<commit_message>
Se actualiza hasta los últimos cambios
</commit_message>
<xml_diff>
--- a/Documents/Actividades realizadas/ActividadesN_.xlsx
+++ b/Documents/Actividades realizadas/ActividadesN_.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\VioletaSystem\Documents\Actividades realizadas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64CC2A07-E266-4772-B141-5324CA61F895}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{240C5E9F-C3C0-45AF-A80C-3746677EF770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HORAS" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="295">
   <si>
     <t>Descripción</t>
   </si>
@@ -907,6 +907,18 @@
   </si>
   <si>
     <t>rediseño de inventario fíciso código</t>
+  </si>
+  <si>
+    <t>Agregar sección de cambio de contraseña y de código de autorización</t>
+  </si>
+  <si>
+    <t>Impresión de código de barra de producto</t>
+  </si>
+  <si>
+    <t>Poner quien aprueba las devoluciones</t>
+  </si>
+  <si>
+    <t>Si cambian de tipo de venta a taller y ya tiene algun producto seleccuionado que lo limpie</t>
   </si>
 </sst>
 </file>
@@ -1134,6 +1146,9 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1187,9 +1202,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1507,11 +1519,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K285"/>
+  <dimension ref="A1:K287"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A236" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G242" sqref="G242"/>
+      <selection pane="bottomLeft" activeCell="G244" sqref="G244"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6362,6 +6374,7 @@
     </row>
     <row r="239" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A239" s="5"/>
+      <c r="C239" s="39"/>
       <c r="D239" t="s">
         <v>287</v>
       </c>
@@ -6377,6 +6390,7 @@
     </row>
     <row r="240" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A240" s="5"/>
+      <c r="C240" s="39"/>
       <c r="D240" t="s">
         <v>288</v>
       </c>
@@ -6392,6 +6406,7 @@
     </row>
     <row r="241" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A241" s="5"/>
+      <c r="C241" s="39"/>
       <c r="D241" t="s">
         <v>289</v>
       </c>
@@ -6407,13 +6422,34 @@
     </row>
     <row r="242" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A242" s="5"/>
-      <c r="E242" s="2"/>
-      <c r="F242" s="2"/>
+      <c r="C242" s="39"/>
+      <c r="D242" t="s">
+        <v>291</v>
+      </c>
+      <c r="E242" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F242" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="G242" s="15">
+        <v>3</v>
+      </c>
     </row>
     <row r="243" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A243" s="5"/>
-      <c r="E243" s="2"/>
-      <c r="F243" s="2"/>
+      <c r="D243" t="s">
+        <v>292</v>
+      </c>
+      <c r="E243" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F243" s="2">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="G243" s="15">
+        <v>5</v>
+      </c>
     </row>
     <row r="244" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A244" s="5"/>
@@ -6426,207 +6462,201 @@
       <c r="F245" s="2"/>
     </row>
     <row r="246" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A246" s="43" t="s">
+      <c r="A246" s="5"/>
+      <c r="E246" s="2"/>
+      <c r="F246" s="2"/>
+    </row>
+    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A247" s="5"/>
+      <c r="E247" s="2"/>
+      <c r="F247" s="2"/>
+    </row>
+    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A248" s="44" t="s">
         <v>165</v>
       </c>
-      <c r="B246" s="43"/>
-      <c r="C246" s="43"/>
-      <c r="D246" s="43"/>
-      <c r="E246" s="43"/>
-      <c r="F246" s="43"/>
-      <c r="G246" s="17">
-        <f>SUM(G2:G245)</f>
-        <v>277.78999999999996</v>
-      </c>
-      <c r="H246" s="17">
-        <f>SUM(H2:H245)</f>
+      <c r="B248" s="44"/>
+      <c r="C248" s="44"/>
+      <c r="D248" s="44"/>
+      <c r="E248" s="44"/>
+      <c r="F248" s="44"/>
+      <c r="G248" s="17">
+        <f>SUM(G2:G247)</f>
+        <v>285.78999999999996</v>
+      </c>
+      <c r="H248" s="17">
+        <f>SUM(H2:H247)</f>
         <v>43.8</v>
       </c>
     </row>
-    <row r="247" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A247" s="43" t="s">
+    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A249" s="44" t="s">
         <v>139</v>
       </c>
-      <c r="B247" s="43"/>
-      <c r="C247" s="43"/>
-      <c r="D247" s="43"/>
-      <c r="E247" s="43"/>
-      <c r="F247" s="43"/>
-      <c r="G247" s="17">
+      <c r="B249" s="44"/>
+      <c r="C249" s="44"/>
+      <c r="D249" s="44"/>
+      <c r="E249" s="44"/>
+      <c r="F249" s="44"/>
+      <c r="G249" s="17">
         <v>200</v>
       </c>
-      <c r="H247" s="17">
+      <c r="H249" s="17">
         <v>300</v>
       </c>
     </row>
-    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A248" s="43" t="s">
+    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A250" s="44" t="s">
         <v>166</v>
       </c>
-      <c r="B248" s="43"/>
-      <c r="C248" s="43"/>
-      <c r="D248" s="43"/>
-      <c r="E248" s="43"/>
-      <c r="F248" s="43"/>
-      <c r="G248" s="18">
-        <f>G247*G246</f>
-        <v>55557.999999999993</v>
-      </c>
-      <c r="H248" s="19">
-        <f>H247*H246</f>
+      <c r="B250" s="44"/>
+      <c r="C250" s="44"/>
+      <c r="D250" s="44"/>
+      <c r="E250" s="44"/>
+      <c r="F250" s="44"/>
+      <c r="G250" s="18">
+        <f>G249*G248</f>
+        <v>57157.999999999993</v>
+      </c>
+      <c r="H250" s="19">
+        <f>H249*H248</f>
         <v>13140</v>
       </c>
-      <c r="J248">
+      <c r="J250">
         <v>-500</v>
       </c>
     </row>
-    <row r="249" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A249" s="43" t="s">
+    <row r="251" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A251" s="44" t="s">
         <v>140</v>
       </c>
-      <c r="B249" s="43"/>
-      <c r="C249" s="43"/>
-      <c r="D249" s="43"/>
-      <c r="E249" s="43"/>
-      <c r="F249" s="43"/>
-      <c r="G249" s="48">
-        <f>G248+H248</f>
-        <v>68698</v>
-      </c>
-      <c r="H249" s="48"/>
-    </row>
-    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A250" s="11"/>
-      <c r="B250" s="51" t="s">
+      <c r="B251" s="44"/>
+      <c r="C251" s="44"/>
+      <c r="D251" s="44"/>
+      <c r="E251" s="44"/>
+      <c r="F251" s="44"/>
+      <c r="G251" s="49">
+        <f>G250+H250</f>
+        <v>70298</v>
+      </c>
+      <c r="H251" s="49"/>
+    </row>
+    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A252" s="11"/>
+      <c r="B252" s="52" t="s">
         <v>142</v>
       </c>
-      <c r="C250" s="51"/>
-      <c r="D250" s="51"/>
-      <c r="E250" s="51"/>
-      <c r="F250" s="51"/>
-      <c r="G250" s="22"/>
-    </row>
-    <row r="251" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A251" s="12">
-        <v>45109</v>
-      </c>
-      <c r="B251" s="52" t="s">
-        <v>141</v>
-      </c>
-      <c r="C251" s="52"/>
-      <c r="D251" s="52"/>
-      <c r="E251" s="52"/>
-      <c r="F251" s="52"/>
-      <c r="G251" s="53">
-        <v>10000</v>
-      </c>
-      <c r="H251" s="53"/>
-    </row>
-    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A252" s="12"/>
-      <c r="B252" s="55" t="s">
-        <v>178</v>
-      </c>
-      <c r="C252" s="55"/>
-      <c r="D252" s="55"/>
-      <c r="E252" s="55"/>
-      <c r="F252" s="55"/>
-      <c r="G252" s="53">
-        <v>5000</v>
-      </c>
-      <c r="H252" s="53"/>
+      <c r="C252" s="52"/>
+      <c r="D252" s="52"/>
+      <c r="E252" s="52"/>
+      <c r="F252" s="52"/>
+      <c r="G252" s="22"/>
     </row>
     <row r="253" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A253" s="12">
-        <v>45278</v>
-      </c>
-      <c r="B253" s="44" t="s">
-        <v>178</v>
-      </c>
-      <c r="C253" s="44"/>
-      <c r="D253" s="44"/>
-      <c r="E253" s="44"/>
-      <c r="F253" s="44"/>
-      <c r="G253" s="53">
-        <v>9800</v>
-      </c>
-      <c r="H253" s="53"/>
+        <v>45109</v>
+      </c>
+      <c r="B253" s="53" t="s">
+        <v>141</v>
+      </c>
+      <c r="C253" s="53"/>
+      <c r="D253" s="53"/>
+      <c r="E253" s="53"/>
+      <c r="F253" s="53"/>
+      <c r="G253" s="54">
+        <v>10000</v>
+      </c>
+      <c r="H253" s="54"/>
     </row>
     <row r="254" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A254" s="12"/>
-      <c r="B254" s="44"/>
-      <c r="C254" s="44"/>
-      <c r="D254" s="44"/>
-      <c r="E254" s="44"/>
-      <c r="F254" s="44"/>
-      <c r="G254" s="54"/>
+      <c r="B254" s="56" t="s">
+        <v>178</v>
+      </c>
+      <c r="C254" s="56"/>
+      <c r="D254" s="56"/>
+      <c r="E254" s="56"/>
+      <c r="F254" s="56"/>
+      <c r="G254" s="54">
+        <v>5000</v>
+      </c>
       <c r="H254" s="54"/>
     </row>
     <row r="255" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A255" s="12"/>
-      <c r="B255" s="44"/>
-      <c r="C255" s="44"/>
-      <c r="D255" s="44"/>
-      <c r="E255" s="44"/>
-      <c r="F255" s="44"/>
-      <c r="G255" s="54"/>
+      <c r="A255" s="12">
+        <v>45278</v>
+      </c>
+      <c r="B255" s="45" t="s">
+        <v>178</v>
+      </c>
+      <c r="C255" s="45"/>
+      <c r="D255" s="45"/>
+      <c r="E255" s="45"/>
+      <c r="F255" s="45"/>
+      <c r="G255" s="54">
+        <v>9800</v>
+      </c>
       <c r="H255" s="54"/>
     </row>
     <row r="256" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A256" s="12"/>
-      <c r="B256" s="44"/>
-      <c r="C256" s="44"/>
-      <c r="D256" s="44"/>
-      <c r="E256" s="44"/>
-      <c r="F256" s="44"/>
-      <c r="G256" s="54"/>
-      <c r="H256" s="54"/>
+      <c r="B256" s="45"/>
+      <c r="C256" s="45"/>
+      <c r="D256" s="45"/>
+      <c r="E256" s="45"/>
+      <c r="F256" s="45"/>
+      <c r="G256" s="55"/>
+      <c r="H256" s="55"/>
     </row>
     <row r="257" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A257" s="12"/>
-      <c r="B257" s="44" t="s">
-        <v>144</v>
-      </c>
-      <c r="C257" s="44"/>
-      <c r="D257" s="44"/>
-      <c r="E257" s="44"/>
-      <c r="F257" s="44"/>
-      <c r="G257" s="53">
-        <f>SUM(G251:H256)</f>
-        <v>24800</v>
-      </c>
-      <c r="H257" s="53"/>
-    </row>
-    <row r="258" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A258" s="49" t="s">
-        <v>143</v>
-      </c>
-      <c r="B258" s="49"/>
-      <c r="C258" s="49"/>
-      <c r="D258" s="49"/>
-      <c r="E258" s="49"/>
-      <c r="F258" s="49"/>
-      <c r="G258" s="50">
-        <f>G249-G257</f>
-        <v>43898</v>
-      </c>
-      <c r="H258" s="50"/>
+      <c r="B257" s="45"/>
+      <c r="C257" s="45"/>
+      <c r="D257" s="45"/>
+      <c r="E257" s="45"/>
+      <c r="F257" s="45"/>
+      <c r="G257" s="55"/>
+      <c r="H257" s="55"/>
+    </row>
+    <row r="258" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A258" s="12"/>
+      <c r="B258" s="45"/>
+      <c r="C258" s="45"/>
+      <c r="D258" s="45"/>
+      <c r="E258" s="45"/>
+      <c r="F258" s="45"/>
+      <c r="G258" s="55"/>
+      <c r="H258" s="55"/>
     </row>
     <row r="259" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A259" s="12"/>
-      <c r="B259" s="13"/>
-      <c r="C259" s="13"/>
-      <c r="D259" s="13"/>
-      <c r="E259" s="13"/>
-      <c r="F259" s="13"/>
-    </row>
-    <row r="260" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A260" s="12"/>
-      <c r="B260" s="13"/>
-      <c r="C260" s="13"/>
-      <c r="D260" s="13"/>
-      <c r="E260" s="13"/>
-      <c r="F260" s="13"/>
+      <c r="B259" s="45" t="s">
+        <v>144</v>
+      </c>
+      <c r="C259" s="45"/>
+      <c r="D259" s="45"/>
+      <c r="E259" s="45"/>
+      <c r="F259" s="45"/>
+      <c r="G259" s="54">
+        <f>SUM(G253:H258)</f>
+        <v>24800</v>
+      </c>
+      <c r="H259" s="54"/>
+    </row>
+    <row r="260" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A260" s="50" t="s">
+        <v>143</v>
+      </c>
+      <c r="B260" s="50"/>
+      <c r="C260" s="50"/>
+      <c r="D260" s="50"/>
+      <c r="E260" s="50"/>
+      <c r="F260" s="50"/>
+      <c r="G260" s="51">
+        <f>G251-G259</f>
+        <v>45498</v>
+      </c>
+      <c r="H260" s="51"/>
     </row>
     <row r="261" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A261" s="12"/>
@@ -6757,190 +6787,206 @@
       <c r="F276" s="13"/>
     </row>
     <row r="277" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A277" s="10"/>
-      <c r="B277" s="45" t="s">
+      <c r="A277" s="12"/>
+      <c r="B277" s="13"/>
+      <c r="C277" s="13"/>
+      <c r="D277" s="13"/>
+      <c r="E277" s="13"/>
+      <c r="F277" s="13"/>
+    </row>
+    <row r="278" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A278" s="12"/>
+      <c r="B278" s="13"/>
+      <c r="C278" s="13"/>
+      <c r="D278" s="13"/>
+      <c r="E278" s="13"/>
+      <c r="F278" s="13"/>
+    </row>
+    <row r="279" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A279" s="10"/>
+      <c r="B279" s="46" t="s">
         <v>138</v>
-      </c>
-      <c r="C277" s="45"/>
-      <c r="D277" s="45"/>
-      <c r="E277" s="45"/>
-      <c r="F277" s="45"/>
-      <c r="G277" s="21"/>
-      <c r="H277" s="21"/>
-      <c r="I277" s="8">
-        <f>G246+H246</f>
-        <v>321.58999999999997</v>
-      </c>
-      <c r="J277" s="8">
-        <f>I277</f>
-        <v>321.58999999999997</v>
-      </c>
-    </row>
-    <row r="278" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A278" s="5"/>
-      <c r="B278" s="46" t="s">
-        <v>139</v>
-      </c>
-      <c r="C278" s="46"/>
-      <c r="D278" s="46"/>
-      <c r="E278" s="46"/>
-      <c r="F278" s="46"/>
-      <c r="I278" s="8">
-        <v>300</v>
-      </c>
-      <c r="J278" s="8">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="279" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A279" s="5"/>
-      <c r="B279" s="46" t="s">
-        <v>140</v>
       </c>
       <c r="C279" s="46"/>
       <c r="D279" s="46"/>
       <c r="E279" s="46"/>
       <c r="F279" s="46"/>
-      <c r="I279" s="9">
-        <f>I278*I277</f>
-        <v>96476.999999999985</v>
-      </c>
-      <c r="J279" s="9">
-        <f>J278*J277</f>
-        <v>64317.999999999993</v>
+      <c r="G279" s="21"/>
+      <c r="H279" s="21"/>
+      <c r="I279" s="8">
+        <f>G248+H248</f>
+        <v>329.59</v>
+      </c>
+      <c r="J279" s="8">
+        <f>I279</f>
+        <v>329.59</v>
       </c>
     </row>
     <row r="280" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A280" s="23"/>
+      <c r="A280" s="5"/>
       <c r="B280" s="47" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C280" s="47"/>
       <c r="D280" s="47"/>
       <c r="E280" s="47"/>
       <c r="F280" s="47"/>
-      <c r="G280" s="24"/>
-      <c r="H280" s="24"/>
-      <c r="I280" s="25"/>
-      <c r="J280" s="25"/>
-    </row>
-    <row r="281" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A281" s="26">
+      <c r="I280" s="8">
+        <v>300</v>
+      </c>
+      <c r="J280" s="8">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="281" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A281" s="5"/>
+      <c r="B281" s="47" t="s">
+        <v>140</v>
+      </c>
+      <c r="C281" s="47"/>
+      <c r="D281" s="47"/>
+      <c r="E281" s="47"/>
+      <c r="F281" s="47"/>
+      <c r="I281" s="9">
+        <f>I280*I279</f>
+        <v>98876.999999999985</v>
+      </c>
+      <c r="J281" s="9">
+        <f>J280*J279</f>
+        <v>65918</v>
+      </c>
+    </row>
+    <row r="282" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A282" s="23"/>
+      <c r="B282" s="48" t="s">
+        <v>142</v>
+      </c>
+      <c r="C282" s="48"/>
+      <c r="D282" s="48"/>
+      <c r="E282" s="48"/>
+      <c r="F282" s="48"/>
+      <c r="G282" s="24"/>
+      <c r="H282" s="24"/>
+      <c r="I282" s="25"/>
+      <c r="J282" s="25"/>
+    </row>
+    <row r="283" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A283" s="26">
         <v>45109</v>
       </c>
-      <c r="B281" s="41" t="s">
+      <c r="B283" s="42" t="s">
         <v>141</v>
       </c>
-      <c r="C281" s="41"/>
-      <c r="D281" s="41"/>
-      <c r="E281" s="41"/>
-      <c r="F281" s="41"/>
-      <c r="G281" s="27"/>
-      <c r="H281" s="27"/>
-      <c r="I281" s="28">
-        <v>10000</v>
-      </c>
-      <c r="J281" s="28">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="282" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A282" s="26"/>
-      <c r="B282" s="29"/>
-      <c r="C282" s="29"/>
-      <c r="D282" s="29"/>
-      <c r="E282" s="29"/>
-      <c r="F282" s="29"/>
-      <c r="G282" s="27"/>
-      <c r="H282" s="27"/>
-      <c r="I282" s="30"/>
-      <c r="J282" s="30"/>
-    </row>
-    <row r="283" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A283" s="26"/>
-      <c r="B283" s="29"/>
-      <c r="C283" s="29"/>
-      <c r="D283" s="29"/>
-      <c r="E283" s="29"/>
-      <c r="F283" s="29"/>
+      <c r="C283" s="42"/>
+      <c r="D283" s="42"/>
+      <c r="E283" s="42"/>
+      <c r="F283" s="42"/>
       <c r="G283" s="27"/>
       <c r="H283" s="27"/>
-      <c r="I283" s="30"/>
-      <c r="J283" s="30"/>
-    </row>
-    <row r="284" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="I283" s="28">
+        <v>10000</v>
+      </c>
+      <c r="J283" s="28">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="284" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A284" s="26"/>
-      <c r="B284" s="42" t="s">
-        <v>144</v>
-      </c>
-      <c r="C284" s="42"/>
-      <c r="D284" s="42"/>
-      <c r="E284" s="42"/>
-      <c r="F284" s="42"/>
+      <c r="B284" s="29"/>
+      <c r="C284" s="29"/>
+      <c r="D284" s="29"/>
+      <c r="E284" s="29"/>
+      <c r="F284" s="29"/>
       <c r="G284" s="27"/>
       <c r="H284" s="27"/>
-      <c r="I284" s="31">
-        <f>SUM(I281:I283)</f>
+      <c r="I284" s="30"/>
+      <c r="J284" s="30"/>
+    </row>
+    <row r="285" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A285" s="26"/>
+      <c r="B285" s="29"/>
+      <c r="C285" s="29"/>
+      <c r="D285" s="29"/>
+      <c r="E285" s="29"/>
+      <c r="F285" s="29"/>
+      <c r="G285" s="27"/>
+      <c r="H285" s="27"/>
+      <c r="I285" s="30"/>
+      <c r="J285" s="30"/>
+    </row>
+    <row r="286" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A286" s="26"/>
+      <c r="B286" s="43" t="s">
+        <v>144</v>
+      </c>
+      <c r="C286" s="43"/>
+      <c r="D286" s="43"/>
+      <c r="E286" s="43"/>
+      <c r="F286" s="43"/>
+      <c r="G286" s="27"/>
+      <c r="H286" s="27"/>
+      <c r="I286" s="31">
+        <f>SUM(I283:I285)</f>
         <v>10000</v>
       </c>
-      <c r="J284" s="31">
-        <f>SUM(J281:J283)</f>
+      <c r="J286" s="31">
+        <f>SUM(J283:J285)</f>
         <v>10000</v>
       </c>
     </row>
-    <row r="285" spans="1:10" ht="33.75" x14ac:dyDescent="0.5">
-      <c r="A285" s="32">
+    <row r="287" spans="1:10" ht="33.75" x14ac:dyDescent="0.5">
+      <c r="A287" s="32">
         <v>45109</v>
       </c>
-      <c r="B285" s="40" t="s">
+      <c r="B287" s="41" t="s">
         <v>143</v>
       </c>
-      <c r="C285" s="40"/>
-      <c r="D285" s="40"/>
-      <c r="E285" s="40"/>
-      <c r="F285" s="40"/>
-      <c r="G285" s="33"/>
-      <c r="H285" s="33"/>
-      <c r="I285" s="34">
-        <f>I279-I284</f>
-        <v>86476.999999999985</v>
-      </c>
-      <c r="J285" s="34">
-        <f>J279-J284</f>
-        <v>54317.999999999993</v>
+      <c r="C287" s="41"/>
+      <c r="D287" s="41"/>
+      <c r="E287" s="41"/>
+      <c r="F287" s="41"/>
+      <c r="G287" s="33"/>
+      <c r="H287" s="33"/>
+      <c r="I287" s="34">
+        <f>I281-I286</f>
+        <v>88876.999999999985</v>
+      </c>
+      <c r="J287" s="34">
+        <f>J281-J286</f>
+        <v>55918</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="G249:H249"/>
-    <mergeCell ref="A258:F258"/>
+    <mergeCell ref="G251:H251"/>
+    <mergeCell ref="A260:F260"/>
+    <mergeCell ref="G260:H260"/>
+    <mergeCell ref="B252:F252"/>
+    <mergeCell ref="B253:F253"/>
+    <mergeCell ref="B259:F259"/>
+    <mergeCell ref="G253:H253"/>
+    <mergeCell ref="G254:H254"/>
+    <mergeCell ref="G259:H259"/>
+    <mergeCell ref="G256:H256"/>
+    <mergeCell ref="G257:H257"/>
     <mergeCell ref="G258:H258"/>
-    <mergeCell ref="B250:F250"/>
-    <mergeCell ref="B251:F251"/>
+    <mergeCell ref="G255:H255"/>
+    <mergeCell ref="B255:F255"/>
+    <mergeCell ref="B254:F254"/>
+    <mergeCell ref="B256:F256"/>
+    <mergeCell ref="B287:F287"/>
+    <mergeCell ref="B283:F283"/>
+    <mergeCell ref="B286:F286"/>
+    <mergeCell ref="A249:F249"/>
+    <mergeCell ref="A248:F248"/>
+    <mergeCell ref="A250:F250"/>
+    <mergeCell ref="A251:F251"/>
     <mergeCell ref="B257:F257"/>
-    <mergeCell ref="G251:H251"/>
-    <mergeCell ref="G252:H252"/>
-    <mergeCell ref="G257:H257"/>
-    <mergeCell ref="G254:H254"/>
-    <mergeCell ref="G255:H255"/>
-    <mergeCell ref="G256:H256"/>
-    <mergeCell ref="G253:H253"/>
-    <mergeCell ref="B253:F253"/>
-    <mergeCell ref="B252:F252"/>
-    <mergeCell ref="B254:F254"/>
-    <mergeCell ref="B285:F285"/>
-    <mergeCell ref="B281:F281"/>
-    <mergeCell ref="B284:F284"/>
-    <mergeCell ref="A247:F247"/>
-    <mergeCell ref="A246:F246"/>
-    <mergeCell ref="A248:F248"/>
-    <mergeCell ref="A249:F249"/>
-    <mergeCell ref="B255:F255"/>
-    <mergeCell ref="B256:F256"/>
-    <mergeCell ref="B277:F277"/>
-    <mergeCell ref="B278:F278"/>
+    <mergeCell ref="B258:F258"/>
     <mergeCell ref="B279:F279"/>
     <mergeCell ref="B280:F280"/>
+    <mergeCell ref="B281:F281"/>
+    <mergeCell ref="B282:F282"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -6949,10 +6995,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7248,8 +7294,32 @@
       <c r="C30" t="s">
         <v>290</v>
       </c>
-      <c r="E30" s="58" t="s">
+      <c r="E30" s="40" t="s">
         <v>238</v>
+      </c>
+    </row>
+    <row r="31" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>291</v>
+      </c>
+      <c r="E31" s="36" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="32" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>293</v>
+      </c>
+      <c r="E32" s="37" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="33" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="C33" s="14" t="s">
+        <v>294</v>
+      </c>
+      <c r="E33" s="37" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -7290,12 +7360,12 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="56"/>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -7598,12 +7668,12 @@
       <c r="D30" s="6"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="57" t="s">
+      <c r="A31" s="58" t="s">
         <v>43</v>
       </c>
-      <c r="B31" s="57"/>
-      <c r="C31" s="57"/>
-      <c r="D31" s="57"/>
+      <c r="B31" s="58"/>
+      <c r="C31" s="58"/>
+      <c r="D31" s="58"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
@@ -8232,10 +8302,10 @@
       <c r="D97" s="6"/>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="57"/>
-      <c r="B98" s="57"/>
-      <c r="C98" s="57"/>
-      <c r="D98" s="57"/>
+      <c r="A98" s="58"/>
+      <c r="B98" s="58"/>
+      <c r="C98" s="58"/>
+      <c r="D98" s="58"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Se arregla reimpresión de pagos, y se limpian productos cuando cambian el tipo de venta a taller
</commit_message>
<xml_diff>
--- a/Documents/Actividades realizadas/ActividadesN_.xlsx
+++ b/Documents/Actividades realizadas/ActividadesN_.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\VioletaSystem\Documents\Actividades realizadas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{240C5E9F-C3C0-45AF-A80C-3746677EF770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C52BFC6B-5E35-4B6F-90D9-9E34CC4C86E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HORAS" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="298">
   <si>
     <t>Descripción</t>
   </si>
@@ -918,7 +918,16 @@
     <t>Poner quien aprueba las devoluciones</t>
   </si>
   <si>
-    <t>Si cambian de tipo de venta a taller y ya tiene algun producto seleccuionado que lo limpie</t>
+    <t>Si cambian de tipo de venta a taller y ya tiene algun producto seleccionado que lo limpie</t>
+  </si>
+  <si>
+    <t>Configuración de código de barras en impresora de oficina</t>
+  </si>
+  <si>
+    <t>Modificaciones de impresión de ticket de notas, Corte de Caja, Egresos, Ingresos y pagos</t>
+  </si>
+  <si>
+    <t>Si se cancela una venta que salió de una consignación, dene regresar el producto a la consignación no al inventario</t>
   </si>
 </sst>
 </file>
@@ -1065,7 +1074,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1147,6 +1156,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1519,11 +1531,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K287"/>
+  <dimension ref="A1:K291"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A236" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G244" sqref="G244"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A239" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F249" sqref="F249"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6453,13 +6465,33 @@
     </row>
     <row r="244" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A244" s="5"/>
-      <c r="E244" s="2"/>
-      <c r="F244" s="2"/>
-    </row>
-    <row r="245" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D244" t="s">
+        <v>295</v>
+      </c>
+      <c r="E244" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="F244" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="G244" s="15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="245" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A245" s="5"/>
-      <c r="E245" s="2"/>
-      <c r="F245" s="2"/>
+      <c r="D245" s="14" t="s">
+        <v>296</v>
+      </c>
+      <c r="E245" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="F245" s="2">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="G245" s="15">
+        <v>2</v>
+      </c>
     </row>
     <row r="246" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A246" s="5"/>
@@ -6472,223 +6504,211 @@
       <c r="F247" s="2"/>
     </row>
     <row r="248" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A248" s="44" t="s">
+      <c r="A248" s="5"/>
+      <c r="E248" s="2"/>
+      <c r="F248" s="2"/>
+    </row>
+    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A249" s="5"/>
+      <c r="E249" s="2"/>
+      <c r="F249" s="2"/>
+    </row>
+    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A250" s="5"/>
+      <c r="E250" s="2"/>
+      <c r="F250" s="2"/>
+    </row>
+    <row r="251" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A251" s="5"/>
+      <c r="E251" s="2"/>
+      <c r="F251" s="2"/>
+    </row>
+    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A252" s="45" t="s">
         <v>165</v>
       </c>
-      <c r="B248" s="44"/>
-      <c r="C248" s="44"/>
-      <c r="D248" s="44"/>
-      <c r="E248" s="44"/>
-      <c r="F248" s="44"/>
-      <c r="G248" s="17">
-        <f>SUM(G2:G247)</f>
-        <v>285.78999999999996</v>
-      </c>
-      <c r="H248" s="17">
-        <f>SUM(H2:H247)</f>
+      <c r="B252" s="45"/>
+      <c r="C252" s="45"/>
+      <c r="D252" s="45"/>
+      <c r="E252" s="45"/>
+      <c r="F252" s="45"/>
+      <c r="G252" s="17">
+        <f>SUM(G2:G251)</f>
+        <v>293.78999999999996</v>
+      </c>
+      <c r="H252" s="17">
+        <f>SUM(H2:H251)</f>
         <v>43.8</v>
       </c>
     </row>
-    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A249" s="44" t="s">
+    <row r="253" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A253" s="45" t="s">
         <v>139</v>
       </c>
-      <c r="B249" s="44"/>
-      <c r="C249" s="44"/>
-      <c r="D249" s="44"/>
-      <c r="E249" s="44"/>
-      <c r="F249" s="44"/>
-      <c r="G249" s="17">
+      <c r="B253" s="45"/>
+      <c r="C253" s="45"/>
+      <c r="D253" s="45"/>
+      <c r="E253" s="45"/>
+      <c r="F253" s="45"/>
+      <c r="G253" s="17">
         <v>200</v>
       </c>
-      <c r="H249" s="17">
+      <c r="H253" s="17">
         <v>300</v>
       </c>
     </row>
-    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A250" s="44" t="s">
+    <row r="254" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A254" s="45" t="s">
         <v>166</v>
       </c>
-      <c r="B250" s="44"/>
-      <c r="C250" s="44"/>
-      <c r="D250" s="44"/>
-      <c r="E250" s="44"/>
-      <c r="F250" s="44"/>
-      <c r="G250" s="18">
-        <f>G249*G248</f>
-        <v>57157.999999999993</v>
-      </c>
-      <c r="H250" s="19">
-        <f>H249*H248</f>
+      <c r="B254" s="45"/>
+      <c r="C254" s="45"/>
+      <c r="D254" s="45"/>
+      <c r="E254" s="45"/>
+      <c r="F254" s="45"/>
+      <c r="G254" s="18">
+        <f>G253*G252</f>
+        <v>58757.999999999993</v>
+      </c>
+      <c r="H254" s="19">
+        <f>H253*H252</f>
         <v>13140</v>
       </c>
-      <c r="J250">
+      <c r="J254">
         <v>-500</v>
       </c>
     </row>
-    <row r="251" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A251" s="44" t="s">
+    <row r="255" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A255" s="45" t="s">
         <v>140</v>
       </c>
-      <c r="B251" s="44"/>
-      <c r="C251" s="44"/>
-      <c r="D251" s="44"/>
-      <c r="E251" s="44"/>
-      <c r="F251" s="44"/>
-      <c r="G251" s="49">
-        <f>G250+H250</f>
-        <v>70298</v>
-      </c>
-      <c r="H251" s="49"/>
-    </row>
-    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A252" s="11"/>
-      <c r="B252" s="52" t="s">
-        <v>142</v>
-      </c>
-      <c r="C252" s="52"/>
-      <c r="D252" s="52"/>
-      <c r="E252" s="52"/>
-      <c r="F252" s="52"/>
-      <c r="G252" s="22"/>
-    </row>
-    <row r="253" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A253" s="12">
-        <v>45109</v>
-      </c>
-      <c r="B253" s="53" t="s">
-        <v>141</v>
-      </c>
-      <c r="C253" s="53"/>
-      <c r="D253" s="53"/>
-      <c r="E253" s="53"/>
-      <c r="F253" s="53"/>
-      <c r="G253" s="54">
-        <v>10000</v>
-      </c>
-      <c r="H253" s="54"/>
-    </row>
-    <row r="254" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A254" s="12"/>
-      <c r="B254" s="56" t="s">
-        <v>178</v>
-      </c>
-      <c r="C254" s="56"/>
-      <c r="D254" s="56"/>
-      <c r="E254" s="56"/>
-      <c r="F254" s="56"/>
-      <c r="G254" s="54">
-        <v>5000</v>
-      </c>
-      <c r="H254" s="54"/>
-    </row>
-    <row r="255" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A255" s="12">
-        <v>45278</v>
-      </c>
-      <c r="B255" s="45" t="s">
-        <v>178</v>
-      </c>
+      <c r="B255" s="45"/>
       <c r="C255" s="45"/>
       <c r="D255" s="45"/>
       <c r="E255" s="45"/>
       <c r="F255" s="45"/>
-      <c r="G255" s="54">
-        <v>9800</v>
-      </c>
-      <c r="H255" s="54"/>
+      <c r="G255" s="50">
+        <f>G254+H254</f>
+        <v>71898</v>
+      </c>
+      <c r="H255" s="50"/>
     </row>
     <row r="256" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A256" s="12"/>
-      <c r="B256" s="45"/>
-      <c r="C256" s="45"/>
-      <c r="D256" s="45"/>
-      <c r="E256" s="45"/>
-      <c r="F256" s="45"/>
-      <c r="G256" s="55"/>
-      <c r="H256" s="55"/>
+      <c r="A256" s="11"/>
+      <c r="B256" s="53" t="s">
+        <v>142</v>
+      </c>
+      <c r="C256" s="53"/>
+      <c r="D256" s="53"/>
+      <c r="E256" s="53"/>
+      <c r="F256" s="53"/>
+      <c r="G256" s="22"/>
     </row>
     <row r="257" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A257" s="12"/>
-      <c r="B257" s="45"/>
-      <c r="C257" s="45"/>
-      <c r="D257" s="45"/>
-      <c r="E257" s="45"/>
-      <c r="F257" s="45"/>
-      <c r="G257" s="55"/>
+      <c r="A257" s="12">
+        <v>45109</v>
+      </c>
+      <c r="B257" s="54" t="s">
+        <v>141</v>
+      </c>
+      <c r="C257" s="54"/>
+      <c r="D257" s="54"/>
+      <c r="E257" s="54"/>
+      <c r="F257" s="54"/>
+      <c r="G257" s="55">
+        <v>10000</v>
+      </c>
       <c r="H257" s="55"/>
     </row>
     <row r="258" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A258" s="12"/>
-      <c r="B258" s="45"/>
-      <c r="C258" s="45"/>
-      <c r="D258" s="45"/>
-      <c r="E258" s="45"/>
-      <c r="F258" s="45"/>
-      <c r="G258" s="55"/>
+      <c r="B258" s="57" t="s">
+        <v>178</v>
+      </c>
+      <c r="C258" s="57"/>
+      <c r="D258" s="57"/>
+      <c r="E258" s="57"/>
+      <c r="F258" s="57"/>
+      <c r="G258" s="55">
+        <v>5000</v>
+      </c>
       <c r="H258" s="55"/>
     </row>
     <row r="259" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A259" s="12"/>
-      <c r="B259" s="45" t="s">
-        <v>144</v>
-      </c>
-      <c r="C259" s="45"/>
-      <c r="D259" s="45"/>
-      <c r="E259" s="45"/>
-      <c r="F259" s="45"/>
-      <c r="G259" s="54">
-        <f>SUM(G253:H258)</f>
-        <v>24800</v>
-      </c>
-      <c r="H259" s="54"/>
-    </row>
-    <row r="260" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A260" s="50" t="s">
-        <v>143</v>
-      </c>
-      <c r="B260" s="50"/>
-      <c r="C260" s="50"/>
-      <c r="D260" s="50"/>
-      <c r="E260" s="50"/>
-      <c r="F260" s="50"/>
-      <c r="G260" s="51">
-        <f>G251-G259</f>
-        <v>45498</v>
-      </c>
-      <c r="H260" s="51"/>
+      <c r="A259" s="12">
+        <v>45278</v>
+      </c>
+      <c r="B259" s="46" t="s">
+        <v>178</v>
+      </c>
+      <c r="C259" s="46"/>
+      <c r="D259" s="46"/>
+      <c r="E259" s="46"/>
+      <c r="F259" s="46"/>
+      <c r="G259" s="55">
+        <v>9800</v>
+      </c>
+      <c r="H259" s="55"/>
+    </row>
+    <row r="260" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A260" s="12"/>
+      <c r="B260" s="46"/>
+      <c r="C260" s="46"/>
+      <c r="D260" s="46"/>
+      <c r="E260" s="46"/>
+      <c r="F260" s="46"/>
+      <c r="G260" s="56"/>
+      <c r="H260" s="56"/>
     </row>
     <row r="261" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A261" s="12"/>
-      <c r="B261" s="13"/>
-      <c r="C261" s="13"/>
-      <c r="D261" s="13"/>
-      <c r="E261" s="13"/>
-      <c r="F261" s="13"/>
+      <c r="B261" s="46"/>
+      <c r="C261" s="46"/>
+      <c r="D261" s="46"/>
+      <c r="E261" s="46"/>
+      <c r="F261" s="46"/>
+      <c r="G261" s="56"/>
+      <c r="H261" s="56"/>
     </row>
     <row r="262" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A262" s="12"/>
-      <c r="B262" s="13"/>
-      <c r="C262" s="13"/>
-      <c r="D262" s="13"/>
-      <c r="E262" s="13"/>
-      <c r="F262" s="13"/>
+      <c r="B262" s="46"/>
+      <c r="C262" s="46"/>
+      <c r="D262" s="46"/>
+      <c r="E262" s="46"/>
+      <c r="F262" s="46"/>
+      <c r="G262" s="56"/>
+      <c r="H262" s="56"/>
     </row>
     <row r="263" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A263" s="12"/>
-      <c r="B263" s="13"/>
-      <c r="C263" s="13"/>
-      <c r="D263" s="13"/>
-      <c r="E263" s="13"/>
-      <c r="F263" s="13"/>
-    </row>
-    <row r="264" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A264" s="12"/>
-      <c r="B264" s="13"/>
-      <c r="C264" s="13"/>
-      <c r="D264" s="13"/>
-      <c r="E264" s="13"/>
-      <c r="F264" s="13"/>
+      <c r="B263" s="46" t="s">
+        <v>144</v>
+      </c>
+      <c r="C263" s="46"/>
+      <c r="D263" s="46"/>
+      <c r="E263" s="46"/>
+      <c r="F263" s="46"/>
+      <c r="G263" s="55">
+        <f>SUM(G257:H262)</f>
+        <v>24800</v>
+      </c>
+      <c r="H263" s="55"/>
+    </row>
+    <row r="264" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A264" s="51" t="s">
+        <v>143</v>
+      </c>
+      <c r="B264" s="51"/>
+      <c r="C264" s="51"/>
+      <c r="D264" s="51"/>
+      <c r="E264" s="51"/>
+      <c r="F264" s="51"/>
+      <c r="G264" s="52">
+        <f>G255-G263</f>
+        <v>47098</v>
+      </c>
+      <c r="H264" s="52"/>
     </row>
     <row r="265" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A265" s="12"/>
@@ -6803,190 +6823,222 @@
       <c r="F278" s="13"/>
     </row>
     <row r="279" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A279" s="10"/>
-      <c r="B279" s="46" t="s">
+      <c r="A279" s="12"/>
+      <c r="B279" s="13"/>
+      <c r="C279" s="13"/>
+      <c r="D279" s="13"/>
+      <c r="E279" s="13"/>
+      <c r="F279" s="13"/>
+    </row>
+    <row r="280" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A280" s="12"/>
+      <c r="B280" s="13"/>
+      <c r="C280" s="13"/>
+      <c r="D280" s="13"/>
+      <c r="E280" s="13"/>
+      <c r="F280" s="13"/>
+    </row>
+    <row r="281" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A281" s="12"/>
+      <c r="B281" s="13"/>
+      <c r="C281" s="13"/>
+      <c r="D281" s="13"/>
+      <c r="E281" s="13"/>
+      <c r="F281" s="13"/>
+    </row>
+    <row r="282" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A282" s="12"/>
+      <c r="B282" s="13"/>
+      <c r="C282" s="13"/>
+      <c r="D282" s="13"/>
+      <c r="E282" s="13"/>
+      <c r="F282" s="13"/>
+    </row>
+    <row r="283" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A283" s="10"/>
+      <c r="B283" s="47" t="s">
         <v>138</v>
       </c>
-      <c r="C279" s="46"/>
-      <c r="D279" s="46"/>
-      <c r="E279" s="46"/>
-      <c r="F279" s="46"/>
-      <c r="G279" s="21"/>
-      <c r="H279" s="21"/>
-      <c r="I279" s="8">
-        <f>G248+H248</f>
-        <v>329.59</v>
-      </c>
-      <c r="J279" s="8">
-        <f>I279</f>
-        <v>329.59</v>
-      </c>
-    </row>
-    <row r="280" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A280" s="5"/>
-      <c r="B280" s="47" t="s">
+      <c r="C283" s="47"/>
+      <c r="D283" s="47"/>
+      <c r="E283" s="47"/>
+      <c r="F283" s="47"/>
+      <c r="G283" s="21"/>
+      <c r="H283" s="21"/>
+      <c r="I283" s="8">
+        <f>G252+H252</f>
+        <v>337.59</v>
+      </c>
+      <c r="J283" s="8">
+        <f>I283</f>
+        <v>337.59</v>
+      </c>
+    </row>
+    <row r="284" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A284" s="5"/>
+      <c r="B284" s="48" t="s">
         <v>139</v>
       </c>
-      <c r="C280" s="47"/>
-      <c r="D280" s="47"/>
-      <c r="E280" s="47"/>
-      <c r="F280" s="47"/>
-      <c r="I280" s="8">
+      <c r="C284" s="48"/>
+      <c r="D284" s="48"/>
+      <c r="E284" s="48"/>
+      <c r="F284" s="48"/>
+      <c r="I284" s="8">
         <v>300</v>
       </c>
-      <c r="J280" s="8">
+      <c r="J284" s="8">
         <v>200</v>
       </c>
     </row>
-    <row r="281" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A281" s="5"/>
-      <c r="B281" s="47" t="s">
+    <row r="285" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A285" s="5"/>
+      <c r="B285" s="48" t="s">
         <v>140</v>
       </c>
-      <c r="C281" s="47"/>
-      <c r="D281" s="47"/>
-      <c r="E281" s="47"/>
-      <c r="F281" s="47"/>
-      <c r="I281" s="9">
-        <f>I280*I279</f>
-        <v>98876.999999999985</v>
-      </c>
-      <c r="J281" s="9">
-        <f>J280*J279</f>
-        <v>65918</v>
-      </c>
-    </row>
-    <row r="282" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A282" s="23"/>
-      <c r="B282" s="48" t="s">
+      <c r="C285" s="48"/>
+      <c r="D285" s="48"/>
+      <c r="E285" s="48"/>
+      <c r="F285" s="48"/>
+      <c r="I285" s="9">
+        <f>I284*I283</f>
+        <v>101276.99999999999</v>
+      </c>
+      <c r="J285" s="9">
+        <f>J284*J283</f>
+        <v>67518</v>
+      </c>
+    </row>
+    <row r="286" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A286" s="23"/>
+      <c r="B286" s="49" t="s">
         <v>142</v>
       </c>
-      <c r="C282" s="48"/>
-      <c r="D282" s="48"/>
-      <c r="E282" s="48"/>
-      <c r="F282" s="48"/>
-      <c r="G282" s="24"/>
-      <c r="H282" s="24"/>
-      <c r="I282" s="25"/>
-      <c r="J282" s="25"/>
-    </row>
-    <row r="283" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A283" s="26">
+      <c r="C286" s="49"/>
+      <c r="D286" s="49"/>
+      <c r="E286" s="49"/>
+      <c r="F286" s="49"/>
+      <c r="G286" s="24"/>
+      <c r="H286" s="24"/>
+      <c r="I286" s="25"/>
+      <c r="J286" s="25"/>
+    </row>
+    <row r="287" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A287" s="26">
         <v>45109</v>
       </c>
-      <c r="B283" s="42" t="s">
+      <c r="B287" s="43" t="s">
         <v>141</v>
       </c>
-      <c r="C283" s="42"/>
-      <c r="D283" s="42"/>
-      <c r="E283" s="42"/>
-      <c r="F283" s="42"/>
-      <c r="G283" s="27"/>
-      <c r="H283" s="27"/>
-      <c r="I283" s="28">
+      <c r="C287" s="43"/>
+      <c r="D287" s="43"/>
+      <c r="E287" s="43"/>
+      <c r="F287" s="43"/>
+      <c r="G287" s="27"/>
+      <c r="H287" s="27"/>
+      <c r="I287" s="28">
         <v>10000</v>
       </c>
-      <c r="J283" s="28">
+      <c r="J287" s="28">
         <v>10000</v>
       </c>
     </row>
-    <row r="284" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A284" s="26"/>
-      <c r="B284" s="29"/>
-      <c r="C284" s="29"/>
-      <c r="D284" s="29"/>
-      <c r="E284" s="29"/>
-      <c r="F284" s="29"/>
-      <c r="G284" s="27"/>
-      <c r="H284" s="27"/>
-      <c r="I284" s="30"/>
-      <c r="J284" s="30"/>
-    </row>
-    <row r="285" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A285" s="26"/>
-      <c r="B285" s="29"/>
-      <c r="C285" s="29"/>
-      <c r="D285" s="29"/>
-      <c r="E285" s="29"/>
-      <c r="F285" s="29"/>
-      <c r="G285" s="27"/>
-      <c r="H285" s="27"/>
-      <c r="I285" s="30"/>
-      <c r="J285" s="30"/>
-    </row>
-    <row r="286" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A286" s="26"/>
-      <c r="B286" s="43" t="s">
+    <row r="288" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A288" s="26"/>
+      <c r="B288" s="29"/>
+      <c r="C288" s="29"/>
+      <c r="D288" s="29"/>
+      <c r="E288" s="29"/>
+      <c r="F288" s="29"/>
+      <c r="G288" s="27"/>
+      <c r="H288" s="27"/>
+      <c r="I288" s="30"/>
+      <c r="J288" s="30"/>
+    </row>
+    <row r="289" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A289" s="26"/>
+      <c r="B289" s="29"/>
+      <c r="C289" s="29"/>
+      <c r="D289" s="29"/>
+      <c r="E289" s="29"/>
+      <c r="F289" s="29"/>
+      <c r="G289" s="27"/>
+      <c r="H289" s="27"/>
+      <c r="I289" s="30"/>
+      <c r="J289" s="30"/>
+    </row>
+    <row r="290" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A290" s="26"/>
+      <c r="B290" s="44" t="s">
         <v>144</v>
       </c>
-      <c r="C286" s="43"/>
-      <c r="D286" s="43"/>
-      <c r="E286" s="43"/>
-      <c r="F286" s="43"/>
-      <c r="G286" s="27"/>
-      <c r="H286" s="27"/>
-      <c r="I286" s="31">
-        <f>SUM(I283:I285)</f>
+      <c r="C290" s="44"/>
+      <c r="D290" s="44"/>
+      <c r="E290" s="44"/>
+      <c r="F290" s="44"/>
+      <c r="G290" s="27"/>
+      <c r="H290" s="27"/>
+      <c r="I290" s="31">
+        <f>SUM(I287:I289)</f>
         <v>10000</v>
       </c>
-      <c r="J286" s="31">
-        <f>SUM(J283:J285)</f>
+      <c r="J290" s="31">
+        <f>SUM(J287:J289)</f>
         <v>10000</v>
       </c>
     </row>
-    <row r="287" spans="1:10" ht="33.75" x14ac:dyDescent="0.5">
-      <c r="A287" s="32">
+    <row r="291" spans="1:10" ht="33.75" x14ac:dyDescent="0.5">
+      <c r="A291" s="32">
         <v>45109</v>
       </c>
-      <c r="B287" s="41" t="s">
+      <c r="B291" s="42" t="s">
         <v>143</v>
       </c>
-      <c r="C287" s="41"/>
-      <c r="D287" s="41"/>
-      <c r="E287" s="41"/>
-      <c r="F287" s="41"/>
-      <c r="G287" s="33"/>
-      <c r="H287" s="33"/>
-      <c r="I287" s="34">
-        <f>I281-I286</f>
-        <v>88876.999999999985</v>
-      </c>
-      <c r="J287" s="34">
-        <f>J281-J286</f>
-        <v>55918</v>
+      <c r="C291" s="42"/>
+      <c r="D291" s="42"/>
+      <c r="E291" s="42"/>
+      <c r="F291" s="42"/>
+      <c r="G291" s="33"/>
+      <c r="H291" s="33"/>
+      <c r="I291" s="34">
+        <f>I285-I290</f>
+        <v>91276.999999999985</v>
+      </c>
+      <c r="J291" s="34">
+        <f>J285-J290</f>
+        <v>57518</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="G251:H251"/>
-    <mergeCell ref="A260:F260"/>
-    <mergeCell ref="G260:H260"/>
-    <mergeCell ref="B252:F252"/>
-    <mergeCell ref="B253:F253"/>
-    <mergeCell ref="B259:F259"/>
-    <mergeCell ref="G253:H253"/>
-    <mergeCell ref="G254:H254"/>
-    <mergeCell ref="G259:H259"/>
-    <mergeCell ref="G256:H256"/>
+    <mergeCell ref="G255:H255"/>
+    <mergeCell ref="A264:F264"/>
+    <mergeCell ref="G264:H264"/>
+    <mergeCell ref="B256:F256"/>
+    <mergeCell ref="B257:F257"/>
+    <mergeCell ref="B263:F263"/>
     <mergeCell ref="G257:H257"/>
     <mergeCell ref="G258:H258"/>
-    <mergeCell ref="G255:H255"/>
-    <mergeCell ref="B255:F255"/>
-    <mergeCell ref="B254:F254"/>
-    <mergeCell ref="B256:F256"/>
+    <mergeCell ref="G263:H263"/>
+    <mergeCell ref="G260:H260"/>
+    <mergeCell ref="G261:H261"/>
+    <mergeCell ref="G262:H262"/>
+    <mergeCell ref="G259:H259"/>
+    <mergeCell ref="B259:F259"/>
+    <mergeCell ref="B258:F258"/>
+    <mergeCell ref="B260:F260"/>
+    <mergeCell ref="B291:F291"/>
     <mergeCell ref="B287:F287"/>
+    <mergeCell ref="B290:F290"/>
+    <mergeCell ref="A253:F253"/>
+    <mergeCell ref="A252:F252"/>
+    <mergeCell ref="A254:F254"/>
+    <mergeCell ref="A255:F255"/>
+    <mergeCell ref="B261:F261"/>
+    <mergeCell ref="B262:F262"/>
     <mergeCell ref="B283:F283"/>
+    <mergeCell ref="B284:F284"/>
+    <mergeCell ref="B285:F285"/>
     <mergeCell ref="B286:F286"/>
-    <mergeCell ref="A249:F249"/>
-    <mergeCell ref="A248:F248"/>
-    <mergeCell ref="A250:F250"/>
-    <mergeCell ref="A251:F251"/>
-    <mergeCell ref="B257:F257"/>
-    <mergeCell ref="B258:F258"/>
-    <mergeCell ref="B279:F279"/>
-    <mergeCell ref="B280:F280"/>
-    <mergeCell ref="B281:F281"/>
-    <mergeCell ref="B282:F282"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -6995,10 +7047,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7238,8 +7290,8 @@
       <c r="C23" t="s">
         <v>274</v>
       </c>
-      <c r="E23" s="37" t="s">
-        <v>143</v>
+      <c r="E23" s="36" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="24" spans="3:5" x14ac:dyDescent="0.25">
@@ -7319,6 +7371,14 @@
         <v>294</v>
       </c>
       <c r="E33" s="37" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="34" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="C34" s="14" t="s">
+        <v>297</v>
+      </c>
+      <c r="E34" s="41" t="s">
         <v>143</v>
       </c>
     </row>
@@ -7360,12 +7420,12 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
+      <c r="B2" s="58"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -7668,12 +7728,12 @@
       <c r="D30" s="6"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="58" t="s">
+      <c r="A31" s="59" t="s">
         <v>43</v>
       </c>
-      <c r="B31" s="58"/>
-      <c r="C31" s="58"/>
-      <c r="D31" s="58"/>
+      <c r="B31" s="59"/>
+      <c r="C31" s="59"/>
+      <c r="D31" s="59"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
@@ -8302,10 +8362,10 @@
       <c r="D97" s="6"/>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="58"/>
-      <c r="B98" s="58"/>
-      <c r="C98" s="58"/>
-      <c r="D98" s="58"/>
+      <c r="A98" s="59"/>
+      <c r="B98" s="59"/>
+      <c r="C98" s="59"/>
+      <c r="D98" s="59"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Se agrega reporte de Pagos, y permiso para ver los costos
</commit_message>
<xml_diff>
--- a/Documents/Actividades realizadas/ActividadesN_.xlsx
+++ b/Documents/Actividades realizadas/ActividadesN_.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\VioletaSystem\Documents\Actividades realizadas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1DDBD58-7F07-4893-A465-3059D01ECBD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D92E0B4D-7D4E-4C82-96DB-D14C62F93DEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="303">
   <si>
     <t>Descripción</t>
   </si>
@@ -937,6 +937,12 @@
   </si>
   <si>
     <t>Configuracion de impresora en merceria</t>
+  </si>
+  <si>
+    <t>Reporte de pagos</t>
+  </si>
+  <si>
+    <t>Permiso para poder ver los costos de los productos en el reporte de ventas</t>
   </si>
 </sst>
 </file>
@@ -1170,6 +1176,30 @@
     <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="44" fontId="3" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1185,9 +1215,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1196,27 +1223,6 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1540,11 +1546,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K291"/>
+  <dimension ref="A1:K296"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A239" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H246" sqref="H246"/>
+      <pane ySplit="1" topLeftCell="A236" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D256" sqref="D256"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1552,7 +1558,7 @@
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" customWidth="1"/>
     <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="64.5703125" customWidth="1"/>
+    <col min="4" max="4" width="72.28515625" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="1"/>
     <col min="6" max="6" width="14.7109375" style="1" customWidth="1"/>
     <col min="7" max="8" width="14.7109375" style="15" customWidth="1"/>
@@ -6425,7 +6431,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="241" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A241" s="5"/>
       <c r="C241" s="39"/>
       <c r="D241" t="s">
@@ -6441,7 +6447,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="242" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A242" s="5"/>
       <c r="C242" s="39"/>
       <c r="D242" t="s">
@@ -6457,7 +6463,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="243" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A243" s="5"/>
       <c r="C243" s="39"/>
       <c r="D243" t="s">
@@ -6473,7 +6479,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="244" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A244" s="5"/>
       <c r="C244" s="39"/>
       <c r="D244" t="s">
@@ -6489,7 +6495,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="245" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A245" s="5"/>
       <c r="C245" s="39"/>
       <c r="D245" s="14" t="s">
@@ -6505,8 +6511,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="246" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A246" s="5"/>
+      <c r="C246" s="39"/>
       <c r="D246" t="s">
         <v>298</v>
       </c>
@@ -6520,8 +6527,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="247" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A247" s="5"/>
+      <c r="C247" s="39"/>
       <c r="D247" s="14" t="s">
         <v>299</v>
       </c>
@@ -6535,8 +6543,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="248" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A248" s="5"/>
+      <c r="C248" s="39"/>
       <c r="D248" t="s">
         <v>300</v>
       </c>
@@ -6550,249 +6559,255 @@
         <v>2</v>
       </c>
     </row>
-    <row r="249" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A249" s="5"/>
-      <c r="E249" s="2"/>
-      <c r="F249" s="2"/>
-    </row>
-    <row r="250" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C249" s="39"/>
+      <c r="D249" s="14" t="s">
+        <v>301</v>
+      </c>
+      <c r="E249" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F249" s="2">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="H249" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="250" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A250" s="5"/>
-      <c r="E250" s="2"/>
-      <c r="F250" s="2"/>
-    </row>
-    <row r="251" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D250" t="s">
+        <v>302</v>
+      </c>
+      <c r="E250" s="2">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="F250" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="H250" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="251" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A251" s="5"/>
       <c r="E251" s="2"/>
       <c r="F251" s="2"/>
     </row>
-    <row r="252" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A252" s="54" t="s">
+    <row r="252" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A252" s="5"/>
+      <c r="E252" s="2"/>
+      <c r="F252" s="2"/>
+    </row>
+    <row r="253" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A253" s="5"/>
+      <c r="E253" s="2"/>
+      <c r="F253" s="2"/>
+    </row>
+    <row r="254" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A254" s="5"/>
+      <c r="E254" s="2"/>
+      <c r="F254" s="2"/>
+    </row>
+    <row r="255" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A255" s="5"/>
+      <c r="E255" s="2"/>
+      <c r="F255" s="2"/>
+    </row>
+    <row r="256" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A256" s="5"/>
+      <c r="E256" s="2"/>
+      <c r="F256" s="2"/>
+    </row>
+    <row r="257" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A257" s="45" t="s">
         <v>165</v>
       </c>
-      <c r="B252" s="54"/>
-      <c r="C252" s="54"/>
-      <c r="D252" s="54"/>
-      <c r="E252" s="54"/>
-      <c r="F252" s="54"/>
-      <c r="G252" s="17">
-        <f>SUM(G2:G251)</f>
+      <c r="B257" s="45"/>
+      <c r="C257" s="45"/>
+      <c r="D257" s="45"/>
+      <c r="E257" s="45"/>
+      <c r="F257" s="45"/>
+      <c r="G257" s="17">
+        <f>SUM(G2:G256)</f>
         <v>293.78999999999996</v>
       </c>
-      <c r="H252" s="17">
-        <f>SUM(H2:H251)</f>
-        <v>48.8</v>
-      </c>
-    </row>
-    <row r="253" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A253" s="54" t="s">
+      <c r="H257" s="17">
+        <f>SUM(H2:H256)</f>
+        <v>52.8</v>
+      </c>
+    </row>
+    <row r="258" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A258" s="45" t="s">
         <v>139</v>
       </c>
-      <c r="B253" s="54"/>
-      <c r="C253" s="54"/>
-      <c r="D253" s="54"/>
-      <c r="E253" s="54"/>
-      <c r="F253" s="54"/>
-      <c r="G253" s="17">
+      <c r="B258" s="45"/>
+      <c r="C258" s="45"/>
+      <c r="D258" s="45"/>
+      <c r="E258" s="45"/>
+      <c r="F258" s="45"/>
+      <c r="G258" s="17">
         <v>200</v>
       </c>
-      <c r="H253" s="17">
+      <c r="H258" s="17">
         <v>300</v>
       </c>
     </row>
-    <row r="254" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A254" s="54" t="s">
+    <row r="259" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A259" s="45" t="s">
         <v>166</v>
       </c>
-      <c r="B254" s="54"/>
-      <c r="C254" s="54"/>
-      <c r="D254" s="54"/>
-      <c r="E254" s="54"/>
-      <c r="F254" s="54"/>
-      <c r="G254" s="18">
-        <f>G253*G252</f>
+      <c r="B259" s="45"/>
+      <c r="C259" s="45"/>
+      <c r="D259" s="45"/>
+      <c r="E259" s="45"/>
+      <c r="F259" s="45"/>
+      <c r="G259" s="18">
+        <f>G258*G257</f>
         <v>58757.999999999993</v>
       </c>
-      <c r="H254" s="19">
-        <f>H253*H252</f>
-        <v>14640</v>
-      </c>
-      <c r="J254">
+      <c r="H259" s="19">
+        <f>H258*H257</f>
+        <v>15840</v>
+      </c>
+      <c r="J259">
         <v>-500</v>
       </c>
     </row>
-    <row r="255" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A255" s="54" t="s">
+    <row r="260" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A260" s="45" t="s">
         <v>140</v>
       </c>
-      <c r="B255" s="54"/>
-      <c r="C255" s="54"/>
-      <c r="D255" s="54"/>
-      <c r="E255" s="54"/>
-      <c r="F255" s="54"/>
-      <c r="G255" s="42">
-        <f>G254+H254</f>
-        <v>73398</v>
-      </c>
-      <c r="H255" s="42"/>
-    </row>
-    <row r="256" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A256" s="11"/>
-      <c r="B256" s="45" t="s">
+      <c r="B260" s="45"/>
+      <c r="C260" s="45"/>
+      <c r="D260" s="45"/>
+      <c r="E260" s="45"/>
+      <c r="F260" s="45"/>
+      <c r="G260" s="50">
+        <f>G259+H259</f>
+        <v>74598</v>
+      </c>
+      <c r="H260" s="50"/>
+    </row>
+    <row r="261" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A261" s="11"/>
+      <c r="B261" s="53" t="s">
         <v>142</v>
       </c>
-      <c r="C256" s="45"/>
-      <c r="D256" s="45"/>
-      <c r="E256" s="45"/>
-      <c r="F256" s="45"/>
-      <c r="G256" s="22"/>
-    </row>
-    <row r="257" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A257" s="12">
+      <c r="C261" s="53"/>
+      <c r="D261" s="53"/>
+      <c r="E261" s="53"/>
+      <c r="F261" s="53"/>
+      <c r="G261" s="22"/>
+    </row>
+    <row r="262" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A262" s="12">
         <v>45109</v>
       </c>
-      <c r="B257" s="46" t="s">
+      <c r="B262" s="54" t="s">
         <v>141</v>
       </c>
-      <c r="C257" s="46"/>
-      <c r="D257" s="46"/>
-      <c r="E257" s="46"/>
-      <c r="F257" s="46"/>
-      <c r="G257" s="48">
+      <c r="C262" s="54"/>
+      <c r="D262" s="54"/>
+      <c r="E262" s="54"/>
+      <c r="F262" s="54"/>
+      <c r="G262" s="55">
         <v>10000</v>
       </c>
-      <c r="H257" s="48"/>
-    </row>
-    <row r="258" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A258" s="12"/>
-      <c r="B258" s="50" t="s">
+      <c r="H262" s="55"/>
+    </row>
+    <row r="263" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A263" s="12"/>
+      <c r="B263" s="57" t="s">
         <v>178</v>
       </c>
-      <c r="C258" s="50"/>
-      <c r="D258" s="50"/>
-      <c r="E258" s="50"/>
-      <c r="F258" s="50"/>
-      <c r="G258" s="48">
+      <c r="C263" s="57"/>
+      <c r="D263" s="57"/>
+      <c r="E263" s="57"/>
+      <c r="F263" s="57"/>
+      <c r="G263" s="55">
         <v>5000</v>
       </c>
-      <c r="H258" s="48"/>
-    </row>
-    <row r="259" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A259" s="12">
+      <c r="H263" s="55"/>
+    </row>
+    <row r="264" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A264" s="12">
         <v>45278</v>
       </c>
-      <c r="B259" s="47" t="s">
+      <c r="B264" s="46" t="s">
         <v>178</v>
       </c>
-      <c r="C259" s="47"/>
-      <c r="D259" s="47"/>
-      <c r="E259" s="47"/>
-      <c r="F259" s="47"/>
-      <c r="G259" s="48">
+      <c r="C264" s="46"/>
+      <c r="D264" s="46"/>
+      <c r="E264" s="46"/>
+      <c r="F264" s="46"/>
+      <c r="G264" s="55">
         <v>9800</v>
       </c>
-      <c r="H259" s="48"/>
-    </row>
-    <row r="260" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A260" s="12"/>
-      <c r="B260" s="47"/>
-      <c r="C260" s="47"/>
-      <c r="D260" s="47"/>
-      <c r="E260" s="47"/>
-      <c r="F260" s="47"/>
-      <c r="G260" s="49"/>
-      <c r="H260" s="49"/>
-    </row>
-    <row r="261" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A261" s="12"/>
-      <c r="B261" s="47"/>
-      <c r="C261" s="47"/>
-      <c r="D261" s="47"/>
-      <c r="E261" s="47"/>
-      <c r="F261" s="47"/>
-      <c r="G261" s="49"/>
-      <c r="H261" s="49"/>
-    </row>
-    <row r="262" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A262" s="12"/>
-      <c r="B262" s="47"/>
-      <c r="C262" s="47"/>
-      <c r="D262" s="47"/>
-      <c r="E262" s="47"/>
-      <c r="F262" s="47"/>
-      <c r="G262" s="49"/>
-      <c r="H262" s="49"/>
-    </row>
-    <row r="263" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A263" s="12"/>
-      <c r="B263" s="47" t="s">
+      <c r="H264" s="55"/>
+    </row>
+    <row r="265" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A265" s="12"/>
+      <c r="B265" s="46"/>
+      <c r="C265" s="46"/>
+      <c r="D265" s="46"/>
+      <c r="E265" s="46"/>
+      <c r="F265" s="46"/>
+      <c r="G265" s="56"/>
+      <c r="H265" s="56"/>
+    </row>
+    <row r="266" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A266" s="12"/>
+      <c r="B266" s="46"/>
+      <c r="C266" s="46"/>
+      <c r="D266" s="46"/>
+      <c r="E266" s="46"/>
+      <c r="F266" s="46"/>
+      <c r="G266" s="56"/>
+      <c r="H266" s="56"/>
+    </row>
+    <row r="267" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A267" s="12"/>
+      <c r="B267" s="46"/>
+      <c r="C267" s="46"/>
+      <c r="D267" s="46"/>
+      <c r="E267" s="46"/>
+      <c r="F267" s="46"/>
+      <c r="G267" s="56"/>
+      <c r="H267" s="56"/>
+    </row>
+    <row r="268" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A268" s="12"/>
+      <c r="B268" s="46" t="s">
         <v>144</v>
       </c>
-      <c r="C263" s="47"/>
-      <c r="D263" s="47"/>
-      <c r="E263" s="47"/>
-      <c r="F263" s="47"/>
-      <c r="G263" s="48">
-        <f>SUM(G257:H262)</f>
+      <c r="C268" s="46"/>
+      <c r="D268" s="46"/>
+      <c r="E268" s="46"/>
+      <c r="F268" s="46"/>
+      <c r="G268" s="55">
+        <f>SUM(G262:H267)</f>
         <v>24800</v>
       </c>
-      <c r="H263" s="48"/>
-    </row>
-    <row r="264" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A264" s="43" t="s">
+      <c r="H268" s="55"/>
+    </row>
+    <row r="269" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A269" s="51" t="s">
         <v>143</v>
       </c>
-      <c r="B264" s="43"/>
-      <c r="C264" s="43"/>
-      <c r="D264" s="43"/>
-      <c r="E264" s="43"/>
-      <c r="F264" s="43"/>
-      <c r="G264" s="44">
-        <f>G255-G263</f>
-        <v>48598</v>
-      </c>
-      <c r="H264" s="44"/>
-    </row>
-    <row r="265" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A265" s="12"/>
-      <c r="B265" s="13"/>
-      <c r="C265" s="13"/>
-      <c r="D265" s="13"/>
-      <c r="E265" s="13"/>
-      <c r="F265" s="13"/>
-    </row>
-    <row r="266" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A266" s="12"/>
-      <c r="B266" s="13"/>
-      <c r="C266" s="13"/>
-      <c r="D266" s="13"/>
-      <c r="E266" s="13"/>
-      <c r="F266" s="13"/>
-    </row>
-    <row r="267" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A267" s="12"/>
-      <c r="B267" s="13"/>
-      <c r="C267" s="13"/>
-      <c r="D267" s="13"/>
-      <c r="E267" s="13"/>
-      <c r="F267" s="13"/>
-    </row>
-    <row r="268" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A268" s="12"/>
-      <c r="B268" s="13"/>
-      <c r="C268" s="13"/>
-      <c r="D268" s="13"/>
-      <c r="E268" s="13"/>
-      <c r="F268" s="13"/>
-    </row>
-    <row r="269" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A269" s="12"/>
-      <c r="B269" s="13"/>
-      <c r="C269" s="13"/>
-      <c r="D269" s="13"/>
-      <c r="E269" s="13"/>
-      <c r="F269" s="13"/>
-    </row>
-    <row r="270" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B269" s="51"/>
+      <c r="C269" s="51"/>
+      <c r="D269" s="51"/>
+      <c r="E269" s="51"/>
+      <c r="F269" s="51"/>
+      <c r="G269" s="52">
+        <f>G260-G268</f>
+        <v>49798</v>
+      </c>
+      <c r="H269" s="52"/>
+    </row>
+    <row r="270" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A270" s="12"/>
       <c r="B270" s="13"/>
       <c r="C270" s="13"/>
@@ -6800,7 +6815,7 @@
       <c r="E270" s="13"/>
       <c r="F270" s="13"/>
     </row>
-    <row r="271" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A271" s="12"/>
       <c r="B271" s="13"/>
       <c r="C271" s="13"/>
@@ -6808,7 +6823,7 @@
       <c r="E271" s="13"/>
       <c r="F271" s="13"/>
     </row>
-    <row r="272" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A272" s="12"/>
       <c r="B272" s="13"/>
       <c r="C272" s="13"/>
@@ -6897,190 +6912,230 @@
       <c r="F282" s="13"/>
     </row>
     <row r="283" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A283" s="10"/>
-      <c r="B283" s="55" t="s">
+      <c r="A283" s="12"/>
+      <c r="B283" s="13"/>
+      <c r="C283" s="13"/>
+      <c r="D283" s="13"/>
+      <c r="E283" s="13"/>
+      <c r="F283" s="13"/>
+    </row>
+    <row r="284" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A284" s="12"/>
+      <c r="B284" s="13"/>
+      <c r="C284" s="13"/>
+      <c r="D284" s="13"/>
+      <c r="E284" s="13"/>
+      <c r="F284" s="13"/>
+    </row>
+    <row r="285" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A285" s="12"/>
+      <c r="B285" s="13"/>
+      <c r="C285" s="13"/>
+      <c r="D285" s="13"/>
+      <c r="E285" s="13"/>
+      <c r="F285" s="13"/>
+    </row>
+    <row r="286" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A286" s="12"/>
+      <c r="B286" s="13"/>
+      <c r="C286" s="13"/>
+      <c r="D286" s="13"/>
+      <c r="E286" s="13"/>
+      <c r="F286" s="13"/>
+    </row>
+    <row r="287" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A287" s="12"/>
+      <c r="B287" s="13"/>
+      <c r="C287" s="13"/>
+      <c r="D287" s="13"/>
+      <c r="E287" s="13"/>
+      <c r="F287" s="13"/>
+    </row>
+    <row r="288" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A288" s="10"/>
+      <c r="B288" s="47" t="s">
         <v>138</v>
       </c>
-      <c r="C283" s="55"/>
-      <c r="D283" s="55"/>
-      <c r="E283" s="55"/>
-      <c r="F283" s="55"/>
-      <c r="G283" s="21"/>
-      <c r="H283" s="21"/>
-      <c r="I283" s="8">
-        <f>G252+H252</f>
-        <v>342.59</v>
-      </c>
-      <c r="J283" s="8">
-        <f>I283</f>
-        <v>342.59</v>
-      </c>
-    </row>
-    <row r="284" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A284" s="5"/>
-      <c r="B284" s="56" t="s">
+      <c r="C288" s="47"/>
+      <c r="D288" s="47"/>
+      <c r="E288" s="47"/>
+      <c r="F288" s="47"/>
+      <c r="G288" s="21"/>
+      <c r="H288" s="21"/>
+      <c r="I288" s="8">
+        <f>G257+H257</f>
+        <v>346.59</v>
+      </c>
+      <c r="J288" s="8">
+        <f>I288</f>
+        <v>346.59</v>
+      </c>
+    </row>
+    <row r="289" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A289" s="5"/>
+      <c r="B289" s="48" t="s">
         <v>139</v>
       </c>
-      <c r="C284" s="56"/>
-      <c r="D284" s="56"/>
-      <c r="E284" s="56"/>
-      <c r="F284" s="56"/>
-      <c r="I284" s="8">
+      <c r="C289" s="48"/>
+      <c r="D289" s="48"/>
+      <c r="E289" s="48"/>
+      <c r="F289" s="48"/>
+      <c r="I289" s="8">
         <v>300</v>
       </c>
-      <c r="J284" s="8">
+      <c r="J289" s="8">
         <v>200</v>
       </c>
     </row>
-    <row r="285" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A285" s="5"/>
-      <c r="B285" s="56" t="s">
+    <row r="290" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A290" s="5"/>
+      <c r="B290" s="48" t="s">
         <v>140</v>
       </c>
-      <c r="C285" s="56"/>
-      <c r="D285" s="56"/>
-      <c r="E285" s="56"/>
-      <c r="F285" s="56"/>
-      <c r="I285" s="9">
-        <f>I284*I283</f>
-        <v>102776.99999999999</v>
-      </c>
-      <c r="J285" s="9">
-        <f>J284*J283</f>
-        <v>68518</v>
-      </c>
-    </row>
-    <row r="286" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A286" s="23"/>
-      <c r="B286" s="57" t="s">
+      <c r="C290" s="48"/>
+      <c r="D290" s="48"/>
+      <c r="E290" s="48"/>
+      <c r="F290" s="48"/>
+      <c r="I290" s="9">
+        <f>I289*I288</f>
+        <v>103976.99999999999</v>
+      </c>
+      <c r="J290" s="9">
+        <f>J289*J288</f>
+        <v>69318</v>
+      </c>
+    </row>
+    <row r="291" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A291" s="23"/>
+      <c r="B291" s="49" t="s">
         <v>142</v>
       </c>
-      <c r="C286" s="57"/>
-      <c r="D286" s="57"/>
-      <c r="E286" s="57"/>
-      <c r="F286" s="57"/>
-      <c r="G286" s="24"/>
-      <c r="H286" s="24"/>
-      <c r="I286" s="25"/>
-      <c r="J286" s="25"/>
-    </row>
-    <row r="287" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A287" s="26">
+      <c r="C291" s="49"/>
+      <c r="D291" s="49"/>
+      <c r="E291" s="49"/>
+      <c r="F291" s="49"/>
+      <c r="G291" s="24"/>
+      <c r="H291" s="24"/>
+      <c r="I291" s="25"/>
+      <c r="J291" s="25"/>
+    </row>
+    <row r="292" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A292" s="26">
         <v>45109</v>
       </c>
-      <c r="B287" s="52" t="s">
+      <c r="B292" s="43" t="s">
         <v>141</v>
       </c>
-      <c r="C287" s="52"/>
-      <c r="D287" s="52"/>
-      <c r="E287" s="52"/>
-      <c r="F287" s="52"/>
-      <c r="G287" s="27"/>
-      <c r="H287" s="27"/>
-      <c r="I287" s="28">
+      <c r="C292" s="43"/>
+      <c r="D292" s="43"/>
+      <c r="E292" s="43"/>
+      <c r="F292" s="43"/>
+      <c r="G292" s="27"/>
+      <c r="H292" s="27"/>
+      <c r="I292" s="28">
         <v>10000</v>
       </c>
-      <c r="J287" s="28">
+      <c r="J292" s="28">
         <v>10000</v>
       </c>
     </row>
-    <row r="288" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A288" s="26"/>
-      <c r="B288" s="29"/>
-      <c r="C288" s="29"/>
-      <c r="D288" s="29"/>
-      <c r="E288" s="29"/>
-      <c r="F288" s="29"/>
-      <c r="G288" s="27"/>
-      <c r="H288" s="27"/>
-      <c r="I288" s="30"/>
-      <c r="J288" s="30"/>
-    </row>
-    <row r="289" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A289" s="26"/>
-      <c r="B289" s="29"/>
-      <c r="C289" s="29"/>
-      <c r="D289" s="29"/>
-      <c r="E289" s="29"/>
-      <c r="F289" s="29"/>
-      <c r="G289" s="27"/>
-      <c r="H289" s="27"/>
-      <c r="I289" s="30"/>
-      <c r="J289" s="30"/>
-    </row>
-    <row r="290" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A290" s="26"/>
-      <c r="B290" s="53" t="s">
+    <row r="293" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A293" s="26"/>
+      <c r="B293" s="29"/>
+      <c r="C293" s="29"/>
+      <c r="D293" s="29"/>
+      <c r="E293" s="29"/>
+      <c r="F293" s="29"/>
+      <c r="G293" s="27"/>
+      <c r="H293" s="27"/>
+      <c r="I293" s="30"/>
+      <c r="J293" s="30"/>
+    </row>
+    <row r="294" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A294" s="26"/>
+      <c r="B294" s="29"/>
+      <c r="C294" s="29"/>
+      <c r="D294" s="29"/>
+      <c r="E294" s="29"/>
+      <c r="F294" s="29"/>
+      <c r="G294" s="27"/>
+      <c r="H294" s="27"/>
+      <c r="I294" s="30"/>
+      <c r="J294" s="30"/>
+    </row>
+    <row r="295" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A295" s="26"/>
+      <c r="B295" s="44" t="s">
         <v>144</v>
       </c>
-      <c r="C290" s="53"/>
-      <c r="D290" s="53"/>
-      <c r="E290" s="53"/>
-      <c r="F290" s="53"/>
-      <c r="G290" s="27"/>
-      <c r="H290" s="27"/>
-      <c r="I290" s="31">
-        <f>SUM(I287:I289)</f>
+      <c r="C295" s="44"/>
+      <c r="D295" s="44"/>
+      <c r="E295" s="44"/>
+      <c r="F295" s="44"/>
+      <c r="G295" s="27"/>
+      <c r="H295" s="27"/>
+      <c r="I295" s="31">
+        <f>SUM(I292:I294)</f>
         <v>10000</v>
       </c>
-      <c r="J290" s="31">
-        <f>SUM(J287:J289)</f>
+      <c r="J295" s="31">
+        <f>SUM(J292:J294)</f>
         <v>10000</v>
       </c>
     </row>
-    <row r="291" spans="1:10" ht="33.75" x14ac:dyDescent="0.5">
-      <c r="A291" s="32">
+    <row r="296" spans="1:10" ht="33.75" x14ac:dyDescent="0.5">
+      <c r="A296" s="32">
         <v>45109</v>
       </c>
-      <c r="B291" s="51" t="s">
+      <c r="B296" s="42" t="s">
         <v>143</v>
       </c>
-      <c r="C291" s="51"/>
-      <c r="D291" s="51"/>
-      <c r="E291" s="51"/>
-      <c r="F291" s="51"/>
-      <c r="G291" s="33"/>
-      <c r="H291" s="33"/>
-      <c r="I291" s="34">
-        <f>I285-I290</f>
-        <v>92776.999999999985</v>
-      </c>
-      <c r="J291" s="34">
-        <f>J285-J290</f>
-        <v>58518</v>
+      <c r="C296" s="42"/>
+      <c r="D296" s="42"/>
+      <c r="E296" s="42"/>
+      <c r="F296" s="42"/>
+      <c r="G296" s="33"/>
+      <c r="H296" s="33"/>
+      <c r="I296" s="34">
+        <f>I290-I295</f>
+        <v>93976.999999999985</v>
+      </c>
+      <c r="J296" s="34">
+        <f>J290-J295</f>
+        <v>59318</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="B291:F291"/>
-    <mergeCell ref="B287:F287"/>
-    <mergeCell ref="B290:F290"/>
-    <mergeCell ref="A253:F253"/>
-    <mergeCell ref="A252:F252"/>
-    <mergeCell ref="A254:F254"/>
-    <mergeCell ref="A255:F255"/>
+    <mergeCell ref="G260:H260"/>
+    <mergeCell ref="A269:F269"/>
+    <mergeCell ref="G269:H269"/>
     <mergeCell ref="B261:F261"/>
     <mergeCell ref="B262:F262"/>
-    <mergeCell ref="B283:F283"/>
-    <mergeCell ref="B284:F284"/>
-    <mergeCell ref="B285:F285"/>
-    <mergeCell ref="B286:F286"/>
-    <mergeCell ref="G255:H255"/>
-    <mergeCell ref="A264:F264"/>
+    <mergeCell ref="B268:F268"/>
+    <mergeCell ref="G262:H262"/>
+    <mergeCell ref="G263:H263"/>
+    <mergeCell ref="G268:H268"/>
+    <mergeCell ref="G265:H265"/>
+    <mergeCell ref="G266:H266"/>
+    <mergeCell ref="G267:H267"/>
     <mergeCell ref="G264:H264"/>
-    <mergeCell ref="B256:F256"/>
-    <mergeCell ref="B257:F257"/>
+    <mergeCell ref="B264:F264"/>
     <mergeCell ref="B263:F263"/>
-    <mergeCell ref="G257:H257"/>
-    <mergeCell ref="G258:H258"/>
-    <mergeCell ref="G263:H263"/>
-    <mergeCell ref="G260:H260"/>
-    <mergeCell ref="G261:H261"/>
-    <mergeCell ref="G262:H262"/>
-    <mergeCell ref="G259:H259"/>
-    <mergeCell ref="B259:F259"/>
-    <mergeCell ref="B258:F258"/>
-    <mergeCell ref="B260:F260"/>
+    <mergeCell ref="B265:F265"/>
+    <mergeCell ref="B296:F296"/>
+    <mergeCell ref="B292:F292"/>
+    <mergeCell ref="B295:F295"/>
+    <mergeCell ref="A258:F258"/>
+    <mergeCell ref="A257:F257"/>
+    <mergeCell ref="A259:F259"/>
+    <mergeCell ref="A260:F260"/>
+    <mergeCell ref="B266:F266"/>
+    <mergeCell ref="B267:F267"/>
+    <mergeCell ref="B288:F288"/>
+    <mergeCell ref="B289:F289"/>
+    <mergeCell ref="B290:F290"/>
+    <mergeCell ref="B291:F291"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Se actualizan cambios antes de hacer cambios en la BD
</commit_message>
<xml_diff>
--- a/Documents/Actividades realizadas/ActividadesN_.xlsx
+++ b/Documents/Actividades realizadas/ActividadesN_.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\VioletaSystem\Documents\Actividades realizadas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2E75748-2456-46A7-ADE1-818375607F3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C16D57A-46F7-4A29-9EC7-94804E6C5B9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HORAS" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="311">
   <si>
     <t>Descripción</t>
   </si>
@@ -964,6 +964,9 @@
   </si>
   <si>
     <t>Agregar fecha de entrega/recibido</t>
+  </si>
+  <si>
+    <t>Modificar el ticket de taller y la nota de taller para agregar la fecha de Entrega</t>
   </si>
 </sst>
 </file>
@@ -1197,6 +1200,30 @@
     <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="44" fontId="3" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1212,9 +1239,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1223,27 +1247,6 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1569,9 +1572,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K301"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A242" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G258" sqref="G258"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A247" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D257" sqref="D257:D258"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6717,8 +6720,18 @@
     </row>
     <row r="258" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A258" s="5"/>
-      <c r="E258" s="2"/>
-      <c r="F258" s="2"/>
+      <c r="D258" t="s">
+        <v>310</v>
+      </c>
+      <c r="E258" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="F258" s="2">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="G258" s="15">
+        <v>2</v>
+      </c>
     </row>
     <row r="259" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A259" s="5"/>
@@ -6736,17 +6749,17 @@
       <c r="F261" s="2"/>
     </row>
     <row r="262" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A262" s="54" t="s">
+      <c r="A262" s="45" t="s">
         <v>165</v>
       </c>
-      <c r="B262" s="54"/>
-      <c r="C262" s="54"/>
-      <c r="D262" s="54"/>
-      <c r="E262" s="54"/>
-      <c r="F262" s="54"/>
+      <c r="B262" s="45"/>
+      <c r="C262" s="45"/>
+      <c r="D262" s="45"/>
+      <c r="E262" s="45"/>
+      <c r="F262" s="45"/>
       <c r="G262" s="17">
         <f>SUM(G2:G261)</f>
-        <v>306.78999999999996</v>
+        <v>308.78999999999996</v>
       </c>
       <c r="H262" s="17">
         <f>SUM(H2:H261)</f>
@@ -6754,14 +6767,14 @@
       </c>
     </row>
     <row r="263" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A263" s="54" t="s">
+      <c r="A263" s="45" t="s">
         <v>139</v>
       </c>
-      <c r="B263" s="54"/>
-      <c r="C263" s="54"/>
-      <c r="D263" s="54"/>
-      <c r="E263" s="54"/>
-      <c r="F263" s="54"/>
+      <c r="B263" s="45"/>
+      <c r="C263" s="45"/>
+      <c r="D263" s="45"/>
+      <c r="E263" s="45"/>
+      <c r="F263" s="45"/>
       <c r="G263" s="17">
         <v>200</v>
       </c>
@@ -6770,17 +6783,17 @@
       </c>
     </row>
     <row r="264" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A264" s="54" t="s">
+      <c r="A264" s="45" t="s">
         <v>166</v>
       </c>
-      <c r="B264" s="54"/>
-      <c r="C264" s="54"/>
-      <c r="D264" s="54"/>
-      <c r="E264" s="54"/>
-      <c r="F264" s="54"/>
+      <c r="B264" s="45"/>
+      <c r="C264" s="45"/>
+      <c r="D264" s="45"/>
+      <c r="E264" s="45"/>
+      <c r="F264" s="45"/>
       <c r="G264" s="18">
         <f>G263*G262</f>
-        <v>61357.999999999993</v>
+        <v>61757.999999999993</v>
       </c>
       <c r="H264" s="19">
         <f>H263*H262</f>
@@ -6791,136 +6804,136 @@
       </c>
     </row>
     <row r="265" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A265" s="54" t="s">
+      <c r="A265" s="45" t="s">
         <v>140</v>
       </c>
-      <c r="B265" s="54"/>
-      <c r="C265" s="54"/>
-      <c r="D265" s="54"/>
-      <c r="E265" s="54"/>
-      <c r="F265" s="54"/>
-      <c r="G265" s="42">
+      <c r="B265" s="45"/>
+      <c r="C265" s="45"/>
+      <c r="D265" s="45"/>
+      <c r="E265" s="45"/>
+      <c r="F265" s="45"/>
+      <c r="G265" s="50">
         <f>G264+H264</f>
-        <v>77198</v>
-      </c>
-      <c r="H265" s="42"/>
+        <v>77598</v>
+      </c>
+      <c r="H265" s="50"/>
     </row>
     <row r="266" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A266" s="11"/>
-      <c r="B266" s="45" t="s">
+      <c r="B266" s="53" t="s">
         <v>142</v>
       </c>
-      <c r="C266" s="45"/>
-      <c r="D266" s="45"/>
-      <c r="E266" s="45"/>
-      <c r="F266" s="45"/>
+      <c r="C266" s="53"/>
+      <c r="D266" s="53"/>
+      <c r="E266" s="53"/>
+      <c r="F266" s="53"/>
       <c r="G266" s="22"/>
     </row>
     <row r="267" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A267" s="12">
         <v>45109</v>
       </c>
-      <c r="B267" s="46" t="s">
+      <c r="B267" s="54" t="s">
         <v>141</v>
       </c>
-      <c r="C267" s="46"/>
-      <c r="D267" s="46"/>
-      <c r="E267" s="46"/>
-      <c r="F267" s="46"/>
-      <c r="G267" s="48">
+      <c r="C267" s="54"/>
+      <c r="D267" s="54"/>
+      <c r="E267" s="54"/>
+      <c r="F267" s="54"/>
+      <c r="G267" s="55">
         <v>10000</v>
       </c>
-      <c r="H267" s="48"/>
+      <c r="H267" s="55"/>
     </row>
     <row r="268" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A268" s="12"/>
-      <c r="B268" s="50" t="s">
+      <c r="B268" s="57" t="s">
         <v>178</v>
       </c>
-      <c r="C268" s="50"/>
-      <c r="D268" s="50"/>
-      <c r="E268" s="50"/>
-      <c r="F268" s="50"/>
-      <c r="G268" s="48">
+      <c r="C268" s="57"/>
+      <c r="D268" s="57"/>
+      <c r="E268" s="57"/>
+      <c r="F268" s="57"/>
+      <c r="G268" s="55">
         <v>5000</v>
       </c>
-      <c r="H268" s="48"/>
+      <c r="H268" s="55"/>
     </row>
     <row r="269" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A269" s="12">
         <v>45278</v>
       </c>
-      <c r="B269" s="47" t="s">
+      <c r="B269" s="46" t="s">
         <v>178</v>
       </c>
-      <c r="C269" s="47"/>
-      <c r="D269" s="47"/>
-      <c r="E269" s="47"/>
-      <c r="F269" s="47"/>
-      <c r="G269" s="48">
+      <c r="C269" s="46"/>
+      <c r="D269" s="46"/>
+      <c r="E269" s="46"/>
+      <c r="F269" s="46"/>
+      <c r="G269" s="55">
         <v>9800</v>
       </c>
-      <c r="H269" s="48"/>
+      <c r="H269" s="55"/>
     </row>
     <row r="270" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A270" s="12"/>
-      <c r="B270" s="47"/>
-      <c r="C270" s="47"/>
-      <c r="D270" s="47"/>
-      <c r="E270" s="47"/>
-      <c r="F270" s="47"/>
-      <c r="G270" s="49"/>
-      <c r="H270" s="49"/>
+      <c r="B270" s="46"/>
+      <c r="C270" s="46"/>
+      <c r="D270" s="46"/>
+      <c r="E270" s="46"/>
+      <c r="F270" s="46"/>
+      <c r="G270" s="56"/>
+      <c r="H270" s="56"/>
     </row>
     <row r="271" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A271" s="12"/>
-      <c r="B271" s="47"/>
-      <c r="C271" s="47"/>
-      <c r="D271" s="47"/>
-      <c r="E271" s="47"/>
-      <c r="F271" s="47"/>
-      <c r="G271" s="49"/>
-      <c r="H271" s="49"/>
+      <c r="B271" s="46"/>
+      <c r="C271" s="46"/>
+      <c r="D271" s="46"/>
+      <c r="E271" s="46"/>
+      <c r="F271" s="46"/>
+      <c r="G271" s="56"/>
+      <c r="H271" s="56"/>
     </row>
     <row r="272" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A272" s="12"/>
-      <c r="B272" s="47"/>
-      <c r="C272" s="47"/>
-      <c r="D272" s="47"/>
-      <c r="E272" s="47"/>
-      <c r="F272" s="47"/>
-      <c r="G272" s="49"/>
-      <c r="H272" s="49"/>
+      <c r="B272" s="46"/>
+      <c r="C272" s="46"/>
+      <c r="D272" s="46"/>
+      <c r="E272" s="46"/>
+      <c r="F272" s="46"/>
+      <c r="G272" s="56"/>
+      <c r="H272" s="56"/>
     </row>
     <row r="273" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A273" s="12"/>
-      <c r="B273" s="47" t="s">
+      <c r="B273" s="46" t="s">
         <v>144</v>
       </c>
-      <c r="C273" s="47"/>
-      <c r="D273" s="47"/>
-      <c r="E273" s="47"/>
-      <c r="F273" s="47"/>
-      <c r="G273" s="48">
+      <c r="C273" s="46"/>
+      <c r="D273" s="46"/>
+      <c r="E273" s="46"/>
+      <c r="F273" s="46"/>
+      <c r="G273" s="55">
         <f>SUM(G267:H272)</f>
         <v>24800</v>
       </c>
-      <c r="H273" s="48"/>
+      <c r="H273" s="55"/>
     </row>
     <row r="274" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A274" s="43" t="s">
+      <c r="A274" s="51" t="s">
         <v>143</v>
       </c>
-      <c r="B274" s="43"/>
-      <c r="C274" s="43"/>
-      <c r="D274" s="43"/>
-      <c r="E274" s="43"/>
-      <c r="F274" s="43"/>
-      <c r="G274" s="44">
+      <c r="B274" s="51"/>
+      <c r="C274" s="51"/>
+      <c r="D274" s="51"/>
+      <c r="E274" s="51"/>
+      <c r="F274" s="51"/>
+      <c r="G274" s="52">
         <f>G265-G273</f>
-        <v>52398</v>
-      </c>
-      <c r="H274" s="44"/>
+        <v>52798</v>
+      </c>
+      <c r="H274" s="52"/>
     </row>
     <row r="275" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A275" s="12"/>
@@ -7068,33 +7081,33 @@
     </row>
     <row r="293" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A293" s="10"/>
-      <c r="B293" s="55" t="s">
+      <c r="B293" s="47" t="s">
         <v>138</v>
       </c>
-      <c r="C293" s="55"/>
-      <c r="D293" s="55"/>
-      <c r="E293" s="55"/>
-      <c r="F293" s="55"/>
+      <c r="C293" s="47"/>
+      <c r="D293" s="47"/>
+      <c r="E293" s="47"/>
+      <c r="F293" s="47"/>
       <c r="G293" s="21"/>
       <c r="H293" s="21"/>
       <c r="I293" s="8">
         <f>G262+H262</f>
-        <v>359.59</v>
+        <v>361.59</v>
       </c>
       <c r="J293" s="8">
         <f>I293</f>
-        <v>359.59</v>
+        <v>361.59</v>
       </c>
     </row>
     <row r="294" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A294" s="5"/>
-      <c r="B294" s="56" t="s">
+      <c r="B294" s="48" t="s">
         <v>139</v>
       </c>
-      <c r="C294" s="56"/>
-      <c r="D294" s="56"/>
-      <c r="E294" s="56"/>
-      <c r="F294" s="56"/>
+      <c r="C294" s="48"/>
+      <c r="D294" s="48"/>
+      <c r="E294" s="48"/>
+      <c r="F294" s="48"/>
       <c r="I294" s="8">
         <v>300</v>
       </c>
@@ -7104,31 +7117,31 @@
     </row>
     <row r="295" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A295" s="5"/>
-      <c r="B295" s="56" t="s">
+      <c r="B295" s="48" t="s">
         <v>140</v>
       </c>
-      <c r="C295" s="56"/>
-      <c r="D295" s="56"/>
-      <c r="E295" s="56"/>
-      <c r="F295" s="56"/>
+      <c r="C295" s="48"/>
+      <c r="D295" s="48"/>
+      <c r="E295" s="48"/>
+      <c r="F295" s="48"/>
       <c r="I295" s="9">
         <f>I294*I293</f>
-        <v>107876.99999999999</v>
+        <v>108476.99999999999</v>
       </c>
       <c r="J295" s="9">
         <f>J294*J293</f>
-        <v>71918</v>
+        <v>72318</v>
       </c>
     </row>
     <row r="296" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A296" s="23"/>
-      <c r="B296" s="57" t="s">
+      <c r="B296" s="49" t="s">
         <v>142</v>
       </c>
-      <c r="C296" s="57"/>
-      <c r="D296" s="57"/>
-      <c r="E296" s="57"/>
-      <c r="F296" s="57"/>
+      <c r="C296" s="49"/>
+      <c r="D296" s="49"/>
+      <c r="E296" s="49"/>
+      <c r="F296" s="49"/>
       <c r="G296" s="24"/>
       <c r="H296" s="24"/>
       <c r="I296" s="25"/>
@@ -7138,13 +7151,13 @@
       <c r="A297" s="26">
         <v>45109</v>
       </c>
-      <c r="B297" s="52" t="s">
+      <c r="B297" s="43" t="s">
         <v>141</v>
       </c>
-      <c r="C297" s="52"/>
-      <c r="D297" s="52"/>
-      <c r="E297" s="52"/>
-      <c r="F297" s="52"/>
+      <c r="C297" s="43"/>
+      <c r="D297" s="43"/>
+      <c r="E297" s="43"/>
+      <c r="F297" s="43"/>
       <c r="G297" s="27"/>
       <c r="H297" s="27"/>
       <c r="I297" s="28">
@@ -7180,13 +7193,13 @@
     </row>
     <row r="300" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A300" s="26"/>
-      <c r="B300" s="53" t="s">
+      <c r="B300" s="44" t="s">
         <v>144</v>
       </c>
-      <c r="C300" s="53"/>
-      <c r="D300" s="53"/>
-      <c r="E300" s="53"/>
-      <c r="F300" s="53"/>
+      <c r="C300" s="44"/>
+      <c r="D300" s="44"/>
+      <c r="E300" s="44"/>
+      <c r="F300" s="44"/>
       <c r="G300" s="27"/>
       <c r="H300" s="27"/>
       <c r="I300" s="31">
@@ -7202,39 +7215,26 @@
       <c r="A301" s="32">
         <v>45109</v>
       </c>
-      <c r="B301" s="51" t="s">
+      <c r="B301" s="42" t="s">
         <v>143</v>
       </c>
-      <c r="C301" s="51"/>
-      <c r="D301" s="51"/>
-      <c r="E301" s="51"/>
-      <c r="F301" s="51"/>
+      <c r="C301" s="42"/>
+      <c r="D301" s="42"/>
+      <c r="E301" s="42"/>
+      <c r="F301" s="42"/>
       <c r="G301" s="33"/>
       <c r="H301" s="33"/>
       <c r="I301" s="34">
         <f>I295-I300</f>
-        <v>97876.999999999985</v>
+        <v>98476.999999999985</v>
       </c>
       <c r="J301" s="34">
         <f>J295-J300</f>
-        <v>61918</v>
+        <v>62318</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="B301:F301"/>
-    <mergeCell ref="B297:F297"/>
-    <mergeCell ref="B300:F300"/>
-    <mergeCell ref="A263:F263"/>
-    <mergeCell ref="A262:F262"/>
-    <mergeCell ref="A264:F264"/>
-    <mergeCell ref="A265:F265"/>
-    <mergeCell ref="B271:F271"/>
-    <mergeCell ref="B272:F272"/>
-    <mergeCell ref="B293:F293"/>
-    <mergeCell ref="B294:F294"/>
-    <mergeCell ref="B295:F295"/>
-    <mergeCell ref="B296:F296"/>
     <mergeCell ref="G265:H265"/>
     <mergeCell ref="A274:F274"/>
     <mergeCell ref="G274:H274"/>
@@ -7251,6 +7251,19 @@
     <mergeCell ref="B269:F269"/>
     <mergeCell ref="B268:F268"/>
     <mergeCell ref="B270:F270"/>
+    <mergeCell ref="B301:F301"/>
+    <mergeCell ref="B297:F297"/>
+    <mergeCell ref="B300:F300"/>
+    <mergeCell ref="A263:F263"/>
+    <mergeCell ref="A262:F262"/>
+    <mergeCell ref="A264:F264"/>
+    <mergeCell ref="A265:F265"/>
+    <mergeCell ref="B271:F271"/>
+    <mergeCell ref="B272:F272"/>
+    <mergeCell ref="B293:F293"/>
+    <mergeCell ref="B294:F294"/>
+    <mergeCell ref="B295:F295"/>
+    <mergeCell ref="B296:F296"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Cambio en historial de abonos
</commit_message>
<xml_diff>
--- a/Documents/Actividades realizadas/ActividadesN_.xlsx
+++ b/Documents/Actividades realizadas/ActividadesN_.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\VioletaSystem\Documents\Actividades realizadas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E530D103-CB49-4B27-B1BA-EE88F1E57F14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DD075BD-5B2F-4D8E-936B-92AC9A16C134}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HORAS" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="313">
   <si>
     <t>Descripción</t>
   </si>
@@ -970,6 +970,9 @@
   </si>
   <si>
     <t>Se soluciona la incidencia de Ids del detalle de las ventas y de el hostorial de consignación</t>
+  </si>
+  <si>
+    <t>Soporte con los Ids de los productos</t>
   </si>
 </sst>
 </file>
@@ -1203,6 +1206,30 @@
     <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="44" fontId="3" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1218,9 +1245,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1229,27 +1253,6 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1573,11 +1576,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K302"/>
+  <dimension ref="A1:K304"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A247" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G260" sqref="G260"/>
+      <pane ySplit="1" topLeftCell="A253" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D262" sqref="D262"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6708,6 +6711,7 @@
     </row>
     <row r="257" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A257" s="5"/>
+      <c r="C257" s="39"/>
       <c r="D257" s="14" t="s">
         <v>309</v>
       </c>
@@ -6723,6 +6727,7 @@
     </row>
     <row r="258" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A258" s="5"/>
+      <c r="C258" s="39"/>
       <c r="D258" t="s">
         <v>310</v>
       </c>
@@ -6753,11 +6758,22 @@
     </row>
     <row r="260" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A260" s="5"/>
-      <c r="E260" s="2"/>
-      <c r="F260" s="2"/>
+      <c r="D260" s="14" t="s">
+        <v>312</v>
+      </c>
+      <c r="E260" s="2">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="F260" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="H260" s="15">
+        <v>2</v>
+      </c>
     </row>
     <row r="261" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A261" s="5"/>
+      <c r="D261" s="14"/>
       <c r="E261" s="2"/>
       <c r="F261" s="2"/>
     </row>
@@ -6767,207 +6783,201 @@
       <c r="F262" s="2"/>
     </row>
     <row r="263" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A263" s="54" t="s">
+      <c r="A263" s="5"/>
+      <c r="E263" s="2"/>
+      <c r="F263" s="2"/>
+    </row>
+    <row r="264" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A264" s="5"/>
+      <c r="E264" s="2"/>
+      <c r="F264" s="2"/>
+    </row>
+    <row r="265" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A265" s="45" t="s">
         <v>165</v>
       </c>
-      <c r="B263" s="54"/>
-      <c r="C263" s="54"/>
-      <c r="D263" s="54"/>
-      <c r="E263" s="54"/>
-      <c r="F263" s="54"/>
-      <c r="G263" s="17">
-        <f>SUM(G2:G262)</f>
+      <c r="B265" s="45"/>
+      <c r="C265" s="45"/>
+      <c r="D265" s="45"/>
+      <c r="E265" s="45"/>
+      <c r="F265" s="45"/>
+      <c r="G265" s="17">
+        <f>SUM(G2:G264)</f>
         <v>310.78999999999996</v>
       </c>
-      <c r="H263" s="17">
-        <f>SUM(H2:H262)</f>
-        <v>52.8</v>
-      </c>
-    </row>
-    <row r="264" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A264" s="54" t="s">
+      <c r="H265" s="17">
+        <f>SUM(H2:H264)</f>
+        <v>54.8</v>
+      </c>
+    </row>
+    <row r="266" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A266" s="45" t="s">
         <v>139</v>
       </c>
-      <c r="B264" s="54"/>
-      <c r="C264" s="54"/>
-      <c r="D264" s="54"/>
-      <c r="E264" s="54"/>
-      <c r="F264" s="54"/>
-      <c r="G264" s="17">
+      <c r="B266" s="45"/>
+      <c r="C266" s="45"/>
+      <c r="D266" s="45"/>
+      <c r="E266" s="45"/>
+      <c r="F266" s="45"/>
+      <c r="G266" s="17">
         <v>200</v>
       </c>
-      <c r="H264" s="17">
+      <c r="H266" s="17">
         <v>300</v>
       </c>
     </row>
-    <row r="265" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A265" s="54" t="s">
+    <row r="267" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A267" s="45" t="s">
         <v>166</v>
       </c>
-      <c r="B265" s="54"/>
-      <c r="C265" s="54"/>
-      <c r="D265" s="54"/>
-      <c r="E265" s="54"/>
-      <c r="F265" s="54"/>
-      <c r="G265" s="18">
-        <f>G264*G263</f>
-        <v>62157.999999999993</v>
-      </c>
-      <c r="H265" s="19">
-        <f>H264*H263</f>
-        <v>15840</v>
-      </c>
-      <c r="J265">
-        <v>-500</v>
-      </c>
-    </row>
-    <row r="266" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A266" s="54" t="s">
-        <v>140</v>
-      </c>
-      <c r="B266" s="54"/>
-      <c r="C266" s="54"/>
-      <c r="D266" s="54"/>
-      <c r="E266" s="54"/>
-      <c r="F266" s="54"/>
-      <c r="G266" s="42">
-        <f>G265+H265</f>
-        <v>77998</v>
-      </c>
-      <c r="H266" s="42"/>
-    </row>
-    <row r="267" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A267" s="11"/>
-      <c r="B267" s="45" t="s">
-        <v>142</v>
-      </c>
+      <c r="B267" s="45"/>
       <c r="C267" s="45"/>
       <c r="D267" s="45"/>
       <c r="E267" s="45"/>
       <c r="F267" s="45"/>
-      <c r="G267" s="22"/>
-    </row>
-    <row r="268" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A268" s="12">
-        <v>45109</v>
-      </c>
-      <c r="B268" s="46" t="s">
-        <v>141</v>
-      </c>
-      <c r="C268" s="46"/>
-      <c r="D268" s="46"/>
-      <c r="E268" s="46"/>
-      <c r="F268" s="46"/>
-      <c r="G268" s="48">
-        <v>10000</v>
-      </c>
-      <c r="H268" s="48"/>
+      <c r="G267" s="18">
+        <f>G266*G265</f>
+        <v>62157.999999999993</v>
+      </c>
+      <c r="H267" s="19">
+        <f>H266*H265</f>
+        <v>16440</v>
+      </c>
+      <c r="J267">
+        <v>-500</v>
+      </c>
+    </row>
+    <row r="268" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A268" s="45" t="s">
+        <v>140</v>
+      </c>
+      <c r="B268" s="45"/>
+      <c r="C268" s="45"/>
+      <c r="D268" s="45"/>
+      <c r="E268" s="45"/>
+      <c r="F268" s="45"/>
+      <c r="G268" s="50">
+        <f>G267+H267</f>
+        <v>78598</v>
+      </c>
+      <c r="H268" s="50"/>
     </row>
     <row r="269" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A269" s="12"/>
-      <c r="B269" s="50" t="s">
-        <v>178</v>
-      </c>
-      <c r="C269" s="50"/>
-      <c r="D269" s="50"/>
-      <c r="E269" s="50"/>
-      <c r="F269" s="50"/>
-      <c r="G269" s="48">
-        <v>5000</v>
-      </c>
-      <c r="H269" s="48"/>
+      <c r="A269" s="11"/>
+      <c r="B269" s="53" t="s">
+        <v>142</v>
+      </c>
+      <c r="C269" s="53"/>
+      <c r="D269" s="53"/>
+      <c r="E269" s="53"/>
+      <c r="F269" s="53"/>
+      <c r="G269" s="22"/>
     </row>
     <row r="270" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A270" s="12">
-        <v>45278</v>
-      </c>
-      <c r="B270" s="47" t="s">
-        <v>178</v>
-      </c>
-      <c r="C270" s="47"/>
-      <c r="D270" s="47"/>
-      <c r="E270" s="47"/>
-      <c r="F270" s="47"/>
-      <c r="G270" s="48">
-        <v>9800</v>
-      </c>
-      <c r="H270" s="48"/>
+        <v>45109</v>
+      </c>
+      <c r="B270" s="54" t="s">
+        <v>141</v>
+      </c>
+      <c r="C270" s="54"/>
+      <c r="D270" s="54"/>
+      <c r="E270" s="54"/>
+      <c r="F270" s="54"/>
+      <c r="G270" s="55">
+        <v>10000</v>
+      </c>
+      <c r="H270" s="55"/>
     </row>
     <row r="271" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A271" s="12"/>
-      <c r="B271" s="47"/>
-      <c r="C271" s="47"/>
-      <c r="D271" s="47"/>
-      <c r="E271" s="47"/>
-      <c r="F271" s="47"/>
-      <c r="G271" s="49"/>
-      <c r="H271" s="49"/>
+      <c r="B271" s="57" t="s">
+        <v>178</v>
+      </c>
+      <c r="C271" s="57"/>
+      <c r="D271" s="57"/>
+      <c r="E271" s="57"/>
+      <c r="F271" s="57"/>
+      <c r="G271" s="55">
+        <v>5000</v>
+      </c>
+      <c r="H271" s="55"/>
     </row>
     <row r="272" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A272" s="12"/>
-      <c r="B272" s="47"/>
-      <c r="C272" s="47"/>
-      <c r="D272" s="47"/>
-      <c r="E272" s="47"/>
-      <c r="F272" s="47"/>
-      <c r="G272" s="49"/>
-      <c r="H272" s="49"/>
+      <c r="A272" s="12">
+        <v>45278</v>
+      </c>
+      <c r="B272" s="46" t="s">
+        <v>178</v>
+      </c>
+      <c r="C272" s="46"/>
+      <c r="D272" s="46"/>
+      <c r="E272" s="46"/>
+      <c r="F272" s="46"/>
+      <c r="G272" s="55">
+        <v>9800</v>
+      </c>
+      <c r="H272" s="55"/>
     </row>
     <row r="273" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A273" s="12"/>
-      <c r="B273" s="47"/>
-      <c r="C273" s="47"/>
-      <c r="D273" s="47"/>
-      <c r="E273" s="47"/>
-      <c r="F273" s="47"/>
-      <c r="G273" s="49"/>
-      <c r="H273" s="49"/>
+      <c r="B273" s="46"/>
+      <c r="C273" s="46"/>
+      <c r="D273" s="46"/>
+      <c r="E273" s="46"/>
+      <c r="F273" s="46"/>
+      <c r="G273" s="56"/>
+      <c r="H273" s="56"/>
     </row>
     <row r="274" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A274" s="12"/>
-      <c r="B274" s="47" t="s">
-        <v>144</v>
-      </c>
-      <c r="C274" s="47"/>
-      <c r="D274" s="47"/>
-      <c r="E274" s="47"/>
-      <c r="F274" s="47"/>
-      <c r="G274" s="48">
-        <f>SUM(G268:H273)</f>
-        <v>24800</v>
-      </c>
-      <c r="H274" s="48"/>
-    </row>
-    <row r="275" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A275" s="43" t="s">
-        <v>143</v>
-      </c>
-      <c r="B275" s="43"/>
-      <c r="C275" s="43"/>
-      <c r="D275" s="43"/>
-      <c r="E275" s="43"/>
-      <c r="F275" s="43"/>
-      <c r="G275" s="44">
-        <f>G266-G274</f>
-        <v>53198</v>
-      </c>
-      <c r="H275" s="44"/>
+      <c r="B274" s="46"/>
+      <c r="C274" s="46"/>
+      <c r="D274" s="46"/>
+      <c r="E274" s="46"/>
+      <c r="F274" s="46"/>
+      <c r="G274" s="56"/>
+      <c r="H274" s="56"/>
+    </row>
+    <row r="275" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A275" s="12"/>
+      <c r="B275" s="46"/>
+      <c r="C275" s="46"/>
+      <c r="D275" s="46"/>
+      <c r="E275" s="46"/>
+      <c r="F275" s="46"/>
+      <c r="G275" s="56"/>
+      <c r="H275" s="56"/>
     </row>
     <row r="276" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A276" s="12"/>
-      <c r="B276" s="13"/>
-      <c r="C276" s="13"/>
-      <c r="D276" s="13"/>
-      <c r="E276" s="13"/>
-      <c r="F276" s="13"/>
-    </row>
-    <row r="277" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A277" s="12"/>
-      <c r="B277" s="13"/>
-      <c r="C277" s="13"/>
-      <c r="D277" s="13"/>
-      <c r="E277" s="13"/>
-      <c r="F277" s="13"/>
+      <c r="B276" s="46" t="s">
+        <v>144</v>
+      </c>
+      <c r="C276" s="46"/>
+      <c r="D276" s="46"/>
+      <c r="E276" s="46"/>
+      <c r="F276" s="46"/>
+      <c r="G276" s="55">
+        <f>SUM(G270:H275)</f>
+        <v>24800</v>
+      </c>
+      <c r="H276" s="55"/>
+    </row>
+    <row r="277" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A277" s="51" t="s">
+        <v>143</v>
+      </c>
+      <c r="B277" s="51"/>
+      <c r="C277" s="51"/>
+      <c r="D277" s="51"/>
+      <c r="E277" s="51"/>
+      <c r="F277" s="51"/>
+      <c r="G277" s="52">
+        <f>G268-G276</f>
+        <v>53798</v>
+      </c>
+      <c r="H277" s="52"/>
     </row>
     <row r="278" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A278" s="12"/>
@@ -7098,190 +7108,206 @@
       <c r="F293" s="13"/>
     </row>
     <row r="294" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A294" s="10"/>
-      <c r="B294" s="55" t="s">
+      <c r="A294" s="12"/>
+      <c r="B294" s="13"/>
+      <c r="C294" s="13"/>
+      <c r="D294" s="13"/>
+      <c r="E294" s="13"/>
+      <c r="F294" s="13"/>
+    </row>
+    <row r="295" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A295" s="12"/>
+      <c r="B295" s="13"/>
+      <c r="C295" s="13"/>
+      <c r="D295" s="13"/>
+      <c r="E295" s="13"/>
+      <c r="F295" s="13"/>
+    </row>
+    <row r="296" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A296" s="10"/>
+      <c r="B296" s="47" t="s">
         <v>138</v>
       </c>
-      <c r="C294" s="55"/>
-      <c r="D294" s="55"/>
-      <c r="E294" s="55"/>
-      <c r="F294" s="55"/>
-      <c r="G294" s="21"/>
-      <c r="H294" s="21"/>
-      <c r="I294" s="8">
-        <f>G263+H263</f>
-        <v>363.59</v>
-      </c>
-      <c r="J294" s="8">
-        <f>I294</f>
-        <v>363.59</v>
-      </c>
-    </row>
-    <row r="295" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A295" s="5"/>
-      <c r="B295" s="56" t="s">
+      <c r="C296" s="47"/>
+      <c r="D296" s="47"/>
+      <c r="E296" s="47"/>
+      <c r="F296" s="47"/>
+      <c r="G296" s="21"/>
+      <c r="H296" s="21"/>
+      <c r="I296" s="8">
+        <f>G265+H265</f>
+        <v>365.59</v>
+      </c>
+      <c r="J296" s="8">
+        <f>I296</f>
+        <v>365.59</v>
+      </c>
+    </row>
+    <row r="297" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A297" s="5"/>
+      <c r="B297" s="48" t="s">
         <v>139</v>
       </c>
-      <c r="C295" s="56"/>
-      <c r="D295" s="56"/>
-      <c r="E295" s="56"/>
-      <c r="F295" s="56"/>
-      <c r="I295" s="8">
+      <c r="C297" s="48"/>
+      <c r="D297" s="48"/>
+      <c r="E297" s="48"/>
+      <c r="F297" s="48"/>
+      <c r="I297" s="8">
         <v>300</v>
       </c>
-      <c r="J295" s="8">
+      <c r="J297" s="8">
         <v>200</v>
       </c>
     </row>
-    <row r="296" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A296" s="5"/>
-      <c r="B296" s="56" t="s">
+    <row r="298" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A298" s="5"/>
+      <c r="B298" s="48" t="s">
         <v>140</v>
       </c>
-      <c r="C296" s="56"/>
-      <c r="D296" s="56"/>
-      <c r="E296" s="56"/>
-      <c r="F296" s="56"/>
-      <c r="I296" s="9">
-        <f>I295*I294</f>
-        <v>109076.99999999999</v>
-      </c>
-      <c r="J296" s="9">
-        <f>J295*J294</f>
-        <v>72718</v>
-      </c>
-    </row>
-    <row r="297" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A297" s="23"/>
-      <c r="B297" s="57" t="s">
+      <c r="C298" s="48"/>
+      <c r="D298" s="48"/>
+      <c r="E298" s="48"/>
+      <c r="F298" s="48"/>
+      <c r="I298" s="9">
+        <f>I297*I296</f>
+        <v>109676.99999999999</v>
+      </c>
+      <c r="J298" s="9">
+        <f>J297*J296</f>
+        <v>73118</v>
+      </c>
+    </row>
+    <row r="299" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A299" s="23"/>
+      <c r="B299" s="49" t="s">
         <v>142</v>
       </c>
-      <c r="C297" s="57"/>
-      <c r="D297" s="57"/>
-      <c r="E297" s="57"/>
-      <c r="F297" s="57"/>
-      <c r="G297" s="24"/>
-      <c r="H297" s="24"/>
-      <c r="I297" s="25"/>
-      <c r="J297" s="25"/>
-    </row>
-    <row r="298" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A298" s="26">
+      <c r="C299" s="49"/>
+      <c r="D299" s="49"/>
+      <c r="E299" s="49"/>
+      <c r="F299" s="49"/>
+      <c r="G299" s="24"/>
+      <c r="H299" s="24"/>
+      <c r="I299" s="25"/>
+      <c r="J299" s="25"/>
+    </row>
+    <row r="300" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A300" s="26">
         <v>45109</v>
       </c>
-      <c r="B298" s="52" t="s">
+      <c r="B300" s="43" t="s">
         <v>141</v>
       </c>
-      <c r="C298" s="52"/>
-      <c r="D298" s="52"/>
-      <c r="E298" s="52"/>
-      <c r="F298" s="52"/>
-      <c r="G298" s="27"/>
-      <c r="H298" s="27"/>
-      <c r="I298" s="28">
-        <v>10000</v>
-      </c>
-      <c r="J298" s="28">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="299" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A299" s="26"/>
-      <c r="B299" s="29"/>
-      <c r="C299" s="29"/>
-      <c r="D299" s="29"/>
-      <c r="E299" s="29"/>
-      <c r="F299" s="29"/>
-      <c r="G299" s="27"/>
-      <c r="H299" s="27"/>
-      <c r="I299" s="30"/>
-      <c r="J299" s="30"/>
-    </row>
-    <row r="300" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A300" s="26"/>
-      <c r="B300" s="29"/>
-      <c r="C300" s="29"/>
-      <c r="D300" s="29"/>
-      <c r="E300" s="29"/>
-      <c r="F300" s="29"/>
+      <c r="C300" s="43"/>
+      <c r="D300" s="43"/>
+      <c r="E300" s="43"/>
+      <c r="F300" s="43"/>
       <c r="G300" s="27"/>
       <c r="H300" s="27"/>
-      <c r="I300" s="30"/>
-      <c r="J300" s="30"/>
-    </row>
-    <row r="301" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="I300" s="28">
+        <v>10000</v>
+      </c>
+      <c r="J300" s="28">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="301" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A301" s="26"/>
-      <c r="B301" s="53" t="s">
-        <v>144</v>
-      </c>
-      <c r="C301" s="53"/>
-      <c r="D301" s="53"/>
-      <c r="E301" s="53"/>
-      <c r="F301" s="53"/>
+      <c r="B301" s="29"/>
+      <c r="C301" s="29"/>
+      <c r="D301" s="29"/>
+      <c r="E301" s="29"/>
+      <c r="F301" s="29"/>
       <c r="G301" s="27"/>
       <c r="H301" s="27"/>
-      <c r="I301" s="31">
-        <f>SUM(I298:I300)</f>
+      <c r="I301" s="30"/>
+      <c r="J301" s="30"/>
+    </row>
+    <row r="302" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A302" s="26"/>
+      <c r="B302" s="29"/>
+      <c r="C302" s="29"/>
+      <c r="D302" s="29"/>
+      <c r="E302" s="29"/>
+      <c r="F302" s="29"/>
+      <c r="G302" s="27"/>
+      <c r="H302" s="27"/>
+      <c r="I302" s="30"/>
+      <c r="J302" s="30"/>
+    </row>
+    <row r="303" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A303" s="26"/>
+      <c r="B303" s="44" t="s">
+        <v>144</v>
+      </c>
+      <c r="C303" s="44"/>
+      <c r="D303" s="44"/>
+      <c r="E303" s="44"/>
+      <c r="F303" s="44"/>
+      <c r="G303" s="27"/>
+      <c r="H303" s="27"/>
+      <c r="I303" s="31">
+        <f>SUM(I300:I302)</f>
         <v>10000</v>
       </c>
-      <c r="J301" s="31">
-        <f>SUM(J298:J300)</f>
+      <c r="J303" s="31">
+        <f>SUM(J300:J302)</f>
         <v>10000</v>
       </c>
     </row>
-    <row r="302" spans="1:10" ht="33.75" x14ac:dyDescent="0.5">
-      <c r="A302" s="32">
+    <row r="304" spans="1:10" ht="33.75" x14ac:dyDescent="0.5">
+      <c r="A304" s="32">
         <v>45109</v>
       </c>
-      <c r="B302" s="51" t="s">
+      <c r="B304" s="42" t="s">
         <v>143</v>
       </c>
-      <c r="C302" s="51"/>
-      <c r="D302" s="51"/>
-      <c r="E302" s="51"/>
-      <c r="F302" s="51"/>
-      <c r="G302" s="33"/>
-      <c r="H302" s="33"/>
-      <c r="I302" s="34">
-        <f>I296-I301</f>
-        <v>99076.999999999985</v>
-      </c>
-      <c r="J302" s="34">
-        <f>J296-J301</f>
-        <v>62718</v>
+      <c r="C304" s="42"/>
+      <c r="D304" s="42"/>
+      <c r="E304" s="42"/>
+      <c r="F304" s="42"/>
+      <c r="G304" s="33"/>
+      <c r="H304" s="33"/>
+      <c r="I304" s="34">
+        <f>I298-I303</f>
+        <v>99676.999999999985</v>
+      </c>
+      <c r="J304" s="34">
+        <f>J298-J303</f>
+        <v>63118</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="B302:F302"/>
-    <mergeCell ref="B298:F298"/>
-    <mergeCell ref="B301:F301"/>
-    <mergeCell ref="A264:F264"/>
-    <mergeCell ref="A263:F263"/>
+    <mergeCell ref="G268:H268"/>
+    <mergeCell ref="A277:F277"/>
+    <mergeCell ref="G277:H277"/>
+    <mergeCell ref="B269:F269"/>
+    <mergeCell ref="B270:F270"/>
+    <mergeCell ref="B276:F276"/>
+    <mergeCell ref="G270:H270"/>
+    <mergeCell ref="G271:H271"/>
+    <mergeCell ref="G276:H276"/>
+    <mergeCell ref="G273:H273"/>
+    <mergeCell ref="G274:H274"/>
+    <mergeCell ref="G275:H275"/>
+    <mergeCell ref="G272:H272"/>
+    <mergeCell ref="B272:F272"/>
+    <mergeCell ref="B271:F271"/>
+    <mergeCell ref="B273:F273"/>
+    <mergeCell ref="B304:F304"/>
+    <mergeCell ref="B300:F300"/>
+    <mergeCell ref="B303:F303"/>
+    <mergeCell ref="A266:F266"/>
     <mergeCell ref="A265:F265"/>
-    <mergeCell ref="A266:F266"/>
-    <mergeCell ref="B272:F272"/>
-    <mergeCell ref="B273:F273"/>
-    <mergeCell ref="B294:F294"/>
-    <mergeCell ref="B295:F295"/>
+    <mergeCell ref="A267:F267"/>
+    <mergeCell ref="A268:F268"/>
+    <mergeCell ref="B274:F274"/>
+    <mergeCell ref="B275:F275"/>
     <mergeCell ref="B296:F296"/>
     <mergeCell ref="B297:F297"/>
-    <mergeCell ref="G266:H266"/>
-    <mergeCell ref="A275:F275"/>
-    <mergeCell ref="G275:H275"/>
-    <mergeCell ref="B267:F267"/>
-    <mergeCell ref="B268:F268"/>
-    <mergeCell ref="B274:F274"/>
-    <mergeCell ref="G268:H268"/>
-    <mergeCell ref="G269:H269"/>
-    <mergeCell ref="G274:H274"/>
-    <mergeCell ref="G271:H271"/>
-    <mergeCell ref="G272:H272"/>
-    <mergeCell ref="G273:H273"/>
-    <mergeCell ref="G270:H270"/>
-    <mergeCell ref="B270:F270"/>
-    <mergeCell ref="B269:F269"/>
-    <mergeCell ref="B271:F271"/>
+    <mergeCell ref="B298:F298"/>
+    <mergeCell ref="B299:F299"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Se agregan los siguientes camibios
1.- Se soluciona la incidencia de Ids del detalle de las ventas y de el hostorial de consignación
2.- Soporte con los Ids de los productos
3.- Revisión y ajuste de Sarita enbase a violeta
4.- Revisión de los Ids de las comisiones
5.- Cancelación de devoluciones
6.- Sección de finanzas con el reporte de información financiera
7.- Graficación en reporte de información financiera y código de barras de producto en ticket
</commit_message>
<xml_diff>
--- a/Documents/Actividades realizadas/ActividadesN_.xlsx
+++ b/Documents/Actividades realizadas/ActividadesN_.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\VioletaSystem\Documents\Actividades realizadas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DD075BD-5B2F-4D8E-936B-92AC9A16C134}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3EBA53F-17B0-4428-A230-FF8E5D289FC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HORAS" sheetId="1" r:id="rId1"/>
-    <sheet name="Pendientes" sheetId="3" r:id="rId2"/>
-    <sheet name="Cotización vs Real" sheetId="2" r:id="rId3"/>
-    <sheet name="Hoja1" sheetId="4" r:id="rId4"/>
+    <sheet name="Abonos" sheetId="5" r:id="rId2"/>
+    <sheet name="Pendientes" sheetId="3" r:id="rId3"/>
+    <sheet name="Cotización vs Real" sheetId="2" r:id="rId4"/>
+    <sheet name="Hoja1" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="359">
   <si>
     <t>Descripción</t>
   </si>
@@ -973,6 +974,144 @@
   </si>
   <si>
     <t>Soporte con los Ids de los productos</t>
+  </si>
+  <si>
+    <t>Revisión y ajuste de Sarita enbase a violeta</t>
+  </si>
+  <si>
+    <t>Concepto</t>
+  </si>
+  <si>
+    <t>Monto</t>
+  </si>
+  <si>
+    <t>Cotización del sistema</t>
+  </si>
+  <si>
+    <t>Modificaciones en varias pantallas, reportes nuevos, comisiones, cancelaciones, inventarios físicos, autorizaciones por código, manejo de sobre de taller, proveedores entre otros cambios que han surjido</t>
+  </si>
+  <si>
+    <t>Verificaciones de inventario, autorizaciones de salidas de inventario, reporte de movimientos de dinero electrónico, pantalla de permisos al menú para usuarios y roles, programa para realizar carga inicial de productos e inventarios por Excel</t>
+  </si>
+  <si>
+    <t>Soporte en conexiones, Revisiones de redondeo, Verificación de inventario por selección, Separar taller y agregar ingreso real en Corte de Caja</t>
+  </si>
+  <si>
+    <t>Reporte de ventas, restriccion para que pida autorización al crear consignación a nombre de martin, instalación y configuración de impresora</t>
+  </si>
+  <si>
+    <t>Agregar el descuento pero en pesos en la pantalla de ventas, solucionar detalle de los decimales en los pagos, Crear sección de devolución de inventario con autorizaciones de mostrador como de Martín, Permiso y cambio de precio de los productos en nota de venta</t>
+  </si>
+  <si>
+    <t>Agregar margen del 30% del costo en los descuentos, Al agregar descuento por precio que salga alerta de si está seguro, cerrar ventana de Cliente cuando se agrega o se actualiza, agregar atajo de inventario de producto desde la consulta, obligatoria la descripción al agregar dinero electrónico de forma manual, en la cancelación de pago, que sea obligatorio seleccionar una de las dos ociones, dinero electronico o el egreso, Se agrega control de quien agrega movimientos en el dinero electrónico de los clientes, Se deshabilita el check en la pantalla de clientes, deshabilitar check de activos en clientes, usuarios y roles</t>
+  </si>
+  <si>
+    <t>Manejo de estatus para los sobres de taller, que aparezca el status de los sobres en la consulta de ventas, agregar botones de exportar a excel en el inventario físico para poder imprimir</t>
+  </si>
+  <si>
+    <t>Se agrega pantalla de Ingresos manuales, Se modifican los Cortes de caja para considerar los ingresos Manuales, Se optimiza el Corte de caja para no manejar transacciones</t>
+  </si>
+  <si>
+    <t>Agregar lista de Egresos, Ingresos y pagos cancelados en la pantalla de Corte de caja, Cancelación de los ingresos con autorización y revisión de impresión de ticket para corte de caja, Reporte de pagos cancelados, Cancelación de venta con pagos cortados</t>
+  </si>
+  <si>
+    <t>Instalación y configuración del Sistema para la merceria Sarita</t>
+  </si>
+  <si>
+    <t>Poner NOTA PAGADA cuando pagan una nota, Agregar el cambio en el ticket de Pagos, Agregar sonidos a la verificación de inventario físico, Agregar sección de cambio de contraseña y de código de autorización</t>
+  </si>
+  <si>
+    <t>Impresión de código de barra de producto, Configuración de código de barras en impresora de oficina, Modificaciones de impresión de ticket de notas, Corte de Caja, Egresos, Ingresos y pagos</t>
+  </si>
+  <si>
+    <t>Agregar el nombre del vendedor en el Ticket del pago, Soporte para migrar de servidor a Sarita y sacar Pagos de los cortes del 29 de junio, Configuracion de impresora en merceria</t>
+  </si>
+  <si>
+    <t>Permiso para poder ver los costos de los productos en el reporte de ventas, Agregar las cotizaciones en la sección de ventas y que no bajen inventario, quitar de merceria el imprimir el código de barras, Que pueda agregar más de una vez el mismo producto, Que la cotización pueda mezclarse como si fuera de taller tambien, Cambiar el pie de página, para que diga que la cotizacion puede cambiar</t>
+  </si>
+  <si>
+    <t>Agregar fecha de entrega/recibido, Modificar el ticket de taller y la nota de taller para agregar la fecha de Entrega</t>
+  </si>
+  <si>
+    <t>total acomulado</t>
+  </si>
+  <si>
+    <t>Anticipo</t>
+  </si>
+  <si>
+    <t>Abono</t>
+  </si>
+  <si>
+    <t>Abono Martin</t>
+  </si>
+  <si>
+    <t>Abono de Amelia</t>
+  </si>
+  <si>
+    <t>Total de abonos</t>
+  </si>
+  <si>
+    <t>Pendiente</t>
+  </si>
+  <si>
+    <t>Permiso para poder ver los costos de los productos en el reporte de ventas, Agregar las cotizaciones en la sección de ventas y que no bajen inventario, quitar de merceria el imprimir el código de barras, quitar de merceria el imprimir el código de barras, Que pueda agregar más de una vez el mismo producto, Que la cotización pueda mezclarse como si fuera de taller tambien, Cambiar el pie de página, para que diga que la cotizacion puede cambiar</t>
+  </si>
+  <si>
+    <t>Revisión de los Ids de las comisiones</t>
+  </si>
+  <si>
+    <t>Cancelación de devoluciones</t>
+  </si>
+  <si>
+    <t>MEDALLA</t>
+  </si>
+  <si>
+    <t>PRECIO</t>
+  </si>
+  <si>
+    <t>COSTO</t>
+  </si>
+  <si>
+    <t>UTILIDAD</t>
+  </si>
+  <si>
+    <t>MO JDA</t>
+  </si>
+  <si>
+    <t>P0000257</t>
+  </si>
+  <si>
+    <t>00006725</t>
+  </si>
+  <si>
+    <t>plata</t>
+  </si>
+  <si>
+    <t>oro</t>
+  </si>
+  <si>
+    <t>Precio</t>
+  </si>
+  <si>
+    <t>Equivalencia</t>
+  </si>
+  <si>
+    <t>Utilidad</t>
+  </si>
+  <si>
+    <t>correspondiente del pago</t>
+  </si>
+  <si>
+    <t>Costo</t>
+  </si>
+  <si>
+    <t>cor del pago</t>
+  </si>
+  <si>
+    <t>Sección de finanzas con el reporte de información financiera</t>
+  </si>
+  <si>
+    <t>Graficación en reporte de información financiera y código de barras de producto en ticket</t>
   </si>
 </sst>
 </file>
@@ -983,7 +1122,7 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1048,8 +1187,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF212529"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1104,8 +1249,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -1113,13 +1270,76 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1206,6 +1426,38 @@
     <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="0" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="0" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="0" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="44" fontId="0" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1254,17 +1506,46 @@
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="44" fontId="0" fillId="11" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="11" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="11" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Millares" xfId="2" builtinId="3"/>
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Porcentaje" xfId="3" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1576,11 +1857,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K304"/>
+  <dimension ref="A1:K309"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A253" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D262" sqref="D262"/>
+      <selection pane="bottomLeft" activeCell="D262" sqref="D262:D265"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6743,6 +7024,7 @@
     </row>
     <row r="259" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A259" s="5"/>
+      <c r="C259" s="39"/>
       <c r="D259" s="14" t="s">
         <v>311</v>
       </c>
@@ -6758,6 +7040,7 @@
     </row>
     <row r="260" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A260" s="5"/>
+      <c r="C260" s="39"/>
       <c r="D260" s="14" t="s">
         <v>312</v>
       </c>
@@ -6773,251 +7056,288 @@
     </row>
     <row r="261" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A261" s="5"/>
-      <c r="D261" s="14"/>
-      <c r="E261" s="2"/>
-      <c r="F261" s="2"/>
+      <c r="C261" s="39"/>
+      <c r="D261" s="14" t="s">
+        <v>313</v>
+      </c>
+      <c r="E261" s="2">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="F261" s="2">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="G261" s="15">
+        <v>2</v>
+      </c>
     </row>
     <row r="262" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A262" s="5"/>
-      <c r="E262" s="2"/>
-      <c r="F262" s="2"/>
+      <c r="D262" s="14" t="s">
+        <v>340</v>
+      </c>
+      <c r="E262" s="2">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="F262" s="2">
+        <v>0.5625</v>
+      </c>
+      <c r="H262" s="15">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="263" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A263" s="5"/>
-      <c r="E263" s="2"/>
-      <c r="F263" s="2"/>
+      <c r="D263" s="14" t="s">
+        <v>341</v>
+      </c>
+      <c r="E263" s="2">
+        <v>0.5625</v>
+      </c>
+      <c r="F263" s="2">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="H263" s="15">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="264" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A264" s="5"/>
-      <c r="E264" s="2"/>
-      <c r="F264" s="2"/>
-    </row>
-    <row r="265" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A265" s="45" t="s">
+      <c r="D264" s="14" t="s">
+        <v>357</v>
+      </c>
+      <c r="E264" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="F264" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="H264" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="265" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A265" s="5"/>
+      <c r="D265" s="14" t="s">
+        <v>358</v>
+      </c>
+      <c r="E265" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="F265" s="2">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="G265" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="266" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A266" s="5"/>
+      <c r="D266" s="14"/>
+      <c r="E266" s="2"/>
+      <c r="F266" s="2"/>
+    </row>
+    <row r="267" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A267" s="5"/>
+      <c r="D267" s="14"/>
+      <c r="E267" s="2"/>
+      <c r="F267" s="2"/>
+    </row>
+    <row r="268" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A268" s="5"/>
+      <c r="E268" s="2"/>
+      <c r="F268" s="2"/>
+    </row>
+    <row r="269" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A269" s="5"/>
+      <c r="E269" s="2"/>
+      <c r="F269" s="2"/>
+    </row>
+    <row r="270" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A270" s="63" t="s">
         <v>165</v>
       </c>
-      <c r="B265" s="45"/>
-      <c r="C265" s="45"/>
-      <c r="D265" s="45"/>
-      <c r="E265" s="45"/>
-      <c r="F265" s="45"/>
-      <c r="G265" s="17">
-        <f>SUM(G2:G264)</f>
-        <v>310.78999999999996</v>
-      </c>
-      <c r="H265" s="17">
-        <f>SUM(H2:H264)</f>
-        <v>54.8</v>
-      </c>
-    </row>
-    <row r="266" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A266" s="45" t="s">
+      <c r="B270" s="63"/>
+      <c r="C270" s="63"/>
+      <c r="D270" s="63"/>
+      <c r="E270" s="63"/>
+      <c r="F270" s="63"/>
+      <c r="G270" s="17">
+        <f>SUM(G2:G269)</f>
+        <v>314.78999999999996</v>
+      </c>
+      <c r="H270" s="17">
+        <f>SUM(H2:H269)</f>
+        <v>59.8</v>
+      </c>
+    </row>
+    <row r="271" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A271" s="63" t="s">
         <v>139</v>
       </c>
-      <c r="B266" s="45"/>
-      <c r="C266" s="45"/>
-      <c r="D266" s="45"/>
-      <c r="E266" s="45"/>
-      <c r="F266" s="45"/>
-      <c r="G266" s="17">
+      <c r="B271" s="63"/>
+      <c r="C271" s="63"/>
+      <c r="D271" s="63"/>
+      <c r="E271" s="63"/>
+      <c r="F271" s="63"/>
+      <c r="G271" s="17">
         <v>200</v>
       </c>
-      <c r="H266" s="17">
+      <c r="H271" s="17">
         <v>300</v>
       </c>
     </row>
-    <row r="267" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A267" s="45" t="s">
+    <row r="272" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A272" s="63" t="s">
         <v>166</v>
       </c>
-      <c r="B267" s="45"/>
-      <c r="C267" s="45"/>
-      <c r="D267" s="45"/>
-      <c r="E267" s="45"/>
-      <c r="F267" s="45"/>
-      <c r="G267" s="18">
-        <f>G266*G265</f>
-        <v>62157.999999999993</v>
-      </c>
-      <c r="H267" s="19">
-        <f>H266*H265</f>
-        <v>16440</v>
-      </c>
-      <c r="J267">
+      <c r="B272" s="63"/>
+      <c r="C272" s="63"/>
+      <c r="D272" s="63"/>
+      <c r="E272" s="63"/>
+      <c r="F272" s="63"/>
+      <c r="G272" s="18">
+        <f>G271*G270</f>
+        <v>62957.999999999993</v>
+      </c>
+      <c r="H272" s="19">
+        <f>H271*H270</f>
+        <v>17940</v>
+      </c>
+      <c r="J272">
         <v>-500</v>
       </c>
     </row>
-    <row r="268" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A268" s="45" t="s">
+    <row r="273" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A273" s="63" t="s">
         <v>140</v>
       </c>
-      <c r="B268" s="45"/>
-      <c r="C268" s="45"/>
-      <c r="D268" s="45"/>
-      <c r="E268" s="45"/>
-      <c r="F268" s="45"/>
-      <c r="G268" s="50">
-        <f>G267+H267</f>
-        <v>78598</v>
-      </c>
-      <c r="H268" s="50"/>
-    </row>
-    <row r="269" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A269" s="11"/>
-      <c r="B269" s="53" t="s">
+      <c r="B273" s="63"/>
+      <c r="C273" s="63"/>
+      <c r="D273" s="63"/>
+      <c r="E273" s="63"/>
+      <c r="F273" s="63"/>
+      <c r="G273" s="68">
+        <f>G272+H272</f>
+        <v>80898</v>
+      </c>
+      <c r="H273" s="68"/>
+    </row>
+    <row r="274" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A274" s="11"/>
+      <c r="B274" s="71" t="s">
         <v>142</v>
       </c>
-      <c r="C269" s="53"/>
-      <c r="D269" s="53"/>
-      <c r="E269" s="53"/>
-      <c r="F269" s="53"/>
-      <c r="G269" s="22"/>
-    </row>
-    <row r="270" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A270" s="12">
+      <c r="C274" s="71"/>
+      <c r="D274" s="71"/>
+      <c r="E274" s="71"/>
+      <c r="F274" s="71"/>
+      <c r="G274" s="22"/>
+    </row>
+    <row r="275" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A275" s="12">
         <v>45109</v>
       </c>
-      <c r="B270" s="54" t="s">
+      <c r="B275" s="72" t="s">
         <v>141</v>
       </c>
-      <c r="C270" s="54"/>
-      <c r="D270" s="54"/>
-      <c r="E270" s="54"/>
-      <c r="F270" s="54"/>
-      <c r="G270" s="55">
+      <c r="C275" s="72"/>
+      <c r="D275" s="72"/>
+      <c r="E275" s="72"/>
+      <c r="F275" s="72"/>
+      <c r="G275" s="73">
         <v>10000</v>
       </c>
-      <c r="H270" s="55"/>
-    </row>
-    <row r="271" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A271" s="12"/>
-      <c r="B271" s="57" t="s">
-        <v>178</v>
-      </c>
-      <c r="C271" s="57"/>
-      <c r="D271" s="57"/>
-      <c r="E271" s="57"/>
-      <c r="F271" s="57"/>
-      <c r="G271" s="55">
-        <v>5000</v>
-      </c>
-      <c r="H271" s="55"/>
-    </row>
-    <row r="272" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A272" s="12">
-        <v>45278</v>
-      </c>
-      <c r="B272" s="46" t="s">
-        <v>178</v>
-      </c>
-      <c r="C272" s="46"/>
-      <c r="D272" s="46"/>
-      <c r="E272" s="46"/>
-      <c r="F272" s="46"/>
-      <c r="G272" s="55">
-        <v>9800</v>
-      </c>
-      <c r="H272" s="55"/>
-    </row>
-    <row r="273" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A273" s="12"/>
-      <c r="B273" s="46"/>
-      <c r="C273" s="46"/>
-      <c r="D273" s="46"/>
-      <c r="E273" s="46"/>
-      <c r="F273" s="46"/>
-      <c r="G273" s="56"/>
-      <c r="H273" s="56"/>
-    </row>
-    <row r="274" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A274" s="12"/>
-      <c r="B274" s="46"/>
-      <c r="C274" s="46"/>
-      <c r="D274" s="46"/>
-      <c r="E274" s="46"/>
-      <c r="F274" s="46"/>
-      <c r="G274" s="56"/>
-      <c r="H274" s="56"/>
-    </row>
-    <row r="275" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A275" s="12"/>
-      <c r="B275" s="46"/>
-      <c r="C275" s="46"/>
-      <c r="D275" s="46"/>
-      <c r="E275" s="46"/>
-      <c r="F275" s="46"/>
-      <c r="G275" s="56"/>
-      <c r="H275" s="56"/>
+      <c r="H275" s="73"/>
     </row>
     <row r="276" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A276" s="12"/>
-      <c r="B276" s="46" t="s">
-        <v>144</v>
-      </c>
-      <c r="C276" s="46"/>
-      <c r="D276" s="46"/>
-      <c r="E276" s="46"/>
-      <c r="F276" s="46"/>
-      <c r="G276" s="55">
-        <f>SUM(G270:H275)</f>
-        <v>24800</v>
-      </c>
-      <c r="H276" s="55"/>
-    </row>
-    <row r="277" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A277" s="51" t="s">
-        <v>143</v>
-      </c>
-      <c r="B277" s="51"/>
-      <c r="C277" s="51"/>
-      <c r="D277" s="51"/>
-      <c r="E277" s="51"/>
-      <c r="F277" s="51"/>
-      <c r="G277" s="52">
-        <f>G268-G276</f>
-        <v>53798</v>
-      </c>
-      <c r="H277" s="52"/>
+      <c r="B276" s="75" t="s">
+        <v>178</v>
+      </c>
+      <c r="C276" s="75"/>
+      <c r="D276" s="75"/>
+      <c r="E276" s="75"/>
+      <c r="F276" s="75"/>
+      <c r="G276" s="73">
+        <v>5000</v>
+      </c>
+      <c r="H276" s="73"/>
+    </row>
+    <row r="277" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A277" s="12">
+        <v>45278</v>
+      </c>
+      <c r="B277" s="64" t="s">
+        <v>178</v>
+      </c>
+      <c r="C277" s="64"/>
+      <c r="D277" s="64"/>
+      <c r="E277" s="64"/>
+      <c r="F277" s="64"/>
+      <c r="G277" s="73">
+        <v>9800</v>
+      </c>
+      <c r="H277" s="73"/>
     </row>
     <row r="278" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A278" s="12"/>
-      <c r="B278" s="13"/>
-      <c r="C278" s="13"/>
-      <c r="D278" s="13"/>
-      <c r="E278" s="13"/>
-      <c r="F278" s="13"/>
+      <c r="B278" s="64"/>
+      <c r="C278" s="64"/>
+      <c r="D278" s="64"/>
+      <c r="E278" s="64"/>
+      <c r="F278" s="64"/>
+      <c r="G278" s="74"/>
+      <c r="H278" s="74"/>
     </row>
     <row r="279" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A279" s="12"/>
-      <c r="B279" s="13"/>
-      <c r="C279" s="13"/>
-      <c r="D279" s="13"/>
-      <c r="E279" s="13"/>
-      <c r="F279" s="13"/>
+      <c r="B279" s="64"/>
+      <c r="C279" s="64"/>
+      <c r="D279" s="64"/>
+      <c r="E279" s="64"/>
+      <c r="F279" s="64"/>
+      <c r="G279" s="74"/>
+      <c r="H279" s="74"/>
     </row>
     <row r="280" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A280" s="12"/>
-      <c r="B280" s="13"/>
-      <c r="C280" s="13"/>
-      <c r="D280" s="13"/>
-      <c r="E280" s="13"/>
-      <c r="F280" s="13"/>
+      <c r="B280" s="64"/>
+      <c r="C280" s="64"/>
+      <c r="D280" s="64"/>
+      <c r="E280" s="64"/>
+      <c r="F280" s="64"/>
+      <c r="G280" s="74"/>
+      <c r="H280" s="74"/>
     </row>
     <row r="281" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A281" s="12"/>
-      <c r="B281" s="13"/>
-      <c r="C281" s="13"/>
-      <c r="D281" s="13"/>
-      <c r="E281" s="13"/>
-      <c r="F281" s="13"/>
-    </row>
-    <row r="282" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A282" s="12"/>
-      <c r="B282" s="13"/>
-      <c r="C282" s="13"/>
-      <c r="D282" s="13"/>
-      <c r="E282" s="13"/>
-      <c r="F282" s="13"/>
+      <c r="B281" s="64" t="s">
+        <v>144</v>
+      </c>
+      <c r="C281" s="64"/>
+      <c r="D281" s="64"/>
+      <c r="E281" s="64"/>
+      <c r="F281" s="64"/>
+      <c r="G281" s="73">
+        <f>SUM(G275:H280)</f>
+        <v>24800</v>
+      </c>
+      <c r="H281" s="73"/>
+    </row>
+    <row r="282" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A282" s="69" t="s">
+        <v>143</v>
+      </c>
+      <c r="B282" s="69"/>
+      <c r="C282" s="69"/>
+      <c r="D282" s="69"/>
+      <c r="E282" s="69"/>
+      <c r="F282" s="69"/>
+      <c r="G282" s="70">
+        <f>G273-G281</f>
+        <v>56098</v>
+      </c>
+      <c r="H282" s="70"/>
     </row>
     <row r="283" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A283" s="12"/>
@@ -7124,190 +7444,230 @@
       <c r="F295" s="13"/>
     </row>
     <row r="296" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A296" s="10"/>
-      <c r="B296" s="47" t="s">
+      <c r="A296" s="12"/>
+      <c r="B296" s="13"/>
+      <c r="C296" s="13"/>
+      <c r="D296" s="13"/>
+      <c r="E296" s="13"/>
+      <c r="F296" s="13"/>
+    </row>
+    <row r="297" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A297" s="12"/>
+      <c r="B297" s="13"/>
+      <c r="C297" s="13"/>
+      <c r="D297" s="13"/>
+      <c r="E297" s="13"/>
+      <c r="F297" s="13"/>
+    </row>
+    <row r="298" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A298" s="12"/>
+      <c r="B298" s="13"/>
+      <c r="C298" s="13"/>
+      <c r="D298" s="13"/>
+      <c r="E298" s="13"/>
+      <c r="F298" s="13"/>
+    </row>
+    <row r="299" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A299" s="12"/>
+      <c r="B299" s="13"/>
+      <c r="C299" s="13"/>
+      <c r="D299" s="13"/>
+      <c r="E299" s="13"/>
+      <c r="F299" s="13"/>
+    </row>
+    <row r="300" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A300" s="12"/>
+      <c r="B300" s="13"/>
+      <c r="C300" s="13"/>
+      <c r="D300" s="13"/>
+      <c r="E300" s="13"/>
+      <c r="F300" s="13"/>
+    </row>
+    <row r="301" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A301" s="10"/>
+      <c r="B301" s="65" t="s">
         <v>138</v>
       </c>
-      <c r="C296" s="47"/>
-      <c r="D296" s="47"/>
-      <c r="E296" s="47"/>
-      <c r="F296" s="47"/>
-      <c r="G296" s="21"/>
-      <c r="H296" s="21"/>
-      <c r="I296" s="8">
-        <f>G265+H265</f>
-        <v>365.59</v>
-      </c>
-      <c r="J296" s="8">
-        <f>I296</f>
-        <v>365.59</v>
-      </c>
-    </row>
-    <row r="297" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A297" s="5"/>
-      <c r="B297" s="48" t="s">
+      <c r="C301" s="65"/>
+      <c r="D301" s="65"/>
+      <c r="E301" s="65"/>
+      <c r="F301" s="65"/>
+      <c r="G301" s="21"/>
+      <c r="H301" s="21"/>
+      <c r="I301" s="8">
+        <f>G270+H270</f>
+        <v>374.59</v>
+      </c>
+      <c r="J301" s="8">
+        <f>I301</f>
+        <v>374.59</v>
+      </c>
+    </row>
+    <row r="302" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A302" s="5"/>
+      <c r="B302" s="66" t="s">
         <v>139</v>
       </c>
-      <c r="C297" s="48"/>
-      <c r="D297" s="48"/>
-      <c r="E297" s="48"/>
-      <c r="F297" s="48"/>
-      <c r="I297" s="8">
+      <c r="C302" s="66"/>
+      <c r="D302" s="66"/>
+      <c r="E302" s="66"/>
+      <c r="F302" s="66"/>
+      <c r="I302" s="8">
         <v>300</v>
       </c>
-      <c r="J297" s="8">
+      <c r="J302" s="8">
         <v>200</v>
       </c>
     </row>
-    <row r="298" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A298" s="5"/>
-      <c r="B298" s="48" t="s">
+    <row r="303" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A303" s="5"/>
+      <c r="B303" s="66" t="s">
         <v>140</v>
       </c>
-      <c r="C298" s="48"/>
-      <c r="D298" s="48"/>
-      <c r="E298" s="48"/>
-      <c r="F298" s="48"/>
-      <c r="I298" s="9">
-        <f>I297*I296</f>
-        <v>109676.99999999999</v>
-      </c>
-      <c r="J298" s="9">
-        <f>J297*J296</f>
-        <v>73118</v>
-      </c>
-    </row>
-    <row r="299" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A299" s="23"/>
-      <c r="B299" s="49" t="s">
+      <c r="C303" s="66"/>
+      <c r="D303" s="66"/>
+      <c r="E303" s="66"/>
+      <c r="F303" s="66"/>
+      <c r="I303" s="9">
+        <f>I302*I301</f>
+        <v>112376.99999999999</v>
+      </c>
+      <c r="J303" s="9">
+        <f>J302*J301</f>
+        <v>74918</v>
+      </c>
+    </row>
+    <row r="304" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A304" s="23"/>
+      <c r="B304" s="67" t="s">
         <v>142</v>
       </c>
-      <c r="C299" s="49"/>
-      <c r="D299" s="49"/>
-      <c r="E299" s="49"/>
-      <c r="F299" s="49"/>
-      <c r="G299" s="24"/>
-      <c r="H299" s="24"/>
-      <c r="I299" s="25"/>
-      <c r="J299" s="25"/>
-    </row>
-    <row r="300" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A300" s="26">
+      <c r="C304" s="67"/>
+      <c r="D304" s="67"/>
+      <c r="E304" s="67"/>
+      <c r="F304" s="67"/>
+      <c r="G304" s="24"/>
+      <c r="H304" s="24"/>
+      <c r="I304" s="25"/>
+      <c r="J304" s="25"/>
+    </row>
+    <row r="305" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A305" s="26">
         <v>45109</v>
       </c>
-      <c r="B300" s="43" t="s">
+      <c r="B305" s="61" t="s">
         <v>141</v>
       </c>
-      <c r="C300" s="43"/>
-      <c r="D300" s="43"/>
-      <c r="E300" s="43"/>
-      <c r="F300" s="43"/>
-      <c r="G300" s="27"/>
-      <c r="H300" s="27"/>
-      <c r="I300" s="28">
+      <c r="C305" s="61"/>
+      <c r="D305" s="61"/>
+      <c r="E305" s="61"/>
+      <c r="F305" s="61"/>
+      <c r="G305" s="27"/>
+      <c r="H305" s="27"/>
+      <c r="I305" s="28">
         <v>10000</v>
       </c>
-      <c r="J300" s="28">
+      <c r="J305" s="28">
         <v>10000</v>
       </c>
     </row>
-    <row r="301" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A301" s="26"/>
-      <c r="B301" s="29"/>
-      <c r="C301" s="29"/>
-      <c r="D301" s="29"/>
-      <c r="E301" s="29"/>
-      <c r="F301" s="29"/>
-      <c r="G301" s="27"/>
-      <c r="H301" s="27"/>
-      <c r="I301" s="30"/>
-      <c r="J301" s="30"/>
-    </row>
-    <row r="302" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A302" s="26"/>
-      <c r="B302" s="29"/>
-      <c r="C302" s="29"/>
-      <c r="D302" s="29"/>
-      <c r="E302" s="29"/>
-      <c r="F302" s="29"/>
-      <c r="G302" s="27"/>
-      <c r="H302" s="27"/>
-      <c r="I302" s="30"/>
-      <c r="J302" s="30"/>
-    </row>
-    <row r="303" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A303" s="26"/>
-      <c r="B303" s="44" t="s">
+    <row r="306" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A306" s="26"/>
+      <c r="B306" s="29"/>
+      <c r="C306" s="29"/>
+      <c r="D306" s="29"/>
+      <c r="E306" s="29"/>
+      <c r="F306" s="29"/>
+      <c r="G306" s="27"/>
+      <c r="H306" s="27"/>
+      <c r="I306" s="30"/>
+      <c r="J306" s="30"/>
+    </row>
+    <row r="307" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A307" s="26"/>
+      <c r="B307" s="29"/>
+      <c r="C307" s="29"/>
+      <c r="D307" s="29"/>
+      <c r="E307" s="29"/>
+      <c r="F307" s="29"/>
+      <c r="G307" s="27"/>
+      <c r="H307" s="27"/>
+      <c r="I307" s="30"/>
+      <c r="J307" s="30"/>
+    </row>
+    <row r="308" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A308" s="26"/>
+      <c r="B308" s="62" t="s">
         <v>144</v>
       </c>
-      <c r="C303" s="44"/>
-      <c r="D303" s="44"/>
-      <c r="E303" s="44"/>
-      <c r="F303" s="44"/>
-      <c r="G303" s="27"/>
-      <c r="H303" s="27"/>
-      <c r="I303" s="31">
-        <f>SUM(I300:I302)</f>
+      <c r="C308" s="62"/>
+      <c r="D308" s="62"/>
+      <c r="E308" s="62"/>
+      <c r="F308" s="62"/>
+      <c r="G308" s="27"/>
+      <c r="H308" s="27"/>
+      <c r="I308" s="31">
+        <f>SUM(I305:I307)</f>
         <v>10000</v>
       </c>
-      <c r="J303" s="31">
-        <f>SUM(J300:J302)</f>
+      <c r="J308" s="31">
+        <f>SUM(J305:J307)</f>
         <v>10000</v>
       </c>
     </row>
-    <row r="304" spans="1:10" ht="33.75" x14ac:dyDescent="0.5">
-      <c r="A304" s="32">
+    <row r="309" spans="1:10" ht="33.75" x14ac:dyDescent="0.5">
+      <c r="A309" s="32">
         <v>45109</v>
       </c>
-      <c r="B304" s="42" t="s">
+      <c r="B309" s="60" t="s">
         <v>143</v>
       </c>
-      <c r="C304" s="42"/>
-      <c r="D304" s="42"/>
-      <c r="E304" s="42"/>
-      <c r="F304" s="42"/>
-      <c r="G304" s="33"/>
-      <c r="H304" s="33"/>
-      <c r="I304" s="34">
-        <f>I298-I303</f>
-        <v>99676.999999999985</v>
-      </c>
-      <c r="J304" s="34">
-        <f>J298-J303</f>
-        <v>63118</v>
+      <c r="C309" s="60"/>
+      <c r="D309" s="60"/>
+      <c r="E309" s="60"/>
+      <c r="F309" s="60"/>
+      <c r="G309" s="33"/>
+      <c r="H309" s="33"/>
+      <c r="I309" s="34">
+        <f>I303-I308</f>
+        <v>102376.99999999999</v>
+      </c>
+      <c r="J309" s="34">
+        <f>J303-J308</f>
+        <v>64918</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="G268:H268"/>
-    <mergeCell ref="A277:F277"/>
-    <mergeCell ref="G277:H277"/>
-    <mergeCell ref="B269:F269"/>
-    <mergeCell ref="B270:F270"/>
-    <mergeCell ref="B276:F276"/>
-    <mergeCell ref="G270:H270"/>
-    <mergeCell ref="G271:H271"/>
-    <mergeCell ref="G276:H276"/>
     <mergeCell ref="G273:H273"/>
-    <mergeCell ref="G274:H274"/>
-    <mergeCell ref="G275:H275"/>
-    <mergeCell ref="G272:H272"/>
-    <mergeCell ref="B272:F272"/>
-    <mergeCell ref="B271:F271"/>
-    <mergeCell ref="B273:F273"/>
-    <mergeCell ref="B304:F304"/>
-    <mergeCell ref="B300:F300"/>
-    <mergeCell ref="B303:F303"/>
-    <mergeCell ref="A266:F266"/>
-    <mergeCell ref="A265:F265"/>
-    <mergeCell ref="A267:F267"/>
-    <mergeCell ref="A268:F268"/>
+    <mergeCell ref="A282:F282"/>
+    <mergeCell ref="G282:H282"/>
     <mergeCell ref="B274:F274"/>
     <mergeCell ref="B275:F275"/>
-    <mergeCell ref="B296:F296"/>
-    <mergeCell ref="B297:F297"/>
-    <mergeCell ref="B298:F298"/>
-    <mergeCell ref="B299:F299"/>
+    <mergeCell ref="B281:F281"/>
+    <mergeCell ref="G275:H275"/>
+    <mergeCell ref="G276:H276"/>
+    <mergeCell ref="G281:H281"/>
+    <mergeCell ref="G278:H278"/>
+    <mergeCell ref="G279:H279"/>
+    <mergeCell ref="G280:H280"/>
+    <mergeCell ref="G277:H277"/>
+    <mergeCell ref="B277:F277"/>
+    <mergeCell ref="B276:F276"/>
+    <mergeCell ref="B278:F278"/>
+    <mergeCell ref="B309:F309"/>
+    <mergeCell ref="B305:F305"/>
+    <mergeCell ref="B308:F308"/>
+    <mergeCell ref="A271:F271"/>
+    <mergeCell ref="A270:F270"/>
+    <mergeCell ref="A272:F272"/>
+    <mergeCell ref="A273:F273"/>
+    <mergeCell ref="B279:F279"/>
+    <mergeCell ref="B280:F280"/>
+    <mergeCell ref="B301:F301"/>
+    <mergeCell ref="B302:F302"/>
+    <mergeCell ref="B303:F303"/>
+    <mergeCell ref="B304:F304"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -7315,6 +7675,488 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3B2F9DB-D849-4B99-B5E6-70BB7408BE44}">
+  <dimension ref="A1:C72"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.140625" customWidth="1"/>
+    <col min="2" max="2" width="76.140625" customWidth="1"/>
+    <col min="3" max="3" width="24" style="8" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>314</v>
+      </c>
+      <c r="C1" s="48" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="49"/>
+      <c r="B2" s="49" t="s">
+        <v>316</v>
+      </c>
+      <c r="C2" s="50">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="49"/>
+      <c r="B3" s="51" t="s">
+        <v>317</v>
+      </c>
+      <c r="C3" s="50">
+        <v>21000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="49"/>
+      <c r="B4" s="51" t="s">
+        <v>318</v>
+      </c>
+      <c r="C4" s="50">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="49"/>
+      <c r="B5" s="51" t="s">
+        <v>319</v>
+      </c>
+      <c r="C5" s="50">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="49"/>
+      <c r="B6" s="51" t="s">
+        <v>320</v>
+      </c>
+      <c r="C6" s="50">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="49"/>
+      <c r="B7" s="51" t="s">
+        <v>321</v>
+      </c>
+      <c r="C7" s="50">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="A8" s="49"/>
+      <c r="B8" s="51" t="s">
+        <v>322</v>
+      </c>
+      <c r="C8" s="50">
+        <v>2300</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="49"/>
+      <c r="B9" s="51" t="s">
+        <v>323</v>
+      </c>
+      <c r="C9" s="50">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="49"/>
+      <c r="B10" s="51" t="s">
+        <v>324</v>
+      </c>
+      <c r="C10" s="50">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="49"/>
+      <c r="B11" s="51" t="s">
+        <v>325</v>
+      </c>
+      <c r="C11" s="50">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="49"/>
+      <c r="B12" s="51" t="s">
+        <v>326</v>
+      </c>
+      <c r="C12" s="50">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="49"/>
+      <c r="B13" s="51" t="s">
+        <v>327</v>
+      </c>
+      <c r="C13" s="50">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="49"/>
+      <c r="B14" s="51" t="s">
+        <v>328</v>
+      </c>
+      <c r="C14" s="50">
+        <v>2600</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="49"/>
+      <c r="B15" s="51" t="s">
+        <v>329</v>
+      </c>
+      <c r="C15" s="50">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="49"/>
+      <c r="B16" s="51" t="s">
+        <v>301</v>
+      </c>
+      <c r="C16" s="50">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A17" s="49"/>
+      <c r="B17" s="51" t="s">
+        <v>330</v>
+      </c>
+      <c r="C17" s="50">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="49"/>
+      <c r="B18" s="51" t="s">
+        <v>331</v>
+      </c>
+      <c r="C18" s="50">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="49"/>
+      <c r="B19" s="57" t="s">
+        <v>311</v>
+      </c>
+      <c r="C19" s="76">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="49"/>
+      <c r="B20" s="58" t="s">
+        <v>312</v>
+      </c>
+      <c r="C20" s="77"/>
+    </row>
+    <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="49"/>
+      <c r="B21" s="59" t="s">
+        <v>313</v>
+      </c>
+      <c r="C21" s="78"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="49"/>
+      <c r="B22" s="57" t="s">
+        <v>340</v>
+      </c>
+      <c r="C22" s="76">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="49"/>
+      <c r="B23" s="59" t="s">
+        <v>341</v>
+      </c>
+      <c r="C23" s="78"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="49"/>
+      <c r="B24" s="57" t="s">
+        <v>340</v>
+      </c>
+      <c r="C24" s="76">
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="49"/>
+      <c r="B25" s="58" t="s">
+        <v>341</v>
+      </c>
+      <c r="C25" s="77"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="49"/>
+      <c r="B26" s="58" t="s">
+        <v>357</v>
+      </c>
+      <c r="C26" s="77"/>
+    </row>
+    <row r="27" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="49"/>
+      <c r="B27" s="59" t="s">
+        <v>358</v>
+      </c>
+      <c r="C27" s="78"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="49"/>
+      <c r="B28" s="81"/>
+      <c r="C28" s="82"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="49"/>
+      <c r="B29" s="81"/>
+      <c r="C29" s="82"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="49"/>
+      <c r="B30" s="81"/>
+      <c r="C30" s="82"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="49"/>
+      <c r="B31" s="81"/>
+      <c r="C31" s="82"/>
+    </row>
+    <row r="32" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="52"/>
+      <c r="B32" s="53"/>
+      <c r="C32" s="54"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="44"/>
+      <c r="B33" s="44" t="s">
+        <v>332</v>
+      </c>
+      <c r="C33" s="47">
+        <f>SUM(C2:C32)</f>
+        <v>88600</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="45">
+        <v>45109</v>
+      </c>
+      <c r="B35" s="42" t="s">
+        <v>333</v>
+      </c>
+      <c r="C35" s="46">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="42"/>
+      <c r="B36" s="42" t="s">
+        <v>334</v>
+      </c>
+      <c r="C36" s="46">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="45">
+        <v>45278</v>
+      </c>
+      <c r="B37" s="42" t="s">
+        <v>334</v>
+      </c>
+      <c r="C37" s="46">
+        <v>9800</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="45">
+        <v>45347</v>
+      </c>
+      <c r="B38" s="42" t="s">
+        <v>334</v>
+      </c>
+      <c r="C38" s="46">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="45">
+        <v>45383</v>
+      </c>
+      <c r="B39" s="42" t="s">
+        <v>334</v>
+      </c>
+      <c r="C39" s="46">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="45">
+        <v>45384</v>
+      </c>
+      <c r="B40" s="42" t="s">
+        <v>334</v>
+      </c>
+      <c r="C40" s="46">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="56">
+        <v>45419</v>
+      </c>
+      <c r="B41" s="49" t="s">
+        <v>334</v>
+      </c>
+      <c r="C41" s="55">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="56">
+        <v>45449</v>
+      </c>
+      <c r="B42" s="49" t="s">
+        <v>334</v>
+      </c>
+      <c r="C42" s="55">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="56">
+        <v>45465</v>
+      </c>
+      <c r="B43" s="49" t="s">
+        <v>335</v>
+      </c>
+      <c r="C43" s="55">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="56"/>
+      <c r="B44" s="49" t="s">
+        <v>336</v>
+      </c>
+      <c r="C44" s="55">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="56">
+        <v>45506</v>
+      </c>
+      <c r="B45" s="49" t="s">
+        <v>335</v>
+      </c>
+      <c r="C45" s="55">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="56">
+        <v>45556</v>
+      </c>
+      <c r="B46" s="49" t="s">
+        <v>334</v>
+      </c>
+      <c r="C46" s="55">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="56"/>
+      <c r="B47" s="49" t="s">
+        <v>334</v>
+      </c>
+      <c r="C47" s="55">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="49"/>
+      <c r="B48" s="49"/>
+      <c r="C48" s="55"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="49"/>
+      <c r="B49" s="49"/>
+      <c r="C49" s="55"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="44"/>
+      <c r="B50" s="44" t="s">
+        <v>337</v>
+      </c>
+      <c r="C50" s="47">
+        <f>SUM(C34:C49)</f>
+        <v>84800</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="7"/>
+      <c r="B51" s="7" t="s">
+        <v>338</v>
+      </c>
+      <c r="C51" s="48">
+        <f>C33-C50</f>
+        <v>3800</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B56" s="14"/>
+    </row>
+    <row r="67" spans="2:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="B67" s="14" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B68" s="14"/>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B70" s="14"/>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B72" s="14"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C19:C21"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="C24:C27"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F34"/>
   <sheetViews>
@@ -7657,7 +8499,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D98"/>
   <sheetViews>
@@ -7689,12 +8531,12 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="58" t="s">
+      <c r="A2" s="79" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="58"/>
-      <c r="C2" s="58"/>
-      <c r="D2" s="58"/>
+      <c r="B2" s="79"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="79"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -7997,12 +8839,12 @@
       <c r="D30" s="6"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="59" t="s">
+      <c r="A31" s="80" t="s">
         <v>43</v>
       </c>
-      <c r="B31" s="59"/>
-      <c r="C31" s="59"/>
-      <c r="D31" s="59"/>
+      <c r="B31" s="80"/>
+      <c r="C31" s="80"/>
+      <c r="D31" s="80"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
@@ -8631,10 +9473,10 @@
       <c r="D97" s="6"/>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="59"/>
-      <c r="B98" s="59"/>
-      <c r="C98" s="59"/>
-      <c r="D98" s="59"/>
+      <c r="A98" s="80"/>
+      <c r="B98" s="80"/>
+      <c r="C98" s="80"/>
+      <c r="D98" s="80"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -8646,17 +9488,21 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="E5:F8"/>
+  <dimension ref="A5:F30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7:F8"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="5" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E5" t="s">
         <v>283</v>
       </c>
@@ -8664,7 +9510,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="6" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E6" t="s">
         <v>285</v>
       </c>
@@ -8672,7 +9518,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="7" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E7" t="s">
         <v>284</v>
       </c>
@@ -8680,7 +9526,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="8" spans="5:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E8" t="s">
         <v>283</v>
       </c>
@@ -8688,7 +9534,180 @@
         <v>3000</v>
       </c>
     </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>344</v>
+      </c>
+      <c r="C16" t="s">
+        <v>343</v>
+      </c>
+      <c r="D16" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>342</v>
+      </c>
+      <c r="B17" s="8">
+        <v>1116</v>
+      </c>
+      <c r="C17" s="8">
+        <v>3800</v>
+      </c>
+      <c r="D17" s="8">
+        <f>C17-B17</f>
+        <v>2684</v>
+      </c>
+      <c r="E17" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>346</v>
+      </c>
+      <c r="B18" s="8">
+        <v>200</v>
+      </c>
+      <c r="C18" s="8">
+        <v>500</v>
+      </c>
+      <c r="D18" s="8">
+        <f>C18-B18</f>
+        <v>300</v>
+      </c>
+      <c r="E18" t="s">
+        <v>349</v>
+      </c>
+      <c r="F18" s="85" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F19" s="84" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="83">
+        <f>SUM(B17:B19)</f>
+        <v>1316</v>
+      </c>
+      <c r="C20" s="83">
+        <f>SUM(C17:C19)</f>
+        <v>4300</v>
+      </c>
+      <c r="D20" s="83">
+        <f>SUM(D17:D19)</f>
+        <v>2984</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B23" s="87" t="s">
+        <v>334</v>
+      </c>
+      <c r="C23" s="87" t="s">
+        <v>351</v>
+      </c>
+      <c r="D23" s="87" t="s">
+        <v>352</v>
+      </c>
+      <c r="E23" s="87" t="s">
+        <v>353</v>
+      </c>
+      <c r="F23" s="88" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="8">
+        <v>1800</v>
+      </c>
+      <c r="C24" s="8">
+        <v>3800</v>
+      </c>
+      <c r="D24" s="86">
+        <f>C24*100/4300/100</f>
+        <v>0.88372093023255816</v>
+      </c>
+      <c r="E24" s="83">
+        <f>B24*D24-B17</f>
+        <v>474.69767441860472</v>
+      </c>
+      <c r="F24" s="8">
+        <f>B24*D24</f>
+        <v>1590.6976744186047</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="8">
+        <v>1800</v>
+      </c>
+      <c r="C25" s="8">
+        <v>500</v>
+      </c>
+      <c r="D25" s="86">
+        <f>C25*100/4300/100</f>
+        <v>0.11627906976744186</v>
+      </c>
+      <c r="E25" s="83">
+        <f>B25*D25-B18</f>
+        <v>9.3023255813953369</v>
+      </c>
+      <c r="F25" s="8">
+        <f>B25*D25</f>
+        <v>209.30232558139534</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B28" s="87" t="s">
+        <v>334</v>
+      </c>
+      <c r="C28" s="87" t="s">
+        <v>355</v>
+      </c>
+      <c r="D28" s="87" t="s">
+        <v>352</v>
+      </c>
+      <c r="E28" s="89" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="8">
+        <v>1800</v>
+      </c>
+      <c r="C29" s="8">
+        <v>1116</v>
+      </c>
+      <c r="D29" s="86">
+        <f>C29*100/1316/100</f>
+        <v>0.84802431610942253</v>
+      </c>
+      <c r="E29" s="8">
+        <f>B29*D29</f>
+        <v>1526.4437689969604</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B30" s="8">
+        <v>1800</v>
+      </c>
+      <c r="C30" s="8">
+        <v>200</v>
+      </c>
+      <c r="D30" s="86">
+        <f>C30*100/1316/100</f>
+        <v>0.1519756838905775</v>
+      </c>
+      <c r="E30" s="8">
+        <f>B30*D30</f>
+        <v>273.5562310030395</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se versiona la ultima liberación
</commit_message>
<xml_diff>
--- a/Documents/Actividades realizadas/ActividadesN_.xlsx
+++ b/Documents/Actividades realizadas/ActividadesN_.xlsx
@@ -8,16 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\VioletaSystem\Documents\Actividades realizadas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3EBA53F-17B0-4428-A230-FF8E5D289FC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C59D8D3-7D92-4CFE-9F34-8FC8B0C07BD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HORAS" sheetId="1" r:id="rId1"/>
     <sheet name="Abonos" sheetId="5" r:id="rId2"/>
-    <sheet name="Pendientes" sheetId="3" r:id="rId3"/>
-    <sheet name="Cotización vs Real" sheetId="2" r:id="rId4"/>
-    <sheet name="Hoja1" sheetId="4" r:id="rId5"/>
+    <sheet name="Abonos 2" sheetId="7" r:id="rId3"/>
+    <sheet name="Hoja2" sheetId="6" r:id="rId4"/>
+    <sheet name="Pendientes" sheetId="3" r:id="rId5"/>
+    <sheet name="Cotización vs Real" sheetId="2" r:id="rId6"/>
+    <sheet name="Hoja1" sheetId="4" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="363">
   <si>
     <t>Descripción</t>
   </si>
@@ -1112,6 +1114,18 @@
   </si>
   <si>
     <t>Graficación en reporte de información financiera y código de barras de producto en ticket</t>
+  </si>
+  <si>
+    <t>Apartado</t>
+  </si>
+  <si>
+    <t>Contado</t>
+  </si>
+  <si>
+    <t>Credito</t>
+  </si>
+  <si>
+    <t>Instalación y configuración de impresora en Sarita</t>
   </si>
 </sst>
 </file>
@@ -1122,7 +1136,7 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1190,6 +1204,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF212529"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1262,7 +1282,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -1332,6 +1352,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1339,7 +1385,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1458,69 +1504,6 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="11" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="11" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="11" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1539,6 +1522,76 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="11" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="11" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="11" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="11" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1860,8 +1913,8 @@
   <dimension ref="A1:K309"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A253" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D262" sqref="D262:D265"/>
+      <pane ySplit="1" topLeftCell="A256" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G265" sqref="G265"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7153,14 +7206,14 @@
       <c r="F269" s="2"/>
     </row>
     <row r="270" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A270" s="63" t="s">
+      <c r="A270" s="81" t="s">
         <v>165</v>
       </c>
-      <c r="B270" s="63"/>
-      <c r="C270" s="63"/>
-      <c r="D270" s="63"/>
-      <c r="E270" s="63"/>
-      <c r="F270" s="63"/>
+      <c r="B270" s="81"/>
+      <c r="C270" s="81"/>
+      <c r="D270" s="81"/>
+      <c r="E270" s="81"/>
+      <c r="F270" s="81"/>
       <c r="G270" s="17">
         <f>SUM(G2:G269)</f>
         <v>314.78999999999996</v>
@@ -7171,14 +7224,14 @@
       </c>
     </row>
     <row r="271" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A271" s="63" t="s">
+      <c r="A271" s="81" t="s">
         <v>139</v>
       </c>
-      <c r="B271" s="63"/>
-      <c r="C271" s="63"/>
-      <c r="D271" s="63"/>
-      <c r="E271" s="63"/>
-      <c r="F271" s="63"/>
+      <c r="B271" s="81"/>
+      <c r="C271" s="81"/>
+      <c r="D271" s="81"/>
+      <c r="E271" s="81"/>
+      <c r="F271" s="81"/>
       <c r="G271" s="17">
         <v>200</v>
       </c>
@@ -7187,14 +7240,14 @@
       </c>
     </row>
     <row r="272" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A272" s="63" t="s">
+      <c r="A272" s="81" t="s">
         <v>166</v>
       </c>
-      <c r="B272" s="63"/>
-      <c r="C272" s="63"/>
-      <c r="D272" s="63"/>
-      <c r="E272" s="63"/>
-      <c r="F272" s="63"/>
+      <c r="B272" s="81"/>
+      <c r="C272" s="81"/>
+      <c r="D272" s="81"/>
+      <c r="E272" s="81"/>
+      <c r="F272" s="81"/>
       <c r="G272" s="18">
         <f>G271*G270</f>
         <v>62957.999999999993</v>
@@ -7208,136 +7261,136 @@
       </c>
     </row>
     <row r="273" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A273" s="63" t="s">
+      <c r="A273" s="81" t="s">
         <v>140</v>
       </c>
-      <c r="B273" s="63"/>
-      <c r="C273" s="63"/>
-      <c r="D273" s="63"/>
-      <c r="E273" s="63"/>
-      <c r="F273" s="63"/>
-      <c r="G273" s="68">
+      <c r="B273" s="81"/>
+      <c r="C273" s="81"/>
+      <c r="D273" s="81"/>
+      <c r="E273" s="81"/>
+      <c r="F273" s="81"/>
+      <c r="G273" s="69">
         <f>G272+H272</f>
         <v>80898</v>
       </c>
-      <c r="H273" s="68"/>
+      <c r="H273" s="69"/>
     </row>
     <row r="274" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A274" s="11"/>
-      <c r="B274" s="71" t="s">
+      <c r="B274" s="72" t="s">
         <v>142</v>
       </c>
-      <c r="C274" s="71"/>
-      <c r="D274" s="71"/>
-      <c r="E274" s="71"/>
-      <c r="F274" s="71"/>
+      <c r="C274" s="72"/>
+      <c r="D274" s="72"/>
+      <c r="E274" s="72"/>
+      <c r="F274" s="72"/>
       <c r="G274" s="22"/>
     </row>
     <row r="275" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A275" s="12">
         <v>45109</v>
       </c>
-      <c r="B275" s="72" t="s">
+      <c r="B275" s="73" t="s">
         <v>141</v>
       </c>
-      <c r="C275" s="72"/>
-      <c r="D275" s="72"/>
-      <c r="E275" s="72"/>
-      <c r="F275" s="72"/>
-      <c r="G275" s="73">
+      <c r="C275" s="73"/>
+      <c r="D275" s="73"/>
+      <c r="E275" s="73"/>
+      <c r="F275" s="73"/>
+      <c r="G275" s="75">
         <v>10000</v>
       </c>
-      <c r="H275" s="73"/>
+      <c r="H275" s="75"/>
     </row>
     <row r="276" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A276" s="12"/>
-      <c r="B276" s="75" t="s">
+      <c r="B276" s="77" t="s">
         <v>178</v>
       </c>
-      <c r="C276" s="75"/>
-      <c r="D276" s="75"/>
-      <c r="E276" s="75"/>
-      <c r="F276" s="75"/>
-      <c r="G276" s="73">
+      <c r="C276" s="77"/>
+      <c r="D276" s="77"/>
+      <c r="E276" s="77"/>
+      <c r="F276" s="77"/>
+      <c r="G276" s="75">
         <v>5000</v>
       </c>
-      <c r="H276" s="73"/>
+      <c r="H276" s="75"/>
     </row>
     <row r="277" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A277" s="12">
         <v>45278</v>
       </c>
-      <c r="B277" s="64" t="s">
+      <c r="B277" s="74" t="s">
         <v>178</v>
       </c>
-      <c r="C277" s="64"/>
-      <c r="D277" s="64"/>
-      <c r="E277" s="64"/>
-      <c r="F277" s="64"/>
-      <c r="G277" s="73">
+      <c r="C277" s="74"/>
+      <c r="D277" s="74"/>
+      <c r="E277" s="74"/>
+      <c r="F277" s="74"/>
+      <c r="G277" s="75">
         <v>9800</v>
       </c>
-      <c r="H277" s="73"/>
+      <c r="H277" s="75"/>
     </row>
     <row r="278" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A278" s="12"/>
-      <c r="B278" s="64"/>
-      <c r="C278" s="64"/>
-      <c r="D278" s="64"/>
-      <c r="E278" s="64"/>
-      <c r="F278" s="64"/>
-      <c r="G278" s="74"/>
-      <c r="H278" s="74"/>
+      <c r="B278" s="74"/>
+      <c r="C278" s="74"/>
+      <c r="D278" s="74"/>
+      <c r="E278" s="74"/>
+      <c r="F278" s="74"/>
+      <c r="G278" s="76"/>
+      <c r="H278" s="76"/>
     </row>
     <row r="279" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A279" s="12"/>
-      <c r="B279" s="64"/>
-      <c r="C279" s="64"/>
-      <c r="D279" s="64"/>
-      <c r="E279" s="64"/>
-      <c r="F279" s="64"/>
-      <c r="G279" s="74"/>
-      <c r="H279" s="74"/>
+      <c r="B279" s="74"/>
+      <c r="C279" s="74"/>
+      <c r="D279" s="74"/>
+      <c r="E279" s="74"/>
+      <c r="F279" s="74"/>
+      <c r="G279" s="76"/>
+      <c r="H279" s="76"/>
     </row>
     <row r="280" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A280" s="12"/>
-      <c r="B280" s="64"/>
-      <c r="C280" s="64"/>
-      <c r="D280" s="64"/>
-      <c r="E280" s="64"/>
-      <c r="F280" s="64"/>
-      <c r="G280" s="74"/>
-      <c r="H280" s="74"/>
+      <c r="B280" s="74"/>
+      <c r="C280" s="74"/>
+      <c r="D280" s="74"/>
+      <c r="E280" s="74"/>
+      <c r="F280" s="74"/>
+      <c r="G280" s="76"/>
+      <c r="H280" s="76"/>
     </row>
     <row r="281" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A281" s="12"/>
-      <c r="B281" s="64" t="s">
+      <c r="B281" s="74" t="s">
         <v>144</v>
       </c>
-      <c r="C281" s="64"/>
-      <c r="D281" s="64"/>
-      <c r="E281" s="64"/>
-      <c r="F281" s="64"/>
-      <c r="G281" s="73">
+      <c r="C281" s="74"/>
+      <c r="D281" s="74"/>
+      <c r="E281" s="74"/>
+      <c r="F281" s="74"/>
+      <c r="G281" s="75">
         <f>SUM(G275:H280)</f>
         <v>24800</v>
       </c>
-      <c r="H281" s="73"/>
+      <c r="H281" s="75"/>
     </row>
     <row r="282" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A282" s="69" t="s">
+      <c r="A282" s="70" t="s">
         <v>143</v>
       </c>
-      <c r="B282" s="69"/>
-      <c r="C282" s="69"/>
-      <c r="D282" s="69"/>
-      <c r="E282" s="69"/>
-      <c r="F282" s="69"/>
-      <c r="G282" s="70">
+      <c r="B282" s="70"/>
+      <c r="C282" s="70"/>
+      <c r="D282" s="70"/>
+      <c r="E282" s="70"/>
+      <c r="F282" s="70"/>
+      <c r="G282" s="71">
         <f>G273-G281</f>
         <v>56098</v>
       </c>
-      <c r="H282" s="70"/>
+      <c r="H282" s="71"/>
     </row>
     <row r="283" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A283" s="12"/>
@@ -7485,13 +7538,13 @@
     </row>
     <row r="301" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A301" s="10"/>
-      <c r="B301" s="65" t="s">
+      <c r="B301" s="82" t="s">
         <v>138</v>
       </c>
-      <c r="C301" s="65"/>
-      <c r="D301" s="65"/>
-      <c r="E301" s="65"/>
-      <c r="F301" s="65"/>
+      <c r="C301" s="82"/>
+      <c r="D301" s="82"/>
+      <c r="E301" s="82"/>
+      <c r="F301" s="82"/>
       <c r="G301" s="21"/>
       <c r="H301" s="21"/>
       <c r="I301" s="8">
@@ -7505,13 +7558,13 @@
     </row>
     <row r="302" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A302" s="5"/>
-      <c r="B302" s="66" t="s">
+      <c r="B302" s="83" t="s">
         <v>139</v>
       </c>
-      <c r="C302" s="66"/>
-      <c r="D302" s="66"/>
-      <c r="E302" s="66"/>
-      <c r="F302" s="66"/>
+      <c r="C302" s="83"/>
+      <c r="D302" s="83"/>
+      <c r="E302" s="83"/>
+      <c r="F302" s="83"/>
       <c r="I302" s="8">
         <v>300</v>
       </c>
@@ -7521,13 +7574,13 @@
     </row>
     <row r="303" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A303" s="5"/>
-      <c r="B303" s="66" t="s">
+      <c r="B303" s="83" t="s">
         <v>140</v>
       </c>
-      <c r="C303" s="66"/>
-      <c r="D303" s="66"/>
-      <c r="E303" s="66"/>
-      <c r="F303" s="66"/>
+      <c r="C303" s="83"/>
+      <c r="D303" s="83"/>
+      <c r="E303" s="83"/>
+      <c r="F303" s="83"/>
       <c r="I303" s="9">
         <f>I302*I301</f>
         <v>112376.99999999999</v>
@@ -7539,13 +7592,13 @@
     </row>
     <row r="304" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A304" s="23"/>
-      <c r="B304" s="67" t="s">
+      <c r="B304" s="84" t="s">
         <v>142</v>
       </c>
-      <c r="C304" s="67"/>
-      <c r="D304" s="67"/>
-      <c r="E304" s="67"/>
-      <c r="F304" s="67"/>
+      <c r="C304" s="84"/>
+      <c r="D304" s="84"/>
+      <c r="E304" s="84"/>
+      <c r="F304" s="84"/>
       <c r="G304" s="24"/>
       <c r="H304" s="24"/>
       <c r="I304" s="25"/>
@@ -7555,13 +7608,13 @@
       <c r="A305" s="26">
         <v>45109</v>
       </c>
-      <c r="B305" s="61" t="s">
+      <c r="B305" s="79" t="s">
         <v>141</v>
       </c>
-      <c r="C305" s="61"/>
-      <c r="D305" s="61"/>
-      <c r="E305" s="61"/>
-      <c r="F305" s="61"/>
+      <c r="C305" s="79"/>
+      <c r="D305" s="79"/>
+      <c r="E305" s="79"/>
+      <c r="F305" s="79"/>
       <c r="G305" s="27"/>
       <c r="H305" s="27"/>
       <c r="I305" s="28">
@@ -7597,13 +7650,13 @@
     </row>
     <row r="308" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A308" s="26"/>
-      <c r="B308" s="62" t="s">
+      <c r="B308" s="80" t="s">
         <v>144</v>
       </c>
-      <c r="C308" s="62"/>
-      <c r="D308" s="62"/>
-      <c r="E308" s="62"/>
-      <c r="F308" s="62"/>
+      <c r="C308" s="80"/>
+      <c r="D308" s="80"/>
+      <c r="E308" s="80"/>
+      <c r="F308" s="80"/>
       <c r="G308" s="27"/>
       <c r="H308" s="27"/>
       <c r="I308" s="31">
@@ -7619,13 +7672,13 @@
       <c r="A309" s="32">
         <v>45109</v>
       </c>
-      <c r="B309" s="60" t="s">
+      <c r="B309" s="78" t="s">
         <v>143</v>
       </c>
-      <c r="C309" s="60"/>
-      <c r="D309" s="60"/>
-      <c r="E309" s="60"/>
-      <c r="F309" s="60"/>
+      <c r="C309" s="78"/>
+      <c r="D309" s="78"/>
+      <c r="E309" s="78"/>
+      <c r="F309" s="78"/>
       <c r="G309" s="33"/>
       <c r="H309" s="33"/>
       <c r="I309" s="34">
@@ -7639,6 +7692,19 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="B309:F309"/>
+    <mergeCell ref="B305:F305"/>
+    <mergeCell ref="B308:F308"/>
+    <mergeCell ref="A271:F271"/>
+    <mergeCell ref="A270:F270"/>
+    <mergeCell ref="A272:F272"/>
+    <mergeCell ref="A273:F273"/>
+    <mergeCell ref="B279:F279"/>
+    <mergeCell ref="B280:F280"/>
+    <mergeCell ref="B301:F301"/>
+    <mergeCell ref="B302:F302"/>
+    <mergeCell ref="B303:F303"/>
+    <mergeCell ref="B304:F304"/>
     <mergeCell ref="G273:H273"/>
     <mergeCell ref="A282:F282"/>
     <mergeCell ref="G282:H282"/>
@@ -7655,19 +7721,6 @@
     <mergeCell ref="B277:F277"/>
     <mergeCell ref="B276:F276"/>
     <mergeCell ref="B278:F278"/>
-    <mergeCell ref="B309:F309"/>
-    <mergeCell ref="B305:F305"/>
-    <mergeCell ref="B308:F308"/>
-    <mergeCell ref="A271:F271"/>
-    <mergeCell ref="A270:F270"/>
-    <mergeCell ref="A272:F272"/>
-    <mergeCell ref="A273:F273"/>
-    <mergeCell ref="B279:F279"/>
-    <mergeCell ref="B280:F280"/>
-    <mergeCell ref="B301:F301"/>
-    <mergeCell ref="B302:F302"/>
-    <mergeCell ref="B303:F303"/>
-    <mergeCell ref="B304:F304"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -7678,8 +7731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3B2F9DB-D849-4B99-B5E6-70BB7408BE44}">
   <dimension ref="A1:C72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7858,7 +7911,7 @@
       <c r="B19" s="57" t="s">
         <v>311</v>
       </c>
-      <c r="C19" s="76">
+      <c r="C19" s="85">
         <v>1100</v>
       </c>
     </row>
@@ -7867,21 +7920,21 @@
       <c r="B20" s="58" t="s">
         <v>312</v>
       </c>
-      <c r="C20" s="77"/>
+      <c r="C20" s="86"/>
     </row>
     <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="49"/>
       <c r="B21" s="59" t="s">
         <v>313</v>
       </c>
-      <c r="C21" s="78"/>
+      <c r="C21" s="87"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="49"/>
       <c r="B22" s="57" t="s">
         <v>340</v>
       </c>
-      <c r="C22" s="76">
+      <c r="C22" s="85">
         <v>600</v>
       </c>
     </row>
@@ -7890,57 +7943,59 @@
       <c r="B23" s="59" t="s">
         <v>341</v>
       </c>
-      <c r="C23" s="78"/>
+      <c r="C23" s="87"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="49"/>
       <c r="B24" s="57" t="s">
         <v>340</v>
       </c>
-      <c r="C24" s="76">
-        <v>2100</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C24" s="85">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="49"/>
-      <c r="B25" s="58" t="s">
+      <c r="B25" s="59" t="s">
         <v>341</v>
       </c>
-      <c r="C25" s="77"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C25" s="87"/>
+    </row>
+    <row r="26" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="49"/>
       <c r="B26" s="58" t="s">
         <v>357</v>
       </c>
-      <c r="C26" s="77"/>
-    </row>
-    <row r="27" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C26" s="86">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="30.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="49"/>
       <c r="B27" s="59" t="s">
         <v>358</v>
       </c>
-      <c r="C27" s="78"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C27" s="87"/>
+    </row>
+    <row r="28" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="49"/>
-      <c r="B28" s="81"/>
-      <c r="C28" s="82"/>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="60"/>
+      <c r="C28" s="61"/>
+    </row>
+    <row r="29" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="49"/>
-      <c r="B29" s="81"/>
-      <c r="C29" s="82"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="60"/>
+      <c r="C29" s="61"/>
+    </row>
+    <row r="30" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="49"/>
-      <c r="B30" s="81"/>
-      <c r="C30" s="82"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B30" s="60"/>
+      <c r="C30" s="61"/>
+    </row>
+    <row r="31" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="49"/>
-      <c r="B31" s="81"/>
-      <c r="C31" s="82"/>
+      <c r="B31" s="60"/>
+      <c r="C31" s="61"/>
     </row>
     <row r="32" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="52"/>
@@ -8147,16 +8202,289 @@
       <c r="B72" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="C19:C21"/>
     <mergeCell ref="C22:C23"/>
-    <mergeCell ref="C24:C27"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="C26:C27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6078F90-1BFA-44D9-9906-5A72B5F0645C}">
+  <dimension ref="A1:C35"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.140625" customWidth="1"/>
+    <col min="2" max="2" width="76.140625" customWidth="1"/>
+    <col min="3" max="3" width="24" style="8" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>314</v>
+      </c>
+      <c r="C1" s="48" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="49"/>
+      <c r="B2" s="57" t="s">
+        <v>311</v>
+      </c>
+      <c r="C2" s="85">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="49"/>
+      <c r="B3" s="58" t="s">
+        <v>312</v>
+      </c>
+      <c r="C3" s="86"/>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="49"/>
+      <c r="B4" s="59" t="s">
+        <v>313</v>
+      </c>
+      <c r="C4" s="87"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="49"/>
+      <c r="B5" s="57" t="s">
+        <v>340</v>
+      </c>
+      <c r="C5" s="85">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="49"/>
+      <c r="B6" s="59" t="s">
+        <v>341</v>
+      </c>
+      <c r="C6" s="87"/>
+    </row>
+    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="49"/>
+      <c r="B7" s="91" t="s">
+        <v>362</v>
+      </c>
+      <c r="C7" s="92">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="52"/>
+      <c r="B8" s="53"/>
+      <c r="C8" s="54"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="44"/>
+      <c r="B9" s="44" t="s">
+        <v>332</v>
+      </c>
+      <c r="C9" s="47">
+        <f>SUM(C2:C8)</f>
+        <v>2300</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="49"/>
+      <c r="B11" s="49"/>
+      <c r="C11" s="55"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="49"/>
+      <c r="B12" s="49"/>
+      <c r="C12" s="55"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="44"/>
+      <c r="B13" s="44" t="s">
+        <v>337</v>
+      </c>
+      <c r="C13" s="47">
+        <f>SUM(C10:C12)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="7"/>
+      <c r="B14" s="7" t="s">
+        <v>338</v>
+      </c>
+      <c r="C14" s="48">
+        <f>C9-C13</f>
+        <v>2300</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="14"/>
+    </row>
+    <row r="30" spans="2:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="B30" s="14" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B31" s="14"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="14"/>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="14"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="C5:C6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18A08465-7957-474D-A298-889861A0696A}">
+  <dimension ref="A1:H12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C11:C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="23.5703125" style="8" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="8" width="11.42578125" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B1" s="8">
+        <v>946859</v>
+      </c>
+      <c r="C1" s="8">
+        <v>530000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>359</v>
+      </c>
+      <c r="B2" s="8">
+        <v>104471</v>
+      </c>
+      <c r="C2" s="8">
+        <v>42200</v>
+      </c>
+      <c r="D2" s="8">
+        <v>62271</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>360</v>
+      </c>
+      <c r="B3" s="8">
+        <v>438939</v>
+      </c>
+      <c r="C3" s="8">
+        <v>439939</v>
+      </c>
+      <c r="D3" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="8">
+        <v>9430</v>
+      </c>
+      <c r="C4" s="8">
+        <v>0</v>
+      </c>
+      <c r="D4" s="8">
+        <v>9430</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="8">
+        <f>SUM(B2:B5)</f>
+        <v>552840</v>
+      </c>
+      <c r="C6" s="8">
+        <f>SUM(C2:C5)</f>
+        <v>482139</v>
+      </c>
+      <c r="D6" s="8">
+        <f>SUM(D2:D5)</f>
+        <v>71701</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>359</v>
+      </c>
+      <c r="B10" s="90">
+        <v>2685</v>
+      </c>
+      <c r="F10" s="8">
+        <v>21820</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>360</v>
+      </c>
+      <c r="B11" s="90">
+        <v>13210</v>
+      </c>
+      <c r="C11" s="8">
+        <v>13210</v>
+      </c>
+      <c r="F11" s="8">
+        <v>16675</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>361</v>
+      </c>
+      <c r="B12" s="90">
+        <v>2340</v>
+      </c>
+      <c r="C12" s="8">
+        <v>7930</v>
+      </c>
+      <c r="F12" s="8">
+        <f>F10-F11</f>
+        <v>5145</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F34"/>
   <sheetViews>
@@ -8499,7 +8827,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D98"/>
   <sheetViews>
@@ -8531,12 +8859,12 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="79" t="s">
+      <c r="A2" s="88" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="79"/>
-      <c r="C2" s="79"/>
-      <c r="D2" s="79"/>
+      <c r="B2" s="88"/>
+      <c r="C2" s="88"/>
+      <c r="D2" s="88"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -8839,12 +9167,12 @@
       <c r="D30" s="6"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="80" t="s">
+      <c r="A31" s="89" t="s">
         <v>43</v>
       </c>
-      <c r="B31" s="80"/>
-      <c r="C31" s="80"/>
-      <c r="D31" s="80"/>
+      <c r="B31" s="89"/>
+      <c r="C31" s="89"/>
+      <c r="D31" s="89"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
@@ -9473,10 +9801,10 @@
       <c r="D97" s="6"/>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="80"/>
-      <c r="B98" s="80"/>
-      <c r="C98" s="80"/>
-      <c r="D98" s="80"/>
+      <c r="A98" s="89"/>
+      <c r="B98" s="89"/>
+      <c r="C98" s="89"/>
+      <c r="D98" s="89"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -9488,11 +9816,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A5:F30"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
@@ -9580,43 +9908,43 @@
       <c r="E18" t="s">
         <v>349</v>
       </c>
-      <c r="F18" s="85" t="s">
+      <c r="F18" s="64" t="s">
         <v>348</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F19" s="84" t="s">
+      <c r="F19" s="63" t="s">
         <v>347</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="83">
+      <c r="B20" s="62">
         <f>SUM(B17:B19)</f>
         <v>1316</v>
       </c>
-      <c r="C20" s="83">
+      <c r="C20" s="62">
         <f>SUM(C17:C19)</f>
         <v>4300</v>
       </c>
-      <c r="D20" s="83">
+      <c r="D20" s="62">
         <f>SUM(D17:D19)</f>
         <v>2984</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B23" s="87" t="s">
+      <c r="B23" s="66" t="s">
         <v>334</v>
       </c>
-      <c r="C23" s="87" t="s">
+      <c r="C23" s="66" t="s">
         <v>351</v>
       </c>
-      <c r="D23" s="87" t="s">
+      <c r="D23" s="66" t="s">
         <v>352</v>
       </c>
-      <c r="E23" s="87" t="s">
+      <c r="E23" s="66" t="s">
         <v>353</v>
       </c>
-      <c r="F23" s="88" t="s">
+      <c r="F23" s="67" t="s">
         <v>354</v>
       </c>
     </row>
@@ -9627,11 +9955,11 @@
       <c r="C24" s="8">
         <v>3800</v>
       </c>
-      <c r="D24" s="86">
+      <c r="D24" s="65">
         <f>C24*100/4300/100</f>
         <v>0.88372093023255816</v>
       </c>
-      <c r="E24" s="83">
+      <c r="E24" s="62">
         <f>B24*D24-B17</f>
         <v>474.69767441860472</v>
       </c>
@@ -9647,11 +9975,11 @@
       <c r="C25" s="8">
         <v>500</v>
       </c>
-      <c r="D25" s="86">
+      <c r="D25" s="65">
         <f>C25*100/4300/100</f>
         <v>0.11627906976744186</v>
       </c>
-      <c r="E25" s="83">
+      <c r="E25" s="62">
         <f>B25*D25-B18</f>
         <v>9.3023255813953369</v>
       </c>
@@ -9661,16 +9989,16 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B28" s="87" t="s">
+      <c r="B28" s="66" t="s">
         <v>334</v>
       </c>
-      <c r="C28" s="87" t="s">
+      <c r="C28" s="66" t="s">
         <v>355</v>
       </c>
-      <c r="D28" s="87" t="s">
+      <c r="D28" s="66" t="s">
         <v>352</v>
       </c>
-      <c r="E28" s="89" t="s">
+      <c r="E28" s="68" t="s">
         <v>356</v>
       </c>
     </row>
@@ -9681,7 +10009,7 @@
       <c r="C29" s="8">
         <v>1116</v>
       </c>
-      <c r="D29" s="86">
+      <c r="D29" s="65">
         <f>C29*100/1316/100</f>
         <v>0.84802431610942253</v>
       </c>
@@ -9697,7 +10025,7 @@
       <c r="C30" s="8">
         <v>200</v>
       </c>
-      <c r="D30" s="86">
+      <c r="D30" s="65">
         <f>C30*100/1316/100</f>
         <v>0.1519756838905775</v>
       </c>

</xml_diff>

<commit_message>
Se suben cambios de código, lo último que se genera es al impresión de evaluaciones.
</commit_message>
<xml_diff>
--- a/Documents/Actividades realizadas/ActividadesN_.xlsx
+++ b/Documents/Actividades realizadas/ActividadesN_.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\VioletaSystem\Documents\Actividades realizadas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C59D8D3-7D92-4CFE-9F34-8FC8B0C07BD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F447B8BB-5F87-4D18-B33A-D3496475045E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HORAS" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="363">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="370">
   <si>
     <t>Descripción</t>
   </si>
@@ -1126,6 +1126,27 @@
   </si>
   <si>
     <t>Instalación y configuración de impresora en Sarita</t>
+  </si>
+  <si>
+    <t>Configuración para dar acceso a inventario físico a los vendedores master y configuracion de permiso para que no puedan ver los costos y los precios</t>
+  </si>
+  <si>
+    <t>Ajustes para diferenciar los inventarios físicos de los verdaderos y modificacion de procesos de cierre para que no afecten en inventarios, Eliminación de verificacion para cambio de precio en venta de sarita</t>
+  </si>
+  <si>
+    <t>Ajuste al input de la verificación de permisos</t>
+  </si>
+  <si>
+    <t>Modificación de ticket para agregar impresión de calificación</t>
+  </si>
+  <si>
+    <t>Configuración al mostrador</t>
+  </si>
+  <si>
+    <t>Modificación de ticket para agregar impresión de sarita</t>
+  </si>
+  <si>
+    <t>Instalación de código en violeta y servicio de impresión</t>
   </si>
 </sst>
 </file>
@@ -1523,6 +1544,37 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="11" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="44" fontId="3" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1538,9 +1590,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1549,27 +1598,6 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="11" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1585,13 +1613,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="11" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1910,11 +1931,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K309"/>
+  <dimension ref="A1:K314"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A256" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G265" sqref="G265"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A265" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C268" sqref="C268:C272"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7043,7 +7064,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="257" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A257" s="5"/>
       <c r="C257" s="39"/>
       <c r="D257" s="14" t="s">
@@ -7059,7 +7080,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="258" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A258" s="5"/>
       <c r="C258" s="39"/>
       <c r="D258" t="s">
@@ -7075,7 +7096,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="259" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A259" s="5"/>
       <c r="C259" s="39"/>
       <c r="D259" s="14" t="s">
@@ -7091,7 +7112,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="260" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A260" s="5"/>
       <c r="C260" s="39"/>
       <c r="D260" s="14" t="s">
@@ -7107,7 +7128,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="261" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A261" s="5"/>
       <c r="C261" s="39"/>
       <c r="D261" s="14" t="s">
@@ -7123,8 +7144,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="262" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A262" s="5"/>
+      <c r="C262" s="39"/>
       <c r="D262" s="14" t="s">
         <v>340</v>
       </c>
@@ -7138,8 +7160,9 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="263" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A263" s="5"/>
+      <c r="C263" s="39"/>
       <c r="D263" s="14" t="s">
         <v>341</v>
       </c>
@@ -7153,8 +7176,9 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="264" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A264" s="5"/>
+      <c r="C264" s="39"/>
       <c r="D264" s="14" t="s">
         <v>357</v>
       </c>
@@ -7168,8 +7192,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="265" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A265" s="5"/>
+      <c r="C265" s="39"/>
       <c r="D265" s="14" t="s">
         <v>358</v>
       </c>
@@ -7183,256 +7208,324 @@
         <v>2</v>
       </c>
     </row>
-    <row r="266" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A266" s="5"/>
-      <c r="D266" s="14"/>
-      <c r="E266" s="2"/>
-      <c r="F266" s="2"/>
-    </row>
-    <row r="267" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C266" s="39"/>
+      <c r="D266" s="14" t="s">
+        <v>363</v>
+      </c>
+      <c r="E266" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="F266" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="H266" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="267" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A267" s="5"/>
-      <c r="D267" s="14"/>
-      <c r="E267" s="2"/>
-      <c r="F267" s="2"/>
-    </row>
-    <row r="268" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C267" s="39"/>
+      <c r="D267" s="14" t="s">
+        <v>364</v>
+      </c>
+      <c r="E267" s="2">
+        <v>0.59722222222222221</v>
+      </c>
+      <c r="F267" s="2">
+        <v>0.6875</v>
+      </c>
+      <c r="H267" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="268" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A268" s="5"/>
-      <c r="E268" s="2"/>
-      <c r="F268" s="2"/>
-    </row>
-    <row r="269" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C268" s="39"/>
+      <c r="D268" s="14" t="s">
+        <v>365</v>
+      </c>
+      <c r="E268" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="F268" s="2">
+        <v>0.40277777777777779</v>
+      </c>
+      <c r="H268" s="15">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="269" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A269" s="5"/>
-      <c r="E269" s="2"/>
-      <c r="F269" s="2"/>
-    </row>
-    <row r="270" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A270" s="81" t="s">
+      <c r="C269" s="10">
+        <v>45748</v>
+      </c>
+      <c r="D269" s="14" t="s">
+        <v>366</v>
+      </c>
+      <c r="E269" s="2">
+        <v>0.68680555555555556</v>
+      </c>
+      <c r="F269" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="H269" s="15">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="270" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A270" s="5"/>
+      <c r="C270" s="10">
+        <v>45748</v>
+      </c>
+      <c r="D270" s="14" t="s">
+        <v>367</v>
+      </c>
+      <c r="E270" s="2">
+        <v>0.76041666666666663</v>
+      </c>
+      <c r="F270" s="2">
+        <v>0.78680555555555554</v>
+      </c>
+      <c r="H270" s="15">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="271" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A271" s="5"/>
+      <c r="C271" s="10">
+        <v>45748</v>
+      </c>
+      <c r="D271" s="14" t="s">
+        <v>368</v>
+      </c>
+      <c r="E271" s="2">
+        <v>0.41805555555555557</v>
+      </c>
+      <c r="F271" s="2">
+        <v>0.47222222222222221</v>
+      </c>
+      <c r="H271" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="272" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A272" s="5"/>
+      <c r="C272" s="10">
+        <v>45749</v>
+      </c>
+      <c r="D272" s="14" t="s">
+        <v>369</v>
+      </c>
+      <c r="E272" s="2">
+        <v>0.51388888888888884</v>
+      </c>
+      <c r="F272" s="2">
+        <v>0.53541666666666665</v>
+      </c>
+      <c r="H272" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="273" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A273" s="5"/>
+      <c r="E273" s="2"/>
+      <c r="F273" s="2"/>
+    </row>
+    <row r="274" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A274" s="5"/>
+      <c r="E274" s="2"/>
+      <c r="F274" s="2"/>
+    </row>
+    <row r="275" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A275" s="75" t="s">
         <v>165</v>
       </c>
-      <c r="B270" s="81"/>
-      <c r="C270" s="81"/>
-      <c r="D270" s="81"/>
-      <c r="E270" s="81"/>
-      <c r="F270" s="81"/>
-      <c r="G270" s="17">
-        <f>SUM(G2:G269)</f>
+      <c r="B275" s="75"/>
+      <c r="C275" s="75"/>
+      <c r="D275" s="75"/>
+      <c r="E275" s="75"/>
+      <c r="F275" s="75"/>
+      <c r="G275" s="17">
+        <f>SUM(G2:G274)</f>
         <v>314.78999999999996</v>
       </c>
-      <c r="H270" s="17">
-        <f>SUM(H2:H269)</f>
-        <v>59.8</v>
-      </c>
-    </row>
-    <row r="271" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A271" s="81" t="s">
+      <c r="H275" s="17">
+        <f>SUM(H2:H274)</f>
+        <v>67.3</v>
+      </c>
+    </row>
+    <row r="276" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A276" s="75" t="s">
         <v>139</v>
       </c>
-      <c r="B271" s="81"/>
-      <c r="C271" s="81"/>
-      <c r="D271" s="81"/>
-      <c r="E271" s="81"/>
-      <c r="F271" s="81"/>
-      <c r="G271" s="17">
+      <c r="B276" s="75"/>
+      <c r="C276" s="75"/>
+      <c r="D276" s="75"/>
+      <c r="E276" s="75"/>
+      <c r="F276" s="75"/>
+      <c r="G276" s="17">
         <v>200</v>
       </c>
-      <c r="H271" s="17">
+      <c r="H276" s="17">
         <v>300</v>
       </c>
     </row>
-    <row r="272" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A272" s="81" t="s">
+    <row r="277" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A277" s="75" t="s">
         <v>166</v>
       </c>
-      <c r="B272" s="81"/>
-      <c r="C272" s="81"/>
-      <c r="D272" s="81"/>
-      <c r="E272" s="81"/>
-      <c r="F272" s="81"/>
-      <c r="G272" s="18">
-        <f>G271*G270</f>
+      <c r="B277" s="75"/>
+      <c r="C277" s="75"/>
+      <c r="D277" s="75"/>
+      <c r="E277" s="75"/>
+      <c r="F277" s="75"/>
+      <c r="G277" s="18">
+        <f>G276*G275</f>
         <v>62957.999999999993</v>
       </c>
-      <c r="H272" s="19">
-        <f>H271*H270</f>
-        <v>17940</v>
-      </c>
-      <c r="J272">
+      <c r="H277" s="19">
+        <f>H276*H275</f>
+        <v>20190</v>
+      </c>
+      <c r="J277">
         <v>-500</v>
       </c>
     </row>
-    <row r="273" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A273" s="81" t="s">
+    <row r="278" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A278" s="75" t="s">
         <v>140</v>
       </c>
-      <c r="B273" s="81"/>
-      <c r="C273" s="81"/>
-      <c r="D273" s="81"/>
-      <c r="E273" s="81"/>
-      <c r="F273" s="81"/>
-      <c r="G273" s="69">
-        <f>G272+H272</f>
-        <v>80898</v>
-      </c>
-      <c r="H273" s="69"/>
-    </row>
-    <row r="274" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A274" s="11"/>
-      <c r="B274" s="72" t="s">
+      <c r="B278" s="75"/>
+      <c r="C278" s="75"/>
+      <c r="D278" s="75"/>
+      <c r="E278" s="75"/>
+      <c r="F278" s="75"/>
+      <c r="G278" s="80">
+        <f>G277+H277</f>
+        <v>83148</v>
+      </c>
+      <c r="H278" s="80"/>
+    </row>
+    <row r="279" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A279" s="11"/>
+      <c r="B279" s="83" t="s">
         <v>142</v>
       </c>
-      <c r="C274" s="72"/>
-      <c r="D274" s="72"/>
-      <c r="E274" s="72"/>
-      <c r="F274" s="72"/>
-      <c r="G274" s="22"/>
-    </row>
-    <row r="275" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A275" s="12">
+      <c r="C279" s="83"/>
+      <c r="D279" s="83"/>
+      <c r="E279" s="83"/>
+      <c r="F279" s="83"/>
+      <c r="G279" s="22"/>
+    </row>
+    <row r="280" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A280" s="12">
         <v>45109</v>
       </c>
-      <c r="B275" s="73" t="s">
+      <c r="B280" s="84" t="s">
         <v>141</v>
       </c>
-      <c r="C275" s="73"/>
-      <c r="D275" s="73"/>
-      <c r="E275" s="73"/>
-      <c r="F275" s="73"/>
-      <c r="G275" s="75">
+      <c r="C280" s="84"/>
+      <c r="D280" s="84"/>
+      <c r="E280" s="84"/>
+      <c r="F280" s="84"/>
+      <c r="G280" s="85">
         <v>10000</v>
       </c>
-      <c r="H275" s="75"/>
-    </row>
-    <row r="276" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A276" s="12"/>
-      <c r="B276" s="77" t="s">
+      <c r="H280" s="85"/>
+    </row>
+    <row r="281" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A281" s="12"/>
+      <c r="B281" s="87" t="s">
         <v>178</v>
       </c>
-      <c r="C276" s="77"/>
-      <c r="D276" s="77"/>
-      <c r="E276" s="77"/>
-      <c r="F276" s="77"/>
-      <c r="G276" s="75">
+      <c r="C281" s="87"/>
+      <c r="D281" s="87"/>
+      <c r="E281" s="87"/>
+      <c r="F281" s="87"/>
+      <c r="G281" s="85">
         <v>5000</v>
       </c>
-      <c r="H276" s="75"/>
-    </row>
-    <row r="277" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A277" s="12">
+      <c r="H281" s="85"/>
+    </row>
+    <row r="282" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A282" s="12">
         <v>45278</v>
       </c>
-      <c r="B277" s="74" t="s">
+      <c r="B282" s="76" t="s">
         <v>178</v>
       </c>
-      <c r="C277" s="74"/>
-      <c r="D277" s="74"/>
-      <c r="E277" s="74"/>
-      <c r="F277" s="74"/>
-      <c r="G277" s="75">
+      <c r="C282" s="76"/>
+      <c r="D282" s="76"/>
+      <c r="E282" s="76"/>
+      <c r="F282" s="76"/>
+      <c r="G282" s="85">
         <v>9800</v>
       </c>
-      <c r="H277" s="75"/>
-    </row>
-    <row r="278" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A278" s="12"/>
-      <c r="B278" s="74"/>
-      <c r="C278" s="74"/>
-      <c r="D278" s="74"/>
-      <c r="E278" s="74"/>
-      <c r="F278" s="74"/>
-      <c r="G278" s="76"/>
-      <c r="H278" s="76"/>
-    </row>
-    <row r="279" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A279" s="12"/>
-      <c r="B279" s="74"/>
-      <c r="C279" s="74"/>
-      <c r="D279" s="74"/>
-      <c r="E279" s="74"/>
-      <c r="F279" s="74"/>
-      <c r="G279" s="76"/>
-      <c r="H279" s="76"/>
-    </row>
-    <row r="280" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A280" s="12"/>
-      <c r="B280" s="74"/>
-      <c r="C280" s="74"/>
-      <c r="D280" s="74"/>
-      <c r="E280" s="74"/>
-      <c r="F280" s="74"/>
-      <c r="G280" s="76"/>
-      <c r="H280" s="76"/>
-    </row>
-    <row r="281" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A281" s="12"/>
-      <c r="B281" s="74" t="s">
+      <c r="H282" s="85"/>
+    </row>
+    <row r="283" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A283" s="12"/>
+      <c r="B283" s="76"/>
+      <c r="C283" s="76"/>
+      <c r="D283" s="76"/>
+      <c r="E283" s="76"/>
+      <c r="F283" s="76"/>
+      <c r="G283" s="86"/>
+      <c r="H283" s="86"/>
+    </row>
+    <row r="284" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A284" s="12"/>
+      <c r="B284" s="76"/>
+      <c r="C284" s="76"/>
+      <c r="D284" s="76"/>
+      <c r="E284" s="76"/>
+      <c r="F284" s="76"/>
+      <c r="G284" s="86"/>
+      <c r="H284" s="86"/>
+    </row>
+    <row r="285" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A285" s="12"/>
+      <c r="B285" s="76"/>
+      <c r="C285" s="76"/>
+      <c r="D285" s="76"/>
+      <c r="E285" s="76"/>
+      <c r="F285" s="76"/>
+      <c r="G285" s="86"/>
+      <c r="H285" s="86"/>
+    </row>
+    <row r="286" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A286" s="12"/>
+      <c r="B286" s="76" t="s">
         <v>144</v>
       </c>
-      <c r="C281" s="74"/>
-      <c r="D281" s="74"/>
-      <c r="E281" s="74"/>
-      <c r="F281" s="74"/>
-      <c r="G281" s="75">
-        <f>SUM(G275:H280)</f>
+      <c r="C286" s="76"/>
+      <c r="D286" s="76"/>
+      <c r="E286" s="76"/>
+      <c r="F286" s="76"/>
+      <c r="G286" s="85">
+        <f>SUM(G280:H285)</f>
         <v>24800</v>
       </c>
-      <c r="H281" s="75"/>
-    </row>
-    <row r="282" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A282" s="70" t="s">
+      <c r="H286" s="85"/>
+    </row>
+    <row r="287" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A287" s="81" t="s">
         <v>143</v>
       </c>
-      <c r="B282" s="70"/>
-      <c r="C282" s="70"/>
-      <c r="D282" s="70"/>
-      <c r="E282" s="70"/>
-      <c r="F282" s="70"/>
-      <c r="G282" s="71">
-        <f>G273-G281</f>
-        <v>56098</v>
-      </c>
-      <c r="H282" s="71"/>
-    </row>
-    <row r="283" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A283" s="12"/>
-      <c r="B283" s="13"/>
-      <c r="C283" s="13"/>
-      <c r="D283" s="13"/>
-      <c r="E283" s="13"/>
-      <c r="F283" s="13"/>
-    </row>
-    <row r="284" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A284" s="12"/>
-      <c r="B284" s="13"/>
-      <c r="C284" s="13"/>
-      <c r="D284" s="13"/>
-      <c r="E284" s="13"/>
-      <c r="F284" s="13"/>
-    </row>
-    <row r="285" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A285" s="12"/>
-      <c r="B285" s="13"/>
-      <c r="C285" s="13"/>
-      <c r="D285" s="13"/>
-      <c r="E285" s="13"/>
-      <c r="F285" s="13"/>
-    </row>
-    <row r="286" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A286" s="12"/>
-      <c r="B286" s="13"/>
-      <c r="C286" s="13"/>
-      <c r="D286" s="13"/>
-      <c r="E286" s="13"/>
-      <c r="F286" s="13"/>
-    </row>
-    <row r="287" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A287" s="12"/>
-      <c r="B287" s="13"/>
-      <c r="C287" s="13"/>
-      <c r="D287" s="13"/>
-      <c r="E287" s="13"/>
-      <c r="F287" s="13"/>
-    </row>
-    <row r="288" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B287" s="81"/>
+      <c r="C287" s="81"/>
+      <c r="D287" s="81"/>
+      <c r="E287" s="81"/>
+      <c r="F287" s="81"/>
+      <c r="G287" s="82">
+        <f>G278-G286</f>
+        <v>58348</v>
+      </c>
+      <c r="H287" s="82"/>
+    </row>
+    <row r="288" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A288" s="12"/>
       <c r="B288" s="13"/>
       <c r="C288" s="13"/>
@@ -7440,7 +7533,7 @@
       <c r="E288" s="13"/>
       <c r="F288" s="13"/>
     </row>
-    <row r="289" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A289" s="12"/>
       <c r="B289" s="13"/>
       <c r="C289" s="13"/>
@@ -7448,7 +7541,7 @@
       <c r="E289" s="13"/>
       <c r="F289" s="13"/>
     </row>
-    <row r="290" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A290" s="12"/>
       <c r="B290" s="13"/>
       <c r="C290" s="13"/>
@@ -7456,7 +7549,7 @@
       <c r="E290" s="13"/>
       <c r="F290" s="13"/>
     </row>
-    <row r="291" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A291" s="12"/>
       <c r="B291" s="13"/>
       <c r="C291" s="13"/>
@@ -7464,7 +7557,7 @@
       <c r="E291" s="13"/>
       <c r="F291" s="13"/>
     </row>
-    <row r="292" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A292" s="12"/>
       <c r="B292" s="13"/>
       <c r="C292" s="13"/>
@@ -7472,7 +7565,7 @@
       <c r="E292" s="13"/>
       <c r="F292" s="13"/>
     </row>
-    <row r="293" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A293" s="12"/>
       <c r="B293" s="13"/>
       <c r="C293" s="13"/>
@@ -7480,7 +7573,7 @@
       <c r="E293" s="13"/>
       <c r="F293" s="13"/>
     </row>
-    <row r="294" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A294" s="12"/>
       <c r="B294" s="13"/>
       <c r="C294" s="13"/>
@@ -7488,7 +7581,7 @@
       <c r="E294" s="13"/>
       <c r="F294" s="13"/>
     </row>
-    <row r="295" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A295" s="12"/>
       <c r="B295" s="13"/>
       <c r="C295" s="13"/>
@@ -7496,7 +7589,7 @@
       <c r="E295" s="13"/>
       <c r="F295" s="13"/>
     </row>
-    <row r="296" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A296" s="12"/>
       <c r="B296" s="13"/>
       <c r="C296" s="13"/>
@@ -7504,7 +7597,7 @@
       <c r="E296" s="13"/>
       <c r="F296" s="13"/>
     </row>
-    <row r="297" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A297" s="12"/>
       <c r="B297" s="13"/>
       <c r="C297" s="13"/>
@@ -7512,7 +7605,7 @@
       <c r="E297" s="13"/>
       <c r="F297" s="13"/>
     </row>
-    <row r="298" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A298" s="12"/>
       <c r="B298" s="13"/>
       <c r="C298" s="13"/>
@@ -7520,7 +7613,7 @@
       <c r="E298" s="13"/>
       <c r="F298" s="13"/>
     </row>
-    <row r="299" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A299" s="12"/>
       <c r="B299" s="13"/>
       <c r="C299" s="13"/>
@@ -7528,7 +7621,7 @@
       <c r="E299" s="13"/>
       <c r="F299" s="13"/>
     </row>
-    <row r="300" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A300" s="12"/>
       <c r="B300" s="13"/>
       <c r="C300" s="13"/>
@@ -7536,191 +7629,231 @@
       <c r="E300" s="13"/>
       <c r="F300" s="13"/>
     </row>
-    <row r="301" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A301" s="10"/>
-      <c r="B301" s="82" t="s">
+    <row r="301" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A301" s="12"/>
+      <c r="B301" s="13"/>
+      <c r="C301" s="13"/>
+      <c r="D301" s="13"/>
+      <c r="E301" s="13"/>
+      <c r="F301" s="13"/>
+    </row>
+    <row r="302" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A302" s="12"/>
+      <c r="B302" s="13"/>
+      <c r="C302" s="13"/>
+      <c r="D302" s="13"/>
+      <c r="E302" s="13"/>
+      <c r="F302" s="13"/>
+    </row>
+    <row r="303" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A303" s="12"/>
+      <c r="B303" s="13"/>
+      <c r="C303" s="13"/>
+      <c r="D303" s="13"/>
+      <c r="E303" s="13"/>
+      <c r="F303" s="13"/>
+    </row>
+    <row r="304" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A304" s="12"/>
+      <c r="B304" s="13"/>
+      <c r="C304" s="13"/>
+      <c r="D304" s="13"/>
+      <c r="E304" s="13"/>
+      <c r="F304" s="13"/>
+    </row>
+    <row r="305" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A305" s="12"/>
+      <c r="B305" s="13"/>
+      <c r="C305" s="13"/>
+      <c r="D305" s="13"/>
+      <c r="E305" s="13"/>
+      <c r="F305" s="13"/>
+    </row>
+    <row r="306" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A306" s="10"/>
+      <c r="B306" s="77" t="s">
         <v>138</v>
       </c>
-      <c r="C301" s="82"/>
-      <c r="D301" s="82"/>
-      <c r="E301" s="82"/>
-      <c r="F301" s="82"/>
-      <c r="G301" s="21"/>
-      <c r="H301" s="21"/>
-      <c r="I301" s="8">
-        <f>G270+H270</f>
-        <v>374.59</v>
-      </c>
-      <c r="J301" s="8">
-        <f>I301</f>
-        <v>374.59</v>
-      </c>
-    </row>
-    <row r="302" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A302" s="5"/>
-      <c r="B302" s="83" t="s">
+      <c r="C306" s="77"/>
+      <c r="D306" s="77"/>
+      <c r="E306" s="77"/>
+      <c r="F306" s="77"/>
+      <c r="G306" s="21"/>
+      <c r="H306" s="21"/>
+      <c r="I306" s="8">
+        <f>G275+H275</f>
+        <v>382.09</v>
+      </c>
+      <c r="J306" s="8">
+        <f>I306</f>
+        <v>382.09</v>
+      </c>
+    </row>
+    <row r="307" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A307" s="5"/>
+      <c r="B307" s="78" t="s">
         <v>139</v>
       </c>
-      <c r="C302" s="83"/>
-      <c r="D302" s="83"/>
-      <c r="E302" s="83"/>
-      <c r="F302" s="83"/>
-      <c r="I302" s="8">
+      <c r="C307" s="78"/>
+      <c r="D307" s="78"/>
+      <c r="E307" s="78"/>
+      <c r="F307" s="78"/>
+      <c r="I307" s="8">
         <v>300</v>
       </c>
-      <c r="J302" s="8">
+      <c r="J307" s="8">
         <v>200</v>
       </c>
     </row>
-    <row r="303" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A303" s="5"/>
-      <c r="B303" s="83" t="s">
+    <row r="308" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A308" s="5"/>
+      <c r="B308" s="78" t="s">
         <v>140</v>
       </c>
-      <c r="C303" s="83"/>
-      <c r="D303" s="83"/>
-      <c r="E303" s="83"/>
-      <c r="F303" s="83"/>
-      <c r="I303" s="9">
-        <f>I302*I301</f>
-        <v>112376.99999999999</v>
-      </c>
-      <c r="J303" s="9">
-        <f>J302*J301</f>
-        <v>74918</v>
-      </c>
-    </row>
-    <row r="304" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A304" s="23"/>
-      <c r="B304" s="84" t="s">
+      <c r="C308" s="78"/>
+      <c r="D308" s="78"/>
+      <c r="E308" s="78"/>
+      <c r="F308" s="78"/>
+      <c r="I308" s="9">
+        <f>I307*I306</f>
+        <v>114626.99999999999</v>
+      </c>
+      <c r="J308" s="9">
+        <f>J307*J306</f>
+        <v>76418</v>
+      </c>
+    </row>
+    <row r="309" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A309" s="23"/>
+      <c r="B309" s="79" t="s">
         <v>142</v>
       </c>
-      <c r="C304" s="84"/>
-      <c r="D304" s="84"/>
-      <c r="E304" s="84"/>
-      <c r="F304" s="84"/>
-      <c r="G304" s="24"/>
-      <c r="H304" s="24"/>
-      <c r="I304" s="25"/>
-      <c r="J304" s="25"/>
-    </row>
-    <row r="305" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A305" s="26">
+      <c r="C309" s="79"/>
+      <c r="D309" s="79"/>
+      <c r="E309" s="79"/>
+      <c r="F309" s="79"/>
+      <c r="G309" s="24"/>
+      <c r="H309" s="24"/>
+      <c r="I309" s="25"/>
+      <c r="J309" s="25"/>
+    </row>
+    <row r="310" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A310" s="26">
         <v>45109</v>
       </c>
-      <c r="B305" s="79" t="s">
+      <c r="B310" s="73" t="s">
         <v>141</v>
       </c>
-      <c r="C305" s="79"/>
-      <c r="D305" s="79"/>
-      <c r="E305" s="79"/>
-      <c r="F305" s="79"/>
-      <c r="G305" s="27"/>
-      <c r="H305" s="27"/>
-      <c r="I305" s="28">
+      <c r="C310" s="73"/>
+      <c r="D310" s="73"/>
+      <c r="E310" s="73"/>
+      <c r="F310" s="73"/>
+      <c r="G310" s="27"/>
+      <c r="H310" s="27"/>
+      <c r="I310" s="28">
         <v>10000</v>
       </c>
-      <c r="J305" s="28">
+      <c r="J310" s="28">
         <v>10000</v>
       </c>
     </row>
-    <row r="306" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A306" s="26"/>
-      <c r="B306" s="29"/>
-      <c r="C306" s="29"/>
-      <c r="D306" s="29"/>
-      <c r="E306" s="29"/>
-      <c r="F306" s="29"/>
-      <c r="G306" s="27"/>
-      <c r="H306" s="27"/>
-      <c r="I306" s="30"/>
-      <c r="J306" s="30"/>
-    </row>
-    <row r="307" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A307" s="26"/>
-      <c r="B307" s="29"/>
-      <c r="C307" s="29"/>
-      <c r="D307" s="29"/>
-      <c r="E307" s="29"/>
-      <c r="F307" s="29"/>
-      <c r="G307" s="27"/>
-      <c r="H307" s="27"/>
-      <c r="I307" s="30"/>
-      <c r="J307" s="30"/>
-    </row>
-    <row r="308" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A308" s="26"/>
-      <c r="B308" s="80" t="s">
+    <row r="311" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A311" s="26"/>
+      <c r="B311" s="29"/>
+      <c r="C311" s="29"/>
+      <c r="D311" s="29"/>
+      <c r="E311" s="29"/>
+      <c r="F311" s="29"/>
+      <c r="G311" s="27"/>
+      <c r="H311" s="27"/>
+      <c r="I311" s="30"/>
+      <c r="J311" s="30"/>
+    </row>
+    <row r="312" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A312" s="26"/>
+      <c r="B312" s="29"/>
+      <c r="C312" s="29"/>
+      <c r="D312" s="29"/>
+      <c r="E312" s="29"/>
+      <c r="F312" s="29"/>
+      <c r="G312" s="27"/>
+      <c r="H312" s="27"/>
+      <c r="I312" s="30"/>
+      <c r="J312" s="30"/>
+    </row>
+    <row r="313" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A313" s="26"/>
+      <c r="B313" s="74" t="s">
         <v>144</v>
       </c>
-      <c r="C308" s="80"/>
-      <c r="D308" s="80"/>
-      <c r="E308" s="80"/>
-      <c r="F308" s="80"/>
-      <c r="G308" s="27"/>
-      <c r="H308" s="27"/>
-      <c r="I308" s="31">
-        <f>SUM(I305:I307)</f>
+      <c r="C313" s="74"/>
+      <c r="D313" s="74"/>
+      <c r="E313" s="74"/>
+      <c r="F313" s="74"/>
+      <c r="G313" s="27"/>
+      <c r="H313" s="27"/>
+      <c r="I313" s="31">
+        <f>SUM(I310:I312)</f>
         <v>10000</v>
       </c>
-      <c r="J308" s="31">
-        <f>SUM(J305:J307)</f>
+      <c r="J313" s="31">
+        <f>SUM(J310:J312)</f>
         <v>10000</v>
       </c>
     </row>
-    <row r="309" spans="1:10" ht="33.75" x14ac:dyDescent="0.5">
-      <c r="A309" s="32">
+    <row r="314" spans="1:10" ht="33.75" x14ac:dyDescent="0.5">
+      <c r="A314" s="32">
         <v>45109</v>
       </c>
-      <c r="B309" s="78" t="s">
+      <c r="B314" s="72" t="s">
         <v>143</v>
       </c>
-      <c r="C309" s="78"/>
-      <c r="D309" s="78"/>
-      <c r="E309" s="78"/>
-      <c r="F309" s="78"/>
-      <c r="G309" s="33"/>
-      <c r="H309" s="33"/>
-      <c r="I309" s="34">
-        <f>I303-I308</f>
-        <v>102376.99999999999</v>
-      </c>
-      <c r="J309" s="34">
-        <f>J303-J308</f>
-        <v>64918</v>
+      <c r="C314" s="72"/>
+      <c r="D314" s="72"/>
+      <c r="E314" s="72"/>
+      <c r="F314" s="72"/>
+      <c r="G314" s="33"/>
+      <c r="H314" s="33"/>
+      <c r="I314" s="34">
+        <f>I308-I313</f>
+        <v>104626.99999999999</v>
+      </c>
+      <c r="J314" s="34">
+        <f>J308-J313</f>
+        <v>66418</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="B309:F309"/>
-    <mergeCell ref="B305:F305"/>
-    <mergeCell ref="B308:F308"/>
-    <mergeCell ref="A271:F271"/>
-    <mergeCell ref="A270:F270"/>
-    <mergeCell ref="A272:F272"/>
-    <mergeCell ref="A273:F273"/>
+    <mergeCell ref="G278:H278"/>
+    <mergeCell ref="A287:F287"/>
+    <mergeCell ref="G287:H287"/>
     <mergeCell ref="B279:F279"/>
     <mergeCell ref="B280:F280"/>
-    <mergeCell ref="B301:F301"/>
-    <mergeCell ref="B302:F302"/>
-    <mergeCell ref="B303:F303"/>
-    <mergeCell ref="B304:F304"/>
-    <mergeCell ref="G273:H273"/>
-    <mergeCell ref="A282:F282"/>
+    <mergeCell ref="B286:F286"/>
+    <mergeCell ref="G280:H280"/>
+    <mergeCell ref="G281:H281"/>
+    <mergeCell ref="G286:H286"/>
+    <mergeCell ref="G283:H283"/>
+    <mergeCell ref="G284:H284"/>
+    <mergeCell ref="G285:H285"/>
     <mergeCell ref="G282:H282"/>
-    <mergeCell ref="B274:F274"/>
-    <mergeCell ref="B275:F275"/>
+    <mergeCell ref="B282:F282"/>
     <mergeCell ref="B281:F281"/>
-    <mergeCell ref="G275:H275"/>
-    <mergeCell ref="G276:H276"/>
-    <mergeCell ref="G281:H281"/>
-    <mergeCell ref="G278:H278"/>
-    <mergeCell ref="G279:H279"/>
-    <mergeCell ref="G280:H280"/>
-    <mergeCell ref="G277:H277"/>
-    <mergeCell ref="B277:F277"/>
-    <mergeCell ref="B276:F276"/>
-    <mergeCell ref="B278:F278"/>
+    <mergeCell ref="B283:F283"/>
+    <mergeCell ref="B314:F314"/>
+    <mergeCell ref="B310:F310"/>
+    <mergeCell ref="B313:F313"/>
+    <mergeCell ref="A276:F276"/>
+    <mergeCell ref="A275:F275"/>
+    <mergeCell ref="A277:F277"/>
+    <mergeCell ref="A278:F278"/>
+    <mergeCell ref="B284:F284"/>
+    <mergeCell ref="B285:F285"/>
+    <mergeCell ref="B306:F306"/>
+    <mergeCell ref="B307:F307"/>
+    <mergeCell ref="B308:F308"/>
+    <mergeCell ref="B309:F309"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -7729,10 +7862,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3B2F9DB-D849-4B99-B5E6-70BB7408BE44}">
-  <dimension ref="A1:C72"/>
+  <dimension ref="A1:C76"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28:C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7911,7 +8044,7 @@
       <c r="B19" s="57" t="s">
         <v>311</v>
       </c>
-      <c r="C19" s="85">
+      <c r="C19" s="88">
         <v>1100</v>
       </c>
     </row>
@@ -7920,21 +8053,21 @@
       <c r="B20" s="58" t="s">
         <v>312</v>
       </c>
-      <c r="C20" s="86"/>
+      <c r="C20" s="89"/>
     </row>
     <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="49"/>
       <c r="B21" s="59" t="s">
         <v>313</v>
       </c>
-      <c r="C21" s="87"/>
+      <c r="C21" s="90"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="49"/>
       <c r="B22" s="57" t="s">
         <v>340</v>
       </c>
-      <c r="C22" s="85">
+      <c r="C22" s="88">
         <v>600</v>
       </c>
     </row>
@@ -7943,14 +8076,14 @@
       <c r="B23" s="59" t="s">
         <v>341</v>
       </c>
-      <c r="C23" s="87"/>
+      <c r="C23" s="90"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="49"/>
       <c r="B24" s="57" t="s">
         <v>340</v>
       </c>
-      <c r="C24" s="85">
+      <c r="C24" s="88">
         <v>600</v>
       </c>
     </row>
@@ -7959,14 +8092,14 @@
       <c r="B25" s="59" t="s">
         <v>341</v>
       </c>
-      <c r="C25" s="87"/>
+      <c r="C25" s="90"/>
     </row>
     <row r="26" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="49"/>
       <c r="B26" s="58" t="s">
         <v>357</v>
       </c>
-      <c r="C26" s="86">
+      <c r="C26" s="89">
         <v>1500</v>
       </c>
     </row>
@@ -7975,94 +8108,82 @@
       <c r="B27" s="59" t="s">
         <v>358</v>
       </c>
-      <c r="C27" s="87"/>
-    </row>
-    <row r="28" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C27" s="90"/>
+    </row>
+    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="49"/>
-      <c r="B28" s="60"/>
-      <c r="C28" s="61"/>
-    </row>
-    <row r="29" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="57" t="s">
+        <v>363</v>
+      </c>
+      <c r="C28" s="88">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="49"/>
-      <c r="B29" s="60"/>
-      <c r="C29" s="61"/>
-    </row>
-    <row r="30" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="59" t="s">
+        <v>364</v>
+      </c>
+      <c r="C29" s="90"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="49"/>
       <c r="B30" s="60"/>
       <c r="C30" s="61"/>
     </row>
-    <row r="31" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="49"/>
       <c r="B31" s="60"/>
       <c r="C31" s="61"/>
     </row>
-    <row r="32" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="52"/>
-      <c r="B32" s="53"/>
-      <c r="C32" s="54"/>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="49"/>
+      <c r="B32" s="60"/>
+      <c r="C32" s="61"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="44"/>
-      <c r="B33" s="44" t="s">
+      <c r="A33" s="49"/>
+      <c r="B33" s="60"/>
+      <c r="C33" s="61"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="49"/>
+      <c r="B34" s="60"/>
+      <c r="C34" s="61"/>
+    </row>
+    <row r="35" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="52"/>
+      <c r="B35" s="53"/>
+      <c r="C35" s="54"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="44"/>
+      <c r="B36" s="44" t="s">
         <v>332</v>
       </c>
-      <c r="C33" s="47">
-        <f>SUM(C2:C32)</f>
-        <v>88600</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
+      <c r="C36" s="47">
+        <f>SUM(C2:C35)</f>
+        <v>89500</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
         <v>120</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="45">
-        <v>45109</v>
-      </c>
-      <c r="B35" s="42" t="s">
-        <v>333</v>
-      </c>
-      <c r="C35" s="46">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="42"/>
-      <c r="B36" s="42" t="s">
-        <v>334</v>
-      </c>
-      <c r="C36" s="46">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="45">
-        <v>45278</v>
-      </c>
-      <c r="B37" s="42" t="s">
-        <v>334</v>
-      </c>
-      <c r="C37" s="46">
-        <v>9800</v>
       </c>
     </row>
     <row r="38" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="45">
-        <v>45347</v>
+        <v>45109</v>
       </c>
       <c r="B38" s="42" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C38" s="46">
-        <v>5000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="39" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="45">
-        <v>45383</v>
-      </c>
+      <c r="A39" s="42"/>
       <c r="B39" s="42" t="s">
         <v>334</v>
       </c>
@@ -8072,52 +8193,54 @@
     </row>
     <row r="40" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="45">
-        <v>45384</v>
+        <v>45278</v>
       </c>
       <c r="B40" s="42" t="s">
         <v>334</v>
       </c>
       <c r="C40" s="46">
+        <v>9800</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="45">
+        <v>45347</v>
+      </c>
+      <c r="B41" s="42" t="s">
+        <v>334</v>
+      </c>
+      <c r="C41" s="46">
         <v>5000</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="56">
+    <row r="42" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="45">
+        <v>45383</v>
+      </c>
+      <c r="B42" s="42" t="s">
+        <v>334</v>
+      </c>
+      <c r="C42" s="46">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="45">
+        <v>45384</v>
+      </c>
+      <c r="B43" s="42" t="s">
+        <v>334</v>
+      </c>
+      <c r="C43" s="46">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="56">
         <v>45419</v>
       </c>
-      <c r="B41" s="49" t="s">
+      <c r="B44" s="49" t="s">
         <v>334</v>
-      </c>
-      <c r="C41" s="55">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="56">
-        <v>45449</v>
-      </c>
-      <c r="B42" s="49" t="s">
-        <v>334</v>
-      </c>
-      <c r="C42" s="55">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="56">
-        <v>45465</v>
-      </c>
-      <c r="B43" s="49" t="s">
-        <v>335</v>
-      </c>
-      <c r="C43" s="55">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="56"/>
-      <c r="B44" s="49" t="s">
-        <v>336</v>
       </c>
       <c r="C44" s="55">
         <v>5000</v>
@@ -8125,88 +8248,129 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="56">
-        <v>45506</v>
+        <v>45449</v>
       </c>
       <c r="B45" s="49" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C45" s="55">
-        <v>15000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="56">
-        <v>45556</v>
+        <v>45465</v>
       </c>
       <c r="B46" s="49" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C46" s="55">
-        <v>5000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="56"/>
       <c r="B47" s="49" t="s">
+        <v>336</v>
+      </c>
+      <c r="C47" s="55">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="56">
+        <v>45506</v>
+      </c>
+      <c r="B48" s="49" t="s">
+        <v>335</v>
+      </c>
+      <c r="C48" s="55">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="56">
+        <v>45556</v>
+      </c>
+      <c r="B49" s="49" t="s">
         <v>334</v>
       </c>
-      <c r="C47" s="55">
+      <c r="C49" s="55">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="56"/>
+      <c r="B50" s="49" t="s">
+        <v>334</v>
+      </c>
+      <c r="C50" s="55">
         <v>3000</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="49"/>
-      <c r="B48" s="49"/>
-      <c r="C48" s="55"/>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="49"/>
-      <c r="B49" s="49"/>
-      <c r="C49" s="55"/>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="44"/>
-      <c r="B50" s="44" t="s">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="49"/>
+      <c r="B51" s="49" t="s">
+        <v>334</v>
+      </c>
+      <c r="C51" s="55">
+        <v>2300</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="49"/>
+      <c r="B52" s="49"/>
+      <c r="C52" s="55"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="49"/>
+      <c r="B53" s="49"/>
+      <c r="C53" s="55"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="44"/>
+      <c r="B54" s="44" t="s">
         <v>337</v>
       </c>
-      <c r="C50" s="47">
-        <f>SUM(C34:C49)</f>
-        <v>84800</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="7"/>
-      <c r="B51" s="7" t="s">
+      <c r="C54" s="47">
+        <f>SUM(C37:C53)</f>
+        <v>87100</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="7"/>
+      <c r="B55" s="7" t="s">
         <v>338</v>
       </c>
-      <c r="C51" s="48">
-        <f>C33-C50</f>
-        <v>3800</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B56" s="14"/>
-    </row>
-    <row r="67" spans="2:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="B67" s="14" t="s">
+      <c r="C55" s="48">
+        <f>C36-C54</f>
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B60" s="14"/>
+    </row>
+    <row r="71" spans="2:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="B71" s="14" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B68" s="14"/>
-    </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B70" s="14"/>
     </row>
     <row r="72" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B72" s="14"/>
     </row>
+    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B74" s="14"/>
+    </row>
+    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B76" s="14"/>
+    </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="C19:C21"/>
     <mergeCell ref="C22:C23"/>
     <mergeCell ref="C24:C25"/>
     <mergeCell ref="C26:C27"/>
+    <mergeCell ref="C28:C29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8214,10 +8378,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6078F90-1BFA-44D9-9906-5A72B5F0645C}">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8243,7 +8407,7 @@
       <c r="B2" s="57" t="s">
         <v>311</v>
       </c>
-      <c r="C2" s="85">
+      <c r="C2" s="88">
         <v>1100</v>
       </c>
     </row>
@@ -8252,21 +8416,21 @@
       <c r="B3" s="58" t="s">
         <v>312</v>
       </c>
-      <c r="C3" s="86"/>
+      <c r="C3" s="89"/>
     </row>
     <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="49"/>
       <c r="B4" s="59" t="s">
         <v>313</v>
       </c>
-      <c r="C4" s="87"/>
+      <c r="C4" s="90"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="49"/>
       <c r="B5" s="57" t="s">
         <v>340</v>
       </c>
-      <c r="C5" s="85">
+      <c r="C5" s="88">
         <v>600</v>
       </c>
     </row>
@@ -8275,88 +8439,174 @@
       <c r="B6" s="59" t="s">
         <v>341</v>
       </c>
-      <c r="C6" s="87"/>
+      <c r="C6" s="90"/>
     </row>
     <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="49"/>
-      <c r="B7" s="91" t="s">
+      <c r="B7" s="70" t="s">
         <v>362</v>
       </c>
-      <c r="C7" s="92">
+      <c r="C7" s="71">
         <v>600</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="52"/>
-      <c r="B8" s="53"/>
-      <c r="C8" s="54"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="44"/>
-      <c r="B9" s="44" t="s">
-        <v>332</v>
-      </c>
-      <c r="C9" s="47">
-        <f>SUM(C2:C8)</f>
-        <v>2300</v>
-      </c>
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="49"/>
+      <c r="B8" s="57" t="s">
+        <v>363</v>
+      </c>
+      <c r="C8" s="88">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="49"/>
+      <c r="B9" s="59" t="s">
+        <v>364</v>
+      </c>
+      <c r="C9" s="90"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>120</v>
+      <c r="A10" s="49"/>
+      <c r="B10" s="57" t="s">
+        <v>365</v>
+      </c>
+      <c r="C10" s="88">
+        <v>1350</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="49"/>
-      <c r="B11" s="49"/>
-      <c r="C11" s="55"/>
+      <c r="B11" s="58" t="s">
+        <v>366</v>
+      </c>
+      <c r="C11" s="89"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="49"/>
-      <c r="B12" s="49"/>
-      <c r="C12" s="55"/>
+      <c r="B12" s="58" t="s">
+        <v>367</v>
+      </c>
+      <c r="C12" s="89"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="44"/>
-      <c r="B13" s="44" t="s">
+      <c r="A13" s="49"/>
+      <c r="B13" s="58" t="s">
+        <v>368</v>
+      </c>
+      <c r="C13" s="89"/>
+    </row>
+    <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="49"/>
+      <c r="B14" s="59" t="s">
+        <v>369</v>
+      </c>
+      <c r="C14" s="90"/>
+    </row>
+    <row r="15" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="52"/>
+      <c r="B15" s="53"/>
+      <c r="C15" s="54"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="44"/>
+      <c r="B16" s="44" t="s">
+        <v>332</v>
+      </c>
+      <c r="C16" s="47">
+        <f>SUM(C2:C15)</f>
+        <v>4550</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="56">
+        <v>45690</v>
+      </c>
+      <c r="B18" s="49" t="s">
+        <v>120</v>
+      </c>
+      <c r="C18" s="55">
+        <v>2300</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="49"/>
+      <c r="B19" s="49"/>
+      <c r="C19" s="55"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="44"/>
+      <c r="B20" s="44" t="s">
         <v>337</v>
       </c>
-      <c r="C13" s="47">
-        <f>SUM(C10:C12)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7" t="s">
+      <c r="C20" s="47">
+        <f>SUM(C17:C19)</f>
+        <v>2300</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="7"/>
+      <c r="B21" s="7" t="s">
         <v>338</v>
       </c>
-      <c r="C14" s="48">
-        <f>C9-C13</f>
-        <v>2300</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B19" s="14"/>
-    </row>
-    <row r="30" spans="2:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="C21" s="48">
+        <f>C16-C20</f>
+        <v>2250</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="14"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="14" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="14" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B30" s="14" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B31" s="14" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B32" s="14" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="B37" s="14" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B31" s="14"/>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" s="14"/>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B35" s="14"/>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B38" s="14"/>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B40" s="14"/>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B42" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="C2:C4"/>
     <mergeCell ref="C5:C6"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C10:C14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8442,7 +8692,7 @@
       <c r="A10" t="s">
         <v>359</v>
       </c>
-      <c r="B10" s="90">
+      <c r="B10" s="69">
         <v>2685</v>
       </c>
       <c r="F10" s="8">
@@ -8453,7 +8703,7 @@
       <c r="A11" t="s">
         <v>360</v>
       </c>
-      <c r="B11" s="90">
+      <c r="B11" s="69">
         <v>13210</v>
       </c>
       <c r="C11" s="8">
@@ -8467,7 +8717,7 @@
       <c r="A12" t="s">
         <v>361</v>
       </c>
-      <c r="B12" s="90">
+      <c r="B12" s="69">
         <v>2340</v>
       </c>
       <c r="C12" s="8">
@@ -8859,12 +9109,12 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="88" t="s">
+      <c r="A2" s="91" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="88"/>
-      <c r="C2" s="88"/>
-      <c r="D2" s="88"/>
+      <c r="B2" s="91"/>
+      <c r="C2" s="91"/>
+      <c r="D2" s="91"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -9167,12 +9417,12 @@
       <c r="D30" s="6"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="89" t="s">
+      <c r="A31" s="92" t="s">
         <v>43</v>
       </c>
-      <c r="B31" s="89"/>
-      <c r="C31" s="89"/>
-      <c r="D31" s="89"/>
+      <c r="B31" s="92"/>
+      <c r="C31" s="92"/>
+      <c r="D31" s="92"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
@@ -9801,10 +10051,10 @@
       <c r="D97" s="6"/>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="89"/>
-      <c r="B98" s="89"/>
-      <c r="C98" s="89"/>
-      <c r="D98" s="89"/>
+      <c r="A98" s="92"/>
+      <c r="B98" s="92"/>
+      <c r="C98" s="92"/>
+      <c r="D98" s="92"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Se hacen instalaciones de los ultimos cambios.
Cambios en el diseño de las tablas de todo el sistema.
Se agrega redondeo en los descuentos de los productos por %.
Se agrega el que revifica y el que recibe en mostrador
</commit_message>
<xml_diff>
--- a/Documents/Actividades realizadas/ActividadesN_.xlsx
+++ b/Documents/Actividades realizadas/ActividadesN_.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\VioletaSystem\Documents\Actividades realizadas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\1.- VioletaSystem\Documents\Actividades realizadas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{457AEA42-EE12-42C9-9FF5-CA2948620F48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9CC6F7E-27CB-4A4D-BDEB-A8B377E734F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21480" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HORAS" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="750" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="777" uniqueCount="378">
   <si>
     <t>Descripción</t>
   </si>
@@ -1150,6 +1150,27 @@
   </si>
   <si>
     <t>Soporte en la red</t>
+  </si>
+  <si>
+    <t>Modificación de impresión de tikcet para quitar evaluación y modificaciones en productos pasarlo a modal y limpiar filtros</t>
+  </si>
+  <si>
+    <t>Modificacion de tickets para agregar logo de la empresa</t>
+  </si>
+  <si>
+    <t>Modificación de tickets para agregar el logo de sarita e instalación</t>
+  </si>
+  <si>
+    <t>Instalación en ambas sucursales tanto el servicio com la actualización de los sitios</t>
+  </si>
+  <si>
+    <t>Pagado</t>
+  </si>
+  <si>
+    <t>Modificación de tickets para agregar el logo de sarita</t>
+  </si>
+  <si>
+    <t>Redondeo de descuento, modificación de producto, Agregar firmas en el inventario log del producto, rediseño de todas las tablas del sistema, mejoras en el performance de la consulta de ventas</t>
   </si>
 </sst>
 </file>
@@ -1415,7 +1436,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1534,12 +1555,6 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
@@ -1560,6 +1575,37 @@
     <xf numFmtId="44" fontId="0" fillId="11" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="11" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="44" fontId="3" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1575,9 +1621,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1586,27 +1629,6 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="11" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1623,7 +1645,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Millares" xfId="2" builtinId="3"/>
@@ -1941,11 +1963,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K315"/>
+  <dimension ref="A1:K323"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A265" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D267" sqref="D267"/>
+      <pane ySplit="1" topLeftCell="A268" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D281" sqref="D281"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7340,7 +7362,7 @@
     </row>
     <row r="273" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A273" s="5"/>
-      <c r="C273" s="93"/>
+      <c r="C273" s="10"/>
       <c r="D273" s="14" t="s">
         <v>370</v>
       </c>
@@ -7354,268 +7376,309 @@
         <v>1</v>
       </c>
     </row>
-    <row r="274" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A274" s="5"/>
-      <c r="E274" s="2"/>
-      <c r="F274" s="2"/>
+      <c r="C274" s="10">
+        <v>45787</v>
+      </c>
+      <c r="D274" s="14" t="s">
+        <v>371</v>
+      </c>
+      <c r="E274" s="2">
+        <v>0.50347222222222221</v>
+      </c>
+      <c r="F274" s="2">
+        <v>0.65625</v>
+      </c>
+      <c r="H274" s="15">
+        <v>3</v>
+      </c>
     </row>
     <row r="275" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A275" s="5"/>
-      <c r="E275" s="2"/>
-      <c r="F275" s="2"/>
+      <c r="C275" s="10">
+        <v>45790</v>
+      </c>
+      <c r="D275" s="14" t="s">
+        <v>372</v>
+      </c>
+      <c r="E275" s="2">
+        <v>0.33680555555555558</v>
+      </c>
+      <c r="F275" s="2">
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="H275" s="15">
+        <v>2</v>
+      </c>
     </row>
     <row r="276" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A276" s="84" t="s">
+      <c r="A276" s="5"/>
+      <c r="C276" s="10">
+        <v>45792</v>
+      </c>
+      <c r="D276" s="14" t="s">
+        <v>373</v>
+      </c>
+      <c r="E276" s="2">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="F276" s="2">
+        <v>0.12847222222222221</v>
+      </c>
+      <c r="H276" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="277" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A277" s="5"/>
+      <c r="C277" s="10">
+        <v>45792</v>
+      </c>
+      <c r="D277" s="14" t="s">
+        <v>374</v>
+      </c>
+      <c r="E277" s="2"/>
+      <c r="F277" s="2"/>
+      <c r="H277" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="278" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A278" s="5"/>
+      <c r="C278" s="94"/>
+      <c r="D278" s="14" t="s">
+        <v>377</v>
+      </c>
+      <c r="E278" s="2">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="F278" s="2">
+        <v>0.97222222222222221</v>
+      </c>
+      <c r="H278" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="279" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A279" s="5"/>
+      <c r="C279" s="94"/>
+      <c r="D279" s="14"/>
+      <c r="E279" s="2"/>
+      <c r="F279" s="2"/>
+    </row>
+    <row r="280" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A280" s="5"/>
+      <c r="C280" s="94"/>
+      <c r="D280" s="14"/>
+      <c r="E280" s="2"/>
+      <c r="F280" s="2"/>
+    </row>
+    <row r="281" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A281" s="5"/>
+      <c r="C281" s="70"/>
+      <c r="D281" s="14"/>
+      <c r="E281" s="2"/>
+      <c r="F281" s="2"/>
+    </row>
+    <row r="282" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A282" s="5"/>
+      <c r="E282" s="2"/>
+      <c r="F282" s="2"/>
+    </row>
+    <row r="283" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A283" s="5"/>
+      <c r="E283" s="2"/>
+      <c r="F283" s="2"/>
+    </row>
+    <row r="284" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A284" s="76" t="s">
         <v>165</v>
       </c>
-      <c r="B276" s="84"/>
-      <c r="C276" s="84"/>
-      <c r="D276" s="84"/>
-      <c r="E276" s="84"/>
-      <c r="F276" s="84"/>
-      <c r="G276" s="17">
-        <f>SUM(G2:G275)</f>
+      <c r="B284" s="76"/>
+      <c r="C284" s="76"/>
+      <c r="D284" s="76"/>
+      <c r="E284" s="76"/>
+      <c r="F284" s="76"/>
+      <c r="G284" s="17">
+        <f>SUM(G2:G283)</f>
         <v>314.78999999999996</v>
       </c>
-      <c r="H276" s="17">
-        <f>SUM(H2:H275)</f>
-        <v>68.3</v>
-      </c>
-    </row>
-    <row r="277" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A277" s="84" t="s">
+      <c r="H284" s="17">
+        <f>SUM(H2:H283)</f>
+        <v>79.3</v>
+      </c>
+    </row>
+    <row r="285" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A285" s="76" t="s">
         <v>139</v>
       </c>
-      <c r="B277" s="84"/>
-      <c r="C277" s="84"/>
-      <c r="D277" s="84"/>
-      <c r="E277" s="84"/>
-      <c r="F277" s="84"/>
-      <c r="G277" s="17">
+      <c r="B285" s="76"/>
+      <c r="C285" s="76"/>
+      <c r="D285" s="76"/>
+      <c r="E285" s="76"/>
+      <c r="F285" s="76"/>
+      <c r="G285" s="17">
         <v>200</v>
       </c>
-      <c r="H277" s="17">
+      <c r="H285" s="17">
         <v>300</v>
       </c>
     </row>
-    <row r="278" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A278" s="84" t="s">
+    <row r="286" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A286" s="76" t="s">
         <v>166</v>
       </c>
-      <c r="B278" s="84"/>
-      <c r="C278" s="84"/>
-      <c r="D278" s="84"/>
-      <c r="E278" s="84"/>
-      <c r="F278" s="84"/>
-      <c r="G278" s="18">
-        <f>G277*G276</f>
+      <c r="B286" s="76"/>
+      <c r="C286" s="76"/>
+      <c r="D286" s="76"/>
+      <c r="E286" s="76"/>
+      <c r="F286" s="76"/>
+      <c r="G286" s="18">
+        <f>G285*G284</f>
         <v>62957.999999999993</v>
       </c>
-      <c r="H278" s="19">
-        <f>H277*H276</f>
-        <v>20490</v>
-      </c>
-      <c r="J278">
+      <c r="H286" s="19">
+        <f>H285*H284</f>
+        <v>23790</v>
+      </c>
+      <c r="J286">
         <v>-500</v>
       </c>
     </row>
-    <row r="279" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A279" s="84" t="s">
+    <row r="287" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A287" s="76" t="s">
         <v>140</v>
       </c>
-      <c r="B279" s="84"/>
-      <c r="C279" s="84"/>
-      <c r="D279" s="84"/>
-      <c r="E279" s="84"/>
-      <c r="F279" s="84"/>
-      <c r="G279" s="72">
-        <f>G278+H278</f>
-        <v>83448</v>
-      </c>
-      <c r="H279" s="72"/>
-    </row>
-    <row r="280" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A280" s="11"/>
-      <c r="B280" s="75" t="s">
+      <c r="B287" s="76"/>
+      <c r="C287" s="76"/>
+      <c r="D287" s="76"/>
+      <c r="E287" s="76"/>
+      <c r="F287" s="76"/>
+      <c r="G287" s="81">
+        <f>G286+H286</f>
+        <v>86748</v>
+      </c>
+      <c r="H287" s="81"/>
+    </row>
+    <row r="288" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A288" s="11"/>
+      <c r="B288" s="84" t="s">
         <v>142</v>
       </c>
-      <c r="C280" s="75"/>
-      <c r="D280" s="75"/>
-      <c r="E280" s="75"/>
-      <c r="F280" s="75"/>
-      <c r="G280" s="22"/>
-    </row>
-    <row r="281" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A281" s="12">
+      <c r="C288" s="84"/>
+      <c r="D288" s="84"/>
+      <c r="E288" s="84"/>
+      <c r="F288" s="84"/>
+      <c r="G288" s="22"/>
+    </row>
+    <row r="289" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A289" s="12">
         <v>45109</v>
       </c>
-      <c r="B281" s="76" t="s">
+      <c r="B289" s="85" t="s">
         <v>141</v>
       </c>
-      <c r="C281" s="76"/>
-      <c r="D281" s="76"/>
-      <c r="E281" s="76"/>
-      <c r="F281" s="76"/>
-      <c r="G281" s="78">
+      <c r="C289" s="85"/>
+      <c r="D289" s="85"/>
+      <c r="E289" s="85"/>
+      <c r="F289" s="85"/>
+      <c r="G289" s="86">
         <v>10000</v>
       </c>
-      <c r="H281" s="78"/>
-    </row>
-    <row r="282" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A282" s="12"/>
-      <c r="B282" s="80" t="s">
+      <c r="H289" s="86"/>
+    </row>
+    <row r="290" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A290" s="12"/>
+      <c r="B290" s="88" t="s">
         <v>178</v>
       </c>
-      <c r="C282" s="80"/>
-      <c r="D282" s="80"/>
-      <c r="E282" s="80"/>
-      <c r="F282" s="80"/>
-      <c r="G282" s="78">
+      <c r="C290" s="88"/>
+      <c r="D290" s="88"/>
+      <c r="E290" s="88"/>
+      <c r="F290" s="88"/>
+      <c r="G290" s="86">
         <v>5000</v>
       </c>
-      <c r="H282" s="78"/>
-    </row>
-    <row r="283" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A283" s="12">
+      <c r="H290" s="86"/>
+    </row>
+    <row r="291" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A291" s="12">
         <v>45278</v>
       </c>
-      <c r="B283" s="77" t="s">
+      <c r="B291" s="77" t="s">
         <v>178</v>
       </c>
-      <c r="C283" s="77"/>
-      <c r="D283" s="77"/>
-      <c r="E283" s="77"/>
-      <c r="F283" s="77"/>
-      <c r="G283" s="78">
+      <c r="C291" s="77"/>
+      <c r="D291" s="77"/>
+      <c r="E291" s="77"/>
+      <c r="F291" s="77"/>
+      <c r="G291" s="86">
         <v>9800</v>
       </c>
-      <c r="H283" s="78"/>
-    </row>
-    <row r="284" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A284" s="12"/>
-      <c r="B284" s="77"/>
-      <c r="C284" s="77"/>
-      <c r="D284" s="77"/>
-      <c r="E284" s="77"/>
-      <c r="F284" s="77"/>
-      <c r="G284" s="79"/>
-      <c r="H284" s="79"/>
-    </row>
-    <row r="285" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A285" s="12"/>
-      <c r="B285" s="77"/>
-      <c r="C285" s="77"/>
-      <c r="D285" s="77"/>
-      <c r="E285" s="77"/>
-      <c r="F285" s="77"/>
-      <c r="G285" s="79"/>
-      <c r="H285" s="79"/>
-    </row>
-    <row r="286" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A286" s="12"/>
-      <c r="B286" s="77"/>
-      <c r="C286" s="77"/>
-      <c r="D286" s="77"/>
-      <c r="E286" s="77"/>
-      <c r="F286" s="77"/>
-      <c r="G286" s="79"/>
-      <c r="H286" s="79"/>
-    </row>
-    <row r="287" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A287" s="12"/>
-      <c r="B287" s="77" t="s">
+      <c r="H291" s="86"/>
+    </row>
+    <row r="292" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A292" s="12"/>
+      <c r="B292" s="77"/>
+      <c r="C292" s="77"/>
+      <c r="D292" s="77"/>
+      <c r="E292" s="77"/>
+      <c r="F292" s="77"/>
+      <c r="G292" s="87"/>
+      <c r="H292" s="87"/>
+    </row>
+    <row r="293" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A293" s="12"/>
+      <c r="B293" s="77"/>
+      <c r="C293" s="77"/>
+      <c r="D293" s="77"/>
+      <c r="E293" s="77"/>
+      <c r="F293" s="77"/>
+      <c r="G293" s="87"/>
+      <c r="H293" s="87"/>
+    </row>
+    <row r="294" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A294" s="12"/>
+      <c r="B294" s="77"/>
+      <c r="C294" s="77"/>
+      <c r="D294" s="77"/>
+      <c r="E294" s="77"/>
+      <c r="F294" s="77"/>
+      <c r="G294" s="87"/>
+      <c r="H294" s="87"/>
+    </row>
+    <row r="295" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A295" s="12"/>
+      <c r="B295" s="77" t="s">
         <v>144</v>
       </c>
-      <c r="C287" s="77"/>
-      <c r="D287" s="77"/>
-      <c r="E287" s="77"/>
-      <c r="F287" s="77"/>
-      <c r="G287" s="78">
-        <f>SUM(G281:H286)</f>
+      <c r="C295" s="77"/>
+      <c r="D295" s="77"/>
+      <c r="E295" s="77"/>
+      <c r="F295" s="77"/>
+      <c r="G295" s="86">
+        <f>SUM(G289:H294)</f>
         <v>24800</v>
       </c>
-      <c r="H287" s="78"/>
-    </row>
-    <row r="288" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A288" s="73" t="s">
+      <c r="H295" s="86"/>
+    </row>
+    <row r="296" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A296" s="82" t="s">
         <v>143</v>
       </c>
-      <c r="B288" s="73"/>
-      <c r="C288" s="73"/>
-      <c r="D288" s="73"/>
-      <c r="E288" s="73"/>
-      <c r="F288" s="73"/>
-      <c r="G288" s="74">
-        <f>G279-G287</f>
-        <v>58648</v>
-      </c>
-      <c r="H288" s="74"/>
-    </row>
-    <row r="289" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A289" s="12"/>
-      <c r="B289" s="13"/>
-      <c r="C289" s="13"/>
-      <c r="D289" s="13"/>
-      <c r="E289" s="13"/>
-      <c r="F289" s="13"/>
-    </row>
-    <row r="290" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A290" s="12"/>
-      <c r="B290" s="13"/>
-      <c r="C290" s="13"/>
-      <c r="D290" s="13"/>
-      <c r="E290" s="13"/>
-      <c r="F290" s="13"/>
-    </row>
-    <row r="291" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A291" s="12"/>
-      <c r="B291" s="13"/>
-      <c r="C291" s="13"/>
-      <c r="D291" s="13"/>
-      <c r="E291" s="13"/>
-      <c r="F291" s="13"/>
-    </row>
-    <row r="292" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A292" s="12"/>
-      <c r="B292" s="13"/>
-      <c r="C292" s="13"/>
-      <c r="D292" s="13"/>
-      <c r="E292" s="13"/>
-      <c r="F292" s="13"/>
-    </row>
-    <row r="293" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A293" s="12"/>
-      <c r="B293" s="13"/>
-      <c r="C293" s="13"/>
-      <c r="D293" s="13"/>
-      <c r="E293" s="13"/>
-      <c r="F293" s="13"/>
-    </row>
-    <row r="294" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A294" s="12"/>
-      <c r="B294" s="13"/>
-      <c r="C294" s="13"/>
-      <c r="D294" s="13"/>
-      <c r="E294" s="13"/>
-      <c r="F294" s="13"/>
-    </row>
-    <row r="295" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A295" s="12"/>
-      <c r="B295" s="13"/>
-      <c r="C295" s="13"/>
-      <c r="D295" s="13"/>
-      <c r="E295" s="13"/>
-      <c r="F295" s="13"/>
-    </row>
-    <row r="296" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A296" s="12"/>
-      <c r="B296" s="13"/>
-      <c r="C296" s="13"/>
-      <c r="D296" s="13"/>
-      <c r="E296" s="13"/>
-      <c r="F296" s="13"/>
-    </row>
-    <row r="297" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B296" s="82"/>
+      <c r="C296" s="82"/>
+      <c r="D296" s="82"/>
+      <c r="E296" s="82"/>
+      <c r="F296" s="82"/>
+      <c r="G296" s="83">
+        <f>G287-G295</f>
+        <v>61948</v>
+      </c>
+      <c r="H296" s="83"/>
+    </row>
+    <row r="297" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A297" s="12"/>
       <c r="B297" s="13"/>
       <c r="C297" s="13"/>
@@ -7623,7 +7686,7 @@
       <c r="E297" s="13"/>
       <c r="F297" s="13"/>
     </row>
-    <row r="298" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A298" s="12"/>
       <c r="B298" s="13"/>
       <c r="C298" s="13"/>
@@ -7631,7 +7694,7 @@
       <c r="E298" s="13"/>
       <c r="F298" s="13"/>
     </row>
-    <row r="299" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A299" s="12"/>
       <c r="B299" s="13"/>
       <c r="C299" s="13"/>
@@ -7639,7 +7702,7 @@
       <c r="E299" s="13"/>
       <c r="F299" s="13"/>
     </row>
-    <row r="300" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A300" s="12"/>
       <c r="B300" s="13"/>
       <c r="C300" s="13"/>
@@ -7647,7 +7710,7 @@
       <c r="E300" s="13"/>
       <c r="F300" s="13"/>
     </row>
-    <row r="301" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A301" s="12"/>
       <c r="B301" s="13"/>
       <c r="C301" s="13"/>
@@ -7655,7 +7718,7 @@
       <c r="E301" s="13"/>
       <c r="F301" s="13"/>
     </row>
-    <row r="302" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A302" s="12"/>
       <c r="B302" s="13"/>
       <c r="C302" s="13"/>
@@ -7663,7 +7726,7 @@
       <c r="E302" s="13"/>
       <c r="F302" s="13"/>
     </row>
-    <row r="303" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A303" s="12"/>
       <c r="B303" s="13"/>
       <c r="C303" s="13"/>
@@ -7671,7 +7734,7 @@
       <c r="E303" s="13"/>
       <c r="F303" s="13"/>
     </row>
-    <row r="304" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A304" s="12"/>
       <c r="B304" s="13"/>
       <c r="C304" s="13"/>
@@ -7696,190 +7759,254 @@
       <c r="F306" s="13"/>
     </row>
     <row r="307" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A307" s="10"/>
-      <c r="B307" s="85" t="s">
+      <c r="A307" s="12"/>
+      <c r="B307" s="13"/>
+      <c r="C307" s="13"/>
+      <c r="D307" s="13"/>
+      <c r="E307" s="13"/>
+      <c r="F307" s="13"/>
+    </row>
+    <row r="308" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A308" s="12"/>
+      <c r="B308" s="13"/>
+      <c r="C308" s="13"/>
+      <c r="D308" s="13"/>
+      <c r="E308" s="13"/>
+      <c r="F308" s="13"/>
+    </row>
+    <row r="309" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A309" s="12"/>
+      <c r="B309" s="13"/>
+      <c r="C309" s="13"/>
+      <c r="D309" s="13"/>
+      <c r="E309" s="13"/>
+      <c r="F309" s="13"/>
+    </row>
+    <row r="310" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A310" s="12"/>
+      <c r="B310" s="13"/>
+      <c r="C310" s="13"/>
+      <c r="D310" s="13"/>
+      <c r="E310" s="13"/>
+      <c r="F310" s="13"/>
+    </row>
+    <row r="311" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A311" s="12"/>
+      <c r="B311" s="13"/>
+      <c r="C311" s="13"/>
+      <c r="D311" s="13"/>
+      <c r="E311" s="13"/>
+      <c r="F311" s="13"/>
+    </row>
+    <row r="312" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A312" s="12"/>
+      <c r="B312" s="13"/>
+      <c r="C312" s="13"/>
+      <c r="D312" s="13"/>
+      <c r="E312" s="13"/>
+      <c r="F312" s="13"/>
+    </row>
+    <row r="313" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A313" s="12"/>
+      <c r="B313" s="13"/>
+      <c r="C313" s="13"/>
+      <c r="D313" s="13"/>
+      <c r="E313" s="13"/>
+      <c r="F313" s="13"/>
+    </row>
+    <row r="314" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A314" s="12"/>
+      <c r="B314" s="13"/>
+      <c r="C314" s="13"/>
+      <c r="D314" s="13"/>
+      <c r="E314" s="13"/>
+      <c r="F314" s="13"/>
+    </row>
+    <row r="315" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A315" s="10"/>
+      <c r="B315" s="78" t="s">
         <v>138</v>
       </c>
-      <c r="C307" s="85"/>
-      <c r="D307" s="85"/>
-      <c r="E307" s="85"/>
-      <c r="F307" s="85"/>
-      <c r="G307" s="21"/>
-      <c r="H307" s="21"/>
-      <c r="I307" s="8">
-        <f>G276+H276</f>
-        <v>383.09</v>
-      </c>
-      <c r="J307" s="8">
-        <f>I307</f>
-        <v>383.09</v>
-      </c>
-    </row>
-    <row r="308" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A308" s="5"/>
-      <c r="B308" s="86" t="s">
+      <c r="C315" s="78"/>
+      <c r="D315" s="78"/>
+      <c r="E315" s="78"/>
+      <c r="F315" s="78"/>
+      <c r="G315" s="21"/>
+      <c r="H315" s="21"/>
+      <c r="I315" s="8">
+        <f>G284+H284</f>
+        <v>394.09</v>
+      </c>
+      <c r="J315" s="8">
+        <f>I315</f>
+        <v>394.09</v>
+      </c>
+    </row>
+    <row r="316" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A316" s="5"/>
+      <c r="B316" s="79" t="s">
         <v>139</v>
       </c>
-      <c r="C308" s="86"/>
-      <c r="D308" s="86"/>
-      <c r="E308" s="86"/>
-      <c r="F308" s="86"/>
-      <c r="I308" s="8">
+      <c r="C316" s="79"/>
+      <c r="D316" s="79"/>
+      <c r="E316" s="79"/>
+      <c r="F316" s="79"/>
+      <c r="I316" s="8">
         <v>300</v>
       </c>
-      <c r="J308" s="8">
+      <c r="J316" s="8">
         <v>200</v>
       </c>
     </row>
-    <row r="309" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A309" s="5"/>
-      <c r="B309" s="86" t="s">
+    <row r="317" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A317" s="5"/>
+      <c r="B317" s="79" t="s">
         <v>140</v>
       </c>
-      <c r="C309" s="86"/>
-      <c r="D309" s="86"/>
-      <c r="E309" s="86"/>
-      <c r="F309" s="86"/>
-      <c r="I309" s="9">
-        <f>I308*I307</f>
-        <v>114926.99999999999</v>
-      </c>
-      <c r="J309" s="9">
-        <f>J308*J307</f>
-        <v>76618</v>
-      </c>
-    </row>
-    <row r="310" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A310" s="23"/>
-      <c r="B310" s="87" t="s">
+      <c r="C317" s="79"/>
+      <c r="D317" s="79"/>
+      <c r="E317" s="79"/>
+      <c r="F317" s="79"/>
+      <c r="I317" s="9">
+        <f>I316*I315</f>
+        <v>118226.99999999999</v>
+      </c>
+      <c r="J317" s="9">
+        <f>J316*J315</f>
+        <v>78818</v>
+      </c>
+    </row>
+    <row r="318" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A318" s="23"/>
+      <c r="B318" s="80" t="s">
         <v>142</v>
       </c>
-      <c r="C310" s="87"/>
-      <c r="D310" s="87"/>
-      <c r="E310" s="87"/>
-      <c r="F310" s="87"/>
-      <c r="G310" s="24"/>
-      <c r="H310" s="24"/>
-      <c r="I310" s="25"/>
-      <c r="J310" s="25"/>
-    </row>
-    <row r="311" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A311" s="26">
+      <c r="C318" s="80"/>
+      <c r="D318" s="80"/>
+      <c r="E318" s="80"/>
+      <c r="F318" s="80"/>
+      <c r="G318" s="24"/>
+      <c r="H318" s="24"/>
+      <c r="I318" s="25"/>
+      <c r="J318" s="25"/>
+    </row>
+    <row r="319" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A319" s="26">
         <v>45109</v>
       </c>
-      <c r="B311" s="82" t="s">
+      <c r="B319" s="74" t="s">
         <v>141</v>
       </c>
-      <c r="C311" s="82"/>
-      <c r="D311" s="82"/>
-      <c r="E311" s="82"/>
-      <c r="F311" s="82"/>
-      <c r="G311" s="27"/>
-      <c r="H311" s="27"/>
-      <c r="I311" s="28">
+      <c r="C319" s="74"/>
+      <c r="D319" s="74"/>
+      <c r="E319" s="74"/>
+      <c r="F319" s="74"/>
+      <c r="G319" s="27"/>
+      <c r="H319" s="27"/>
+      <c r="I319" s="28">
         <v>10000</v>
       </c>
-      <c r="J311" s="28">
+      <c r="J319" s="28">
         <v>10000</v>
       </c>
     </row>
-    <row r="312" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A312" s="26"/>
-      <c r="B312" s="29"/>
-      <c r="C312" s="29"/>
-      <c r="D312" s="29"/>
-      <c r="E312" s="29"/>
-      <c r="F312" s="29"/>
-      <c r="G312" s="27"/>
-      <c r="H312" s="27"/>
-      <c r="I312" s="30"/>
-      <c r="J312" s="30"/>
-    </row>
-    <row r="313" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A313" s="26"/>
-      <c r="B313" s="29"/>
-      <c r="C313" s="29"/>
-      <c r="D313" s="29"/>
-      <c r="E313" s="29"/>
-      <c r="F313" s="29"/>
-      <c r="G313" s="27"/>
-      <c r="H313" s="27"/>
-      <c r="I313" s="30"/>
-      <c r="J313" s="30"/>
-    </row>
-    <row r="314" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A314" s="26"/>
-      <c r="B314" s="83" t="s">
+    <row r="320" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A320" s="26"/>
+      <c r="B320" s="29"/>
+      <c r="C320" s="29"/>
+      <c r="D320" s="29"/>
+      <c r="E320" s="29"/>
+      <c r="F320" s="29"/>
+      <c r="G320" s="27"/>
+      <c r="H320" s="27"/>
+      <c r="I320" s="30"/>
+      <c r="J320" s="30"/>
+    </row>
+    <row r="321" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A321" s="26"/>
+      <c r="B321" s="29"/>
+      <c r="C321" s="29"/>
+      <c r="D321" s="29"/>
+      <c r="E321" s="29"/>
+      <c r="F321" s="29"/>
+      <c r="G321" s="27"/>
+      <c r="H321" s="27"/>
+      <c r="I321" s="30"/>
+      <c r="J321" s="30"/>
+    </row>
+    <row r="322" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A322" s="26"/>
+      <c r="B322" s="75" t="s">
         <v>144</v>
       </c>
-      <c r="C314" s="83"/>
-      <c r="D314" s="83"/>
-      <c r="E314" s="83"/>
-      <c r="F314" s="83"/>
-      <c r="G314" s="27"/>
-      <c r="H314" s="27"/>
-      <c r="I314" s="31">
-        <f>SUM(I311:I313)</f>
+      <c r="C322" s="75"/>
+      <c r="D322" s="75"/>
+      <c r="E322" s="75"/>
+      <c r="F322" s="75"/>
+      <c r="G322" s="27"/>
+      <c r="H322" s="27"/>
+      <c r="I322" s="31">
+        <f>SUM(I319:I321)</f>
         <v>10000</v>
       </c>
-      <c r="J314" s="31">
-        <f>SUM(J311:J313)</f>
+      <c r="J322" s="31">
+        <f>SUM(J319:J321)</f>
         <v>10000</v>
       </c>
     </row>
-    <row r="315" spans="1:10" ht="33.75" x14ac:dyDescent="0.5">
-      <c r="A315" s="32">
+    <row r="323" spans="1:10" ht="33.75" x14ac:dyDescent="0.5">
+      <c r="A323" s="32">
         <v>45109</v>
       </c>
-      <c r="B315" s="81" t="s">
+      <c r="B323" s="73" t="s">
         <v>143</v>
       </c>
-      <c r="C315" s="81"/>
-      <c r="D315" s="81"/>
-      <c r="E315" s="81"/>
-      <c r="F315" s="81"/>
-      <c r="G315" s="33"/>
-      <c r="H315" s="33"/>
-      <c r="I315" s="34">
-        <f>I309-I314</f>
-        <v>104926.99999999999</v>
-      </c>
-      <c r="J315" s="34">
-        <f>J309-J314</f>
-        <v>66618</v>
+      <c r="C323" s="73"/>
+      <c r="D323" s="73"/>
+      <c r="E323" s="73"/>
+      <c r="F323" s="73"/>
+      <c r="G323" s="33"/>
+      <c r="H323" s="33"/>
+      <c r="I323" s="34">
+        <f>I317-I322</f>
+        <v>108226.99999999999</v>
+      </c>
+      <c r="J323" s="34">
+        <f>J317-J322</f>
+        <v>68818</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="G287:H287"/>
+    <mergeCell ref="A296:F296"/>
+    <mergeCell ref="G296:H296"/>
+    <mergeCell ref="B288:F288"/>
+    <mergeCell ref="B289:F289"/>
+    <mergeCell ref="B295:F295"/>
+    <mergeCell ref="G289:H289"/>
+    <mergeCell ref="G290:H290"/>
+    <mergeCell ref="G295:H295"/>
+    <mergeCell ref="G292:H292"/>
+    <mergeCell ref="G293:H293"/>
+    <mergeCell ref="G294:H294"/>
+    <mergeCell ref="G291:H291"/>
+    <mergeCell ref="B291:F291"/>
+    <mergeCell ref="B290:F290"/>
+    <mergeCell ref="B292:F292"/>
+    <mergeCell ref="B323:F323"/>
+    <mergeCell ref="B319:F319"/>
+    <mergeCell ref="B322:F322"/>
+    <mergeCell ref="A285:F285"/>
+    <mergeCell ref="A284:F284"/>
+    <mergeCell ref="A286:F286"/>
+    <mergeCell ref="A287:F287"/>
+    <mergeCell ref="B293:F293"/>
+    <mergeCell ref="B294:F294"/>
     <mergeCell ref="B315:F315"/>
-    <mergeCell ref="B311:F311"/>
-    <mergeCell ref="B314:F314"/>
-    <mergeCell ref="A277:F277"/>
-    <mergeCell ref="A276:F276"/>
-    <mergeCell ref="A278:F278"/>
-    <mergeCell ref="A279:F279"/>
-    <mergeCell ref="B285:F285"/>
-    <mergeCell ref="B286:F286"/>
-    <mergeCell ref="B307:F307"/>
-    <mergeCell ref="B308:F308"/>
-    <mergeCell ref="B309:F309"/>
-    <mergeCell ref="B310:F310"/>
-    <mergeCell ref="G279:H279"/>
-    <mergeCell ref="A288:F288"/>
-    <mergeCell ref="G288:H288"/>
-    <mergeCell ref="B280:F280"/>
-    <mergeCell ref="B281:F281"/>
-    <mergeCell ref="B287:F287"/>
-    <mergeCell ref="G281:H281"/>
-    <mergeCell ref="G282:H282"/>
-    <mergeCell ref="G287:H287"/>
-    <mergeCell ref="G284:H284"/>
-    <mergeCell ref="G285:H285"/>
-    <mergeCell ref="G286:H286"/>
-    <mergeCell ref="G283:H283"/>
-    <mergeCell ref="B283:F283"/>
-    <mergeCell ref="B282:F282"/>
-    <mergeCell ref="B284:F284"/>
+    <mergeCell ref="B316:F316"/>
+    <mergeCell ref="B317:F317"/>
+    <mergeCell ref="B318:F318"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -7888,10 +8015,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3B2F9DB-D849-4B99-B5E6-70BB7408BE44}">
-  <dimension ref="A1:C76"/>
+  <dimension ref="A1:D83"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28:C29"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7901,7 +8028,7 @@
     <col min="3" max="3" width="24" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>5</v>
       </c>
@@ -7912,7 +8039,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="49"/>
       <c r="B2" s="49" t="s">
         <v>316</v>
@@ -7920,8 +8047,9 @@
       <c r="C2" s="50">
         <v>30000</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="D2" s="39"/>
+    </row>
+    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="49"/>
       <c r="B3" s="51" t="s">
         <v>317</v>
@@ -7929,8 +8057,9 @@
       <c r="C3" s="50">
         <v>21000</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="D3" s="39"/>
+    </row>
+    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="49"/>
       <c r="B4" s="51" t="s">
         <v>318</v>
@@ -7938,8 +8067,9 @@
       <c r="C4" s="50">
         <v>4000</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D4" s="39"/>
+    </row>
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="49"/>
       <c r="B5" s="51" t="s">
         <v>319</v>
@@ -7947,8 +8077,9 @@
       <c r="C5" s="50">
         <v>2000</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D5" s="39"/>
+    </row>
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="49"/>
       <c r="B6" s="51" t="s">
         <v>320</v>
@@ -7956,8 +8087,9 @@
       <c r="C6" s="50">
         <v>2500</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="D6" s="39"/>
+    </row>
+    <row r="7" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="49"/>
       <c r="B7" s="51" t="s">
         <v>321</v>
@@ -7965,8 +8097,9 @@
       <c r="C7" s="50">
         <v>2500</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="D7" s="39"/>
+    </row>
+    <row r="8" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A8" s="49"/>
       <c r="B8" s="51" t="s">
         <v>322</v>
@@ -7974,8 +8107,9 @@
       <c r="C8" s="50">
         <v>2300</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="D8" s="39"/>
+    </row>
+    <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="49"/>
       <c r="B9" s="51" t="s">
         <v>323</v>
@@ -7983,8 +8117,9 @@
       <c r="C9" s="50">
         <v>1800</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="D9" s="39"/>
+    </row>
+    <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="49"/>
       <c r="B10" s="51" t="s">
         <v>324</v>
@@ -7992,8 +8127,9 @@
       <c r="C10" s="50">
         <v>1400</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="D10" s="39"/>
+    </row>
+    <row r="11" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A11" s="49"/>
       <c r="B11" s="51" t="s">
         <v>325</v>
@@ -8001,8 +8137,9 @@
       <c r="C11" s="50">
         <v>2500</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" s="39"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="49"/>
       <c r="B12" s="51" t="s">
         <v>326</v>
@@ -8010,8 +8147,9 @@
       <c r="C12" s="50">
         <v>5000</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="D12" s="39"/>
+    </row>
+    <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="49"/>
       <c r="B13" s="51" t="s">
         <v>327</v>
@@ -8019,8 +8157,9 @@
       <c r="C13" s="50">
         <v>1800</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="D13" s="39"/>
+    </row>
+    <row r="14" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="49"/>
       <c r="B14" s="51" t="s">
         <v>328</v>
@@ -8028,8 +8167,9 @@
       <c r="C14" s="50">
         <v>2600</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="D14" s="39"/>
+    </row>
+    <row r="15" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="49"/>
       <c r="B15" s="51" t="s">
         <v>329</v>
@@ -8037,8 +8177,9 @@
       <c r="C15" s="50">
         <v>1500</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" s="39"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="49"/>
       <c r="B16" s="51" t="s">
         <v>301</v>
@@ -8046,8 +8187,9 @@
       <c r="C16" s="50">
         <v>900</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="D16" s="39"/>
+    </row>
+    <row r="17" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A17" s="49"/>
       <c r="B17" s="51" t="s">
         <v>330</v>
@@ -8055,8 +8197,9 @@
       <c r="C17" s="50">
         <v>2200</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D17" s="39"/>
+    </row>
+    <row r="18" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="49"/>
       <c r="B18" s="51" t="s">
         <v>331</v>
@@ -8064,334 +8207,414 @@
       <c r="C18" s="50">
         <v>800</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D18" s="39"/>
+    </row>
+    <row r="19" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="49"/>
       <c r="B19" s="57" t="s">
         <v>311</v>
       </c>
-      <c r="C19" s="88">
+      <c r="C19" s="89">
         <v>1100</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" s="39"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="49"/>
       <c r="B20" s="58" t="s">
         <v>312</v>
       </c>
-      <c r="C20" s="89"/>
-    </row>
-    <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C20" s="90"/>
+      <c r="D20" s="39"/>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="49"/>
       <c r="B21" s="59" t="s">
         <v>313</v>
       </c>
-      <c r="C21" s="90"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C21" s="91"/>
+      <c r="D21" s="39"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="49"/>
       <c r="B22" s="57" t="s">
         <v>340</v>
       </c>
-      <c r="C22" s="88">
+      <c r="C22" s="89">
         <v>600</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D22" s="39"/>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="49"/>
       <c r="B23" s="59" t="s">
         <v>341</v>
       </c>
-      <c r="C23" s="90"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C23" s="91"/>
+      <c r="D23" s="39"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="49"/>
       <c r="B24" s="57" t="s">
         <v>340</v>
       </c>
-      <c r="C24" s="88">
+      <c r="C24" s="89">
         <v>600</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D24" s="39"/>
+    </row>
+    <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="49"/>
       <c r="B25" s="59" t="s">
         <v>341</v>
       </c>
-      <c r="C25" s="90"/>
-    </row>
-    <row r="26" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="C25" s="91"/>
+      <c r="D25" s="39"/>
+    </row>
+    <row r="26" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="49"/>
       <c r="B26" s="58" t="s">
         <v>357</v>
       </c>
-      <c r="C26" s="89">
+      <c r="C26" s="90">
         <v>1500</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" ht="30.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D26" s="39"/>
+    </row>
+    <row r="27" spans="1:4" ht="30.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="49"/>
       <c r="B27" s="59" t="s">
         <v>358</v>
       </c>
-      <c r="C27" s="90"/>
-    </row>
-    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="C27" s="91"/>
+      <c r="D27" s="39"/>
+    </row>
+    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="49"/>
       <c r="B28" s="57" t="s">
         <v>363</v>
       </c>
-      <c r="C28" s="88">
+      <c r="C28" s="89">
         <v>900</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D28" s="39"/>
+    </row>
+    <row r="29" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="49"/>
       <c r="B29" s="59" t="s">
         <v>364</v>
       </c>
-      <c r="C29" s="90"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C29" s="91"/>
+      <c r="D29" s="39"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="49"/>
-      <c r="B30" s="60"/>
-      <c r="C30" s="61"/>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B30" s="57" t="s">
+        <v>365</v>
+      </c>
+      <c r="C30" s="89">
+        <v>1350</v>
+      </c>
+      <c r="D30" s="39"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="49"/>
-      <c r="B31" s="60"/>
-      <c r="C31" s="61"/>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B31" s="58" t="s">
+        <v>366</v>
+      </c>
+      <c r="C31" s="90"/>
+      <c r="D31" s="39"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="49"/>
-      <c r="B32" s="60"/>
-      <c r="C32" s="61"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B32" s="58" t="s">
+        <v>367</v>
+      </c>
+      <c r="C32" s="90"/>
+      <c r="D32" s="39"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="49"/>
-      <c r="B33" s="60"/>
-      <c r="C33" s="61"/>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B33" s="58" t="s">
+        <v>368</v>
+      </c>
+      <c r="C33" s="90"/>
+      <c r="D33" s="39"/>
+    </row>
+    <row r="34" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="49"/>
-      <c r="B34" s="60"/>
-      <c r="C34" s="61"/>
-    </row>
-    <row r="35" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="52"/>
-      <c r="B35" s="53"/>
-      <c r="C35" s="54"/>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="44"/>
-      <c r="B36" s="44" t="s">
+      <c r="B34" s="59" t="s">
+        <v>369</v>
+      </c>
+      <c r="C34" s="91"/>
+      <c r="D34" s="39"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="49"/>
+      <c r="B35" s="57" t="s">
+        <v>370</v>
+      </c>
+      <c r="C35" s="89">
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36" s="49"/>
+      <c r="B36" s="58" t="s">
+        <v>371</v>
+      </c>
+      <c r="C36" s="90"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="49"/>
+      <c r="B37" s="58" t="s">
+        <v>372</v>
+      </c>
+      <c r="C37" s="90"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="49"/>
+      <c r="B38" s="58" t="s">
+        <v>373</v>
+      </c>
+      <c r="C38" s="90"/>
+    </row>
+    <row r="39" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="49"/>
+      <c r="B39" s="59" t="s">
+        <v>374</v>
+      </c>
+      <c r="C39" s="91"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="49"/>
+      <c r="B40" s="71"/>
+      <c r="C40" s="72"/>
+    </row>
+    <row r="41" spans="1:4" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="52"/>
+      <c r="B41" s="53"/>
+      <c r="C41" s="54"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="44"/>
+      <c r="B42" s="44" t="s">
         <v>332</v>
       </c>
-      <c r="C36" s="47">
-        <f>SUM(C2:C35)</f>
-        <v>89500</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
+      <c r="C42" s="47">
+        <f>SUM(C2:C41)</f>
+        <v>93550</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="38" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="45">
+    <row r="44" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="45">
         <v>45109</v>
       </c>
-      <c r="B38" s="42" t="s">
+      <c r="B44" s="42" t="s">
         <v>333</v>
       </c>
-      <c r="C38" s="46">
+      <c r="C44" s="46">
         <v>10000</v>
       </c>
     </row>
-    <row r="39" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="42"/>
-      <c r="B39" s="42" t="s">
+    <row r="45" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="42"/>
+      <c r="B45" s="42" t="s">
         <v>334</v>
       </c>
-      <c r="C39" s="46">
+      <c r="C45" s="46">
         <v>5000</v>
       </c>
     </row>
-    <row r="40" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="45">
+    <row r="46" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="45">
         <v>45278</v>
       </c>
-      <c r="B40" s="42" t="s">
+      <c r="B46" s="42" t="s">
         <v>334</v>
       </c>
-      <c r="C40" s="46">
+      <c r="C46" s="46">
         <v>9800</v>
       </c>
     </row>
-    <row r="41" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="45">
+    <row r="47" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="45">
         <v>45347</v>
       </c>
-      <c r="B41" s="42" t="s">
+      <c r="B47" s="42" t="s">
         <v>334</v>
       </c>
-      <c r="C41" s="46">
+      <c r="C47" s="46">
         <v>5000</v>
       </c>
     </row>
-    <row r="42" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="45">
+    <row r="48" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="45">
         <v>45383</v>
       </c>
-      <c r="B42" s="42" t="s">
+      <c r="B48" s="42" t="s">
         <v>334</v>
       </c>
-      <c r="C42" s="46">
+      <c r="C48" s="46">
         <v>5000</v>
       </c>
     </row>
-    <row r="43" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="45">
+    <row r="49" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="45">
         <v>45384</v>
       </c>
-      <c r="B43" s="42" t="s">
+      <c r="B49" s="42" t="s">
         <v>334</v>
       </c>
-      <c r="C43" s="46">
+      <c r="C49" s="46">
         <v>5000</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="56">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="56">
         <v>45419</v>
       </c>
-      <c r="B44" s="49" t="s">
-        <v>334</v>
-      </c>
-      <c r="C44" s="55">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="56">
-        <v>45449</v>
-      </c>
-      <c r="B45" s="49" t="s">
-        <v>334</v>
-      </c>
-      <c r="C45" s="55">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="56">
-        <v>45465</v>
-      </c>
-      <c r="B46" s="49" t="s">
-        <v>335</v>
-      </c>
-      <c r="C46" s="55">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="56"/>
-      <c r="B47" s="49" t="s">
-        <v>336</v>
-      </c>
-      <c r="C47" s="55">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="56">
-        <v>45506</v>
-      </c>
-      <c r="B48" s="49" t="s">
-        <v>335</v>
-      </c>
-      <c r="C48" s="55">
-        <v>15000</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="56">
-        <v>45556</v>
-      </c>
-      <c r="B49" s="49" t="s">
-        <v>334</v>
-      </c>
-      <c r="C49" s="55">
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="56"/>
       <c r="B50" s="49" t="s">
         <v>334</v>
       </c>
       <c r="C50" s="55">
-        <v>3000</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="49"/>
+      <c r="A51" s="56">
+        <v>45449</v>
+      </c>
       <c r="B51" s="49" t="s">
         <v>334</v>
       </c>
       <c r="C51" s="55">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="56">
+        <v>45465</v>
+      </c>
+      <c r="B52" s="49" t="s">
+        <v>335</v>
+      </c>
+      <c r="C52" s="55">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="56"/>
+      <c r="B53" s="49" t="s">
+        <v>336</v>
+      </c>
+      <c r="C53" s="55">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="56">
+        <v>45506</v>
+      </c>
+      <c r="B54" s="49" t="s">
+        <v>335</v>
+      </c>
+      <c r="C54" s="55">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="56">
+        <v>45556</v>
+      </c>
+      <c r="B55" s="49" t="s">
+        <v>334</v>
+      </c>
+      <c r="C55" s="55">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="56"/>
+      <c r="B56" s="49" t="s">
+        <v>334</v>
+      </c>
+      <c r="C56" s="55">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="49"/>
+      <c r="B57" s="49" t="s">
+        <v>334</v>
+      </c>
+      <c r="C57" s="55">
         <v>2300</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="49"/>
-      <c r="B52" s="49"/>
-      <c r="C52" s="55"/>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="49"/>
-      <c r="B53" s="49"/>
-      <c r="C53" s="55"/>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="44"/>
-      <c r="B54" s="44" t="s">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="49"/>
+      <c r="B58" s="49"/>
+      <c r="C58" s="55">
+        <v>2250</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="49"/>
+      <c r="B59" s="49"/>
+      <c r="C59" s="55"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="49"/>
+      <c r="B60" s="49"/>
+      <c r="C60" s="55"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="44"/>
+      <c r="B61" s="44" t="s">
         <v>337</v>
       </c>
-      <c r="C54" s="47">
-        <f>SUM(C37:C53)</f>
-        <v>87100</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="7"/>
-      <c r="B55" s="7" t="s">
+      <c r="C61" s="47">
+        <f>SUM(C43:C60)</f>
+        <v>89350</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="7"/>
+      <c r="B62" s="7" t="s">
         <v>338</v>
       </c>
-      <c r="C55" s="48">
-        <f>C36-C54</f>
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B60" s="14"/>
-    </row>
-    <row r="71" spans="2:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="B71" s="14" t="s">
+      <c r="C62" s="48">
+        <f>C42-C61</f>
+        <v>4200</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B67" s="14"/>
+    </row>
+    <row r="78" spans="2:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="B78" s="14" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B72" s="14"/>
-    </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B74" s="14"/>
-    </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B76" s="14"/>
+    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B79" s="14"/>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B81" s="14"/>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B83" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
+    <mergeCell ref="C35:C39"/>
+    <mergeCell ref="C30:C34"/>
     <mergeCell ref="C19:C21"/>
     <mergeCell ref="C22:C23"/>
     <mergeCell ref="C24:C25"/>
@@ -8399,15 +8622,16 @@
     <mergeCell ref="C28:C29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="147" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6078F90-1BFA-44D9-9906-5A72B5F0645C}">
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:D57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8417,7 +8641,7 @@
     <col min="3" max="3" width="24" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>5</v>
       </c>
@@ -8427,212 +8651,305 @@
       <c r="C1" s="48" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D1" s="1" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="49"/>
       <c r="B2" s="57" t="s">
         <v>311</v>
       </c>
-      <c r="C2" s="88">
+      <c r="C2" s="89">
         <v>1100</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="39"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="49"/>
       <c r="B3" s="58" t="s">
         <v>312</v>
       </c>
-      <c r="C3" s="89"/>
-    </row>
-    <row r="4" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="90"/>
+      <c r="D3" s="39"/>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="49"/>
       <c r="B4" s="59" t="s">
         <v>313</v>
       </c>
-      <c r="C4" s="90"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C4" s="91"/>
+      <c r="D4" s="39"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="49"/>
       <c r="B5" s="57" t="s">
         <v>340</v>
       </c>
-      <c r="C5" s="88">
+      <c r="C5" s="89">
         <v>600</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D5" s="39"/>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="49"/>
       <c r="B6" s="59" t="s">
         <v>341</v>
       </c>
-      <c r="C6" s="90"/>
-    </row>
-    <row r="7" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="91"/>
+      <c r="D6" s="39"/>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="49"/>
-      <c r="B7" s="70" t="s">
+      <c r="B7" s="68" t="s">
         <v>362</v>
       </c>
-      <c r="C7" s="71">
+      <c r="C7" s="69">
         <v>600</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D7" s="39"/>
+    </row>
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="49"/>
       <c r="B8" s="57" t="s">
         <v>363</v>
       </c>
-      <c r="C8" s="88">
+      <c r="C8" s="89">
         <v>900</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D8" s="39"/>
+    </row>
+    <row r="9" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="49"/>
       <c r="B9" s="59" t="s">
         <v>364</v>
       </c>
-      <c r="C9" s="90"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C9" s="91"/>
+      <c r="D9" s="39"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="49"/>
       <c r="B10" s="57" t="s">
         <v>365</v>
       </c>
-      <c r="C10" s="88">
+      <c r="C10" s="89">
         <v>1350</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" s="39"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="49"/>
       <c r="B11" s="58" t="s">
         <v>366</v>
       </c>
-      <c r="C11" s="89"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C11" s="90"/>
+      <c r="D11" s="39"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="49"/>
       <c r="B12" s="58" t="s">
         <v>367</v>
       </c>
-      <c r="C12" s="89"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C12" s="90"/>
+      <c r="D12" s="39"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="49"/>
       <c r="B13" s="58" t="s">
         <v>368</v>
       </c>
-      <c r="C13" s="89"/>
-    </row>
-    <row r="14" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="90"/>
+      <c r="D13" s="39"/>
+    </row>
+    <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="49"/>
       <c r="B14" s="59" t="s">
         <v>369</v>
       </c>
-      <c r="C14" s="90"/>
-    </row>
-    <row r="15" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="52"/>
-      <c r="B15" s="53"/>
-      <c r="C15" s="54"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="44"/>
-      <c r="B16" s="44" t="s">
+      <c r="C14" s="91"/>
+      <c r="D14" s="39"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="49"/>
+      <c r="B15" s="57" t="s">
+        <v>370</v>
+      </c>
+      <c r="C15" s="89">
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="49"/>
+      <c r="B16" s="58" t="s">
+        <v>371</v>
+      </c>
+      <c r="C16" s="90"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="49"/>
+      <c r="B17" s="58" t="s">
+        <v>372</v>
+      </c>
+      <c r="C17" s="90"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="49"/>
+      <c r="B18" s="58" t="s">
+        <v>376</v>
+      </c>
+      <c r="C18" s="90"/>
+    </row>
+    <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="49"/>
+      <c r="B19" s="59" t="s">
+        <v>374</v>
+      </c>
+      <c r="C19" s="91"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="49"/>
+      <c r="B20" s="71"/>
+      <c r="C20" s="72"/>
+    </row>
+    <row r="21" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="52"/>
+      <c r="B21" s="53"/>
+      <c r="C21" s="54"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="44"/>
+      <c r="B22" s="44" t="s">
         <v>332</v>
       </c>
-      <c r="C16" s="47">
-        <f>SUM(C2:C15)</f>
+      <c r="C22" s="47">
+        <f>SUM(C2:C21)</f>
+        <v>7250</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="56">
+        <v>45690</v>
+      </c>
+      <c r="B24" s="49" t="s">
+        <v>120</v>
+      </c>
+      <c r="C24" s="55">
+        <v>2300</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="56"/>
+      <c r="B25" s="49" t="s">
+        <v>120</v>
+      </c>
+      <c r="C25" s="55">
+        <v>2250</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="49"/>
+      <c r="B26" s="49"/>
+      <c r="C26" s="55"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="44"/>
+      <c r="B27" s="44" t="s">
+        <v>337</v>
+      </c>
+      <c r="C27" s="47">
+        <f>SUM(C23:C26)</f>
         <v>4550</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="56">
-        <v>45690</v>
-      </c>
-      <c r="B18" s="49" t="s">
-        <v>120</v>
-      </c>
-      <c r="C18" s="55">
-        <v>2300</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="49"/>
-      <c r="B19" s="49"/>
-      <c r="C19" s="55"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="44"/>
-      <c r="B20" s="44" t="s">
-        <v>337</v>
-      </c>
-      <c r="C20" s="47">
-        <f>SUM(C17:C19)</f>
-        <v>2300</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="7"/>
+      <c r="B28" s="7" t="s">
         <v>338</v>
       </c>
-      <c r="C21" s="48">
-        <f>C16-C20</f>
-        <v>2250</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B26" s="14"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B28" s="14" t="s">
+      <c r="C28" s="48">
+        <f>C22-C27</f>
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="14"/>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" s="14" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B29" s="14" t="s">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" s="14" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B30" s="14" t="s">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B37" s="14" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B31" s="14" t="s">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B38" s="14" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B32" s="14" t="s">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B39" s="14" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="37" spans="2:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="B37" s="14" t="s">
+    <row r="44" spans="2:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="B44" s="14" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B38" s="14"/>
-    </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B40" s="14"/>
-    </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B42" s="14"/>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B45" s="14"/>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B47" s="14"/>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B49" s="14"/>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B53" s="14" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B54" s="14" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B55" s="14" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B56" s="14" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B57" s="14" t="s">
+        <v>374</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="C2:C4"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="C10:C14"/>
+    <mergeCell ref="C15:C19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8718,7 +9035,7 @@
       <c r="A10" t="s">
         <v>359</v>
       </c>
-      <c r="B10" s="69">
+      <c r="B10" s="67">
         <v>2685</v>
       </c>
       <c r="F10" s="8">
@@ -8729,7 +9046,7 @@
       <c r="A11" t="s">
         <v>360</v>
       </c>
-      <c r="B11" s="69">
+      <c r="B11" s="67">
         <v>13210</v>
       </c>
       <c r="C11" s="8">
@@ -8743,7 +9060,7 @@
       <c r="A12" t="s">
         <v>361</v>
       </c>
-      <c r="B12" s="69">
+      <c r="B12" s="67">
         <v>2340</v>
       </c>
       <c r="C12" s="8">
@@ -8764,8 +9081,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9108,7 +9425,7 @@
   <dimension ref="A1:D98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D95" sqref="D95"/>
     </sheetView>
   </sheetViews>
@@ -9135,12 +9452,12 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="91" t="s">
+      <c r="A2" s="92" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="91"/>
-      <c r="C2" s="91"/>
-      <c r="D2" s="91"/>
+      <c r="B2" s="92"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
@@ -9443,12 +9760,12 @@
       <c r="D30" s="6"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="92" t="s">
+      <c r="A31" s="93" t="s">
         <v>43</v>
       </c>
-      <c r="B31" s="92"/>
-      <c r="C31" s="92"/>
-      <c r="D31" s="92"/>
+      <c r="B31" s="93"/>
+      <c r="C31" s="93"/>
+      <c r="D31" s="93"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
@@ -10077,10 +10394,10 @@
       <c r="D97" s="6"/>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="92"/>
-      <c r="B98" s="92"/>
-      <c r="C98" s="92"/>
-      <c r="D98" s="92"/>
+      <c r="A98" s="93"/>
+      <c r="B98" s="93"/>
+      <c r="C98" s="93"/>
+      <c r="D98" s="93"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -10184,43 +10501,43 @@
       <c r="E18" t="s">
         <v>349</v>
       </c>
-      <c r="F18" s="64" t="s">
+      <c r="F18" s="62" t="s">
         <v>348</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F19" s="63" t="s">
+      <c r="F19" s="61" t="s">
         <v>347</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="62">
+      <c r="B20" s="60">
         <f>SUM(B17:B19)</f>
         <v>1316</v>
       </c>
-      <c r="C20" s="62">
+      <c r="C20" s="60">
         <f>SUM(C17:C19)</f>
         <v>4300</v>
       </c>
-      <c r="D20" s="62">
+      <c r="D20" s="60">
         <f>SUM(D17:D19)</f>
         <v>2984</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B23" s="66" t="s">
+      <c r="B23" s="64" t="s">
         <v>334</v>
       </c>
-      <c r="C23" s="66" t="s">
+      <c r="C23" s="64" t="s">
         <v>351</v>
       </c>
-      <c r="D23" s="66" t="s">
+      <c r="D23" s="64" t="s">
         <v>352</v>
       </c>
-      <c r="E23" s="66" t="s">
+      <c r="E23" s="64" t="s">
         <v>353</v>
       </c>
-      <c r="F23" s="67" t="s">
+      <c r="F23" s="65" t="s">
         <v>354</v>
       </c>
     </row>
@@ -10231,11 +10548,11 @@
       <c r="C24" s="8">
         <v>3800</v>
       </c>
-      <c r="D24" s="65">
+      <c r="D24" s="63">
         <f>C24*100/4300/100</f>
         <v>0.88372093023255816</v>
       </c>
-      <c r="E24" s="62">
+      <c r="E24" s="60">
         <f>B24*D24-B17</f>
         <v>474.69767441860472</v>
       </c>
@@ -10251,11 +10568,11 @@
       <c r="C25" s="8">
         <v>500</v>
       </c>
-      <c r="D25" s="65">
+      <c r="D25" s="63">
         <f>C25*100/4300/100</f>
         <v>0.11627906976744186</v>
       </c>
-      <c r="E25" s="62">
+      <c r="E25" s="60">
         <f>B25*D25-B18</f>
         <v>9.3023255813953369</v>
       </c>
@@ -10265,16 +10582,16 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B28" s="66" t="s">
+      <c r="B28" s="64" t="s">
         <v>334</v>
       </c>
-      <c r="C28" s="66" t="s">
+      <c r="C28" s="64" t="s">
         <v>355</v>
       </c>
-      <c r="D28" s="66" t="s">
+      <c r="D28" s="64" t="s">
         <v>352</v>
       </c>
-      <c r="E28" s="68" t="s">
+      <c r="E28" s="66" t="s">
         <v>356</v>
       </c>
     </row>
@@ -10285,7 +10602,7 @@
       <c r="C29" s="8">
         <v>1116</v>
       </c>
-      <c r="D29" s="65">
+      <c r="D29" s="63">
         <f>C29*100/1316/100</f>
         <v>0.84802431610942253</v>
       </c>
@@ -10301,7 +10618,7 @@
       <c r="C30" s="8">
         <v>200</v>
       </c>
-      <c r="D30" s="65">
+      <c r="D30" s="63">
         <f>C30*100/1316/100</f>
         <v>0.1519756838905775</v>
       </c>

</xml_diff>

<commit_message>
Se suben mejora y avances para no perder código
</commit_message>
<xml_diff>
--- a/Documents/Actividades realizadas/ActividadesN_.xlsx
+++ b/Documents/Actividades realizadas/ActividadesN_.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24334"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\1.- VioletaSystem\Documents\Actividades realizadas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0D9B421-1258-4A58-8A04-C1564597EC1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F66849C2-D332-457D-BB82-2722665BB040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="778" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="386">
   <si>
     <t>Descripción</t>
   </si>
@@ -1174,6 +1174,27 @@
   </si>
   <si>
     <t>Soporte para revisar los inventarios fisicos, hambiene para explicación de reporte financiero</t>
+  </si>
+  <si>
+    <t>Configuracion de impresora nueva en mostrador 1</t>
+  </si>
+  <si>
+    <t>Llamada con martin para dar acceso a Carmen y dudas sobre el proceso</t>
+  </si>
+  <si>
+    <t>Abonos Martin</t>
+  </si>
+  <si>
+    <t>Revisión de la Base de datos para que los productos inactivos no cuenten, neva regla para las acciones, poder administrarlas de otro nivel</t>
+  </si>
+  <si>
+    <t>Instalación de ultimos cambios</t>
+  </si>
+  <si>
+    <t>Soporte devoluciones Sarita con Kamila</t>
+  </si>
+  <si>
+    <t>Creación de servicio de BackUP</t>
   </si>
 </sst>
 </file>
@@ -1586,6 +1607,30 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="44" fontId="3" fillId="8" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1601,9 +1646,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1612,27 +1654,6 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="11" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1966,11 +1987,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K323"/>
+  <dimension ref="A1:K327"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A268" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H280" sqref="H280"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A279" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C286" sqref="C286"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7363,7 +7384,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="273" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A273" s="5"/>
       <c r="C273" s="10"/>
       <c r="D273" s="14" t="s">
@@ -7379,7 +7400,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="274" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A274" s="5"/>
       <c r="C274" s="10">
         <v>45787</v>
@@ -7397,7 +7418,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="275" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A275" s="5"/>
       <c r="C275" s="10">
         <v>45790</v>
@@ -7415,7 +7436,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="276" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A276" s="5"/>
       <c r="C276" s="10">
         <v>45792</v>
@@ -7433,7 +7454,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="277" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A277" s="5"/>
       <c r="C277" s="10">
         <v>45792</v>
@@ -7447,7 +7468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="278" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A278" s="5"/>
       <c r="C278" s="73"/>
       <c r="D278" s="14" t="s">
@@ -7463,7 +7484,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="279" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A279" s="5"/>
       <c r="C279" s="73"/>
       <c r="D279" s="14" t="s">
@@ -7479,250 +7500,312 @@
         <v>1</v>
       </c>
     </row>
-    <row r="280" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A280" s="5"/>
-      <c r="C280" s="73"/>
-      <c r="D280" s="14"/>
-      <c r="E280" s="2"/>
-      <c r="F280" s="2"/>
-    </row>
-    <row r="281" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C280" s="73">
+        <v>45815</v>
+      </c>
+      <c r="D280" s="14" t="s">
+        <v>379</v>
+      </c>
+      <c r="E280" s="2">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="F280" s="2">
+        <v>0.6875</v>
+      </c>
+      <c r="H280" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="281" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A281" s="5"/>
-      <c r="C281" s="70"/>
-      <c r="D281" s="14"/>
-      <c r="E281" s="2"/>
-      <c r="F281" s="2"/>
-    </row>
-    <row r="282" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C281" s="70">
+        <v>45825</v>
+      </c>
+      <c r="D281" s="14" t="s">
+        <v>380</v>
+      </c>
+      <c r="E281" s="2">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="F281" s="2">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="H281" s="15">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="282" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A282" s="5"/>
-      <c r="E282" s="2"/>
-      <c r="F282" s="2"/>
-    </row>
-    <row r="283" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C282" s="70">
+        <v>45831</v>
+      </c>
+      <c r="D282" s="14" t="s">
+        <v>382</v>
+      </c>
+      <c r="E282" s="2">
+        <v>0.35555555555555557</v>
+      </c>
+      <c r="F282" s="2">
+        <v>0.4826388888888889</v>
+      </c>
+      <c r="H282" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="283" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A283" s="5"/>
-      <c r="E283" s="2"/>
-      <c r="F283" s="2"/>
-    </row>
-    <row r="284" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A284" s="86" t="s">
+      <c r="C283" s="70">
+        <v>45831</v>
+      </c>
+      <c r="D283" s="14" t="s">
+        <v>383</v>
+      </c>
+      <c r="E283" s="2">
+        <v>0.48402777777777778</v>
+      </c>
+      <c r="F283" s="2">
+        <v>0.50694444444444442</v>
+      </c>
+      <c r="H283" s="15">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="284" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A284" s="5"/>
+      <c r="C284" s="70">
+        <v>45834</v>
+      </c>
+      <c r="D284" s="14" t="s">
+        <v>384</v>
+      </c>
+      <c r="E284" s="2">
+        <v>0.4513888888888889</v>
+      </c>
+      <c r="F284" s="2">
+        <v>0.47222222222222221</v>
+      </c>
+      <c r="H284" s="15">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="285" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A285" s="5"/>
+      <c r="C285" s="70">
+        <v>45848</v>
+      </c>
+      <c r="D285" s="14" t="s">
+        <v>385</v>
+      </c>
+      <c r="E285" s="2">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="F285" s="2">
+        <v>0.97222222222222221</v>
+      </c>
+      <c r="H285" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="286" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A286" s="5"/>
+      <c r="E286" s="2"/>
+      <c r="F286" s="2"/>
+    </row>
+    <row r="287" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A287" s="5"/>
+      <c r="E287" s="2"/>
+      <c r="F287" s="2"/>
+    </row>
+    <row r="288" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A288" s="77" t="s">
         <v>165</v>
       </c>
-      <c r="B284" s="86"/>
-      <c r="C284" s="86"/>
-      <c r="D284" s="86"/>
-      <c r="E284" s="86"/>
-      <c r="F284" s="86"/>
-      <c r="G284" s="17">
-        <f>SUM(G2:G283)</f>
-        <v>314.78999999999996</v>
-      </c>
-      <c r="H284" s="17">
-        <f>SUM(H2:H283)</f>
-        <v>80.3</v>
-      </c>
-    </row>
-    <row r="285" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A285" s="86" t="s">
-        <v>139</v>
-      </c>
-      <c r="B285" s="86"/>
-      <c r="C285" s="86"/>
-      <c r="D285" s="86"/>
-      <c r="E285" s="86"/>
-      <c r="F285" s="86"/>
-      <c r="G285" s="17">
-        <v>200</v>
-      </c>
-      <c r="H285" s="17">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="286" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A286" s="86" t="s">
-        <v>166</v>
-      </c>
-      <c r="B286" s="86"/>
-      <c r="C286" s="86"/>
-      <c r="D286" s="86"/>
-      <c r="E286" s="86"/>
-      <c r="F286" s="86"/>
-      <c r="G286" s="18">
-        <f>G285*G284</f>
-        <v>62957.999999999993</v>
-      </c>
-      <c r="H286" s="19">
-        <f>H285*H284</f>
-        <v>24090</v>
-      </c>
-      <c r="J286">
-        <v>-500</v>
-      </c>
-    </row>
-    <row r="287" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A287" s="86" t="s">
-        <v>140</v>
-      </c>
-      <c r="B287" s="86"/>
-      <c r="C287" s="86"/>
-      <c r="D287" s="86"/>
-      <c r="E287" s="86"/>
-      <c r="F287" s="86"/>
-      <c r="G287" s="74">
-        <f>G286+H286</f>
-        <v>87048</v>
-      </c>
-      <c r="H287" s="74"/>
-    </row>
-    <row r="288" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A288" s="11"/>
-      <c r="B288" s="77" t="s">
-        <v>142</v>
-      </c>
+      <c r="B288" s="77"/>
       <c r="C288" s="77"/>
       <c r="D288" s="77"/>
       <c r="E288" s="77"/>
       <c r="F288" s="77"/>
-      <c r="G288" s="22"/>
-    </row>
-    <row r="289" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A289" s="12">
+      <c r="G288" s="17">
+        <f>SUM(G2:G287)</f>
+        <v>314.78999999999996</v>
+      </c>
+      <c r="H288" s="17">
+        <f>SUM(H2:H287)</f>
+        <v>88.8</v>
+      </c>
+    </row>
+    <row r="289" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A289" s="77" t="s">
+        <v>139</v>
+      </c>
+      <c r="B289" s="77"/>
+      <c r="C289" s="77"/>
+      <c r="D289" s="77"/>
+      <c r="E289" s="77"/>
+      <c r="F289" s="77"/>
+      <c r="G289" s="17">
+        <v>200</v>
+      </c>
+      <c r="H289" s="17">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="290" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A290" s="77" t="s">
+        <v>166</v>
+      </c>
+      <c r="B290" s="77"/>
+      <c r="C290" s="77"/>
+      <c r="D290" s="77"/>
+      <c r="E290" s="77"/>
+      <c r="F290" s="77"/>
+      <c r="G290" s="18">
+        <f>G289*G288</f>
+        <v>62957.999999999993</v>
+      </c>
+      <c r="H290" s="19">
+        <f>H289*H288</f>
+        <v>26640</v>
+      </c>
+      <c r="J290">
+        <v>-500</v>
+      </c>
+    </row>
+    <row r="291" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A291" s="77" t="s">
+        <v>140</v>
+      </c>
+      <c r="B291" s="77"/>
+      <c r="C291" s="77"/>
+      <c r="D291" s="77"/>
+      <c r="E291" s="77"/>
+      <c r="F291" s="77"/>
+      <c r="G291" s="82">
+        <f>G290+H290</f>
+        <v>89598</v>
+      </c>
+      <c r="H291" s="82"/>
+    </row>
+    <row r="292" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A292" s="11"/>
+      <c r="B292" s="85" t="s">
+        <v>142</v>
+      </c>
+      <c r="C292" s="85"/>
+      <c r="D292" s="85"/>
+      <c r="E292" s="85"/>
+      <c r="F292" s="85"/>
+      <c r="G292" s="22"/>
+    </row>
+    <row r="293" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A293" s="12">
         <v>45109</v>
       </c>
-      <c r="B289" s="78" t="s">
+      <c r="B293" s="86" t="s">
         <v>141</v>
       </c>
-      <c r="C289" s="78"/>
-      <c r="D289" s="78"/>
-      <c r="E289" s="78"/>
-      <c r="F289" s="78"/>
-      <c r="G289" s="80">
+      <c r="C293" s="86"/>
+      <c r="D293" s="86"/>
+      <c r="E293" s="86"/>
+      <c r="F293" s="86"/>
+      <c r="G293" s="87">
         <v>10000</v>
       </c>
-      <c r="H289" s="80"/>
-    </row>
-    <row r="290" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A290" s="12"/>
-      <c r="B290" s="82" t="s">
+      <c r="H293" s="87"/>
+    </row>
+    <row r="294" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A294" s="12"/>
+      <c r="B294" s="89" t="s">
         <v>178</v>
       </c>
-      <c r="C290" s="82"/>
-      <c r="D290" s="82"/>
-      <c r="E290" s="82"/>
-      <c r="F290" s="82"/>
-      <c r="G290" s="80">
+      <c r="C294" s="89"/>
+      <c r="D294" s="89"/>
+      <c r="E294" s="89"/>
+      <c r="F294" s="89"/>
+      <c r="G294" s="87">
         <v>5000</v>
       </c>
-      <c r="H290" s="80"/>
-    </row>
-    <row r="291" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A291" s="12">
+      <c r="H294" s="87"/>
+    </row>
+    <row r="295" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A295" s="12">
         <v>45278</v>
       </c>
-      <c r="B291" s="79" t="s">
+      <c r="B295" s="78" t="s">
         <v>178</v>
       </c>
-      <c r="C291" s="79"/>
-      <c r="D291" s="79"/>
-      <c r="E291" s="79"/>
-      <c r="F291" s="79"/>
-      <c r="G291" s="80">
+      <c r="C295" s="78"/>
+      <c r="D295" s="78"/>
+      <c r="E295" s="78"/>
+      <c r="F295" s="78"/>
+      <c r="G295" s="87">
         <v>9800</v>
       </c>
-      <c r="H291" s="80"/>
-    </row>
-    <row r="292" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A292" s="12"/>
-      <c r="B292" s="79"/>
-      <c r="C292" s="79"/>
-      <c r="D292" s="79"/>
-      <c r="E292" s="79"/>
-      <c r="F292" s="79"/>
-      <c r="G292" s="81"/>
-      <c r="H292" s="81"/>
-    </row>
-    <row r="293" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A293" s="12"/>
-      <c r="B293" s="79"/>
-      <c r="C293" s="79"/>
-      <c r="D293" s="79"/>
-      <c r="E293" s="79"/>
-      <c r="F293" s="79"/>
-      <c r="G293" s="81"/>
-      <c r="H293" s="81"/>
-    </row>
-    <row r="294" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A294" s="12"/>
-      <c r="B294" s="79"/>
-      <c r="C294" s="79"/>
-      <c r="D294" s="79"/>
-      <c r="E294" s="79"/>
-      <c r="F294" s="79"/>
-      <c r="G294" s="81"/>
-      <c r="H294" s="81"/>
-    </row>
-    <row r="295" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A295" s="12"/>
-      <c r="B295" s="79" t="s">
+      <c r="H295" s="87"/>
+    </row>
+    <row r="296" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A296" s="12"/>
+      <c r="B296" s="78"/>
+      <c r="C296" s="78"/>
+      <c r="D296" s="78"/>
+      <c r="E296" s="78"/>
+      <c r="F296" s="78"/>
+      <c r="G296" s="88"/>
+      <c r="H296" s="88"/>
+    </row>
+    <row r="297" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A297" s="12"/>
+      <c r="B297" s="78"/>
+      <c r="C297" s="78"/>
+      <c r="D297" s="78"/>
+      <c r="E297" s="78"/>
+      <c r="F297" s="78"/>
+      <c r="G297" s="88"/>
+      <c r="H297" s="88"/>
+    </row>
+    <row r="298" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A298" s="12"/>
+      <c r="B298" s="78"/>
+      <c r="C298" s="78"/>
+      <c r="D298" s="78"/>
+      <c r="E298" s="78"/>
+      <c r="F298" s="78"/>
+      <c r="G298" s="88"/>
+      <c r="H298" s="88"/>
+    </row>
+    <row r="299" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A299" s="12"/>
+      <c r="B299" s="78" t="s">
         <v>144</v>
       </c>
-      <c r="C295" s="79"/>
-      <c r="D295" s="79"/>
-      <c r="E295" s="79"/>
-      <c r="F295" s="79"/>
-      <c r="G295" s="80">
-        <f>SUM(G289:H294)</f>
+      <c r="C299" s="78"/>
+      <c r="D299" s="78"/>
+      <c r="E299" s="78"/>
+      <c r="F299" s="78"/>
+      <c r="G299" s="87">
+        <f>SUM(G293:H298)</f>
         <v>24800</v>
       </c>
-      <c r="H295" s="80"/>
-    </row>
-    <row r="296" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A296" s="75" t="s">
+      <c r="H299" s="87"/>
+    </row>
+    <row r="300" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A300" s="83" t="s">
         <v>143</v>
       </c>
-      <c r="B296" s="75"/>
-      <c r="C296" s="75"/>
-      <c r="D296" s="75"/>
-      <c r="E296" s="75"/>
-      <c r="F296" s="75"/>
-      <c r="G296" s="76">
-        <f>G287-G295</f>
-        <v>62248</v>
-      </c>
-      <c r="H296" s="76"/>
-    </row>
-    <row r="297" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A297" s="12"/>
-      <c r="B297" s="13"/>
-      <c r="C297" s="13"/>
-      <c r="D297" s="13"/>
-      <c r="E297" s="13"/>
-      <c r="F297" s="13"/>
-    </row>
-    <row r="298" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A298" s="12"/>
-      <c r="B298" s="13"/>
-      <c r="C298" s="13"/>
-      <c r="D298" s="13"/>
-      <c r="E298" s="13"/>
-      <c r="F298" s="13"/>
-    </row>
-    <row r="299" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A299" s="12"/>
-      <c r="B299" s="13"/>
-      <c r="C299" s="13"/>
-      <c r="D299" s="13"/>
-      <c r="E299" s="13"/>
-      <c r="F299" s="13"/>
-    </row>
-    <row r="300" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A300" s="12"/>
-      <c r="B300" s="13"/>
-      <c r="C300" s="13"/>
-      <c r="D300" s="13"/>
-      <c r="E300" s="13"/>
-      <c r="F300" s="13"/>
-    </row>
-    <row r="301" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B300" s="83"/>
+      <c r="C300" s="83"/>
+      <c r="D300" s="83"/>
+      <c r="E300" s="83"/>
+      <c r="F300" s="83"/>
+      <c r="G300" s="84">
+        <f>G291-G299</f>
+        <v>64798</v>
+      </c>
+      <c r="H300" s="84"/>
+    </row>
+    <row r="301" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A301" s="12"/>
       <c r="B301" s="13"/>
       <c r="C301" s="13"/>
@@ -7730,7 +7813,7 @@
       <c r="E301" s="13"/>
       <c r="F301" s="13"/>
     </row>
-    <row r="302" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A302" s="12"/>
       <c r="B302" s="13"/>
       <c r="C302" s="13"/>
@@ -7738,7 +7821,7 @@
       <c r="E302" s="13"/>
       <c r="F302" s="13"/>
     </row>
-    <row r="303" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A303" s="12"/>
       <c r="B303" s="13"/>
       <c r="C303" s="13"/>
@@ -7746,7 +7829,7 @@
       <c r="E303" s="13"/>
       <c r="F303" s="13"/>
     </row>
-    <row r="304" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A304" s="12"/>
       <c r="B304" s="13"/>
       <c r="C304" s="13"/>
@@ -7835,190 +7918,222 @@
       <c r="F314" s="13"/>
     </row>
     <row r="315" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A315" s="10"/>
-      <c r="B315" s="87" t="s">
+      <c r="A315" s="12"/>
+      <c r="B315" s="13"/>
+      <c r="C315" s="13"/>
+      <c r="D315" s="13"/>
+      <c r="E315" s="13"/>
+      <c r="F315" s="13"/>
+    </row>
+    <row r="316" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A316" s="12"/>
+      <c r="B316" s="13"/>
+      <c r="C316" s="13"/>
+      <c r="D316" s="13"/>
+      <c r="E316" s="13"/>
+      <c r="F316" s="13"/>
+    </row>
+    <row r="317" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A317" s="12"/>
+      <c r="B317" s="13"/>
+      <c r="C317" s="13"/>
+      <c r="D317" s="13"/>
+      <c r="E317" s="13"/>
+      <c r="F317" s="13"/>
+    </row>
+    <row r="318" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A318" s="12"/>
+      <c r="B318" s="13"/>
+      <c r="C318" s="13"/>
+      <c r="D318" s="13"/>
+      <c r="E318" s="13"/>
+      <c r="F318" s="13"/>
+    </row>
+    <row r="319" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A319" s="10"/>
+      <c r="B319" s="79" t="s">
         <v>138</v>
       </c>
-      <c r="C315" s="87"/>
-      <c r="D315" s="87"/>
-      <c r="E315" s="87"/>
-      <c r="F315" s="87"/>
-      <c r="G315" s="21"/>
-      <c r="H315" s="21"/>
-      <c r="I315" s="8">
-        <f>G284+H284</f>
-        <v>395.09</v>
-      </c>
-      <c r="J315" s="8">
-        <f>I315</f>
-        <v>395.09</v>
-      </c>
-    </row>
-    <row r="316" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A316" s="5"/>
-      <c r="B316" s="88" t="s">
+      <c r="C319" s="79"/>
+      <c r="D319" s="79"/>
+      <c r="E319" s="79"/>
+      <c r="F319" s="79"/>
+      <c r="G319" s="21"/>
+      <c r="H319" s="21"/>
+      <c r="I319" s="8">
+        <f>G288+H288</f>
+        <v>403.59</v>
+      </c>
+      <c r="J319" s="8">
+        <f>I319</f>
+        <v>403.59</v>
+      </c>
+    </row>
+    <row r="320" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A320" s="5"/>
+      <c r="B320" s="80" t="s">
         <v>139</v>
       </c>
-      <c r="C316" s="88"/>
-      <c r="D316" s="88"/>
-      <c r="E316" s="88"/>
-      <c r="F316" s="88"/>
-      <c r="I316" s="8">
+      <c r="C320" s="80"/>
+      <c r="D320" s="80"/>
+      <c r="E320" s="80"/>
+      <c r="F320" s="80"/>
+      <c r="I320" s="8">
         <v>300</v>
       </c>
-      <c r="J316" s="8">
+      <c r="J320" s="8">
         <v>200</v>
       </c>
     </row>
-    <row r="317" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A317" s="5"/>
-      <c r="B317" s="88" t="s">
+    <row r="321" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A321" s="5"/>
+      <c r="B321" s="80" t="s">
         <v>140</v>
       </c>
-      <c r="C317" s="88"/>
-      <c r="D317" s="88"/>
-      <c r="E317" s="88"/>
-      <c r="F317" s="88"/>
-      <c r="I317" s="9">
-        <f>I316*I315</f>
-        <v>118526.99999999999</v>
-      </c>
-      <c r="J317" s="9">
-        <f>J316*J315</f>
-        <v>79018</v>
-      </c>
-    </row>
-    <row r="318" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A318" s="23"/>
-      <c r="B318" s="89" t="s">
+      <c r="C321" s="80"/>
+      <c r="D321" s="80"/>
+      <c r="E321" s="80"/>
+      <c r="F321" s="80"/>
+      <c r="I321" s="9">
+        <f>I320*I319</f>
+        <v>121076.99999999999</v>
+      </c>
+      <c r="J321" s="9">
+        <f>J320*J319</f>
+        <v>80718</v>
+      </c>
+    </row>
+    <row r="322" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A322" s="23"/>
+      <c r="B322" s="81" t="s">
         <v>142</v>
       </c>
-      <c r="C318" s="89"/>
-      <c r="D318" s="89"/>
-      <c r="E318" s="89"/>
-      <c r="F318" s="89"/>
-      <c r="G318" s="24"/>
-      <c r="H318" s="24"/>
-      <c r="I318" s="25"/>
-      <c r="J318" s="25"/>
-    </row>
-    <row r="319" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A319" s="26">
+      <c r="C322" s="81"/>
+      <c r="D322" s="81"/>
+      <c r="E322" s="81"/>
+      <c r="F322" s="81"/>
+      <c r="G322" s="24"/>
+      <c r="H322" s="24"/>
+      <c r="I322" s="25"/>
+      <c r="J322" s="25"/>
+    </row>
+    <row r="323" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A323" s="26">
         <v>45109</v>
       </c>
-      <c r="B319" s="84" t="s">
+      <c r="B323" s="75" t="s">
         <v>141</v>
       </c>
-      <c r="C319" s="84"/>
-      <c r="D319" s="84"/>
-      <c r="E319" s="84"/>
-      <c r="F319" s="84"/>
-      <c r="G319" s="27"/>
-      <c r="H319" s="27"/>
-      <c r="I319" s="28">
+      <c r="C323" s="75"/>
+      <c r="D323" s="75"/>
+      <c r="E323" s="75"/>
+      <c r="F323" s="75"/>
+      <c r="G323" s="27"/>
+      <c r="H323" s="27"/>
+      <c r="I323" s="28">
         <v>10000</v>
       </c>
-      <c r="J319" s="28">
+      <c r="J323" s="28">
         <v>10000</v>
       </c>
     </row>
-    <row r="320" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A320" s="26"/>
-      <c r="B320" s="29"/>
-      <c r="C320" s="29"/>
-      <c r="D320" s="29"/>
-      <c r="E320" s="29"/>
-      <c r="F320" s="29"/>
-      <c r="G320" s="27"/>
-      <c r="H320" s="27"/>
-      <c r="I320" s="30"/>
-      <c r="J320" s="30"/>
-    </row>
-    <row r="321" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A321" s="26"/>
-      <c r="B321" s="29"/>
-      <c r="C321" s="29"/>
-      <c r="D321" s="29"/>
-      <c r="E321" s="29"/>
-      <c r="F321" s="29"/>
-      <c r="G321" s="27"/>
-      <c r="H321" s="27"/>
-      <c r="I321" s="30"/>
-      <c r="J321" s="30"/>
-    </row>
-    <row r="322" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A322" s="26"/>
-      <c r="B322" s="85" t="s">
+    <row r="324" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A324" s="26"/>
+      <c r="B324" s="29"/>
+      <c r="C324" s="29"/>
+      <c r="D324" s="29"/>
+      <c r="E324" s="29"/>
+      <c r="F324" s="29"/>
+      <c r="G324" s="27"/>
+      <c r="H324" s="27"/>
+      <c r="I324" s="30"/>
+      <c r="J324" s="30"/>
+    </row>
+    <row r="325" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A325" s="26"/>
+      <c r="B325" s="29"/>
+      <c r="C325" s="29"/>
+      <c r="D325" s="29"/>
+      <c r="E325" s="29"/>
+      <c r="F325" s="29"/>
+      <c r="G325" s="27"/>
+      <c r="H325" s="27"/>
+      <c r="I325" s="30"/>
+      <c r="J325" s="30"/>
+    </row>
+    <row r="326" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A326" s="26"/>
+      <c r="B326" s="76" t="s">
         <v>144</v>
       </c>
-      <c r="C322" s="85"/>
-      <c r="D322" s="85"/>
-      <c r="E322" s="85"/>
-      <c r="F322" s="85"/>
-      <c r="G322" s="27"/>
-      <c r="H322" s="27"/>
-      <c r="I322" s="31">
-        <f>SUM(I319:I321)</f>
+      <c r="C326" s="76"/>
+      <c r="D326" s="76"/>
+      <c r="E326" s="76"/>
+      <c r="F326" s="76"/>
+      <c r="G326" s="27"/>
+      <c r="H326" s="27"/>
+      <c r="I326" s="31">
+        <f>SUM(I323:I325)</f>
         <v>10000</v>
       </c>
-      <c r="J322" s="31">
-        <f>SUM(J319:J321)</f>
+      <c r="J326" s="31">
+        <f>SUM(J323:J325)</f>
         <v>10000</v>
       </c>
     </row>
-    <row r="323" spans="1:10" ht="33.75" x14ac:dyDescent="0.5">
-      <c r="A323" s="32">
+    <row r="327" spans="1:10" ht="33.75" x14ac:dyDescent="0.5">
+      <c r="A327" s="32">
         <v>45109</v>
       </c>
-      <c r="B323" s="83" t="s">
+      <c r="B327" s="74" t="s">
         <v>143</v>
       </c>
-      <c r="C323" s="83"/>
-      <c r="D323" s="83"/>
-      <c r="E323" s="83"/>
-      <c r="F323" s="83"/>
-      <c r="G323" s="33"/>
-      <c r="H323" s="33"/>
-      <c r="I323" s="34">
-        <f>I317-I322</f>
-        <v>108526.99999999999</v>
-      </c>
-      <c r="J323" s="34">
-        <f>J317-J322</f>
-        <v>69018</v>
+      <c r="C327" s="74"/>
+      <c r="D327" s="74"/>
+      <c r="E327" s="74"/>
+      <c r="F327" s="74"/>
+      <c r="G327" s="33"/>
+      <c r="H327" s="33"/>
+      <c r="I327" s="34">
+        <f>I321-I326</f>
+        <v>111076.99999999999</v>
+      </c>
+      <c r="J327" s="34">
+        <f>J321-J326</f>
+        <v>70718</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="B323:F323"/>
-    <mergeCell ref="B319:F319"/>
-    <mergeCell ref="B322:F322"/>
-    <mergeCell ref="A285:F285"/>
-    <mergeCell ref="A284:F284"/>
-    <mergeCell ref="A286:F286"/>
-    <mergeCell ref="A287:F287"/>
+    <mergeCell ref="G291:H291"/>
+    <mergeCell ref="A300:F300"/>
+    <mergeCell ref="G300:H300"/>
+    <mergeCell ref="B292:F292"/>
     <mergeCell ref="B293:F293"/>
-    <mergeCell ref="B294:F294"/>
-    <mergeCell ref="B315:F315"/>
-    <mergeCell ref="B316:F316"/>
-    <mergeCell ref="B317:F317"/>
-    <mergeCell ref="B318:F318"/>
-    <mergeCell ref="G287:H287"/>
-    <mergeCell ref="A296:F296"/>
-    <mergeCell ref="G296:H296"/>
-    <mergeCell ref="B288:F288"/>
-    <mergeCell ref="B289:F289"/>
-    <mergeCell ref="B295:F295"/>
-    <mergeCell ref="G289:H289"/>
-    <mergeCell ref="G290:H290"/>
-    <mergeCell ref="G295:H295"/>
-    <mergeCell ref="G292:H292"/>
+    <mergeCell ref="B299:F299"/>
     <mergeCell ref="G293:H293"/>
     <mergeCell ref="G294:H294"/>
-    <mergeCell ref="G291:H291"/>
-    <mergeCell ref="B291:F291"/>
-    <mergeCell ref="B290:F290"/>
-    <mergeCell ref="B292:F292"/>
+    <mergeCell ref="G299:H299"/>
+    <mergeCell ref="G296:H296"/>
+    <mergeCell ref="G297:H297"/>
+    <mergeCell ref="G298:H298"/>
+    <mergeCell ref="G295:H295"/>
+    <mergeCell ref="B295:F295"/>
+    <mergeCell ref="B294:F294"/>
+    <mergeCell ref="B296:F296"/>
+    <mergeCell ref="B327:F327"/>
+    <mergeCell ref="B323:F323"/>
+    <mergeCell ref="B326:F326"/>
+    <mergeCell ref="A289:F289"/>
+    <mergeCell ref="A288:F288"/>
+    <mergeCell ref="A290:F290"/>
+    <mergeCell ref="A291:F291"/>
+    <mergeCell ref="B297:F297"/>
+    <mergeCell ref="B298:F298"/>
+    <mergeCell ref="B319:F319"/>
+    <mergeCell ref="B320:F320"/>
+    <mergeCell ref="B321:F321"/>
+    <mergeCell ref="B322:F322"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -8027,10 +8142,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3B2F9DB-D849-4B99-B5E6-70BB7408BE44}">
-  <dimension ref="A1:D83"/>
+  <dimension ref="A1:D106"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40:C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8283,24 +8398,7 @@
       <c r="C25" s="92"/>
       <c r="D25" s="39"/>
     </row>
-    <row r="26" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="49"/>
-      <c r="B26" s="58" t="s">
-        <v>357</v>
-      </c>
-      <c r="C26" s="91">
-        <v>1500</v>
-      </c>
-      <c r="D26" s="39"/>
-    </row>
-    <row r="27" spans="1:4" ht="30.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="49"/>
-      <c r="B27" s="59" t="s">
-        <v>358</v>
-      </c>
-      <c r="C27" s="92"/>
-      <c r="D27" s="39"/>
-    </row>
+    <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="49"/>
       <c r="B28" s="57" t="s">
@@ -8369,6 +8467,7 @@
       <c r="C35" s="90">
         <v>2700</v>
       </c>
+      <c r="D35" s="39"/>
     </row>
     <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="49"/>
@@ -8376,6 +8475,7 @@
         <v>371</v>
       </c>
       <c r="C36" s="91"/>
+      <c r="D36" s="39"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="49"/>
@@ -8383,6 +8483,7 @@
         <v>372</v>
       </c>
       <c r="C37" s="91"/>
+      <c r="D37" s="39"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="49"/>
@@ -8390,6 +8491,7 @@
         <v>373</v>
       </c>
       <c r="C38" s="91"/>
+      <c r="D38" s="39"/>
     </row>
     <row r="39" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="49"/>
@@ -8397,240 +8499,341 @@
         <v>374</v>
       </c>
       <c r="C39" s="92"/>
+      <c r="D39" s="39"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="49"/>
-      <c r="B40" s="71"/>
-      <c r="C40" s="72"/>
-    </row>
-    <row r="41" spans="1:4" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="52"/>
-      <c r="B41" s="53"/>
-      <c r="C41" s="54"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="44"/>
-      <c r="B42" s="44" t="s">
+      <c r="B40" s="58" t="s">
+        <v>357</v>
+      </c>
+      <c r="C40" s="91">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="49"/>
+      <c r="B41" s="59" t="s">
+        <v>358</v>
+      </c>
+      <c r="C41" s="92"/>
+    </row>
+    <row r="42" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A42" s="49"/>
+      <c r="B42" s="57" t="s">
+        <v>377</v>
+      </c>
+      <c r="C42" s="90">
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="49"/>
+      <c r="B43" s="58" t="s">
+        <v>378</v>
+      </c>
+      <c r="C43" s="91"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="49"/>
+      <c r="B44" s="58" t="s">
+        <v>379</v>
+      </c>
+      <c r="C44" s="91"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="49"/>
+      <c r="B45" s="58" t="s">
+        <v>380</v>
+      </c>
+      <c r="C45" s="91"/>
+    </row>
+    <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" s="49"/>
+      <c r="B46" s="58" t="s">
+        <v>382</v>
+      </c>
+      <c r="C46" s="91"/>
+    </row>
+    <row r="47" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="49"/>
+      <c r="B47" s="59" t="s">
+        <v>383</v>
+      </c>
+      <c r="C47" s="92"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="49"/>
+      <c r="B48" s="71"/>
+      <c r="C48" s="72"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="49"/>
+      <c r="B49" s="71"/>
+      <c r="C49" s="72"/>
+    </row>
+    <row r="50" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="52"/>
+      <c r="B50" s="53"/>
+      <c r="C50" s="54"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="44"/>
+      <c r="B51" s="44" t="s">
         <v>332</v>
       </c>
-      <c r="C42" s="47">
-        <f>SUM(C2:C41)</f>
-        <v>93550</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
+      <c r="C51" s="47">
+        <f>SUM(C2:C50)</f>
+        <v>96250</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="44" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="45">
+    <row r="53" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="45">
         <v>45109</v>
       </c>
-      <c r="B44" s="42" t="s">
+      <c r="B53" s="42" t="s">
         <v>333</v>
       </c>
-      <c r="C44" s="46">
+      <c r="C53" s="46">
         <v>10000</v>
       </c>
     </row>
-    <row r="45" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="42"/>
-      <c r="B45" s="42" t="s">
+    <row r="54" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="42"/>
+      <c r="B54" s="42" t="s">
         <v>334</v>
       </c>
-      <c r="C45" s="46">
+      <c r="C54" s="46">
         <v>5000</v>
       </c>
     </row>
-    <row r="46" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="45">
+    <row r="55" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="45">
         <v>45278</v>
       </c>
-      <c r="B46" s="42" t="s">
+      <c r="B55" s="42" t="s">
         <v>334</v>
       </c>
-      <c r="C46" s="46">
+      <c r="C55" s="46">
         <v>9800</v>
       </c>
     </row>
-    <row r="47" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="45">
+    <row r="56" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="45">
         <v>45347</v>
       </c>
-      <c r="B47" s="42" t="s">
+      <c r="B56" s="42" t="s">
         <v>334</v>
       </c>
-      <c r="C47" s="46">
+      <c r="C56" s="46">
         <v>5000</v>
       </c>
     </row>
-    <row r="48" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="45">
+    <row r="57" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="45">
         <v>45383</v>
       </c>
-      <c r="B48" s="42" t="s">
+      <c r="B57" s="42" t="s">
         <v>334</v>
       </c>
-      <c r="C48" s="46">
+      <c r="C57" s="46">
         <v>5000</v>
       </c>
     </row>
-    <row r="49" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="45">
+    <row r="58" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="45">
         <v>45384</v>
       </c>
-      <c r="B49" s="42" t="s">
+      <c r="B58" s="42" t="s">
         <v>334</v>
       </c>
-      <c r="C49" s="46">
+      <c r="C58" s="46">
         <v>5000</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="56">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="56">
         <v>45419</v>
       </c>
-      <c r="B50" s="49" t="s">
+      <c r="B59" s="49" t="s">
         <v>334</v>
       </c>
-      <c r="C50" s="55">
+      <c r="C59" s="55">
         <v>5000</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="56">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="56">
         <v>45449</v>
       </c>
-      <c r="B51" s="49" t="s">
+      <c r="B60" s="49" t="s">
         <v>334</v>
       </c>
-      <c r="C51" s="55">
+      <c r="C60" s="55">
         <v>10000</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="56">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="56">
         <v>45465</v>
       </c>
-      <c r="B52" s="49" t="s">
+      <c r="B61" s="49" t="s">
         <v>335</v>
       </c>
-      <c r="C52" s="55">
+      <c r="C61" s="55">
         <v>2000</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="56"/>
-      <c r="B53" s="49" t="s">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="56"/>
+      <c r="B62" s="49" t="s">
         <v>336</v>
       </c>
-      <c r="C53" s="55">
+      <c r="C62" s="55">
         <v>5000</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="56">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="56">
         <v>45506</v>
       </c>
-      <c r="B54" s="49" t="s">
+      <c r="B63" s="49" t="s">
         <v>335</v>
       </c>
-      <c r="C54" s="55">
+      <c r="C63" s="55">
         <v>15000</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="56">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="56">
         <v>45556</v>
       </c>
-      <c r="B55" s="49" t="s">
+      <c r="B64" s="49" t="s">
         <v>334</v>
       </c>
-      <c r="C55" s="55">
+      <c r="C64" s="55">
         <v>5000</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="56"/>
-      <c r="B56" s="49" t="s">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="56"/>
+      <c r="B65" s="49" t="s">
         <v>334</v>
       </c>
-      <c r="C56" s="55">
+      <c r="C65" s="55">
         <v>3000</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="49"/>
-      <c r="B57" s="49" t="s">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="49"/>
+      <c r="B66" s="49" t="s">
         <v>334</v>
       </c>
-      <c r="C57" s="55">
+      <c r="C66" s="55">
         <v>2300</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="49"/>
-      <c r="B58" s="49"/>
-      <c r="C58" s="55">
-        <v>2250</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="49"/>
-      <c r="B59" s="49"/>
-      <c r="C59" s="55"/>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="49"/>
-      <c r="B60" s="49"/>
-      <c r="C60" s="55"/>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="44"/>
-      <c r="B61" s="44" t="s">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="56">
+        <v>45804</v>
+      </c>
+      <c r="B67" s="49" t="s">
+        <v>381</v>
+      </c>
+      <c r="C67" s="55">
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="49"/>
+      <c r="B68" s="49"/>
+      <c r="C68" s="55"/>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="49"/>
+      <c r="B69" s="49"/>
+      <c r="C69" s="55"/>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="44"/>
+      <c r="B70" s="44" t="s">
         <v>337</v>
       </c>
-      <c r="C61" s="47">
-        <f>SUM(C43:C60)</f>
-        <v>89350</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="7"/>
-      <c r="B62" s="7" t="s">
+      <c r="C70" s="47">
+        <f>SUM(C52:C69)</f>
+        <v>89800</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="7"/>
+      <c r="B71" s="7" t="s">
         <v>338</v>
       </c>
-      <c r="C62" s="48">
-        <f>C42-C61</f>
-        <v>4200</v>
-      </c>
-    </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B67" s="14"/>
-    </row>
-    <row r="78" spans="2:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="B78" s="14" t="s">
+      <c r="C71" s="48">
+        <f>C51-C70</f>
+        <v>6450</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B76" s="14"/>
+    </row>
+    <row r="87" spans="2:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="B87" s="14" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B79" s="14"/>
-    </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B81" s="14"/>
-    </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B83" s="14"/>
+    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B88" s="14"/>
+    </row>
+    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B90" s="14"/>
+    </row>
+    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B92" s="14"/>
+    </row>
+    <row r="101" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B101" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="102" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B102" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="103" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B103" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="104" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B104" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="105" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B105" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="106" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B106" t="s">
+        <v>383</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
+    <mergeCell ref="C42:C47"/>
     <mergeCell ref="C35:C39"/>
     <mergeCell ref="C30:C34"/>
     <mergeCell ref="C19:C21"/>
     <mergeCell ref="C22:C23"/>
     <mergeCell ref="C24:C25"/>
-    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="C40:C41"/>
     <mergeCell ref="C28:C29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8640,10 +8843,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6078F90-1BFA-44D9-9906-5A72B5F0645C}">
-  <dimension ref="A1:D57"/>
+  <dimension ref="A1:D66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8789,6 +8992,7 @@
       <c r="C15" s="90">
         <v>2700</v>
       </c>
+      <c r="D15" s="39"/>
     </row>
     <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="49"/>
@@ -8796,167 +9000,244 @@
         <v>371</v>
       </c>
       <c r="C16" s="91"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" s="39"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="49"/>
       <c r="B17" s="58" t="s">
         <v>372</v>
       </c>
       <c r="C17" s="91"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" s="39"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="49"/>
       <c r="B18" s="58" t="s">
         <v>376</v>
       </c>
       <c r="C18" s="91"/>
-    </row>
-    <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D18" s="39"/>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="49"/>
       <c r="B19" s="59" t="s">
         <v>374</v>
       </c>
       <c r="C19" s="92"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" s="39"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="49"/>
-      <c r="B20" s="71"/>
-      <c r="C20" s="72"/>
-    </row>
-    <row r="21" spans="1:3" s="43" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="52"/>
-      <c r="B21" s="53"/>
-      <c r="C21" s="54"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="44"/>
-      <c r="B22" s="44" t="s">
+      <c r="B20" s="58" t="s">
+        <v>357</v>
+      </c>
+      <c r="C20" s="91">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="49"/>
+      <c r="B21" s="59" t="s">
+        <v>358</v>
+      </c>
+      <c r="C21" s="92"/>
+    </row>
+    <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="49"/>
+      <c r="B22" s="57" t="s">
+        <v>377</v>
+      </c>
+      <c r="C22" s="90">
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="49"/>
+      <c r="B23" s="58" t="s">
+        <v>378</v>
+      </c>
+      <c r="C23" s="91"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="49"/>
+      <c r="B24" s="58" t="s">
+        <v>379</v>
+      </c>
+      <c r="C24" s="91"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="49"/>
+      <c r="B25" s="58" t="s">
+        <v>380</v>
+      </c>
+      <c r="C25" s="91"/>
+    </row>
+    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="49"/>
+      <c r="B26" s="58" t="s">
+        <v>382</v>
+      </c>
+      <c r="C26" s="91"/>
+    </row>
+    <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="49"/>
+      <c r="B27" s="59" t="s">
+        <v>383</v>
+      </c>
+      <c r="C27" s="92"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="49"/>
+      <c r="B28" s="71"/>
+      <c r="C28" s="72"/>
+    </row>
+    <row r="29" spans="1:4" s="43" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="52"/>
+      <c r="B29" s="53"/>
+      <c r="C29" s="54"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="44"/>
+      <c r="B30" s="44" t="s">
         <v>332</v>
       </c>
-      <c r="C22" s="47">
-        <f>SUM(C2:C21)</f>
+      <c r="C30" s="47">
+        <f>SUM(C2:C29)</f>
+        <v>11450</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="56">
+        <v>45690</v>
+      </c>
+      <c r="B32" s="49" t="s">
+        <v>120</v>
+      </c>
+      <c r="C32" s="55">
+        <v>2300</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="56"/>
+      <c r="B33" s="49" t="s">
+        <v>120</v>
+      </c>
+      <c r="C33" s="55">
+        <v>2250</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="56">
+        <v>45804</v>
+      </c>
+      <c r="B34" s="49" t="s">
+        <v>381</v>
+      </c>
+      <c r="C34" s="55">
+        <v>2700</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="49"/>
+      <c r="B35" s="49"/>
+      <c r="C35" s="55"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="44"/>
+      <c r="B36" s="44" t="s">
+        <v>337</v>
+      </c>
+      <c r="C36" s="47">
+        <f>SUM(C31:C35)</f>
         <v>7250</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="56">
-        <v>45690</v>
-      </c>
-      <c r="B24" s="49" t="s">
-        <v>120</v>
-      </c>
-      <c r="C24" s="55">
-        <v>2300</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="56"/>
-      <c r="B25" s="49" t="s">
-        <v>120</v>
-      </c>
-      <c r="C25" s="55">
-        <v>2250</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="49"/>
-      <c r="B26" s="49"/>
-      <c r="C26" s="55"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="44"/>
-      <c r="B27" s="44" t="s">
-        <v>337</v>
-      </c>
-      <c r="C27" s="47">
-        <f>SUM(C23:C26)</f>
-        <v>4550</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
-      <c r="B28" s="7" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="7"/>
+      <c r="B37" s="7" t="s">
         <v>338</v>
       </c>
-      <c r="C28" s="48">
-        <f>C22-C27</f>
-        <v>2700</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" s="14"/>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B35" s="14" t="s">
+      <c r="C37" s="48">
+        <f>C30-C36</f>
+        <v>4200</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B42" s="14"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B44" s="14" t="s">
         <v>365</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B36" s="14" t="s">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B45" s="14" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B37" s="14" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B46" s="14" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B38" s="14" t="s">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B47" s="14" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B39" s="14" t="s">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B48" s="14" t="s">
         <v>369</v>
       </c>
     </row>
-    <row r="44" spans="2:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="B44" s="14" t="s">
+    <row r="53" spans="2:2" ht="90" x14ac:dyDescent="0.25">
+      <c r="B53" s="14" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B45" s="14"/>
-    </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B47" s="14"/>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B49" s="14"/>
-    </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B53" s="14" t="s">
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B54" s="14"/>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B56" s="14"/>
+    </row>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B58" s="14"/>
+    </row>
+    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B62" s="14" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="54" spans="2:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="B54" s="14" t="s">
+    <row r="63" spans="2:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="B63" s="14" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B55" s="14" t="s">
+    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B64" s="14" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B56" s="14" t="s">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B65" s="14" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B57" s="14" t="s">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B66" s="14" t="s">
         <v>374</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="C22:C27"/>
     <mergeCell ref="C2:C4"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="C8:C9"/>
@@ -8964,6 +9245,7 @@
     <mergeCell ref="C15:C19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Se suben los ajustes.
Funcionalidad de control de acciones y permisos
Agregar el grupo en la descripción del producto en la verificación, catalogos de productos, devolución
Cambio de precio con permiso especial, cambio de precio en verificación de productos, poder asignar precio en el alta de inventario para que se apruebe en la autorización de la entrada
</commit_message>
<xml_diff>
--- a/Documents/Actividades realizadas/ActividadesN_.xlsx
+++ b/Documents/Actividades realizadas/ActividadesN_.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\1.- VioletaSystem\Documents\Actividades realizadas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAAB1EDB-2D42-4952-8641-9CE2F2B9DD1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CDEF212-9CAE-4DA0-A3D0-AD490B8E5DA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HORAS" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="722" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="305">
   <si>
     <t>Descripción</t>
   </si>
@@ -949,6 +949,9 @@
   </si>
   <si>
     <t>Agregar el grupo en la descripción del producto en la verificación, catalogos de productos, devolución</t>
+  </si>
+  <si>
+    <t>Cambio de precio con permiso especial, cambio de precio en verificación de productos, poder asignar precio en el alta de inventario para que se apruebe en la autorización de la entrada</t>
   </si>
 </sst>
 </file>
@@ -1099,7 +1102,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -1227,6 +1230,21 @@
         <color indexed="64"/>
       </right>
       <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -1373,9 +1391,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="9" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="0" fillId="10" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1384,30 +1399,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="3" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1424,6 +1415,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1433,10 +1427,28 @@
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="44" fontId="0" fillId="10" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="10" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="10" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1449,6 +1461,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="10" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="10" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="10" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1769,8 +1787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K338"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A279" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A270" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D295" sqref="D295"/>
     </sheetView>
   </sheetViews>
@@ -7546,12 +7564,23 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="295" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A295" s="5"/>
-      <c r="C295" s="61"/>
-      <c r="D295" s="13"/>
-      <c r="E295" s="2"/>
-      <c r="F295" s="2"/>
+      <c r="C295" s="61">
+        <v>45663</v>
+      </c>
+      <c r="D295" s="13" t="s">
+        <v>304</v>
+      </c>
+      <c r="E295" s="2">
+        <v>0.3611111111111111</v>
+      </c>
+      <c r="F295" s="2">
+        <v>0.49652777777777779</v>
+      </c>
+      <c r="H295" s="14">
+        <v>3</v>
+      </c>
     </row>
     <row r="296" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A296" s="5"/>
@@ -7573,32 +7602,32 @@
       <c r="F298" s="2"/>
     </row>
     <row r="299" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A299" s="73" t="s">
+      <c r="A299" s="81" t="s">
         <v>83</v>
       </c>
-      <c r="B299" s="73"/>
-      <c r="C299" s="73"/>
-      <c r="D299" s="73"/>
-      <c r="E299" s="73"/>
-      <c r="F299" s="73"/>
+      <c r="B299" s="81"/>
+      <c r="C299" s="81"/>
+      <c r="D299" s="81"/>
+      <c r="E299" s="81"/>
+      <c r="F299" s="81"/>
       <c r="G299" s="16">
         <f>SUM(G2:G298)</f>
         <v>314.78999999999996</v>
       </c>
       <c r="H299" s="16">
         <f>SUM(H2:H298)</f>
-        <v>106.3</v>
+        <v>109.3</v>
       </c>
     </row>
     <row r="300" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A300" s="73" t="s">
+      <c r="A300" s="81" t="s">
         <v>57</v>
       </c>
-      <c r="B300" s="73"/>
-      <c r="C300" s="73"/>
-      <c r="D300" s="73"/>
-      <c r="E300" s="73"/>
-      <c r="F300" s="73"/>
+      <c r="B300" s="81"/>
+      <c r="C300" s="81"/>
+      <c r="D300" s="81"/>
+      <c r="E300" s="81"/>
+      <c r="F300" s="81"/>
       <c r="G300" s="16">
         <v>200</v>
       </c>
@@ -7607,81 +7636,81 @@
       </c>
     </row>
     <row r="301" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A301" s="73" t="s">
+      <c r="A301" s="81" t="s">
         <v>84</v>
       </c>
-      <c r="B301" s="73"/>
-      <c r="C301" s="73"/>
-      <c r="D301" s="73"/>
-      <c r="E301" s="73"/>
-      <c r="F301" s="73"/>
+      <c r="B301" s="81"/>
+      <c r="C301" s="81"/>
+      <c r="D301" s="81"/>
+      <c r="E301" s="81"/>
+      <c r="F301" s="81"/>
       <c r="G301" s="17">
         <f>G300*G299</f>
         <v>62957.999999999993</v>
       </c>
       <c r="H301" s="18">
         <f>H300*H299</f>
-        <v>31890</v>
+        <v>32790</v>
       </c>
       <c r="J301">
         <v>-500</v>
       </c>
     </row>
     <row r="302" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A302" s="73" t="s">
+      <c r="A302" s="81" t="s">
         <v>58</v>
       </c>
-      <c r="B302" s="73"/>
-      <c r="C302" s="73"/>
-      <c r="D302" s="73"/>
-      <c r="E302" s="73"/>
-      <c r="F302" s="73"/>
-      <c r="G302" s="78">
+      <c r="B302" s="81"/>
+      <c r="C302" s="81"/>
+      <c r="D302" s="81"/>
+      <c r="E302" s="81"/>
+      <c r="F302" s="81"/>
+      <c r="G302" s="69">
         <f>G301+H301</f>
-        <v>94848</v>
-      </c>
-      <c r="H302" s="78"/>
+        <v>95748</v>
+      </c>
+      <c r="H302" s="69"/>
     </row>
     <row r="303" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A303" s="10"/>
-      <c r="B303" s="81" t="s">
+      <c r="B303" s="72" t="s">
         <v>60</v>
       </c>
-      <c r="C303" s="81"/>
-      <c r="D303" s="81"/>
-      <c r="E303" s="81"/>
-      <c r="F303" s="81"/>
+      <c r="C303" s="72"/>
+      <c r="D303" s="72"/>
+      <c r="E303" s="72"/>
+      <c r="F303" s="72"/>
       <c r="G303" s="21"/>
     </row>
     <row r="304" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A304" s="11">
         <v>45109</v>
       </c>
-      <c r="B304" s="82" t="s">
+      <c r="B304" s="73" t="s">
         <v>59</v>
       </c>
-      <c r="C304" s="82"/>
-      <c r="D304" s="82"/>
-      <c r="E304" s="82"/>
-      <c r="F304" s="82"/>
-      <c r="G304" s="83">
+      <c r="C304" s="73"/>
+      <c r="D304" s="73"/>
+      <c r="E304" s="73"/>
+      <c r="F304" s="73"/>
+      <c r="G304" s="75">
         <v>10000</v>
       </c>
-      <c r="H304" s="83"/>
+      <c r="H304" s="75"/>
     </row>
     <row r="305" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A305" s="11"/>
-      <c r="B305" s="85" t="s">
+      <c r="B305" s="77" t="s">
         <v>96</v>
       </c>
-      <c r="C305" s="85"/>
-      <c r="D305" s="85"/>
-      <c r="E305" s="85"/>
-      <c r="F305" s="85"/>
-      <c r="G305" s="83">
+      <c r="C305" s="77"/>
+      <c r="D305" s="77"/>
+      <c r="E305" s="77"/>
+      <c r="F305" s="77"/>
+      <c r="G305" s="75">
         <v>5000</v>
       </c>
-      <c r="H305" s="83"/>
+      <c r="H305" s="75"/>
     </row>
     <row r="306" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A306" s="11">
@@ -7694,10 +7723,10 @@
       <c r="D306" s="74"/>
       <c r="E306" s="74"/>
       <c r="F306" s="74"/>
-      <c r="G306" s="83">
+      <c r="G306" s="75">
         <v>9800</v>
       </c>
-      <c r="H306" s="83"/>
+      <c r="H306" s="75"/>
     </row>
     <row r="307" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A307" s="11"/>
@@ -7706,8 +7735,8 @@
       <c r="D307" s="74"/>
       <c r="E307" s="74"/>
       <c r="F307" s="74"/>
-      <c r="G307" s="84"/>
-      <c r="H307" s="84"/>
+      <c r="G307" s="76"/>
+      <c r="H307" s="76"/>
     </row>
     <row r="308" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A308" s="11"/>
@@ -7716,8 +7745,8 @@
       <c r="D308" s="74"/>
       <c r="E308" s="74"/>
       <c r="F308" s="74"/>
-      <c r="G308" s="84"/>
-      <c r="H308" s="84"/>
+      <c r="G308" s="76"/>
+      <c r="H308" s="76"/>
     </row>
     <row r="309" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A309" s="11"/>
@@ -7726,8 +7755,8 @@
       <c r="D309" s="74"/>
       <c r="E309" s="74"/>
       <c r="F309" s="74"/>
-      <c r="G309" s="84"/>
-      <c r="H309" s="84"/>
+      <c r="G309" s="76"/>
+      <c r="H309" s="76"/>
     </row>
     <row r="310" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A310" s="11"/>
@@ -7738,26 +7767,26 @@
       <c r="D310" s="74"/>
       <c r="E310" s="74"/>
       <c r="F310" s="74"/>
-      <c r="G310" s="83">
+      <c r="G310" s="75">
         <f>SUM(G304:H309)</f>
         <v>24800</v>
       </c>
-      <c r="H310" s="83"/>
+      <c r="H310" s="75"/>
     </row>
     <row r="311" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A311" s="79" t="s">
+      <c r="A311" s="70" t="s">
         <v>61</v>
       </c>
-      <c r="B311" s="79"/>
-      <c r="C311" s="79"/>
-      <c r="D311" s="79"/>
-      <c r="E311" s="79"/>
-      <c r="F311" s="79"/>
-      <c r="G311" s="80">
+      <c r="B311" s="70"/>
+      <c r="C311" s="70"/>
+      <c r="D311" s="70"/>
+      <c r="E311" s="70"/>
+      <c r="F311" s="70"/>
+      <c r="G311" s="71">
         <f>G302-G310</f>
-        <v>70048</v>
-      </c>
-      <c r="H311" s="80"/>
+        <v>70948</v>
+      </c>
+      <c r="H311" s="71"/>
     </row>
     <row r="312" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A312" s="11"/>
@@ -7905,33 +7934,33 @@
     </row>
     <row r="330" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A330" s="9"/>
-      <c r="B330" s="75" t="s">
+      <c r="B330" s="82" t="s">
         <v>56</v>
       </c>
-      <c r="C330" s="75"/>
-      <c r="D330" s="75"/>
-      <c r="E330" s="75"/>
-      <c r="F330" s="75"/>
+      <c r="C330" s="82"/>
+      <c r="D330" s="82"/>
+      <c r="E330" s="82"/>
+      <c r="F330" s="82"/>
       <c r="G330" s="20"/>
       <c r="H330" s="20"/>
       <c r="I330" s="7">
         <f>G299+H299</f>
-        <v>421.09</v>
+        <v>424.09</v>
       </c>
       <c r="J330" s="7">
         <f>I330</f>
-        <v>421.09</v>
+        <v>424.09</v>
       </c>
     </row>
     <row r="331" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A331" s="5"/>
-      <c r="B331" s="76" t="s">
+      <c r="B331" s="83" t="s">
         <v>57</v>
       </c>
-      <c r="C331" s="76"/>
-      <c r="D331" s="76"/>
-      <c r="E331" s="76"/>
-      <c r="F331" s="76"/>
+      <c r="C331" s="83"/>
+      <c r="D331" s="83"/>
+      <c r="E331" s="83"/>
+      <c r="F331" s="83"/>
       <c r="I331" s="7">
         <v>300</v>
       </c>
@@ -7941,31 +7970,31 @@
     </row>
     <row r="332" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A332" s="5"/>
-      <c r="B332" s="76" t="s">
+      <c r="B332" s="83" t="s">
         <v>58</v>
       </c>
-      <c r="C332" s="76"/>
-      <c r="D332" s="76"/>
-      <c r="E332" s="76"/>
-      <c r="F332" s="76"/>
+      <c r="C332" s="83"/>
+      <c r="D332" s="83"/>
+      <c r="E332" s="83"/>
+      <c r="F332" s="83"/>
       <c r="I332" s="8">
         <f>I331*I330</f>
-        <v>126326.99999999999</v>
+        <v>127226.99999999999</v>
       </c>
       <c r="J332" s="8">
         <f>J331*J330</f>
-        <v>84218</v>
+        <v>84818</v>
       </c>
     </row>
     <row r="333" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A333" s="22"/>
-      <c r="B333" s="77" t="s">
+      <c r="B333" s="84" t="s">
         <v>60</v>
       </c>
-      <c r="C333" s="77"/>
-      <c r="D333" s="77"/>
-      <c r="E333" s="77"/>
-      <c r="F333" s="77"/>
+      <c r="C333" s="84"/>
+      <c r="D333" s="84"/>
+      <c r="E333" s="84"/>
+      <c r="F333" s="84"/>
       <c r="G333" s="23"/>
       <c r="H333" s="23"/>
       <c r="I333" s="24"/>
@@ -7975,13 +8004,13 @@
       <c r="A334" s="25">
         <v>45109</v>
       </c>
-      <c r="B334" s="71" t="s">
+      <c r="B334" s="79" t="s">
         <v>59</v>
       </c>
-      <c r="C334" s="71"/>
-      <c r="D334" s="71"/>
-      <c r="E334" s="71"/>
-      <c r="F334" s="71"/>
+      <c r="C334" s="79"/>
+      <c r="D334" s="79"/>
+      <c r="E334" s="79"/>
+      <c r="F334" s="79"/>
       <c r="G334" s="26"/>
       <c r="H334" s="26"/>
       <c r="I334" s="27">
@@ -8017,13 +8046,13 @@
     </row>
     <row r="337" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A337" s="25"/>
-      <c r="B337" s="72" t="s">
+      <c r="B337" s="80" t="s">
         <v>62</v>
       </c>
-      <c r="C337" s="72"/>
-      <c r="D337" s="72"/>
-      <c r="E337" s="72"/>
-      <c r="F337" s="72"/>
+      <c r="C337" s="80"/>
+      <c r="D337" s="80"/>
+      <c r="E337" s="80"/>
+      <c r="F337" s="80"/>
       <c r="G337" s="26"/>
       <c r="H337" s="26"/>
       <c r="I337" s="30">
@@ -8039,26 +8068,39 @@
       <c r="A338" s="31">
         <v>45109</v>
       </c>
-      <c r="B338" s="70" t="s">
+      <c r="B338" s="78" t="s">
         <v>61</v>
       </c>
-      <c r="C338" s="70"/>
-      <c r="D338" s="70"/>
-      <c r="E338" s="70"/>
-      <c r="F338" s="70"/>
+      <c r="C338" s="78"/>
+      <c r="D338" s="78"/>
+      <c r="E338" s="78"/>
+      <c r="F338" s="78"/>
       <c r="G338" s="32"/>
       <c r="H338" s="32"/>
       <c r="I338" s="33">
         <f>I332-I337</f>
-        <v>116326.99999999999</v>
+        <v>117226.99999999999</v>
       </c>
       <c r="J338" s="33">
         <f>J332-J337</f>
-        <v>74218</v>
+        <v>74818</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="B338:F338"/>
+    <mergeCell ref="B334:F334"/>
+    <mergeCell ref="B337:F337"/>
+    <mergeCell ref="A300:F300"/>
+    <mergeCell ref="A299:F299"/>
+    <mergeCell ref="A301:F301"/>
+    <mergeCell ref="A302:F302"/>
+    <mergeCell ref="B308:F308"/>
+    <mergeCell ref="B309:F309"/>
+    <mergeCell ref="B330:F330"/>
+    <mergeCell ref="B331:F331"/>
+    <mergeCell ref="B332:F332"/>
+    <mergeCell ref="B333:F333"/>
     <mergeCell ref="G302:H302"/>
     <mergeCell ref="A311:F311"/>
     <mergeCell ref="G311:H311"/>
@@ -8075,19 +8117,6 @@
     <mergeCell ref="B306:F306"/>
     <mergeCell ref="B305:F305"/>
     <mergeCell ref="B307:F307"/>
-    <mergeCell ref="B338:F338"/>
-    <mergeCell ref="B334:F334"/>
-    <mergeCell ref="B337:F337"/>
-    <mergeCell ref="A300:F300"/>
-    <mergeCell ref="A299:F299"/>
-    <mergeCell ref="A301:F301"/>
-    <mergeCell ref="A302:F302"/>
-    <mergeCell ref="B308:F308"/>
-    <mergeCell ref="B309:F309"/>
-    <mergeCell ref="B330:F330"/>
-    <mergeCell ref="B331:F331"/>
-    <mergeCell ref="B332:F332"/>
-    <mergeCell ref="B333:F333"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -8295,7 +8324,7 @@
       <c r="B19" s="56" t="s">
         <v>226</v>
       </c>
-      <c r="C19" s="89">
+      <c r="C19" s="87">
         <v>1100</v>
       </c>
       <c r="D19" s="38"/>
@@ -8305,7 +8334,7 @@
       <c r="B20" s="57" t="s">
         <v>227</v>
       </c>
-      <c r="C20" s="90"/>
+      <c r="C20" s="88"/>
       <c r="D20" s="38"/>
     </row>
     <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8313,7 +8342,7 @@
       <c r="B21" s="58" t="s">
         <v>228</v>
       </c>
-      <c r="C21" s="91"/>
+      <c r="C21" s="89"/>
       <c r="D21" s="38"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -8321,7 +8350,7 @@
       <c r="B22" s="56" t="s">
         <v>255</v>
       </c>
-      <c r="C22" s="89">
+      <c r="C22" s="87">
         <v>600</v>
       </c>
       <c r="D22" s="38"/>
@@ -8331,7 +8360,7 @@
       <c r="B23" s="58" t="s">
         <v>256</v>
       </c>
-      <c r="C23" s="91"/>
+      <c r="C23" s="89"/>
       <c r="D23" s="38"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -8339,7 +8368,7 @@
       <c r="B24" s="56" t="s">
         <v>255</v>
       </c>
-      <c r="C24" s="89">
+      <c r="C24" s="87">
         <v>600</v>
       </c>
       <c r="D24" s="38"/>
@@ -8349,7 +8378,7 @@
       <c r="B25" s="58" t="s">
         <v>256</v>
       </c>
-      <c r="C25" s="91"/>
+      <c r="C25" s="89"/>
       <c r="D25" s="38"/>
     </row>
     <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -8358,7 +8387,7 @@
       <c r="B28" s="56" t="s">
         <v>260</v>
       </c>
-      <c r="C28" s="89">
+      <c r="C28" s="87">
         <v>900</v>
       </c>
       <c r="D28" s="38"/>
@@ -8368,7 +8397,7 @@
       <c r="B29" s="58" t="s">
         <v>261</v>
       </c>
-      <c r="C29" s="91"/>
+      <c r="C29" s="89"/>
       <c r="D29" s="38"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -8376,7 +8405,7 @@
       <c r="B30" s="56" t="s">
         <v>262</v>
       </c>
-      <c r="C30" s="89">
+      <c r="C30" s="87">
         <v>1350</v>
       </c>
       <c r="D30" s="38"/>
@@ -8386,7 +8415,7 @@
       <c r="B31" s="57" t="s">
         <v>263</v>
       </c>
-      <c r="C31" s="90"/>
+      <c r="C31" s="88"/>
       <c r="D31" s="38"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -8394,7 +8423,7 @@
       <c r="B32" s="57" t="s">
         <v>264</v>
       </c>
-      <c r="C32" s="90"/>
+      <c r="C32" s="88"/>
       <c r="D32" s="38"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -8402,7 +8431,7 @@
       <c r="B33" s="57" t="s">
         <v>265</v>
       </c>
-      <c r="C33" s="90"/>
+      <c r="C33" s="88"/>
       <c r="D33" s="38"/>
     </row>
     <row r="34" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8410,7 +8439,7 @@
       <c r="B34" s="58" t="s">
         <v>266</v>
       </c>
-      <c r="C34" s="91"/>
+      <c r="C34" s="89"/>
       <c r="D34" s="38"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -8418,7 +8447,7 @@
       <c r="B35" s="56" t="s">
         <v>267</v>
       </c>
-      <c r="C35" s="89">
+      <c r="C35" s="87">
         <v>2700</v>
       </c>
       <c r="D35" s="38"/>
@@ -8428,7 +8457,7 @@
       <c r="B36" s="57" t="s">
         <v>268</v>
       </c>
-      <c r="C36" s="90"/>
+      <c r="C36" s="88"/>
       <c r="D36" s="38"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -8436,7 +8465,7 @@
       <c r="B37" s="57" t="s">
         <v>269</v>
       </c>
-      <c r="C37" s="90"/>
+      <c r="C37" s="88"/>
       <c r="D37" s="38"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -8444,7 +8473,7 @@
       <c r="B38" s="57" t="s">
         <v>270</v>
       </c>
-      <c r="C38" s="90"/>
+      <c r="C38" s="88"/>
       <c r="D38" s="38"/>
     </row>
     <row r="39" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8452,7 +8481,7 @@
       <c r="B39" s="58" t="s">
         <v>271</v>
       </c>
-      <c r="C39" s="91"/>
+      <c r="C39" s="89"/>
       <c r="D39" s="38"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -8460,7 +8489,7 @@
       <c r="B40" s="57" t="s">
         <v>257</v>
       </c>
-      <c r="C40" s="90">
+      <c r="C40" s="88">
         <v>1500</v>
       </c>
     </row>
@@ -8469,14 +8498,14 @@
       <c r="B41" s="58" t="s">
         <v>258</v>
       </c>
-      <c r="C41" s="91"/>
+      <c r="C41" s="89"/>
     </row>
     <row r="42" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="48"/>
       <c r="B42" s="56" t="s">
         <v>274</v>
       </c>
-      <c r="C42" s="89">
+      <c r="C42" s="87">
         <v>2700</v>
       </c>
     </row>
@@ -8485,95 +8514,95 @@
       <c r="B43" s="57" t="s">
         <v>275</v>
       </c>
-      <c r="C43" s="90"/>
+      <c r="C43" s="88"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="48"/>
       <c r="B44" s="57" t="s">
         <v>276</v>
       </c>
-      <c r="C44" s="90"/>
+      <c r="C44" s="88"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="48"/>
       <c r="B45" s="57" t="s">
         <v>277</v>
       </c>
-      <c r="C45" s="90"/>
+      <c r="C45" s="88"/>
     </row>
     <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="48"/>
       <c r="B46" s="57" t="s">
         <v>279</v>
       </c>
-      <c r="C46" s="90"/>
+      <c r="C46" s="88"/>
     </row>
     <row r="47" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="48"/>
       <c r="B47" s="58" t="s">
         <v>280</v>
       </c>
-      <c r="C47" s="91"/>
+      <c r="C47" s="89"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="48"/>
-      <c r="B48" s="67" t="s">
+      <c r="B48" s="66" t="s">
         <v>281</v>
       </c>
-      <c r="C48" s="86">
+      <c r="C48" s="85">
         <v>3000</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="48"/>
-      <c r="B49" s="68" t="s">
+      <c r="B49" s="67" t="s">
         <v>282</v>
       </c>
-      <c r="C49" s="87"/>
+      <c r="C49" s="90"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="48"/>
-      <c r="B50" s="68" t="s">
+      <c r="B50" s="67" t="s">
         <v>287</v>
       </c>
-      <c r="C50" s="87"/>
+      <c r="C50" s="90"/>
     </row>
     <row r="51" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="48"/>
-      <c r="B51" s="69" t="s">
+      <c r="B51" s="68" t="s">
         <v>292</v>
       </c>
-      <c r="C51" s="88"/>
+      <c r="C51" s="86"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="48"/>
-      <c r="B52" s="67" t="s">
+      <c r="B52" s="66" t="s">
         <v>293</v>
       </c>
-      <c r="C52" s="86">
+      <c r="C52" s="85">
         <v>1500</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="48"/>
-      <c r="B53" s="68" t="s">
+      <c r="B53" s="67" t="s">
         <v>294</v>
       </c>
-      <c r="C53" s="87"/>
+      <c r="C53" s="90"/>
     </row>
     <row r="54" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="48"/>
-      <c r="B54" s="69" t="s">
+      <c r="B54" s="68" t="s">
         <v>295</v>
       </c>
-      <c r="C54" s="88"/>
+      <c r="C54" s="86"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="48"/>
       <c r="B55" s="56" t="s">
         <v>302</v>
       </c>
-      <c r="C55" s="86">
+      <c r="C55" s="85">
         <v>1200</v>
       </c>
     </row>
@@ -8582,7 +8611,7 @@
       <c r="B56" s="58" t="s">
         <v>303</v>
       </c>
-      <c r="C56" s="88"/>
+      <c r="C56" s="86"/>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="48"/>
@@ -8903,10 +8932,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6078F90-1BFA-44D9-9906-5A72B5F0645C}">
-  <dimension ref="A1:D54"/>
+  <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8935,7 +8964,7 @@
       <c r="B2" s="56" t="s">
         <v>226</v>
       </c>
-      <c r="C2" s="89">
+      <c r="C2" s="87">
         <v>1100</v>
       </c>
       <c r="D2" s="38"/>
@@ -8945,7 +8974,7 @@
       <c r="B3" s="57" t="s">
         <v>227</v>
       </c>
-      <c r="C3" s="90"/>
+      <c r="C3" s="88"/>
       <c r="D3" s="38"/>
     </row>
     <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8953,7 +8982,7 @@
       <c r="B4" s="58" t="s">
         <v>228</v>
       </c>
-      <c r="C4" s="91"/>
+      <c r="C4" s="89"/>
       <c r="D4" s="38"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -8961,7 +8990,7 @@
       <c r="B5" s="56" t="s">
         <v>255</v>
       </c>
-      <c r="C5" s="89">
+      <c r="C5" s="87">
         <v>600</v>
       </c>
       <c r="D5" s="38"/>
@@ -8971,7 +9000,7 @@
       <c r="B6" s="58" t="s">
         <v>256</v>
       </c>
-      <c r="C6" s="91"/>
+      <c r="C6" s="89"/>
       <c r="D6" s="38"/>
     </row>
     <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8989,7 +9018,7 @@
       <c r="B8" s="56" t="s">
         <v>260</v>
       </c>
-      <c r="C8" s="89">
+      <c r="C8" s="87">
         <v>900</v>
       </c>
       <c r="D8" s="38"/>
@@ -8999,7 +9028,7 @@
       <c r="B9" s="58" t="s">
         <v>261</v>
       </c>
-      <c r="C9" s="91"/>
+      <c r="C9" s="89"/>
       <c r="D9" s="38"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -9007,7 +9036,7 @@
       <c r="B10" s="56" t="s">
         <v>262</v>
       </c>
-      <c r="C10" s="89">
+      <c r="C10" s="87">
         <v>1350</v>
       </c>
       <c r="D10" s="38"/>
@@ -9017,7 +9046,7 @@
       <c r="B11" s="57" t="s">
         <v>263</v>
       </c>
-      <c r="C11" s="90"/>
+      <c r="C11" s="88"/>
       <c r="D11" s="38"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -9025,7 +9054,7 @@
       <c r="B12" s="57" t="s">
         <v>264</v>
       </c>
-      <c r="C12" s="90"/>
+      <c r="C12" s="88"/>
       <c r="D12" s="38"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -9033,7 +9062,7 @@
       <c r="B13" s="57" t="s">
         <v>265</v>
       </c>
-      <c r="C13" s="90"/>
+      <c r="C13" s="88"/>
       <c r="D13" s="38"/>
     </row>
     <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9041,7 +9070,7 @@
       <c r="B14" s="58" t="s">
         <v>266</v>
       </c>
-      <c r="C14" s="91"/>
+      <c r="C14" s="89"/>
       <c r="D14" s="38"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -9049,7 +9078,7 @@
       <c r="B15" s="56" t="s">
         <v>267</v>
       </c>
-      <c r="C15" s="89">
+      <c r="C15" s="87">
         <v>2700</v>
       </c>
       <c r="D15" s="38"/>
@@ -9059,7 +9088,7 @@
       <c r="B16" s="57" t="s">
         <v>268</v>
       </c>
-      <c r="C16" s="90"/>
+      <c r="C16" s="88"/>
       <c r="D16" s="38"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -9067,7 +9096,7 @@
       <c r="B17" s="57" t="s">
         <v>269</v>
       </c>
-      <c r="C17" s="90"/>
+      <c r="C17" s="88"/>
       <c r="D17" s="38"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -9075,7 +9104,7 @@
       <c r="B18" s="57" t="s">
         <v>273</v>
       </c>
-      <c r="C18" s="90"/>
+      <c r="C18" s="88"/>
       <c r="D18" s="38"/>
     </row>
     <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9083,7 +9112,7 @@
       <c r="B19" s="58" t="s">
         <v>271</v>
       </c>
-      <c r="C19" s="91"/>
+      <c r="C19" s="89"/>
       <c r="D19" s="38"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -9091,7 +9120,7 @@
       <c r="B20" s="57" t="s">
         <v>257</v>
       </c>
-      <c r="C20" s="90">
+      <c r="C20" s="88">
         <v>1500</v>
       </c>
       <c r="D20" s="38"/>
@@ -9101,7 +9130,7 @@
       <c r="B21" s="58" t="s">
         <v>258</v>
       </c>
-      <c r="C21" s="91"/>
+      <c r="C21" s="89"/>
       <c r="D21" s="38"/>
     </row>
     <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -9109,7 +9138,7 @@
       <c r="B22" s="56" t="s">
         <v>274</v>
       </c>
-      <c r="C22" s="89">
+      <c r="C22" s="87">
         <v>2700</v>
       </c>
       <c r="D22" s="38"/>
@@ -9119,7 +9148,7 @@
       <c r="B23" s="57" t="s">
         <v>275</v>
       </c>
-      <c r="C23" s="90"/>
+      <c r="C23" s="88"/>
       <c r="D23" s="38"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -9127,7 +9156,7 @@
       <c r="B24" s="57" t="s">
         <v>276</v>
       </c>
-      <c r="C24" s="90"/>
+      <c r="C24" s="88"/>
       <c r="D24" s="38"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -9135,7 +9164,7 @@
       <c r="B25" s="57" t="s">
         <v>277</v>
       </c>
-      <c r="C25" s="90"/>
+      <c r="C25" s="88"/>
       <c r="D25" s="38"/>
     </row>
     <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -9143,7 +9172,7 @@
       <c r="B26" s="57" t="s">
         <v>279</v>
       </c>
-      <c r="C26" s="90"/>
+      <c r="C26" s="88"/>
       <c r="D26" s="38"/>
     </row>
     <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9151,104 +9180,115 @@
       <c r="B27" s="58" t="s">
         <v>280</v>
       </c>
-      <c r="C27" s="91"/>
+      <c r="C27" s="89"/>
       <c r="D27" s="38"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="48"/>
-      <c r="B28" s="67" t="s">
+      <c r="B28" s="66" t="s">
         <v>281</v>
       </c>
-      <c r="C28" s="86">
+      <c r="C28" s="85">
         <v>3000</v>
       </c>
+      <c r="D28" s="38"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="48"/>
-      <c r="B29" s="68" t="s">
+      <c r="B29" s="67" t="s">
         <v>282</v>
       </c>
-      <c r="C29" s="87"/>
+      <c r="C29" s="90"/>
+      <c r="D29" s="38"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="48"/>
-      <c r="B30" s="68" t="s">
+      <c r="B30" s="67" t="s">
         <v>287</v>
       </c>
-      <c r="C30" s="87"/>
+      <c r="C30" s="90"/>
+      <c r="D30" s="38"/>
     </row>
     <row r="31" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="48"/>
-      <c r="B31" s="69" t="s">
+      <c r="B31" s="68" t="s">
         <v>292</v>
       </c>
-      <c r="C31" s="88"/>
+      <c r="C31" s="86"/>
+      <c r="D31" s="38"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="48"/>
-      <c r="B32" s="67" t="s">
+      <c r="B32" s="66" t="s">
         <v>293</v>
       </c>
-      <c r="C32" s="86">
+      <c r="C32" s="85">
         <v>1500</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32" s="38"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="48"/>
-      <c r="B33" s="68" t="s">
+      <c r="B33" s="67" t="s">
         <v>294</v>
       </c>
-      <c r="C33" s="87"/>
-    </row>
-    <row r="34" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C33" s="90"/>
+      <c r="D33" s="38"/>
+    </row>
+    <row r="34" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="48"/>
-      <c r="B34" s="69" t="s">
+      <c r="B34" s="68" t="s">
         <v>295</v>
       </c>
-      <c r="C34" s="88"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C34" s="86"/>
+      <c r="D34" s="38"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="48"/>
       <c r="B35" s="56" t="s">
         <v>302</v>
       </c>
-      <c r="C35" s="86">
+      <c r="C35" s="85">
         <v>1200</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="48"/>
       <c r="B36" s="58" t="s">
         <v>303</v>
       </c>
-      <c r="C36" s="88"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C36" s="86"/>
+    </row>
+    <row r="37" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="48"/>
-      <c r="B37" s="62"/>
-      <c r="C37" s="66"/>
-    </row>
-    <row r="38" spans="1:3" s="42" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="58" t="s">
+        <v>304</v>
+      </c>
+      <c r="C37" s="91">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="51"/>
       <c r="B38" s="52"/>
       <c r="C38" s="53"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="43"/>
       <c r="B39" s="43" t="s">
         <v>247</v>
       </c>
       <c r="C39" s="46">
         <f>SUM(C2:C38)</f>
-        <v>17150</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+        <v>18050</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="55">
         <v>45690</v>
       </c>
@@ -9259,7 +9299,7 @@
         <v>2300</v>
       </c>
     </row>
-    <row r="42" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="55"/>
       <c r="B42" s="48" t="s">
         <v>38</v>
@@ -9268,7 +9308,7 @@
         <v>2250</v>
       </c>
     </row>
-    <row r="43" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="55">
         <v>45804</v>
       </c>
@@ -9279,7 +9319,7 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="44" spans="1:3" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="55">
         <v>45839</v>
       </c>
@@ -9290,75 +9330,70 @@
         <v>4200</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="55"/>
       <c r="B45" s="48"/>
       <c r="C45" s="54">
         <v>4500</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="55"/>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="48"/>
       <c r="B46" s="48"/>
       <c r="C46" s="54"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="48"/>
-      <c r="B47" s="48"/>
-      <c r="C47" s="54"/>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="43"/>
-      <c r="B48" s="43" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="43"/>
+      <c r="B47" s="43" t="s">
         <v>252</v>
       </c>
-      <c r="C48" s="46">
-        <f>SUM(C40:C47)</f>
+      <c r="C47" s="46">
+        <f>SUM(C40:C46)</f>
         <v>15950</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="6"/>
-      <c r="B49" s="6" t="s">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="6"/>
+      <c r="B48" s="6" t="s">
         <v>253</v>
       </c>
-      <c r="C49" s="47">
-        <f>C39-C48</f>
-        <v>1200</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C48" s="47">
+        <f>C39-C47</f>
+        <v>2100</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B50" s="13" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B51" s="13" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B52" s="13" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2" ht="30" x14ac:dyDescent="0.25">
       <c r="B53" s="13" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B54" s="13" t="s">
         <v>292</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C10:C14"/>
+    <mergeCell ref="C15:C19"/>
     <mergeCell ref="C35:C36"/>
     <mergeCell ref="C32:C34"/>
     <mergeCell ref="C28:C31"/>
     <mergeCell ref="C20:C21"/>
     <mergeCell ref="C22:C27"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="C10:C14"/>
-    <mergeCell ref="C15:C19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
@@ -9772,7 +9807,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="46" spans="3:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:6" ht="30" x14ac:dyDescent="0.25">
       <c r="C46" s="13" t="s">
         <v>296</v>
       </c>

</xml_diff>

<commit_message>
Se suben los avances de la pantalla de taller
</commit_message>
<xml_diff>
--- a/Documents/Actividades realizadas/ActividadesN_.xlsx
+++ b/Documents/Actividades realizadas/ActividadesN_.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\1.- VioletaSystem\Documents\Actividades realizadas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0936E55-09A4-4D39-8B25-F631DAF9C565}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBDEFCCC-96C7-4C08-8B17-AFF2E010C79A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="725" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="310">
   <si>
     <t>Descripción</t>
   </si>
@@ -955,6 +955,18 @@
   </si>
   <si>
     <t>Agregar el cambio del costo al producto desde la autorización</t>
+  </si>
+  <si>
+    <t>Inicio de Pantalla de taller</t>
+  </si>
+  <si>
+    <t>Alta de encabezado de taller y refacciones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Consulta de lista de TALLERES </t>
+  </si>
+  <si>
+    <t>Consulta de taller y Lista de refacciones para la pantalla de taller</t>
   </si>
 </sst>
 </file>
@@ -1788,11 +1800,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K338"/>
+  <dimension ref="A1:K345"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A288" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J302" sqref="J302"/>
+      <selection pane="bottomLeft" activeCell="D304" sqref="D304"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7459,7 +7471,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="289" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A289" s="5"/>
       <c r="C289" s="9">
         <v>45872</v>
@@ -7477,7 +7489,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="290" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A290" s="5"/>
       <c r="C290" s="9">
         <v>45872</v>
@@ -7495,7 +7507,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="291" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A291" s="5"/>
       <c r="C291" s="9">
         <v>45939</v>
@@ -7513,7 +7525,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="292" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A292" s="5"/>
       <c r="C292" s="9">
         <v>45941</v>
@@ -7531,7 +7543,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="293" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A293" s="5"/>
       <c r="C293" s="9">
         <v>45941</v>
@@ -7549,7 +7561,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="294" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A294" s="5"/>
       <c r="C294" s="9">
         <v>45942</v>
@@ -7567,7 +7579,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="295" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A295" s="5"/>
       <c r="C295" s="9">
         <v>45663</v>
@@ -7585,7 +7597,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="296" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A296" s="5"/>
       <c r="C296" s="61"/>
       <c r="D296" s="13" t="s">
@@ -7601,262 +7613,310 @@
         <v>2</v>
       </c>
     </row>
-    <row r="297" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A297" s="5"/>
-      <c r="C297" s="61"/>
-      <c r="D297" s="13"/>
-      <c r="E297" s="2"/>
-      <c r="F297" s="2"/>
-    </row>
-    <row r="298" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C297" s="61">
+        <v>46052</v>
+      </c>
+      <c r="D297" s="13" t="s">
+        <v>306</v>
+      </c>
+      <c r="E297" s="2">
+        <v>0.50694444444444442</v>
+      </c>
+      <c r="F297" s="2">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="H297" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="298" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A298" s="5"/>
-      <c r="E298" s="2"/>
-      <c r="F298" s="2"/>
-    </row>
-    <row r="299" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A299" s="73" t="s">
+      <c r="C298" s="61">
+        <v>46052</v>
+      </c>
+      <c r="D298" s="13" t="s">
+        <v>306</v>
+      </c>
+      <c r="E298" s="2">
+        <v>0.65416666666666667</v>
+      </c>
+      <c r="F298" s="2">
+        <v>0.70138888888888884</v>
+      </c>
+      <c r="H298" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="299" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A299" s="5"/>
+      <c r="C299" s="61">
+        <v>46061</v>
+      </c>
+      <c r="D299" s="13" t="s">
+        <v>307</v>
+      </c>
+      <c r="E299" s="2">
+        <v>0.8125</v>
+      </c>
+      <c r="F299" s="2">
+        <v>0.88263888888888886</v>
+      </c>
+      <c r="H299" s="14">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="300" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A300" s="5"/>
+      <c r="C300" s="61">
+        <v>46061</v>
+      </c>
+      <c r="D300" s="13" t="s">
+        <v>308</v>
+      </c>
+      <c r="E300" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="F300" s="2">
+        <v>0.93611111111111112</v>
+      </c>
+      <c r="H300" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="301" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A301" s="5"/>
+      <c r="C301" s="61">
+        <v>46061</v>
+      </c>
+      <c r="D301" s="13" t="s">
+        <v>309</v>
+      </c>
+      <c r="E301" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="F301" s="2">
+        <v>0.47222222222222221</v>
+      </c>
+      <c r="H301" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="302" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A302" s="5"/>
+      <c r="C302" s="61"/>
+      <c r="D302" s="13"/>
+      <c r="E302" s="2"/>
+      <c r="F302" s="2"/>
+    </row>
+    <row r="303" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A303" s="5"/>
+      <c r="C303" s="61"/>
+      <c r="D303" s="13"/>
+      <c r="E303" s="2"/>
+      <c r="F303" s="2"/>
+    </row>
+    <row r="304" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A304" s="5"/>
+      <c r="C304" s="61"/>
+      <c r="D304" s="13"/>
+      <c r="E304" s="2"/>
+      <c r="F304" s="2"/>
+    </row>
+    <row r="305" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A305" s="5"/>
+      <c r="E305" s="2"/>
+      <c r="F305" s="2"/>
+    </row>
+    <row r="306" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A306" s="73" t="s">
         <v>83</v>
       </c>
-      <c r="B299" s="73"/>
-      <c r="C299" s="73"/>
-      <c r="D299" s="73"/>
-      <c r="E299" s="73"/>
-      <c r="F299" s="73"/>
-      <c r="G299" s="16">
-        <f>SUM(G2:G298)</f>
+      <c r="B306" s="73"/>
+      <c r="C306" s="73"/>
+      <c r="D306" s="73"/>
+      <c r="E306" s="73"/>
+      <c r="F306" s="73"/>
+      <c r="G306" s="16">
+        <f>SUM(G2:G305)</f>
         <v>314.78999999999996</v>
       </c>
-      <c r="H299" s="16">
-        <f>SUM(H2:H298)</f>
-        <v>111.3</v>
-      </c>
-    </row>
-    <row r="300" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A300" s="73" t="s">
+      <c r="H306" s="16">
+        <f>SUM(H2:H305)</f>
+        <v>117.8</v>
+      </c>
+    </row>
+    <row r="307" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A307" s="73" t="s">
         <v>57</v>
       </c>
-      <c r="B300" s="73"/>
-      <c r="C300" s="73"/>
-      <c r="D300" s="73"/>
-      <c r="E300" s="73"/>
-      <c r="F300" s="73"/>
-      <c r="G300" s="16">
+      <c r="B307" s="73"/>
+      <c r="C307" s="73"/>
+      <c r="D307" s="73"/>
+      <c r="E307" s="73"/>
+      <c r="F307" s="73"/>
+      <c r="G307" s="16">
         <v>200</v>
       </c>
-      <c r="H300" s="16">
+      <c r="H307" s="16">
         <v>300</v>
       </c>
     </row>
-    <row r="301" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A301" s="73" t="s">
+    <row r="308" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A308" s="73" t="s">
         <v>84</v>
       </c>
-      <c r="B301" s="73"/>
-      <c r="C301" s="73"/>
-      <c r="D301" s="73"/>
-      <c r="E301" s="73"/>
-      <c r="F301" s="73"/>
-      <c r="G301" s="17">
-        <f>G300*G299</f>
+      <c r="B308" s="73"/>
+      <c r="C308" s="73"/>
+      <c r="D308" s="73"/>
+      <c r="E308" s="73"/>
+      <c r="F308" s="73"/>
+      <c r="G308" s="17">
+        <f>G307*G306</f>
         <v>62957.999999999993</v>
       </c>
-      <c r="H301" s="18">
-        <f>H300*H299</f>
-        <v>33390</v>
-      </c>
-      <c r="J301">
+      <c r="H308" s="18">
+        <f>H307*H306</f>
+        <v>35340</v>
+      </c>
+      <c r="J308">
         <v>-500</v>
       </c>
     </row>
-    <row r="302" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A302" s="73" t="s">
+    <row r="309" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A309" s="73" t="s">
         <v>58</v>
       </c>
-      <c r="B302" s="73"/>
-      <c r="C302" s="73"/>
-      <c r="D302" s="73"/>
-      <c r="E302" s="73"/>
-      <c r="F302" s="73"/>
-      <c r="G302" s="78">
-        <f>G301+H301</f>
-        <v>96348</v>
-      </c>
-      <c r="H302" s="78"/>
-    </row>
-    <row r="303" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A303" s="10"/>
-      <c r="B303" s="81" t="s">
+      <c r="B309" s="73"/>
+      <c r="C309" s="73"/>
+      <c r="D309" s="73"/>
+      <c r="E309" s="73"/>
+      <c r="F309" s="73"/>
+      <c r="G309" s="78">
+        <f>G308+H308</f>
+        <v>98298</v>
+      </c>
+      <c r="H309" s="78"/>
+    </row>
+    <row r="310" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A310" s="10"/>
+      <c r="B310" s="81" t="s">
         <v>60</v>
       </c>
-      <c r="C303" s="81"/>
-      <c r="D303" s="81"/>
-      <c r="E303" s="81"/>
-      <c r="F303" s="81"/>
-      <c r="G303" s="21"/>
-    </row>
-    <row r="304" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A304" s="11">
+      <c r="C310" s="81"/>
+      <c r="D310" s="81"/>
+      <c r="E310" s="81"/>
+      <c r="F310" s="81"/>
+      <c r="G310" s="21"/>
+    </row>
+    <row r="311" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A311" s="11">
         <v>45109</v>
       </c>
-      <c r="B304" s="82" t="s">
+      <c r="B311" s="82" t="s">
         <v>59</v>
       </c>
-      <c r="C304" s="82"/>
-      <c r="D304" s="82"/>
-      <c r="E304" s="82"/>
-      <c r="F304" s="82"/>
-      <c r="G304" s="83">
+      <c r="C311" s="82"/>
+      <c r="D311" s="82"/>
+      <c r="E311" s="82"/>
+      <c r="F311" s="82"/>
+      <c r="G311" s="83">
         <v>10000</v>
       </c>
-      <c r="H304" s="83"/>
-    </row>
-    <row r="305" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A305" s="11"/>
-      <c r="B305" s="85" t="s">
+      <c r="H311" s="83"/>
+    </row>
+    <row r="312" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A312" s="11"/>
+      <c r="B312" s="85" t="s">
         <v>96</v>
       </c>
-      <c r="C305" s="85"/>
-      <c r="D305" s="85"/>
-      <c r="E305" s="85"/>
-      <c r="F305" s="85"/>
-      <c r="G305" s="83">
+      <c r="C312" s="85"/>
+      <c r="D312" s="85"/>
+      <c r="E312" s="85"/>
+      <c r="F312" s="85"/>
+      <c r="G312" s="83">
         <v>5000</v>
       </c>
-      <c r="H305" s="83"/>
-    </row>
-    <row r="306" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A306" s="11">
+      <c r="H312" s="83"/>
+    </row>
+    <row r="313" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A313" s="11">
         <v>45278</v>
       </c>
-      <c r="B306" s="74" t="s">
+      <c r="B313" s="74" t="s">
         <v>96</v>
       </c>
-      <c r="C306" s="74"/>
-      <c r="D306" s="74"/>
-      <c r="E306" s="74"/>
-      <c r="F306" s="74"/>
-      <c r="G306" s="83">
+      <c r="C313" s="74"/>
+      <c r="D313" s="74"/>
+      <c r="E313" s="74"/>
+      <c r="F313" s="74"/>
+      <c r="G313" s="83">
         <v>9800</v>
       </c>
-      <c r="H306" s="83"/>
-    </row>
-    <row r="307" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A307" s="11"/>
-      <c r="B307" s="74"/>
-      <c r="C307" s="74"/>
-      <c r="D307" s="74"/>
-      <c r="E307" s="74"/>
-      <c r="F307" s="74"/>
-      <c r="G307" s="84"/>
-      <c r="H307" s="84"/>
-    </row>
-    <row r="308" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A308" s="11"/>
-      <c r="B308" s="74"/>
-      <c r="C308" s="74"/>
-      <c r="D308" s="74"/>
-      <c r="E308" s="74"/>
-      <c r="F308" s="74"/>
-      <c r="G308" s="84"/>
-      <c r="H308" s="84"/>
-    </row>
-    <row r="309" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A309" s="11"/>
-      <c r="B309" s="74"/>
-      <c r="C309" s="74"/>
-      <c r="D309" s="74"/>
-      <c r="E309" s="74"/>
-      <c r="F309" s="74"/>
-      <c r="G309" s="84"/>
-      <c r="H309" s="84"/>
-    </row>
-    <row r="310" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A310" s="11"/>
-      <c r="B310" s="74" t="s">
+      <c r="H313" s="83"/>
+    </row>
+    <row r="314" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A314" s="11"/>
+      <c r="B314" s="74"/>
+      <c r="C314" s="74"/>
+      <c r="D314" s="74"/>
+      <c r="E314" s="74"/>
+      <c r="F314" s="74"/>
+      <c r="G314" s="84"/>
+      <c r="H314" s="84"/>
+    </row>
+    <row r="315" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A315" s="11"/>
+      <c r="B315" s="74"/>
+      <c r="C315" s="74"/>
+      <c r="D315" s="74"/>
+      <c r="E315" s="74"/>
+      <c r="F315" s="74"/>
+      <c r="G315" s="84"/>
+      <c r="H315" s="84"/>
+    </row>
+    <row r="316" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A316" s="11"/>
+      <c r="B316" s="74"/>
+      <c r="C316" s="74"/>
+      <c r="D316" s="74"/>
+      <c r="E316" s="74"/>
+      <c r="F316" s="74"/>
+      <c r="G316" s="84"/>
+      <c r="H316" s="84"/>
+    </row>
+    <row r="317" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A317" s="11"/>
+      <c r="B317" s="74" t="s">
         <v>62</v>
       </c>
-      <c r="C310" s="74"/>
-      <c r="D310" s="74"/>
-      <c r="E310" s="74"/>
-      <c r="F310" s="74"/>
-      <c r="G310" s="83">
-        <f>SUM(G304:H309)</f>
+      <c r="C317" s="74"/>
+      <c r="D317" s="74"/>
+      <c r="E317" s="74"/>
+      <c r="F317" s="74"/>
+      <c r="G317" s="83">
+        <f>SUM(G311:H316)</f>
         <v>24800</v>
       </c>
-      <c r="H310" s="83"/>
-    </row>
-    <row r="311" spans="1:8" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A311" s="79" t="s">
+      <c r="H317" s="83"/>
+    </row>
+    <row r="318" spans="1:10" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="A318" s="79" t="s">
         <v>61</v>
       </c>
-      <c r="B311" s="79"/>
-      <c r="C311" s="79"/>
-      <c r="D311" s="79"/>
-      <c r="E311" s="79"/>
-      <c r="F311" s="79"/>
-      <c r="G311" s="80">
-        <f>G302-G310</f>
-        <v>71548</v>
-      </c>
-      <c r="H311" s="80"/>
-    </row>
-    <row r="312" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A312" s="11"/>
-      <c r="B312" s="12"/>
-      <c r="C312" s="12"/>
-      <c r="D312" s="12"/>
-      <c r="E312" s="12"/>
-      <c r="F312" s="12"/>
-    </row>
-    <row r="313" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A313" s="11"/>
-      <c r="B313" s="12"/>
-      <c r="C313" s="12"/>
-      <c r="D313" s="12"/>
-      <c r="E313" s="12"/>
-      <c r="F313" s="12"/>
-    </row>
-    <row r="314" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A314" s="11"/>
-      <c r="B314" s="12"/>
-      <c r="C314" s="12"/>
-      <c r="D314" s="12"/>
-      <c r="E314" s="12"/>
-      <c r="F314" s="12"/>
-    </row>
-    <row r="315" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A315" s="11"/>
-      <c r="B315" s="12"/>
-      <c r="C315" s="12"/>
-      <c r="D315" s="12"/>
-      <c r="E315" s="12"/>
-      <c r="F315" s="12"/>
-    </row>
-    <row r="316" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A316" s="11"/>
-      <c r="B316" s="12"/>
-      <c r="C316" s="12"/>
-      <c r="D316" s="12"/>
-      <c r="E316" s="12"/>
-      <c r="F316" s="12"/>
-    </row>
-    <row r="317" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A317" s="11"/>
-      <c r="B317" s="12"/>
-      <c r="C317" s="12"/>
-      <c r="D317" s="12"/>
-      <c r="E317" s="12"/>
-      <c r="F317" s="12"/>
-    </row>
-    <row r="318" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A318" s="11"/>
-      <c r="B318" s="12"/>
-      <c r="C318" s="12"/>
-      <c r="D318" s="12"/>
-      <c r="E318" s="12"/>
-      <c r="F318" s="12"/>
-    </row>
-    <row r="319" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B318" s="79"/>
+      <c r="C318" s="79"/>
+      <c r="D318" s="79"/>
+      <c r="E318" s="79"/>
+      <c r="F318" s="79"/>
+      <c r="G318" s="80">
+        <f>G309-G317</f>
+        <v>73498</v>
+      </c>
+      <c r="H318" s="80"/>
+    </row>
+    <row r="319" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A319" s="11"/>
       <c r="B319" s="12"/>
       <c r="C319" s="12"/>
@@ -7864,7 +7924,7 @@
       <c r="E319" s="12"/>
       <c r="F319" s="12"/>
     </row>
-    <row r="320" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A320" s="11"/>
       <c r="B320" s="12"/>
       <c r="C320" s="12"/>
@@ -7872,7 +7932,7 @@
       <c r="E320" s="12"/>
       <c r="F320" s="12"/>
     </row>
-    <row r="321" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A321" s="11"/>
       <c r="B321" s="12"/>
       <c r="C321" s="12"/>
@@ -7880,7 +7940,7 @@
       <c r="E321" s="12"/>
       <c r="F321" s="12"/>
     </row>
-    <row r="322" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A322" s="11"/>
       <c r="B322" s="12"/>
       <c r="C322" s="12"/>
@@ -7888,7 +7948,7 @@
       <c r="E322" s="12"/>
       <c r="F322" s="12"/>
     </row>
-    <row r="323" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A323" s="11"/>
       <c r="B323" s="12"/>
       <c r="C323" s="12"/>
@@ -7896,7 +7956,7 @@
       <c r="E323" s="12"/>
       <c r="F323" s="12"/>
     </row>
-    <row r="324" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A324" s="11"/>
       <c r="B324" s="12"/>
       <c r="C324" s="12"/>
@@ -7904,7 +7964,7 @@
       <c r="E324" s="12"/>
       <c r="F324" s="12"/>
     </row>
-    <row r="325" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A325" s="11"/>
       <c r="B325" s="12"/>
       <c r="C325" s="12"/>
@@ -7912,7 +7972,7 @@
       <c r="E325" s="12"/>
       <c r="F325" s="12"/>
     </row>
-    <row r="326" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A326" s="11"/>
       <c r="B326" s="12"/>
       <c r="C326" s="12"/>
@@ -7920,7 +7980,7 @@
       <c r="E326" s="12"/>
       <c r="F326" s="12"/>
     </row>
-    <row r="327" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A327" s="11"/>
       <c r="B327" s="12"/>
       <c r="C327" s="12"/>
@@ -7928,7 +7988,7 @@
       <c r="E327" s="12"/>
       <c r="F327" s="12"/>
     </row>
-    <row r="328" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A328" s="11"/>
       <c r="B328" s="12"/>
       <c r="C328" s="12"/>
@@ -7936,7 +7996,7 @@
       <c r="E328" s="12"/>
       <c r="F328" s="12"/>
     </row>
-    <row r="329" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A329" s="11"/>
       <c r="B329" s="12"/>
       <c r="C329" s="12"/>
@@ -7944,191 +8004,247 @@
       <c r="E329" s="12"/>
       <c r="F329" s="12"/>
     </row>
-    <row r="330" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A330" s="9"/>
-      <c r="B330" s="75" t="s">
+    <row r="330" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A330" s="11"/>
+      <c r="B330" s="12"/>
+      <c r="C330" s="12"/>
+      <c r="D330" s="12"/>
+      <c r="E330" s="12"/>
+      <c r="F330" s="12"/>
+    </row>
+    <row r="331" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A331" s="11"/>
+      <c r="B331" s="12"/>
+      <c r="C331" s="12"/>
+      <c r="D331" s="12"/>
+      <c r="E331" s="12"/>
+      <c r="F331" s="12"/>
+    </row>
+    <row r="332" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A332" s="11"/>
+      <c r="B332" s="12"/>
+      <c r="C332" s="12"/>
+      <c r="D332" s="12"/>
+      <c r="E332" s="12"/>
+      <c r="F332" s="12"/>
+    </row>
+    <row r="333" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A333" s="11"/>
+      <c r="B333" s="12"/>
+      <c r="C333" s="12"/>
+      <c r="D333" s="12"/>
+      <c r="E333" s="12"/>
+      <c r="F333" s="12"/>
+    </row>
+    <row r="334" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A334" s="11"/>
+      <c r="B334" s="12"/>
+      <c r="C334" s="12"/>
+      <c r="D334" s="12"/>
+      <c r="E334" s="12"/>
+      <c r="F334" s="12"/>
+    </row>
+    <row r="335" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A335" s="11"/>
+      <c r="B335" s="12"/>
+      <c r="C335" s="12"/>
+      <c r="D335" s="12"/>
+      <c r="E335" s="12"/>
+      <c r="F335" s="12"/>
+    </row>
+    <row r="336" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A336" s="11"/>
+      <c r="B336" s="12"/>
+      <c r="C336" s="12"/>
+      <c r="D336" s="12"/>
+      <c r="E336" s="12"/>
+      <c r="F336" s="12"/>
+    </row>
+    <row r="337" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A337" s="9"/>
+      <c r="B337" s="75" t="s">
         <v>56</v>
       </c>
-      <c r="C330" s="75"/>
-      <c r="D330" s="75"/>
-      <c r="E330" s="75"/>
-      <c r="F330" s="75"/>
-      <c r="G330" s="20"/>
-      <c r="H330" s="20"/>
-      <c r="I330" s="7">
-        <f>G299+H299</f>
-        <v>426.09</v>
-      </c>
-      <c r="J330" s="7">
-        <f>I330</f>
-        <v>426.09</v>
-      </c>
-    </row>
-    <row r="331" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A331" s="5"/>
-      <c r="B331" s="76" t="s">
+      <c r="C337" s="75"/>
+      <c r="D337" s="75"/>
+      <c r="E337" s="75"/>
+      <c r="F337" s="75"/>
+      <c r="G337" s="20"/>
+      <c r="H337" s="20"/>
+      <c r="I337" s="7">
+        <f>G306+H306</f>
+        <v>432.59</v>
+      </c>
+      <c r="J337" s="7">
+        <f>I337</f>
+        <v>432.59</v>
+      </c>
+    </row>
+    <row r="338" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A338" s="5"/>
+      <c r="B338" s="76" t="s">
         <v>57</v>
       </c>
-      <c r="C331" s="76"/>
-      <c r="D331" s="76"/>
-      <c r="E331" s="76"/>
-      <c r="F331" s="76"/>
-      <c r="I331" s="7">
+      <c r="C338" s="76"/>
+      <c r="D338" s="76"/>
+      <c r="E338" s="76"/>
+      <c r="F338" s="76"/>
+      <c r="I338" s="7">
         <v>300</v>
       </c>
-      <c r="J331" s="7">
+      <c r="J338" s="7">
         <v>200</v>
       </c>
     </row>
-    <row r="332" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A332" s="5"/>
-      <c r="B332" s="76" t="s">
+    <row r="339" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A339" s="5"/>
+      <c r="B339" s="76" t="s">
         <v>58</v>
       </c>
-      <c r="C332" s="76"/>
-      <c r="D332" s="76"/>
-      <c r="E332" s="76"/>
-      <c r="F332" s="76"/>
-      <c r="I332" s="8">
-        <f>I331*I330</f>
-        <v>127826.99999999999</v>
-      </c>
-      <c r="J332" s="8">
-        <f>J331*J330</f>
-        <v>85218</v>
-      </c>
-    </row>
-    <row r="333" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A333" s="22"/>
-      <c r="B333" s="77" t="s">
+      <c r="C339" s="76"/>
+      <c r="D339" s="76"/>
+      <c r="E339" s="76"/>
+      <c r="F339" s="76"/>
+      <c r="I339" s="8">
+        <f>I338*I337</f>
+        <v>129776.99999999999</v>
+      </c>
+      <c r="J339" s="8">
+        <f>J338*J337</f>
+        <v>86518</v>
+      </c>
+    </row>
+    <row r="340" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A340" s="22"/>
+      <c r="B340" s="77" t="s">
         <v>60</v>
       </c>
-      <c r="C333" s="77"/>
-      <c r="D333" s="77"/>
-      <c r="E333" s="77"/>
-      <c r="F333" s="77"/>
-      <c r="G333" s="23"/>
-      <c r="H333" s="23"/>
-      <c r="I333" s="24"/>
-      <c r="J333" s="24"/>
-    </row>
-    <row r="334" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A334" s="25">
+      <c r="C340" s="77"/>
+      <c r="D340" s="77"/>
+      <c r="E340" s="77"/>
+      <c r="F340" s="77"/>
+      <c r="G340" s="23"/>
+      <c r="H340" s="23"/>
+      <c r="I340" s="24"/>
+      <c r="J340" s="24"/>
+    </row>
+    <row r="341" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A341" s="25">
         <v>45109</v>
       </c>
-      <c r="B334" s="71" t="s">
+      <c r="B341" s="71" t="s">
         <v>59</v>
       </c>
-      <c r="C334" s="71"/>
-      <c r="D334" s="71"/>
-      <c r="E334" s="71"/>
-      <c r="F334" s="71"/>
-      <c r="G334" s="26"/>
-      <c r="H334" s="26"/>
-      <c r="I334" s="27">
+      <c r="C341" s="71"/>
+      <c r="D341" s="71"/>
+      <c r="E341" s="71"/>
+      <c r="F341" s="71"/>
+      <c r="G341" s="26"/>
+      <c r="H341" s="26"/>
+      <c r="I341" s="27">
         <v>10000</v>
       </c>
-      <c r="J334" s="27">
+      <c r="J341" s="27">
         <v>10000</v>
       </c>
     </row>
-    <row r="335" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A335" s="25"/>
-      <c r="B335" s="28"/>
-      <c r="C335" s="28"/>
-      <c r="D335" s="28"/>
-      <c r="E335" s="28"/>
-      <c r="F335" s="28"/>
-      <c r="G335" s="26"/>
-      <c r="H335" s="26"/>
-      <c r="I335" s="29"/>
-      <c r="J335" s="29"/>
-    </row>
-    <row r="336" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A336" s="25"/>
-      <c r="B336" s="28"/>
-      <c r="C336" s="28"/>
-      <c r="D336" s="28"/>
-      <c r="E336" s="28"/>
-      <c r="F336" s="28"/>
-      <c r="G336" s="26"/>
-      <c r="H336" s="26"/>
-      <c r="I336" s="29"/>
-      <c r="J336" s="29"/>
-    </row>
-    <row r="337" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A337" s="25"/>
-      <c r="B337" s="72" t="s">
+    <row r="342" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A342" s="25"/>
+      <c r="B342" s="28"/>
+      <c r="C342" s="28"/>
+      <c r="D342" s="28"/>
+      <c r="E342" s="28"/>
+      <c r="F342" s="28"/>
+      <c r="G342" s="26"/>
+      <c r="H342" s="26"/>
+      <c r="I342" s="29"/>
+      <c r="J342" s="29"/>
+    </row>
+    <row r="343" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A343" s="25"/>
+      <c r="B343" s="28"/>
+      <c r="C343" s="28"/>
+      <c r="D343" s="28"/>
+      <c r="E343" s="28"/>
+      <c r="F343" s="28"/>
+      <c r="G343" s="26"/>
+      <c r="H343" s="26"/>
+      <c r="I343" s="29"/>
+      <c r="J343" s="29"/>
+    </row>
+    <row r="344" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A344" s="25"/>
+      <c r="B344" s="72" t="s">
         <v>62</v>
       </c>
-      <c r="C337" s="72"/>
-      <c r="D337" s="72"/>
-      <c r="E337" s="72"/>
-      <c r="F337" s="72"/>
-      <c r="G337" s="26"/>
-      <c r="H337" s="26"/>
-      <c r="I337" s="30">
-        <f>SUM(I334:I336)</f>
+      <c r="C344" s="72"/>
+      <c r="D344" s="72"/>
+      <c r="E344" s="72"/>
+      <c r="F344" s="72"/>
+      <c r="G344" s="26"/>
+      <c r="H344" s="26"/>
+      <c r="I344" s="30">
+        <f>SUM(I341:I343)</f>
         <v>10000</v>
       </c>
-      <c r="J337" s="30">
-        <f>SUM(J334:J336)</f>
+      <c r="J344" s="30">
+        <f>SUM(J341:J343)</f>
         <v>10000</v>
       </c>
     </row>
-    <row r="338" spans="1:10" ht="33.75" x14ac:dyDescent="0.5">
-      <c r="A338" s="31">
+    <row r="345" spans="1:10" ht="33.75" x14ac:dyDescent="0.5">
+      <c r="A345" s="31">
         <v>45109</v>
       </c>
-      <c r="B338" s="70" t="s">
+      <c r="B345" s="70" t="s">
         <v>61</v>
       </c>
-      <c r="C338" s="70"/>
-      <c r="D338" s="70"/>
-      <c r="E338" s="70"/>
-      <c r="F338" s="70"/>
-      <c r="G338" s="32"/>
-      <c r="H338" s="32"/>
-      <c r="I338" s="33">
-        <f>I332-I337</f>
-        <v>117826.99999999999</v>
-      </c>
-      <c r="J338" s="33">
-        <f>J332-J337</f>
-        <v>75218</v>
+      <c r="C345" s="70"/>
+      <c r="D345" s="70"/>
+      <c r="E345" s="70"/>
+      <c r="F345" s="70"/>
+      <c r="G345" s="32"/>
+      <c r="H345" s="32"/>
+      <c r="I345" s="33">
+        <f>I339-I344</f>
+        <v>119776.99999999999</v>
+      </c>
+      <c r="J345" s="33">
+        <f>J339-J344</f>
+        <v>76518</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="G302:H302"/>
-    <mergeCell ref="A311:F311"/>
+    <mergeCell ref="G309:H309"/>
+    <mergeCell ref="A318:F318"/>
+    <mergeCell ref="G318:H318"/>
+    <mergeCell ref="B310:F310"/>
+    <mergeCell ref="B311:F311"/>
+    <mergeCell ref="B317:F317"/>
     <mergeCell ref="G311:H311"/>
-    <mergeCell ref="B303:F303"/>
-    <mergeCell ref="B304:F304"/>
-    <mergeCell ref="B310:F310"/>
-    <mergeCell ref="G304:H304"/>
-    <mergeCell ref="G305:H305"/>
-    <mergeCell ref="G310:H310"/>
-    <mergeCell ref="G307:H307"/>
-    <mergeCell ref="G308:H308"/>
-    <mergeCell ref="G309:H309"/>
-    <mergeCell ref="G306:H306"/>
-    <mergeCell ref="B306:F306"/>
-    <mergeCell ref="B305:F305"/>
-    <mergeCell ref="B307:F307"/>
+    <mergeCell ref="G312:H312"/>
+    <mergeCell ref="G317:H317"/>
+    <mergeCell ref="G314:H314"/>
+    <mergeCell ref="G315:H315"/>
+    <mergeCell ref="G316:H316"/>
+    <mergeCell ref="G313:H313"/>
+    <mergeCell ref="B313:F313"/>
+    <mergeCell ref="B312:F312"/>
+    <mergeCell ref="B314:F314"/>
+    <mergeCell ref="B345:F345"/>
+    <mergeCell ref="B341:F341"/>
+    <mergeCell ref="B344:F344"/>
+    <mergeCell ref="A307:F307"/>
+    <mergeCell ref="A306:F306"/>
+    <mergeCell ref="A308:F308"/>
+    <mergeCell ref="A309:F309"/>
+    <mergeCell ref="B315:F315"/>
+    <mergeCell ref="B316:F316"/>
+    <mergeCell ref="B337:F337"/>
     <mergeCell ref="B338:F338"/>
-    <mergeCell ref="B334:F334"/>
-    <mergeCell ref="B337:F337"/>
-    <mergeCell ref="A300:F300"/>
-    <mergeCell ref="A299:F299"/>
-    <mergeCell ref="A301:F301"/>
-    <mergeCell ref="A302:F302"/>
-    <mergeCell ref="B308:F308"/>
-    <mergeCell ref="B309:F309"/>
-    <mergeCell ref="B330:F330"/>
-    <mergeCell ref="B331:F331"/>
-    <mergeCell ref="B332:F332"/>
-    <mergeCell ref="B333:F333"/>
+    <mergeCell ref="B339:F339"/>
+    <mergeCell ref="B340:F340"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -8139,7 +8255,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3B2F9DB-D849-4B99-B5E6-70BB7408BE44}">
   <dimension ref="A1:D117"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
+    <sheetView topLeftCell="A49" workbookViewId="0">
       <selection activeCell="B76" sqref="B76"/>
     </sheetView>
   </sheetViews>
@@ -8944,10 +9060,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6078F90-1BFA-44D9-9906-5A72B5F0645C}">
-  <dimension ref="A1:D53"/>
+  <dimension ref="A1:D54"/>
   <sheetViews>
     <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9350,47 +9466,56 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="48"/>
+      <c r="A46" s="55">
+        <v>45901</v>
+      </c>
       <c r="B46" s="48"/>
-      <c r="C46" s="54"/>
+      <c r="C46" s="54">
+        <v>2100</v>
+      </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="43"/>
-      <c r="B47" s="43" t="s">
+      <c r="A47" s="48"/>
+      <c r="B47" s="48"/>
+      <c r="C47" s="54"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="43"/>
+      <c r="B48" s="43" t="s">
         <v>252</v>
       </c>
-      <c r="C47" s="46">
-        <f>SUM(C40:C46)</f>
-        <v>15950</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="6"/>
-      <c r="B48" s="6" t="s">
+      <c r="C48" s="46">
+        <f>SUM(C40:C47)</f>
+        <v>18050</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="6"/>
+      <c r="B49" s="6" t="s">
         <v>253</v>
       </c>
-      <c r="C48" s="47">
-        <f>C39-C47</f>
-        <v>2100</v>
-      </c>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B50" s="13" t="s">
+      <c r="C49" s="47">
+        <f>C39-C48</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B51" s="13" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B51" s="13" t="s">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B52" s="13" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B52" s="13" t="s">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B53" s="13" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="53" spans="2:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="B53" s="13" t="s">
+    <row r="54" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B54" s="13" t="s">
         <v>292</v>
       </c>
     </row>

</xml_diff>